<commit_message>
Created Acuity smoke test case TC01-TC08.
Signed-off-by: Sourabh kumar <sourabh@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Firm" sheetId="1" r:id="rId1"/>
     <sheet name="Contact" sheetId="2" r:id="rId2"/>
     <sheet name="Deal" sheetId="3" r:id="rId3"/>
-    <sheet name="Fund" sheetId="4" r:id="rId4"/>
+    <sheet name="Activity Timeline" sheetId="5" r:id="rId4"/>
+    <sheet name="Acuity" sheetId="6" r:id="rId5"/>
+    <sheet name="Fund" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -30,9 +32,6 @@
     <t>Legal_Name</t>
   </si>
   <si>
-    <t>Module 9</t>
-  </si>
-  <si>
     <t>Record_Type</t>
   </si>
   <si>
@@ -103,6 +102,174 @@
   </si>
   <si>
     <t>Contact_EmailId</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Advance_Due_Date</t>
+  </si>
+  <si>
+    <t>Int Task</t>
+  </si>
+  <si>
+    <t>AT_001</t>
+  </si>
+  <si>
+    <t>Related_To</t>
+  </si>
+  <si>
+    <t>Suggested_Tag</t>
+  </si>
+  <si>
+    <t>Int Fund 01&lt;break&gt;</t>
+  </si>
+  <si>
+    <t>For verification of task fund</t>
+  </si>
+  <si>
+    <t>Int Contact2&lt;break&gt;Int Institution&lt;break&gt;Int Deal 01&lt;break&gt;Int Contact3</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>Deals</t>
+  </si>
+  <si>
+    <t>Companies_Count</t>
+  </si>
+  <si>
+    <t>People_Count</t>
+  </si>
+  <si>
+    <t>Deals_Count</t>
+  </si>
+  <si>
+    <t>Int Institution&lt;break&gt;Int Intermediary</t>
+  </si>
+  <si>
+    <t>Int Contact3</t>
+  </si>
+  <si>
+    <t>Int Deal 01</t>
+  </si>
+  <si>
+    <t>Tagged_001</t>
+  </si>
+  <si>
+    <t>Acuity Smoke Record</t>
+  </si>
+  <si>
+    <t>ASRecord2</t>
+  </si>
+  <si>
+    <t>AS_Contact2</t>
+  </si>
+  <si>
+    <t>Int Contact2</t>
+  </si>
+  <si>
+    <t>Int Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tagged </t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Con_001</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Meetings_And_Calls</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>Int Event</t>
+  </si>
+  <si>
+    <t>Int Contact2&lt;break&gt;Int Institution&lt;break&gt;Int Deal 01&lt;break&gt;Int Fund 01&lt;break&gt;Int Contact1</t>
+  </si>
+  <si>
+    <t>Advance_Start_Date</t>
+  </si>
+  <si>
+    <t>Advance_End_Date</t>
+  </si>
+  <si>
+    <t>Int Intermediary</t>
+  </si>
+  <si>
+    <t>New Event</t>
+  </si>
+  <si>
+    <t>New Task</t>
+  </si>
+  <si>
+    <t>AT_002</t>
+  </si>
+  <si>
+    <t>Action_Type</t>
+  </si>
+  <si>
+    <t>ASRecord3</t>
+  </si>
+  <si>
+    <t>For verification of Meeting Firm Intermediary</t>
+  </si>
+  <si>
+    <t>Tagged_002</t>
+  </si>
+  <si>
+    <t>AS_Contact3</t>
+  </si>
+  <si>
+    <t>ASRecord4</t>
+  </si>
+  <si>
+    <t>Con_002</t>
+  </si>
+  <si>
+    <t>AT_003</t>
+  </si>
+  <si>
+    <t>Log a Call</t>
+  </si>
+  <si>
+    <t>Int Call</t>
+  </si>
+  <si>
+    <t>For verification of Activity</t>
+  </si>
+  <si>
+    <t>ASRecord5</t>
+  </si>
+  <si>
+    <t>Tagged_003</t>
+  </si>
+  <si>
+    <t>AS_Contact4</t>
+  </si>
+  <si>
+    <t>ASRecord6</t>
+  </si>
+  <si>
+    <t>Con_003</t>
   </si>
 </sst>
 </file>
@@ -175,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -187,6 +354,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -471,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" activeCellId="2" sqref="A1 B1 B2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,25 +677,65 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -524,10 +749,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,47 +760,75 @@
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="117" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" customWidth="1"/>
+    <col min="5" max="5" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="117" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -585,9 +838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -602,27 +853,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -631,6 +882,310 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="78" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="7" t="str">
+        <f ca="1">TEXT(TODAY()-5,"mm/dd/yyyy")</f>
+        <v>10/06/2022</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="str">
+        <f ca="1">TEXT(TODAY()+15,"mm/dd/yyyy")</f>
+        <v>10/26/2022</v>
+      </c>
+      <c r="I3" t="str">
+        <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
+        <v>11/05/2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="7" t="str">
+        <f ca="1">TEXT(TODAY()-5,"mm/dd/yyyy")</f>
+        <v>10/06/2022</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -652,27 +1207,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Import datasheet and testcase file.
Signed-off-by: Sourabh kumar <sourabh@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -1,30 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A28622-9A62-41E2-B3D3-6E0BD8160387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Firm" sheetId="1" r:id="rId1"/>
     <sheet name="Contact" sheetId="2" r:id="rId2"/>
     <sheet name="Deal" sheetId="3" r:id="rId3"/>
-    <sheet name="Activity Timeline" sheetId="5" r:id="rId4"/>
-    <sheet name="Acuity" sheetId="6" r:id="rId5"/>
-    <sheet name="Fund" sheetId="4" r:id="rId6"/>
+    <sheet name="Deal Team" sheetId="7" r:id="rId4"/>
+    <sheet name="Activity Timeline" sheetId="5" r:id="rId5"/>
+    <sheet name="Acuity" sheetId="6" r:id="rId6"/>
+    <sheet name="Reports" sheetId="8" r:id="rId7"/>
+    <sheet name="Fund" sheetId="4" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="148">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -125,15 +136,9 @@
     <t>Suggested_Tag</t>
   </si>
   <si>
-    <t>Int Fund 01&lt;break&gt;</t>
-  </si>
-  <si>
     <t>For verification of task fund</t>
   </si>
   <si>
-    <t>Int Contact2&lt;break&gt;Int Institution&lt;break&gt;Int Deal 01&lt;break&gt;Int Contact3</t>
-  </si>
-  <si>
     <t>People</t>
   </si>
   <si>
@@ -203,9 +208,6 @@
     <t>Int Event</t>
   </si>
   <si>
-    <t>Int Contact2&lt;break&gt;Int Institution&lt;break&gt;Int Deal 01&lt;break&gt;Int Fund 01&lt;break&gt;Int Contact1</t>
-  </si>
-  <si>
     <t>Advance_Start_Date</t>
   </si>
   <si>
@@ -270,13 +272,220 @@
   </si>
   <si>
     <t>Con_003</t>
+  </si>
+  <si>
+    <t>AT_004</t>
+  </si>
+  <si>
+    <t>Edit Intermediary 02</t>
+  </si>
+  <si>
+    <t>For verification of Task after Edit</t>
+  </si>
+  <si>
+    <t>AT_005</t>
+  </si>
+  <si>
+    <t>View All Task 1</t>
+  </si>
+  <si>
+    <t>For verification of View All link</t>
+  </si>
+  <si>
+    <t>AT_006</t>
+  </si>
+  <si>
+    <t>ASRecord7</t>
+  </si>
+  <si>
+    <t>AT_007</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>+10</t>
+  </si>
+  <si>
+    <t>-10</t>
+  </si>
+  <si>
+    <t>For verification of Call after Edit</t>
+  </si>
+  <si>
+    <t>View All Task 2</t>
+  </si>
+  <si>
+    <t>AT_008</t>
+  </si>
+  <si>
+    <t>AT_009</t>
+  </si>
+  <si>
+    <t>View All Task 1&lt;break&gt;View All Call 1&lt;break&gt;View All Task 2&lt;break&gt;Int Call&lt;break&gt;Int Task</t>
+  </si>
+  <si>
+    <t>ASRecord8</t>
+  </si>
+  <si>
+    <t>Int Institution</t>
+  </si>
+  <si>
+    <t>ASRecord9</t>
+  </si>
+  <si>
+    <t>Tagged_004</t>
+  </si>
+  <si>
+    <t>Int Contact1</t>
+  </si>
+  <si>
+    <t>AT_010</t>
+  </si>
+  <si>
+    <t>Int Call&lt;break&gt;Int Task</t>
+  </si>
+  <si>
+    <t>CS Company</t>
+  </si>
+  <si>
+    <t>ASRecord10</t>
+  </si>
+  <si>
+    <t>CS&lt;break&gt;CS</t>
+  </si>
+  <si>
+    <t>Contact1&lt;break&gt;Contact2</t>
+  </si>
+  <si>
+    <t>CS Company&lt;break&gt;CS ITM</t>
+  </si>
+  <si>
+    <t>1investorportal+CSContact1@gmail.com&lt;break&gt;1investorportal+CSContact2@gmail.com</t>
+  </si>
+  <si>
+    <t>CTO&lt;break&gt;Dev</t>
+  </si>
+  <si>
+    <t>AS_Contact5</t>
+  </si>
+  <si>
+    <t>CS Deal 01</t>
+  </si>
+  <si>
+    <t>NDA Signed</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>DT_001</t>
+  </si>
+  <si>
+    <t>CS Contact1</t>
+  </si>
+  <si>
+    <t>PE Admin</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>AT_011</t>
+  </si>
+  <si>
+    <t>CS Call</t>
+  </si>
+  <si>
+    <t>CS Call 2</t>
+  </si>
+  <si>
+    <t>AT_012</t>
+  </si>
+  <si>
+    <t>For Verification of Contacts Grid</t>
+  </si>
+  <si>
+    <t>Assigned_To</t>
+  </si>
+  <si>
+    <t>CRM User</t>
+  </si>
+  <si>
+    <t>Company&lt;break&gt;Intermediary</t>
+  </si>
+  <si>
+    <t>AS_Deal2</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>ASRecord11</t>
+  </si>
+  <si>
+    <t>Con_004</t>
+  </si>
+  <si>
+    <t>CTO</t>
+  </si>
+  <si>
+    <t>AS_Contact6</t>
+  </si>
+  <si>
+    <t>ASRecord12</t>
+  </si>
+  <si>
+    <t>Company 1&lt;break&gt;Intermediary 1&lt;break&gt;Institution 1</t>
+  </si>
+  <si>
+    <t>Report_Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>R_001</t>
+  </si>
+  <si>
+    <t>Contact with Activities&lt;break&gt;Activities with Firms-SW&lt;break&gt;Fundraisings with Legal Name -SW</t>
+  </si>
+  <si>
+    <t>Shows the details of Activities Touchpoint corresponding to the Contact- System Wide&lt;break&gt;Shows the details of Activities corresponding to the Firm- System Wide&lt;break&gt;Shows the details of Fundraising corresponding to the Firm- System Wide</t>
+  </si>
+  <si>
+    <t>10/20/2022</t>
+  </si>
+  <si>
+    <t>Int Company&lt;Prefilled&gt;&lt;break&gt;Int Contact2&lt;break&gt;Int Institution&lt;break&gt;Int Deal 01&lt;break&gt;Int Contact3</t>
+  </si>
+  <si>
+    <t>Int Company&lt;Prefilled&gt;&lt;break&gt;Int Contact2&lt;break&gt;Int Institution&lt;break&gt;Int Deal 01&lt;break&gt;Int Fund 01&lt;break&gt;Int Contact1</t>
+  </si>
+  <si>
+    <t>Int Company&lt;Prefilled&gt;&lt;break&gt;Int Intermediary&lt;break&gt;Int Institution&lt;break&gt;Int Contact1&lt;break&gt;Int Contact3</t>
+  </si>
+  <si>
+    <t>10/21/2022</t>
+  </si>
+  <si>
+    <t>11/10/2022</t>
+  </si>
+  <si>
+    <t>AS_Contact7</t>
+  </si>
+  <si>
+    <t>View All Call 1</t>
+  </si>
+  <si>
+    <t>CS Contact1&lt;Prefilled&gt;&lt;break&gt;CS Company&lt;break&gt;CS ITM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +517,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -329,7 +544,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -337,12 +552,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,6 +617,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -655,18 +916,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="73.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="58.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -681,11 +942,11 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="A3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -700,72 +961,124 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:C3"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.33203125" customWidth="1"/>
-    <col min="5" max="5" width="49.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="117" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="117" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -776,7 +1089,7 @@
         <v>21</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -784,8 +1097,11 @@
       <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -802,50 +1118,90 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{0F7A85EA-17C3-430A-A99E-090F70355B23}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -874,6 +1230,20 @@
       </c>
       <c r="D2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -882,33 +1252,91 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32909671-21F3-47D8-B15D-836384415519}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="78" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="78" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>26</v>
@@ -919,119 +1347,270 @@
       <c r="E1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>60</v>
-      </c>
       <c r="I1" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="7" t="str">
-        <f ca="1">TEXT(TODAY()-5,"mm/dd/yyyy")</f>
-        <v>10/06/2022</v>
+        <v>140</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
         <v>65</v>
       </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>68</v>
-      </c>
       <c r="E3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" t="s">
         <v>59</v>
       </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <f ca="1">TEXT(TODAY()+15,"mm/dd/yyyy")</f>
-        <v>10/26/2022</v>
-      </c>
-      <c r="I3" t="str">
+        <v>11/15/2022</v>
+      </c>
+      <c r="J3" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>11/05/2022</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11/25/2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
         <v>73</v>
       </c>
-      <c r="B4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" t="s">
-        <v>76</v>
-      </c>
       <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="7" t="str">
-        <f ca="1">TEXT(TODAY()-5,"mm/dd/yyyy")</f>
-        <v>10/06/2022</v>
+        <v>140</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" t="s">
+        <v>147</v>
+      </c>
+      <c r="K12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" t="s">
+        <v>147</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="4.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -1042,34 +1621,34 @@
         <v>10</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="H1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1077,7 +1656,7 @@
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -1090,44 +1669,58 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
         <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
         <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
         <v>41</v>
       </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1135,7 +1728,7 @@
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -1148,10 +1741,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1159,10 +1752,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1170,24 +1763,85 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K15">
         <v>2</v>
       </c>
     </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" t="s">
+        <v>115</v>
+      </c>
+      <c r="I16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212A931B-B5A0-4D20-AB7B-9542993AD90C}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="72.21875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -1195,11 +1849,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Acuity Deals & Emails and deal team
Signed-off-by: sahil <sbansal@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845D9BFC-F1F1-4AB3-93B1-DDA3C5E4E19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Firm" sheetId="1" r:id="rId1"/>
     <sheet name="Research" sheetId="9" r:id="rId2"/>
     <sheet name="Contact" sheetId="2" r:id="rId3"/>
     <sheet name="Deal" sheetId="3" r:id="rId4"/>
-    <sheet name="Deal Team" sheetId="7" r:id="rId5"/>
-    <sheet name="Activity Timeline" sheetId="5" r:id="rId6"/>
-    <sheet name="Acuity" sheetId="6" r:id="rId7"/>
-    <sheet name="Reports" sheetId="8" r:id="rId8"/>
-    <sheet name="Fund" sheetId="4" r:id="rId9"/>
-    <sheet name="Fundraisings" sheetId="10" r:id="rId10"/>
+    <sheet name="Deals" sheetId="11" r:id="rId5"/>
+    <sheet name="Deal Team" sheetId="7" r:id="rId6"/>
+    <sheet name="Activity Timeline" sheetId="5" r:id="rId7"/>
+    <sheet name="Acuity" sheetId="6" r:id="rId8"/>
+    <sheet name="Reports" sheetId="8" r:id="rId9"/>
+    <sheet name="Fund" sheetId="4" r:id="rId10"/>
+    <sheet name="Fundraisings" sheetId="10" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="383">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -805,12 +805,393 @@
   </si>
   <si>
     <t>FDKRT01&lt;Break&gt;MKDRT01&lt;Break&gt;FDKRT01</t>
+  </si>
+  <si>
+    <t>Acuity Deals &amp; Email</t>
+  </si>
+  <si>
+    <t>ADEIns1</t>
+  </si>
+  <si>
+    <t>ADETestCom</t>
+  </si>
+  <si>
+    <t>ADETestAdvisor</t>
+  </si>
+  <si>
+    <t>ADETestInsti</t>
+  </si>
+  <si>
+    <t>ADETestInt</t>
+  </si>
+  <si>
+    <t>ADETestL</t>
+  </si>
+  <si>
+    <t>ADETestPC</t>
+  </si>
+  <si>
+    <t>ADETestLP</t>
+  </si>
+  <si>
+    <t>ADEIns2</t>
+  </si>
+  <si>
+    <t>ADEIns3</t>
+  </si>
+  <si>
+    <t>ADEIns4</t>
+  </si>
+  <si>
+    <t>ADEIns5</t>
+  </si>
+  <si>
+    <t>ADEIns6</t>
+  </si>
+  <si>
+    <t>ADEIns7</t>
+  </si>
+  <si>
+    <t>Advisor</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>Intermediary</t>
+  </si>
+  <si>
+    <t>Lender</t>
+  </si>
+  <si>
+    <t>Limited Partner</t>
+  </si>
+  <si>
+    <t>Portfolio Company</t>
+  </si>
+  <si>
+    <t>Parent_Institution</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>TC 1</t>
+  </si>
+  <si>
+    <t>TC 5</t>
+  </si>
+  <si>
+    <t>TC 6</t>
+  </si>
+  <si>
+    <t>TC 7</t>
+  </si>
+  <si>
+    <t>TC 8</t>
+  </si>
+  <si>
+    <t>TC 9</t>
+  </si>
+  <si>
+    <t>ADEContact1</t>
+  </si>
+  <si>
+    <t>ADEContact2</t>
+  </si>
+  <si>
+    <t>ADEContact3</t>
+  </si>
+  <si>
+    <t>ADEContact4</t>
+  </si>
+  <si>
+    <t>ADEContact5</t>
+  </si>
+  <si>
+    <t>ADEContact6</t>
+  </si>
+  <si>
+    <t>ADEContact7</t>
+  </si>
+  <si>
+    <t>navatariptesting+43991@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+86328@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+33546@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+49956@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+63716@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+26759@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+47344@gmail.com</t>
+  </si>
+  <si>
+    <t>ADETest</t>
+  </si>
+  <si>
+    <t>ADEIns8</t>
+  </si>
+  <si>
+    <t>ADEIns9</t>
+  </si>
+  <si>
+    <t>OGCOM</t>
+  </si>
+  <si>
+    <t>OGINT</t>
+  </si>
+  <si>
+    <t>ADEContact8</t>
+  </si>
+  <si>
+    <t>TC 10</t>
+  </si>
+  <si>
+    <t>navatariptesting+1115@gmail.com</t>
+  </si>
+  <si>
+    <t>ADEDeal1</t>
+  </si>
+  <si>
+    <t>ADEDeal2</t>
+  </si>
+  <si>
+    <t>ADEDeal3</t>
+  </si>
+  <si>
+    <t>ADEDeal4</t>
+  </si>
+  <si>
+    <t>ADEDeal5</t>
+  </si>
+  <si>
+    <t>ADEDeal6</t>
+  </si>
+  <si>
+    <t>ADEDeal7</t>
+  </si>
+  <si>
+    <t>ADEDeal8</t>
+  </si>
+  <si>
+    <t>ADEDeal9</t>
+  </si>
+  <si>
+    <t>ADEDeal10</t>
+  </si>
+  <si>
+    <t>ADEDeal11</t>
+  </si>
+  <si>
+    <t>ADEDeal12</t>
+  </si>
+  <si>
+    <t>ADEDeal13</t>
+  </si>
+  <si>
+    <t>ADEDeal14</t>
+  </si>
+  <si>
+    <t>ADEDeal15</t>
+  </si>
+  <si>
+    <t>ADEDeal16</t>
+  </si>
+  <si>
+    <t>ADEDeal17</t>
+  </si>
+  <si>
+    <t>ADEDeal18</t>
+  </si>
+  <si>
+    <t>ADEMD</t>
+  </si>
+  <si>
+    <t>ADEMD1</t>
+  </si>
+  <si>
+    <t>ADEMD2</t>
+  </si>
+  <si>
+    <t>ADEMD3</t>
+  </si>
+  <si>
+    <t>ADEMD4</t>
+  </si>
+  <si>
+    <t>ADEMD5</t>
+  </si>
+  <si>
+    <t>ADEMD6</t>
+  </si>
+  <si>
+    <t>ADEMD7</t>
+  </si>
+  <si>
+    <t>ADEMD8</t>
+  </si>
+  <si>
+    <t>ADEMD9</t>
+  </si>
+  <si>
+    <t>ADEMD10</t>
+  </si>
+  <si>
+    <t>ADEMD11</t>
+  </si>
+  <si>
+    <t>ADEMD12</t>
+  </si>
+  <si>
+    <t>ADEMD13</t>
+  </si>
+  <si>
+    <t>ADEMD14</t>
+  </si>
+  <si>
+    <t>ADEMD15</t>
+  </si>
+  <si>
+    <t>ADEMD16</t>
+  </si>
+  <si>
+    <t>ADEMD17</t>
+  </si>
+  <si>
+    <t>Deal Received</t>
+  </si>
+  <si>
+    <t>Management Meeting</t>
+  </si>
+  <si>
+    <t>IOI</t>
+  </si>
+  <si>
+    <t>LOI</t>
+  </si>
+  <si>
+    <t>Due Diligence</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Declined/dead</t>
+  </si>
+  <si>
+    <t>ADETestInt&lt;Break&gt;ADETest TC 5&lt;Break&gt;11/02/2022</t>
+  </si>
+  <si>
+    <t>Company_Name</t>
+  </si>
+  <si>
+    <t>Source_Contact</t>
+  </si>
+  <si>
+    <t>Source_Firm</t>
+  </si>
+  <si>
+    <t>Date Received</t>
+  </si>
+  <si>
+    <t>Investment_Size</t>
+  </si>
+  <si>
+    <t>Updated_Stage</t>
+  </si>
+  <si>
+    <t>Updated_Investment_Size</t>
+  </si>
+  <si>
+    <t>Pipeline_Comments</t>
+  </si>
+  <si>
+    <t>Ashish TC 5</t>
+  </si>
+  <si>
+    <t>ADEMD&lt;Section&gt;ADEMD2&lt;Section&gt;ADEMD3&lt;Section&gt;ADEMD4&lt;Section&gt;ADEMD5&lt;Section&gt;ADEMD6&lt;Section&gt;ADEMD7&lt;Section&gt;ADEMD8&lt;Section&gt;ADEMD9&lt;Section&gt;ADEMD10&lt;Section&gt;ADEMD11&lt;Section&gt;ADEMD12&lt;Section&gt;ADEMD13&lt;Section&gt;ADEMD14&lt;Section&gt;ADEMD15&lt;Section&gt;ADEMD16&lt;Section&gt;ADEMD17&lt;Section&gt;ADEMD18</t>
+  </si>
+  <si>
+    <t>ADETestCom&lt;Section&gt;ADETestCom&lt;Section&gt;ADETestCom&lt;Section&gt;ADETestCom&lt;Section&gt;ADETestInt&lt;Section&gt;ADETestInt&lt;Section&gt;ADETestCom&lt;Section&gt;ADETestCom&lt;Section&gt;ADETestCom&lt;Section&gt;ADETestInt&lt;Section&gt;ADETestInt&lt;Section&gt;ADETestInt&lt;Section&gt;ADETestInt&lt;Section&gt;ADETestInt&lt;Section&gt;ADETestInt&lt;Section&gt;ADETestInt&lt;Section&gt;ADETestInt&lt;Section&gt;ADETestInt</t>
+  </si>
+  <si>
+    <t>Deal Received&lt;Section&gt;NDA Signed&lt;Section&gt;Management Meeting&lt;Section&gt;IOI&lt;Section&gt;LOI&lt;Section&gt;Due Diligence&lt;Section&gt;Closed&lt;Section&gt;Parked&lt;Section&gt;Declined/dead&lt;Section&gt;Deal Received&lt;Section&gt;NDA Signed&lt;Section&gt;Management Meeting&lt;Section&gt;IOI&lt;Section&gt;LOI&lt;Section&gt;Due Diligence&lt;Section&gt;Closed&lt;Section&gt;Parked&lt;Section&gt;Declined/dead</t>
+  </si>
+  <si>
+    <t>ADE1</t>
+  </si>
+  <si>
+    <t>ADE2</t>
+  </si>
+  <si>
+    <t>ADE3</t>
+  </si>
+  <si>
+    <t>ADE4</t>
+  </si>
+  <si>
+    <t>ADE5</t>
+  </si>
+  <si>
+    <t>ADE6</t>
+  </si>
+  <si>
+    <t>ADE7</t>
+  </si>
+  <si>
+    <t>ADE8</t>
+  </si>
+  <si>
+    <t>ADE9</t>
+  </si>
+  <si>
+    <t>ADE10</t>
+  </si>
+  <si>
+    <t>ADE11</t>
+  </si>
+  <si>
+    <t>ADE12</t>
+  </si>
+  <si>
+    <t>ADE13</t>
+  </si>
+  <si>
+    <t>ADE14</t>
+  </si>
+  <si>
+    <t>ADE15</t>
+  </si>
+  <si>
+    <t>ADE16</t>
+  </si>
+  <si>
+    <t>ADE17</t>
+  </si>
+  <si>
+    <t>ADE18</t>
+  </si>
+  <si>
+    <t>Date Received&lt;Section&gt;Date Received&lt;Section&gt;Date Received&lt;Section&gt;Date Received&lt;Section&gt;Date Received&lt;Section&gt;Date Received&lt;Section&gt;Date Received&lt;Section&gt;Date Received&lt;Section&gt;Date Received&lt;Section&gt;Source Contact&lt;Break&gt;Date Received&lt;Section&gt;Source Contact&lt;Break&gt;Date Received&lt;Section&gt;Source Contact&lt;Break&gt;Date Received&lt;Section&gt;Source Contact&lt;Break&gt;Date Received&lt;Section&gt;Source Contact&lt;Break&gt;Date Received&lt;Section&gt;Source Contact&lt;Break&gt;Date Received&lt;Section&gt;Source Contact&lt;Break&gt;Date Received&lt;Section&gt;Source Contact&lt;Break&gt;Date Received&lt;Section&gt;Source Contact&lt;Break&gt;Date Received</t>
+  </si>
+  <si>
+    <t>11/02/2022&lt;Section&gt;11/02/2022&lt;Section&gt;11/02/2022&lt;Section&gt;11/02/2022&lt;Section&gt;11/02/2022&lt;Section&gt;11/02/2022&lt;Section&gt;11/02/2022&lt;Section&gt;11/02/2022&lt;Section&gt;11/02/2022&lt;Section&gt;ADETest TC 5&lt;Break&gt;11/02/2022&lt;Section&gt;ADETest TC 5&lt;Break&gt;11/02/2022&lt;Section&gt;ADETest TC 5&lt;Break&gt;11/02/2022&lt;Section&gt;ADETest TC 5&lt;Break&gt;11/02/2022&lt;Section&gt;ADETest TC 5&lt;Break&gt;11/02/2022&lt;Section&gt;ADETest TC 5&lt;Break&gt;11/02/2022&lt;Section&gt;ADETest TC 5&lt;Break&gt;11/02/2022&lt;Section&gt;ADETest TC 5&lt;Break&gt;11/02/2022&lt;Section&gt;ADETest TC 5&lt;Break&gt;11/02/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -883,7 +1264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -921,13 +1302,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -980,20 +1390,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{11AC1A27-91D3-46F1-A4BA-05D7AA9092AC}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1270,21 +1688,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="73.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="58.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="73.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="58.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1300,15 +1718,18 @@
       <c r="E1" s="21" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+      <c r="F1" s="22" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1319,7 +1740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1327,7 +1748,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1335,7 +1756,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -1343,7 +1764,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -1351,7 +1772,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1359,7 +1780,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -1367,7 +1788,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -1375,7 +1796,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -1383,7 +1804,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -1394,7 +1815,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -1402,7 +1823,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>132</v>
       </c>
@@ -1410,7 +1831,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>158</v>
       </c>
@@ -1421,7 +1842,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>159</v>
       </c>
@@ -1430,7 +1851,7 @@
       </c>
       <c r="C17" s="23"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>160</v>
       </c>
@@ -1439,7 +1860,7 @@
       </c>
       <c r="C18" s="23"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>161</v>
       </c>
@@ -1452,7 +1873,7 @@
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>162</v>
       </c>
@@ -1469,9 +1890,119 @@
         <v>157</v>
       </c>
     </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>257</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>265</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="C25" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>266</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="C26" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="C27" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>268</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="C28" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>269</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="C29" t="s">
+        <v>275</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>270</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>300</v>
+      </c>
+      <c r="B31" t="s">
+        <v>302</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>301</v>
+      </c>
+      <c r="B32" t="s">
+        <v>303</v>
+      </c>
+      <c r="C32" t="s">
+        <v>273</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A23:C23"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1480,41 +2011,137 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174A1CF7-C343-4C2D-9E58-8686B8DBD504}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.1796875" customWidth="1"/>
-    <col min="11" max="11" width="10.90625" customWidth="1"/>
-    <col min="12" max="12" width="24.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>236</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -1529,37 +2156,37 @@
       <c r="H1" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="24" t="s">
         <v>27</v>
       </c>
       <c r="N1" s="21" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26" t="s">
+    <row r="3" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>243</v>
       </c>
@@ -1587,7 +2214,7 @@
       <c r="M4" s="23"/>
       <c r="N4" s="23"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>248</v>
       </c>
@@ -1607,7 +2234,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>250</v>
       </c>
@@ -1642,20 +2269,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA987EBB-87FF-40D2-A16B-E969B1367C61}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1663,13 +2290,13 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="24"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="32"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>167</v>
       </c>
@@ -1677,7 +2304,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>169</v>
       </c>
@@ -1685,7 +2312,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>171</v>
       </c>
@@ -1693,7 +2320,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>173</v>
       </c>
@@ -1701,7 +2328,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>175</v>
       </c>
@@ -1718,24 +2345,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="45.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.36328125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="117" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="117" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="31.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1754,17 +2385,20 @@
       <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1780,8 +2414,9 @@
       <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1789,7 +2424,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1797,7 +2432,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -1805,7 +2440,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -1821,11 +2456,12 @@
       <c r="F6" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -1833,7 +2469,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -1841,7 +2477,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>185</v>
       </c>
@@ -1859,14 +2495,15 @@
         <v>180</v>
       </c>
       <c r="G9" s="23"/>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="23"/>
+      <c r="I9" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="J9" s="23" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>191</v>
       </c>
@@ -1880,8 +2517,9 @@
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10" s="23"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>195</v>
       </c>
@@ -1895,8 +2533,9 @@
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11" s="23"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>196</v>
       </c>
@@ -1912,14 +2551,15 @@
         <v>188</v>
       </c>
       <c r="G12" s="23"/>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="23"/>
+      <c r="I12" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="J12" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>197</v>
       </c>
@@ -1937,34 +2577,183 @@
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+    </row>
+    <row r="16" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>285</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="F17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>286</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="F18" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>287</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="F19" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>288</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="F20" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>289</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="F21" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>290</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="F22" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>291</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>304</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="F24" t="s">
+        <v>306</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A16:C16"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="F6" r:id="rId2" xr:uid="{0F7A85EA-17C3-430A-A99E-090F70355B23}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F6" r:id="rId2"/>
+    <hyperlink ref="F23" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="49.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1990,7 +2779,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2004,7 +2793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -2018,7 +2807,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>203</v>
       </c>
@@ -2042,7 +2831,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>205</v>
       </c>
@@ -2056,7 +2845,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>211</v>
       </c>
@@ -2075,6 +2864,386 @@
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B8" t="s">
+        <v>360</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="F8" t="s">
+        <v>381</v>
+      </c>
+      <c r="G8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>363</v>
+      </c>
+      <c r="B10" t="s">
+        <v>360</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="F10" t="s">
+        <v>354</v>
+      </c>
+      <c r="G10" s="7">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>364</v>
+      </c>
+      <c r="B11" t="s">
+        <v>326</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" t="s">
+        <v>354</v>
+      </c>
+      <c r="G11" s="7">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>365</v>
+      </c>
+      <c r="B12" t="s">
+        <v>327</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="F12" t="s">
+        <v>354</v>
+      </c>
+      <c r="G12" s="7">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>366</v>
+      </c>
+      <c r="B13" t="s">
+        <v>328</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="F13" t="s">
+        <v>354</v>
+      </c>
+      <c r="G13" s="7">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>367</v>
+      </c>
+      <c r="B14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="F14" t="s">
+        <v>354</v>
+      </c>
+      <c r="G14" s="7">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>368</v>
+      </c>
+      <c r="B15" t="s">
+        <v>330</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="F15" t="s">
+        <v>354</v>
+      </c>
+      <c r="G15" s="7">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>369</v>
+      </c>
+      <c r="B16" t="s">
+        <v>331</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="F16" t="s">
+        <v>354</v>
+      </c>
+      <c r="G16" s="7">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>370</v>
+      </c>
+      <c r="B17" t="s">
+        <v>332</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="F17" t="s">
+        <v>354</v>
+      </c>
+      <c r="G17" s="7">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>371</v>
+      </c>
+      <c r="B18" t="s">
+        <v>333</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="F18" t="s">
+        <v>354</v>
+      </c>
+      <c r="G18" s="7">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>372</v>
+      </c>
+      <c r="B19" t="s">
+        <v>334</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="F19" t="s">
+        <v>200</v>
+      </c>
+      <c r="G19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>373</v>
+      </c>
+      <c r="B20" t="s">
+        <v>335</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" t="s">
+        <v>200</v>
+      </c>
+      <c r="G20" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>374</v>
+      </c>
+      <c r="B21" t="s">
+        <v>336</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="F21" t="s">
+        <v>200</v>
+      </c>
+      <c r="G21" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>375</v>
+      </c>
+      <c r="B22" t="s">
+        <v>337</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="F22" t="s">
+        <v>200</v>
+      </c>
+      <c r="G22" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>376</v>
+      </c>
+      <c r="B23" t="s">
+        <v>338</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="F23" t="s">
+        <v>200</v>
+      </c>
+      <c r="G23" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>377</v>
+      </c>
+      <c r="B24" t="s">
+        <v>339</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="F24" t="s">
+        <v>200</v>
+      </c>
+      <c r="G24" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>378</v>
+      </c>
+      <c r="B25" t="s">
+        <v>340</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="F25" t="s">
+        <v>200</v>
+      </c>
+      <c r="G25" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>379</v>
+      </c>
+      <c r="B26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="F26" t="s">
+        <v>200</v>
+      </c>
+      <c r="G26" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>380</v>
+      </c>
+      <c r="B27" t="s">
+        <v>342</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="F27" t="s">
+        <v>200</v>
+      </c>
+      <c r="G27" t="s">
+        <v>350</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2083,23 +3252,1412 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32909671-21F3-47D8-B15D-836384415519}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMO19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1029" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="30"/>
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30"/>
+      <c r="BN1" s="30"/>
+      <c r="BO1" s="30"/>
+      <c r="BP1" s="30"/>
+      <c r="BQ1" s="30"/>
+      <c r="BR1" s="30"/>
+      <c r="BS1" s="30"/>
+      <c r="BT1" s="30"/>
+      <c r="BU1" s="30"/>
+      <c r="BV1" s="30"/>
+      <c r="BW1" s="30"/>
+      <c r="BX1" s="30"/>
+      <c r="BY1" s="30"/>
+      <c r="BZ1" s="30"/>
+      <c r="CA1" s="30"/>
+      <c r="CB1" s="30"/>
+      <c r="CC1" s="30"/>
+      <c r="CD1" s="30"/>
+      <c r="CE1" s="30"/>
+      <c r="CF1" s="30"/>
+      <c r="CG1" s="30"/>
+      <c r="CH1" s="30"/>
+      <c r="CI1" s="30"/>
+      <c r="CJ1" s="30"/>
+      <c r="CK1" s="30"/>
+      <c r="CL1" s="30"/>
+      <c r="CM1" s="30"/>
+      <c r="CN1" s="30"/>
+      <c r="CO1" s="30"/>
+      <c r="CP1" s="30"/>
+      <c r="CQ1" s="30"/>
+      <c r="CR1" s="30"/>
+      <c r="CS1" s="30"/>
+      <c r="CT1" s="30"/>
+      <c r="CU1" s="30"/>
+      <c r="CV1" s="30"/>
+      <c r="CW1" s="30"/>
+      <c r="CX1" s="30"/>
+      <c r="CY1" s="30"/>
+      <c r="CZ1" s="30"/>
+      <c r="DA1" s="30"/>
+      <c r="DB1" s="30"/>
+      <c r="DC1" s="30"/>
+      <c r="DD1" s="30"/>
+      <c r="DE1" s="30"/>
+      <c r="DF1" s="30"/>
+      <c r="DG1" s="30"/>
+      <c r="DH1" s="30"/>
+      <c r="DI1" s="30"/>
+      <c r="DJ1" s="30"/>
+      <c r="DK1" s="30"/>
+      <c r="DL1" s="30"/>
+      <c r="DM1" s="30"/>
+      <c r="DN1" s="30"/>
+      <c r="DO1" s="30"/>
+      <c r="DP1" s="30"/>
+      <c r="DQ1" s="30"/>
+      <c r="DR1" s="30"/>
+      <c r="DS1" s="30"/>
+      <c r="DT1" s="30"/>
+      <c r="DU1" s="30"/>
+      <c r="DV1" s="30"/>
+      <c r="DW1" s="30"/>
+      <c r="DX1" s="30"/>
+      <c r="DY1" s="30"/>
+      <c r="DZ1" s="30"/>
+      <c r="EA1" s="30"/>
+      <c r="EB1" s="30"/>
+      <c r="EC1" s="30"/>
+      <c r="ED1" s="30"/>
+      <c r="EE1" s="30"/>
+      <c r="EF1" s="30"/>
+      <c r="EG1" s="30"/>
+      <c r="EH1" s="30"/>
+      <c r="EI1" s="30"/>
+      <c r="EJ1" s="30"/>
+      <c r="EK1" s="30"/>
+      <c r="EL1" s="30"/>
+      <c r="EM1" s="30"/>
+      <c r="EN1" s="30"/>
+      <c r="EO1" s="30"/>
+      <c r="EP1" s="30"/>
+      <c r="EQ1" s="30"/>
+      <c r="ER1" s="30"/>
+      <c r="ES1" s="30"/>
+      <c r="ET1" s="30"/>
+      <c r="EU1" s="30"/>
+      <c r="EV1" s="30"/>
+      <c r="EW1" s="30"/>
+      <c r="EX1" s="30"/>
+      <c r="EY1" s="30"/>
+      <c r="EZ1" s="30"/>
+      <c r="FA1" s="30"/>
+      <c r="FB1" s="30"/>
+      <c r="FC1" s="30"/>
+      <c r="FD1" s="30"/>
+      <c r="FE1" s="30"/>
+      <c r="FF1" s="30"/>
+      <c r="FG1" s="30"/>
+      <c r="FH1" s="30"/>
+      <c r="FI1" s="30"/>
+      <c r="FJ1" s="30"/>
+      <c r="FK1" s="30"/>
+      <c r="FL1" s="30"/>
+      <c r="FM1" s="30"/>
+      <c r="FN1" s="30"/>
+      <c r="FO1" s="30"/>
+      <c r="FP1" s="30"/>
+      <c r="FQ1" s="30"/>
+      <c r="FR1" s="30"/>
+      <c r="FS1" s="30"/>
+      <c r="FT1" s="30"/>
+      <c r="FU1" s="30"/>
+      <c r="FV1" s="30"/>
+      <c r="FW1" s="30"/>
+      <c r="FX1" s="30"/>
+      <c r="FY1" s="30"/>
+      <c r="FZ1" s="30"/>
+      <c r="GA1" s="30"/>
+      <c r="GB1" s="30"/>
+      <c r="GC1" s="30"/>
+      <c r="GD1" s="30"/>
+      <c r="GE1" s="30"/>
+      <c r="GF1" s="30"/>
+      <c r="GG1" s="30"/>
+      <c r="GH1" s="30"/>
+      <c r="GI1" s="30"/>
+      <c r="GJ1" s="30"/>
+      <c r="GK1" s="30"/>
+      <c r="GL1" s="30"/>
+      <c r="GM1" s="30"/>
+      <c r="GN1" s="30"/>
+      <c r="GO1" s="30"/>
+      <c r="GP1" s="30"/>
+      <c r="GQ1" s="30"/>
+      <c r="GR1" s="30"/>
+      <c r="GS1" s="30"/>
+      <c r="GT1" s="30"/>
+      <c r="GU1" s="30"/>
+      <c r="GV1" s="30"/>
+      <c r="GW1" s="30"/>
+      <c r="GX1" s="30"/>
+      <c r="GY1" s="30"/>
+      <c r="GZ1" s="30"/>
+      <c r="HA1" s="30"/>
+      <c r="HB1" s="30"/>
+      <c r="HC1" s="30"/>
+      <c r="HD1" s="30"/>
+      <c r="HE1" s="30"/>
+      <c r="HF1" s="30"/>
+      <c r="HG1" s="30"/>
+      <c r="HH1" s="30"/>
+      <c r="HI1" s="30"/>
+      <c r="HJ1" s="30"/>
+      <c r="HK1" s="30"/>
+      <c r="HL1" s="30"/>
+      <c r="HM1" s="30"/>
+      <c r="HN1" s="30"/>
+      <c r="HO1" s="30"/>
+      <c r="HP1" s="30"/>
+      <c r="HQ1" s="30"/>
+      <c r="HR1" s="30"/>
+      <c r="HS1" s="30"/>
+      <c r="HT1" s="30"/>
+      <c r="HU1" s="30"/>
+      <c r="HV1" s="30"/>
+      <c r="HW1" s="30"/>
+      <c r="HX1" s="30"/>
+      <c r="HY1" s="30"/>
+      <c r="HZ1" s="30"/>
+      <c r="IA1" s="30"/>
+      <c r="IB1" s="30"/>
+      <c r="IC1" s="30"/>
+      <c r="ID1" s="30"/>
+      <c r="IE1" s="30"/>
+      <c r="IF1" s="30"/>
+      <c r="IG1" s="30"/>
+      <c r="IH1" s="30"/>
+      <c r="II1" s="30"/>
+      <c r="IJ1" s="30"/>
+      <c r="IK1" s="30"/>
+      <c r="IL1" s="30"/>
+      <c r="IM1" s="30"/>
+      <c r="IN1" s="30"/>
+      <c r="IO1" s="30"/>
+      <c r="IP1" s="30"/>
+      <c r="IQ1" s="30"/>
+      <c r="IR1" s="30"/>
+      <c r="IS1" s="30"/>
+      <c r="IT1" s="30"/>
+      <c r="IU1" s="30"/>
+      <c r="IV1" s="30"/>
+      <c r="IW1" s="30"/>
+      <c r="IX1" s="30"/>
+      <c r="IY1" s="30"/>
+      <c r="IZ1" s="30"/>
+      <c r="JA1" s="30"/>
+      <c r="JB1" s="30"/>
+      <c r="JC1" s="30"/>
+      <c r="JD1" s="30"/>
+      <c r="JE1" s="30"/>
+      <c r="JF1" s="30"/>
+      <c r="JG1" s="30"/>
+      <c r="JH1" s="30"/>
+      <c r="JI1" s="30"/>
+      <c r="JJ1" s="30"/>
+      <c r="JK1" s="30"/>
+      <c r="JL1" s="30"/>
+      <c r="JM1" s="30"/>
+      <c r="JN1" s="30"/>
+      <c r="JO1" s="30"/>
+      <c r="JP1" s="30"/>
+      <c r="JQ1" s="30"/>
+      <c r="JR1" s="30"/>
+      <c r="JS1" s="30"/>
+      <c r="JT1" s="30"/>
+      <c r="JU1" s="30"/>
+      <c r="JV1" s="30"/>
+      <c r="JW1" s="30"/>
+      <c r="JX1" s="30"/>
+      <c r="JY1" s="30"/>
+      <c r="JZ1" s="30"/>
+      <c r="KA1" s="30"/>
+      <c r="KB1" s="30"/>
+      <c r="KC1" s="30"/>
+      <c r="KD1" s="30"/>
+      <c r="KE1" s="30"/>
+      <c r="KF1" s="30"/>
+      <c r="KG1" s="30"/>
+      <c r="KH1" s="30"/>
+      <c r="KI1" s="30"/>
+      <c r="KJ1" s="30"/>
+      <c r="KK1" s="30"/>
+      <c r="KL1" s="30"/>
+      <c r="KM1" s="30"/>
+      <c r="KN1" s="30"/>
+      <c r="KO1" s="30"/>
+      <c r="KP1" s="30"/>
+      <c r="KQ1" s="30"/>
+      <c r="KR1" s="30"/>
+      <c r="KS1" s="30"/>
+      <c r="KT1" s="30"/>
+      <c r="KU1" s="30"/>
+      <c r="KV1" s="30"/>
+      <c r="KW1" s="30"/>
+      <c r="KX1" s="30"/>
+      <c r="KY1" s="30"/>
+      <c r="KZ1" s="30"/>
+      <c r="LA1" s="30"/>
+      <c r="LB1" s="30"/>
+      <c r="LC1" s="30"/>
+      <c r="LD1" s="30"/>
+      <c r="LE1" s="30"/>
+      <c r="LF1" s="30"/>
+      <c r="LG1" s="30"/>
+      <c r="LH1" s="30"/>
+      <c r="LI1" s="30"/>
+      <c r="LJ1" s="30"/>
+      <c r="LK1" s="30"/>
+      <c r="LL1" s="30"/>
+      <c r="LM1" s="30"/>
+      <c r="LN1" s="30"/>
+      <c r="LO1" s="30"/>
+      <c r="LP1" s="30"/>
+      <c r="LQ1" s="30"/>
+      <c r="LR1" s="30"/>
+      <c r="LS1" s="30"/>
+      <c r="LT1" s="30"/>
+      <c r="LU1" s="30"/>
+      <c r="LV1" s="30"/>
+      <c r="LW1" s="30"/>
+      <c r="LX1" s="30"/>
+      <c r="LY1" s="30"/>
+      <c r="LZ1" s="30"/>
+      <c r="MA1" s="30"/>
+      <c r="MB1" s="30"/>
+      <c r="MC1" s="30"/>
+      <c r="MD1" s="30"/>
+      <c r="ME1" s="30"/>
+      <c r="MF1" s="30"/>
+      <c r="MG1" s="30"/>
+      <c r="MH1" s="30"/>
+      <c r="MI1" s="30"/>
+      <c r="MJ1" s="30"/>
+      <c r="MK1" s="30"/>
+      <c r="ML1" s="30"/>
+      <c r="MM1" s="30"/>
+      <c r="MN1" s="30"/>
+      <c r="MO1" s="30"/>
+      <c r="MP1" s="30"/>
+      <c r="MQ1" s="30"/>
+      <c r="MR1" s="30"/>
+      <c r="MS1" s="30"/>
+      <c r="MT1" s="30"/>
+      <c r="MU1" s="30"/>
+      <c r="MV1" s="30"/>
+      <c r="MW1" s="30"/>
+      <c r="MX1" s="30"/>
+      <c r="MY1" s="30"/>
+      <c r="MZ1" s="30"/>
+      <c r="NA1" s="30"/>
+      <c r="NB1" s="30"/>
+      <c r="NC1" s="30"/>
+      <c r="ND1" s="30"/>
+      <c r="NE1" s="30"/>
+      <c r="NF1" s="30"/>
+      <c r="NG1" s="30"/>
+      <c r="NH1" s="30"/>
+      <c r="NI1" s="30"/>
+      <c r="NJ1" s="30"/>
+      <c r="NK1" s="30"/>
+      <c r="NL1" s="30"/>
+      <c r="NM1" s="30"/>
+      <c r="NN1" s="30"/>
+      <c r="NO1" s="30"/>
+      <c r="NP1" s="30"/>
+      <c r="NQ1" s="30"/>
+      <c r="NR1" s="30"/>
+      <c r="NS1" s="30"/>
+      <c r="NT1" s="30"/>
+      <c r="NU1" s="30"/>
+      <c r="NV1" s="30"/>
+      <c r="NW1" s="30"/>
+      <c r="NX1" s="30"/>
+      <c r="NY1" s="30"/>
+      <c r="NZ1" s="30"/>
+      <c r="OA1" s="30"/>
+      <c r="OB1" s="30"/>
+      <c r="OC1" s="30"/>
+      <c r="OD1" s="30"/>
+      <c r="OE1" s="30"/>
+      <c r="OF1" s="30"/>
+      <c r="OG1" s="30"/>
+      <c r="OH1" s="30"/>
+      <c r="OI1" s="30"/>
+      <c r="OJ1" s="30"/>
+      <c r="OK1" s="30"/>
+      <c r="OL1" s="30"/>
+      <c r="OM1" s="30"/>
+      <c r="ON1" s="30"/>
+      <c r="OO1" s="30"/>
+      <c r="OP1" s="30"/>
+      <c r="OQ1" s="30"/>
+      <c r="OR1" s="30"/>
+      <c r="OS1" s="30"/>
+      <c r="OT1" s="30"/>
+      <c r="OU1" s="30"/>
+      <c r="OV1" s="30"/>
+      <c r="OW1" s="30"/>
+      <c r="OX1" s="30"/>
+      <c r="OY1" s="30"/>
+      <c r="OZ1" s="30"/>
+      <c r="PA1" s="30"/>
+      <c r="PB1" s="30"/>
+      <c r="PC1" s="30"/>
+      <c r="PD1" s="30"/>
+      <c r="PE1" s="30"/>
+      <c r="PF1" s="30"/>
+      <c r="PG1" s="30"/>
+      <c r="PH1" s="30"/>
+      <c r="PI1" s="30"/>
+      <c r="PJ1" s="30"/>
+      <c r="PK1" s="30"/>
+      <c r="PL1" s="30"/>
+      <c r="PM1" s="30"/>
+      <c r="PN1" s="30"/>
+      <c r="PO1" s="30"/>
+      <c r="PP1" s="30"/>
+      <c r="PQ1" s="30"/>
+      <c r="PR1" s="30"/>
+      <c r="PS1" s="30"/>
+      <c r="PT1" s="30"/>
+      <c r="PU1" s="30"/>
+      <c r="PV1" s="30"/>
+      <c r="PW1" s="30"/>
+      <c r="PX1" s="30"/>
+      <c r="PY1" s="30"/>
+      <c r="PZ1" s="30"/>
+      <c r="QA1" s="30"/>
+      <c r="QB1" s="30"/>
+      <c r="QC1" s="30"/>
+      <c r="QD1" s="30"/>
+      <c r="QE1" s="30"/>
+      <c r="QF1" s="30"/>
+      <c r="QG1" s="30"/>
+      <c r="QH1" s="30"/>
+      <c r="QI1" s="30"/>
+      <c r="QJ1" s="30"/>
+      <c r="QK1" s="30"/>
+      <c r="QL1" s="30"/>
+      <c r="QM1" s="30"/>
+      <c r="QN1" s="30"/>
+      <c r="QO1" s="30"/>
+      <c r="QP1" s="30"/>
+      <c r="QQ1" s="30"/>
+      <c r="QR1" s="30"/>
+      <c r="QS1" s="30"/>
+      <c r="QT1" s="30"/>
+      <c r="QU1" s="30"/>
+      <c r="QV1" s="30"/>
+      <c r="QW1" s="30"/>
+      <c r="QX1" s="30"/>
+      <c r="QY1" s="30"/>
+      <c r="QZ1" s="30"/>
+      <c r="RA1" s="30"/>
+      <c r="RB1" s="30"/>
+      <c r="RC1" s="30"/>
+      <c r="RD1" s="30"/>
+      <c r="RE1" s="30"/>
+      <c r="RF1" s="30"/>
+      <c r="RG1" s="30"/>
+      <c r="RH1" s="30"/>
+      <c r="RI1" s="30"/>
+      <c r="RJ1" s="30"/>
+      <c r="RK1" s="30"/>
+      <c r="RL1" s="30"/>
+      <c r="RM1" s="30"/>
+      <c r="RN1" s="30"/>
+      <c r="RO1" s="30"/>
+      <c r="RP1" s="30"/>
+      <c r="RQ1" s="30"/>
+      <c r="RR1" s="30"/>
+      <c r="RS1" s="30"/>
+      <c r="RT1" s="30"/>
+      <c r="RU1" s="30"/>
+      <c r="RV1" s="30"/>
+      <c r="RW1" s="30"/>
+      <c r="RX1" s="30"/>
+      <c r="RY1" s="30"/>
+      <c r="RZ1" s="30"/>
+      <c r="SA1" s="30"/>
+      <c r="SB1" s="30"/>
+      <c r="SC1" s="30"/>
+      <c r="SD1" s="30"/>
+      <c r="SE1" s="30"/>
+      <c r="SF1" s="30"/>
+      <c r="SG1" s="30"/>
+      <c r="SH1" s="30"/>
+      <c r="SI1" s="30"/>
+      <c r="SJ1" s="30"/>
+      <c r="SK1" s="30"/>
+      <c r="SL1" s="30"/>
+      <c r="SM1" s="30"/>
+      <c r="SN1" s="30"/>
+      <c r="SO1" s="30"/>
+      <c r="SP1" s="30"/>
+      <c r="SQ1" s="30"/>
+      <c r="SR1" s="30"/>
+      <c r="SS1" s="30"/>
+      <c r="ST1" s="30"/>
+      <c r="SU1" s="30"/>
+      <c r="SV1" s="30"/>
+      <c r="SW1" s="30"/>
+      <c r="SX1" s="30"/>
+      <c r="SY1" s="30"/>
+      <c r="SZ1" s="30"/>
+      <c r="TA1" s="30"/>
+      <c r="TB1" s="30"/>
+      <c r="TC1" s="30"/>
+      <c r="TD1" s="30"/>
+      <c r="TE1" s="30"/>
+      <c r="TF1" s="30"/>
+      <c r="TG1" s="30"/>
+      <c r="TH1" s="30"/>
+      <c r="TI1" s="30"/>
+      <c r="TJ1" s="30"/>
+      <c r="TK1" s="30"/>
+      <c r="TL1" s="30"/>
+      <c r="TM1" s="30"/>
+      <c r="TN1" s="30"/>
+      <c r="TO1" s="30"/>
+      <c r="TP1" s="30"/>
+      <c r="TQ1" s="30"/>
+      <c r="TR1" s="30"/>
+      <c r="TS1" s="30"/>
+      <c r="TT1" s="30"/>
+      <c r="TU1" s="30"/>
+      <c r="TV1" s="30"/>
+      <c r="TW1" s="30"/>
+      <c r="TX1" s="30"/>
+      <c r="TY1" s="30"/>
+      <c r="TZ1" s="30"/>
+      <c r="UA1" s="30"/>
+      <c r="UB1" s="30"/>
+      <c r="UC1" s="30"/>
+      <c r="UD1" s="30"/>
+      <c r="UE1" s="30"/>
+      <c r="UF1" s="30"/>
+      <c r="UG1" s="30"/>
+      <c r="UH1" s="30"/>
+      <c r="UI1" s="30"/>
+      <c r="UJ1" s="30"/>
+      <c r="UK1" s="30"/>
+      <c r="UL1" s="30"/>
+      <c r="UM1" s="30"/>
+      <c r="UN1" s="30"/>
+      <c r="UO1" s="30"/>
+      <c r="UP1" s="30"/>
+      <c r="UQ1" s="30"/>
+      <c r="UR1" s="30"/>
+      <c r="US1" s="30"/>
+      <c r="UT1" s="30"/>
+      <c r="UU1" s="30"/>
+      <c r="UV1" s="30"/>
+      <c r="UW1" s="30"/>
+      <c r="UX1" s="30"/>
+      <c r="UY1" s="30"/>
+      <c r="UZ1" s="30"/>
+      <c r="VA1" s="30"/>
+      <c r="VB1" s="30"/>
+      <c r="VC1" s="30"/>
+      <c r="VD1" s="30"/>
+      <c r="VE1" s="30"/>
+      <c r="VF1" s="30"/>
+      <c r="VG1" s="30"/>
+      <c r="VH1" s="30"/>
+      <c r="VI1" s="30"/>
+      <c r="VJ1" s="30"/>
+      <c r="VK1" s="30"/>
+      <c r="VL1" s="30"/>
+      <c r="VM1" s="30"/>
+      <c r="VN1" s="30"/>
+      <c r="VO1" s="30"/>
+      <c r="VP1" s="30"/>
+      <c r="VQ1" s="30"/>
+      <c r="VR1" s="30"/>
+      <c r="VS1" s="30"/>
+      <c r="VT1" s="30"/>
+      <c r="VU1" s="30"/>
+      <c r="VV1" s="30"/>
+      <c r="VW1" s="30"/>
+      <c r="VX1" s="30"/>
+      <c r="VY1" s="30"/>
+      <c r="VZ1" s="30"/>
+      <c r="WA1" s="30"/>
+      <c r="WB1" s="30"/>
+      <c r="WC1" s="30"/>
+      <c r="WD1" s="30"/>
+      <c r="WE1" s="30"/>
+      <c r="WF1" s="30"/>
+      <c r="WG1" s="30"/>
+      <c r="WH1" s="30"/>
+      <c r="WI1" s="30"/>
+      <c r="WJ1" s="30"/>
+      <c r="WK1" s="30"/>
+      <c r="WL1" s="30"/>
+      <c r="WM1" s="30"/>
+      <c r="WN1" s="30"/>
+      <c r="WO1" s="30"/>
+      <c r="WP1" s="30"/>
+      <c r="WQ1" s="30"/>
+      <c r="WR1" s="30"/>
+      <c r="WS1" s="30"/>
+      <c r="WT1" s="30"/>
+      <c r="WU1" s="30"/>
+      <c r="WV1" s="30"/>
+      <c r="WW1" s="30"/>
+      <c r="WX1" s="30"/>
+      <c r="WY1" s="30"/>
+      <c r="WZ1" s="30"/>
+      <c r="XA1" s="30"/>
+      <c r="XB1" s="30"/>
+      <c r="XC1" s="30"/>
+      <c r="XD1" s="30"/>
+      <c r="XE1" s="30"/>
+      <c r="XF1" s="30"/>
+      <c r="XG1" s="30"/>
+      <c r="XH1" s="30"/>
+      <c r="XI1" s="30"/>
+      <c r="XJ1" s="30"/>
+      <c r="XK1" s="30"/>
+      <c r="XL1" s="30"/>
+      <c r="XM1" s="30"/>
+      <c r="XN1" s="30"/>
+      <c r="XO1" s="30"/>
+      <c r="XP1" s="30"/>
+      <c r="XQ1" s="30"/>
+      <c r="XR1" s="30"/>
+      <c r="XS1" s="30"/>
+      <c r="XT1" s="30"/>
+      <c r="XU1" s="30"/>
+      <c r="XV1" s="30"/>
+      <c r="XW1" s="30"/>
+      <c r="XX1" s="30"/>
+      <c r="XY1" s="30"/>
+      <c r="XZ1" s="30"/>
+      <c r="YA1" s="30"/>
+      <c r="YB1" s="30"/>
+      <c r="YC1" s="30"/>
+      <c r="YD1" s="30"/>
+      <c r="YE1" s="30"/>
+      <c r="YF1" s="30"/>
+      <c r="YG1" s="30"/>
+      <c r="YH1" s="30"/>
+      <c r="YI1" s="30"/>
+      <c r="YJ1" s="30"/>
+      <c r="YK1" s="30"/>
+      <c r="YL1" s="30"/>
+      <c r="YM1" s="30"/>
+      <c r="YN1" s="30"/>
+      <c r="YO1" s="30"/>
+      <c r="YP1" s="30"/>
+      <c r="YQ1" s="30"/>
+      <c r="YR1" s="30"/>
+      <c r="YS1" s="30"/>
+      <c r="YT1" s="30"/>
+      <c r="YU1" s="30"/>
+      <c r="YV1" s="30"/>
+      <c r="YW1" s="30"/>
+      <c r="YX1" s="30"/>
+      <c r="YY1" s="30"/>
+      <c r="YZ1" s="30"/>
+      <c r="ZA1" s="30"/>
+      <c r="ZB1" s="30"/>
+      <c r="ZC1" s="30"/>
+      <c r="ZD1" s="30"/>
+      <c r="ZE1" s="30"/>
+      <c r="ZF1" s="30"/>
+      <c r="ZG1" s="30"/>
+      <c r="ZH1" s="30"/>
+      <c r="ZI1" s="30"/>
+      <c r="ZJ1" s="30"/>
+      <c r="ZK1" s="30"/>
+      <c r="ZL1" s="30"/>
+      <c r="ZM1" s="30"/>
+      <c r="ZN1" s="30"/>
+      <c r="ZO1" s="30"/>
+      <c r="ZP1" s="30"/>
+      <c r="ZQ1" s="30"/>
+      <c r="ZR1" s="30"/>
+      <c r="ZS1" s="30"/>
+      <c r="ZT1" s="30"/>
+      <c r="ZU1" s="30"/>
+      <c r="ZV1" s="30"/>
+      <c r="ZW1" s="30"/>
+      <c r="ZX1" s="30"/>
+      <c r="ZY1" s="30"/>
+      <c r="ZZ1" s="30"/>
+      <c r="AAA1" s="30"/>
+      <c r="AAB1" s="30"/>
+      <c r="AAC1" s="30"/>
+      <c r="AAD1" s="30"/>
+      <c r="AAE1" s="30"/>
+      <c r="AAF1" s="30"/>
+      <c r="AAG1" s="30"/>
+      <c r="AAH1" s="30"/>
+      <c r="AAI1" s="30"/>
+      <c r="AAJ1" s="30"/>
+      <c r="AAK1" s="30"/>
+      <c r="AAL1" s="30"/>
+      <c r="AAM1" s="30"/>
+      <c r="AAN1" s="30"/>
+      <c r="AAO1" s="30"/>
+      <c r="AAP1" s="30"/>
+      <c r="AAQ1" s="30"/>
+      <c r="AAR1" s="30"/>
+      <c r="AAS1" s="30"/>
+      <c r="AAT1" s="30"/>
+      <c r="AAU1" s="30"/>
+      <c r="AAV1" s="30"/>
+      <c r="AAW1" s="30"/>
+      <c r="AAX1" s="30"/>
+      <c r="AAY1" s="30"/>
+      <c r="AAZ1" s="30"/>
+      <c r="ABA1" s="30"/>
+      <c r="ABB1" s="30"/>
+      <c r="ABC1" s="30"/>
+      <c r="ABD1" s="30"/>
+      <c r="ABE1" s="30"/>
+      <c r="ABF1" s="30"/>
+      <c r="ABG1" s="30"/>
+      <c r="ABH1" s="30"/>
+      <c r="ABI1" s="30"/>
+      <c r="ABJ1" s="30"/>
+      <c r="ABK1" s="30"/>
+      <c r="ABL1" s="30"/>
+      <c r="ABM1" s="30"/>
+      <c r="ABN1" s="30"/>
+      <c r="ABO1" s="30"/>
+      <c r="ABP1" s="30"/>
+      <c r="ABQ1" s="30"/>
+      <c r="ABR1" s="30"/>
+      <c r="ABS1" s="30"/>
+      <c r="ABT1" s="30"/>
+      <c r="ABU1" s="30"/>
+      <c r="ABV1" s="30"/>
+      <c r="ABW1" s="30"/>
+      <c r="ABX1" s="30"/>
+      <c r="ABY1" s="30"/>
+      <c r="ABZ1" s="30"/>
+      <c r="ACA1" s="30"/>
+      <c r="ACB1" s="30"/>
+      <c r="ACC1" s="30"/>
+      <c r="ACD1" s="30"/>
+      <c r="ACE1" s="30"/>
+      <c r="ACF1" s="30"/>
+      <c r="ACG1" s="30"/>
+      <c r="ACH1" s="30"/>
+      <c r="ACI1" s="30"/>
+      <c r="ACJ1" s="30"/>
+      <c r="ACK1" s="30"/>
+      <c r="ACL1" s="30"/>
+      <c r="ACM1" s="30"/>
+      <c r="ACN1" s="30"/>
+      <c r="ACO1" s="30"/>
+      <c r="ACP1" s="30"/>
+      <c r="ACQ1" s="30"/>
+      <c r="ACR1" s="30"/>
+      <c r="ACS1" s="30"/>
+      <c r="ACT1" s="30"/>
+      <c r="ACU1" s="30"/>
+      <c r="ACV1" s="30"/>
+      <c r="ACW1" s="30"/>
+      <c r="ACX1" s="30"/>
+      <c r="ACY1" s="30"/>
+      <c r="ACZ1" s="30"/>
+      <c r="ADA1" s="30"/>
+      <c r="ADB1" s="30"/>
+      <c r="ADC1" s="30"/>
+      <c r="ADD1" s="30"/>
+      <c r="ADE1" s="30"/>
+      <c r="ADF1" s="30"/>
+      <c r="ADG1" s="30"/>
+      <c r="ADH1" s="30"/>
+      <c r="ADI1" s="30"/>
+      <c r="ADJ1" s="30"/>
+      <c r="ADK1" s="30"/>
+      <c r="ADL1" s="30"/>
+      <c r="ADM1" s="30"/>
+      <c r="ADN1" s="30"/>
+      <c r="ADO1" s="30"/>
+      <c r="ADP1" s="30"/>
+      <c r="ADQ1" s="30"/>
+      <c r="ADR1" s="30"/>
+      <c r="ADS1" s="30"/>
+      <c r="ADT1" s="30"/>
+      <c r="ADU1" s="30"/>
+      <c r="ADV1" s="30"/>
+      <c r="ADW1" s="30"/>
+      <c r="ADX1" s="30"/>
+      <c r="ADY1" s="30"/>
+      <c r="ADZ1" s="30"/>
+      <c r="AEA1" s="30"/>
+      <c r="AEB1" s="30"/>
+      <c r="AEC1" s="30"/>
+      <c r="AED1" s="30"/>
+      <c r="AEE1" s="30"/>
+      <c r="AEF1" s="30"/>
+      <c r="AEG1" s="30"/>
+      <c r="AEH1" s="30"/>
+      <c r="AEI1" s="30"/>
+      <c r="AEJ1" s="30"/>
+      <c r="AEK1" s="30"/>
+      <c r="AEL1" s="30"/>
+      <c r="AEM1" s="30"/>
+      <c r="AEN1" s="30"/>
+      <c r="AEO1" s="30"/>
+      <c r="AEP1" s="30"/>
+      <c r="AEQ1" s="30"/>
+      <c r="AER1" s="30"/>
+      <c r="AES1" s="30"/>
+      <c r="AET1" s="30"/>
+      <c r="AEU1" s="30"/>
+      <c r="AEV1" s="30"/>
+      <c r="AEW1" s="30"/>
+      <c r="AEX1" s="30"/>
+      <c r="AEY1" s="30"/>
+      <c r="AEZ1" s="30"/>
+      <c r="AFA1" s="30"/>
+      <c r="AFB1" s="30"/>
+      <c r="AFC1" s="30"/>
+      <c r="AFD1" s="30"/>
+      <c r="AFE1" s="30"/>
+      <c r="AFF1" s="30"/>
+      <c r="AFG1" s="30"/>
+      <c r="AFH1" s="30"/>
+      <c r="AFI1" s="30"/>
+      <c r="AFJ1" s="30"/>
+      <c r="AFK1" s="30"/>
+      <c r="AFL1" s="30"/>
+      <c r="AFM1" s="30"/>
+      <c r="AFN1" s="30"/>
+      <c r="AFO1" s="30"/>
+      <c r="AFP1" s="30"/>
+      <c r="AFQ1" s="30"/>
+      <c r="AFR1" s="30"/>
+      <c r="AFS1" s="30"/>
+      <c r="AFT1" s="30"/>
+      <c r="AFU1" s="30"/>
+      <c r="AFV1" s="30"/>
+      <c r="AFW1" s="30"/>
+      <c r="AFX1" s="30"/>
+      <c r="AFY1" s="30"/>
+      <c r="AFZ1" s="30"/>
+      <c r="AGA1" s="30"/>
+      <c r="AGB1" s="30"/>
+      <c r="AGC1" s="30"/>
+      <c r="AGD1" s="30"/>
+      <c r="AGE1" s="30"/>
+      <c r="AGF1" s="30"/>
+      <c r="AGG1" s="30"/>
+      <c r="AGH1" s="30"/>
+      <c r="AGI1" s="30"/>
+      <c r="AGJ1" s="30"/>
+      <c r="AGK1" s="30"/>
+      <c r="AGL1" s="30"/>
+      <c r="AGM1" s="30"/>
+      <c r="AGN1" s="30"/>
+      <c r="AGO1" s="30"/>
+      <c r="AGP1" s="30"/>
+      <c r="AGQ1" s="30"/>
+      <c r="AGR1" s="30"/>
+      <c r="AGS1" s="30"/>
+      <c r="AGT1" s="30"/>
+      <c r="AGU1" s="30"/>
+      <c r="AGV1" s="30"/>
+      <c r="AGW1" s="30"/>
+      <c r="AGX1" s="30"/>
+      <c r="AGY1" s="30"/>
+      <c r="AGZ1" s="30"/>
+      <c r="AHA1" s="30"/>
+      <c r="AHB1" s="30"/>
+      <c r="AHC1" s="30"/>
+      <c r="AHD1" s="30"/>
+      <c r="AHE1" s="30"/>
+      <c r="AHF1" s="30"/>
+      <c r="AHG1" s="30"/>
+      <c r="AHH1" s="30"/>
+      <c r="AHI1" s="30"/>
+      <c r="AHJ1" s="30"/>
+      <c r="AHK1" s="30"/>
+      <c r="AHL1" s="30"/>
+      <c r="AHM1" s="30"/>
+      <c r="AHN1" s="30"/>
+      <c r="AHO1" s="30"/>
+      <c r="AHP1" s="30"/>
+      <c r="AHQ1" s="30"/>
+      <c r="AHR1" s="30"/>
+      <c r="AHS1" s="30"/>
+      <c r="AHT1" s="30"/>
+      <c r="AHU1" s="30"/>
+      <c r="AHV1" s="30"/>
+      <c r="AHW1" s="30"/>
+      <c r="AHX1" s="30"/>
+      <c r="AHY1" s="30"/>
+      <c r="AHZ1" s="30"/>
+      <c r="AIA1" s="30"/>
+      <c r="AIB1" s="30"/>
+      <c r="AIC1" s="30"/>
+      <c r="AID1" s="30"/>
+      <c r="AIE1" s="30"/>
+      <c r="AIF1" s="30"/>
+      <c r="AIG1" s="30"/>
+      <c r="AIH1" s="30"/>
+      <c r="AII1" s="30"/>
+      <c r="AIJ1" s="30"/>
+      <c r="AIK1" s="30"/>
+      <c r="AIL1" s="30"/>
+      <c r="AIM1" s="30"/>
+      <c r="AIN1" s="30"/>
+      <c r="AIO1" s="30"/>
+      <c r="AIP1" s="30"/>
+      <c r="AIQ1" s="30"/>
+      <c r="AIR1" s="30"/>
+      <c r="AIS1" s="30"/>
+      <c r="AIT1" s="30"/>
+      <c r="AIU1" s="30"/>
+      <c r="AIV1" s="30"/>
+      <c r="AIW1" s="30"/>
+      <c r="AIX1" s="30"/>
+      <c r="AIY1" s="30"/>
+      <c r="AIZ1" s="30"/>
+      <c r="AJA1" s="30"/>
+      <c r="AJB1" s="30"/>
+      <c r="AJC1" s="30"/>
+      <c r="AJD1" s="30"/>
+      <c r="AJE1" s="30"/>
+      <c r="AJF1" s="30"/>
+      <c r="AJG1" s="30"/>
+      <c r="AJH1" s="30"/>
+      <c r="AJI1" s="30"/>
+      <c r="AJJ1" s="30"/>
+      <c r="AJK1" s="30"/>
+      <c r="AJL1" s="30"/>
+      <c r="AJM1" s="30"/>
+      <c r="AJN1" s="30"/>
+      <c r="AJO1" s="30"/>
+      <c r="AJP1" s="30"/>
+      <c r="AJQ1" s="30"/>
+      <c r="AJR1" s="30"/>
+      <c r="AJS1" s="30"/>
+      <c r="AJT1" s="30"/>
+      <c r="AJU1" s="30"/>
+      <c r="AJV1" s="30"/>
+      <c r="AJW1" s="30"/>
+      <c r="AJX1" s="30"/>
+      <c r="AJY1" s="30"/>
+      <c r="AJZ1" s="30"/>
+      <c r="AKA1" s="30"/>
+      <c r="AKB1" s="30"/>
+      <c r="AKC1" s="30"/>
+      <c r="AKD1" s="30"/>
+      <c r="AKE1" s="30"/>
+      <c r="AKF1" s="30"/>
+      <c r="AKG1" s="30"/>
+      <c r="AKH1" s="30"/>
+      <c r="AKI1" s="30"/>
+      <c r="AKJ1" s="30"/>
+      <c r="AKK1" s="30"/>
+      <c r="AKL1" s="30"/>
+      <c r="AKM1" s="30"/>
+      <c r="AKN1" s="30"/>
+      <c r="AKO1" s="30"/>
+      <c r="AKP1" s="30"/>
+      <c r="AKQ1" s="30"/>
+      <c r="AKR1" s="30"/>
+      <c r="AKS1" s="30"/>
+      <c r="AKT1" s="30"/>
+      <c r="AKU1" s="30"/>
+      <c r="AKV1" s="30"/>
+      <c r="AKW1" s="30"/>
+      <c r="AKX1" s="30"/>
+      <c r="AKY1" s="30"/>
+      <c r="AKZ1" s="30"/>
+      <c r="ALA1" s="30"/>
+      <c r="ALB1" s="30"/>
+      <c r="ALC1" s="30"/>
+      <c r="ALD1" s="30"/>
+      <c r="ALE1" s="30"/>
+      <c r="ALF1" s="30"/>
+      <c r="ALG1" s="30"/>
+      <c r="ALH1" s="30"/>
+      <c r="ALI1" s="30"/>
+      <c r="ALJ1" s="30"/>
+      <c r="ALK1" s="30"/>
+      <c r="ALL1" s="30"/>
+      <c r="ALM1" s="30"/>
+      <c r="ALN1" s="30"/>
+      <c r="ALO1" s="30"/>
+      <c r="ALP1" s="30"/>
+      <c r="ALQ1" s="30"/>
+      <c r="ALR1" s="30"/>
+      <c r="ALS1" s="30"/>
+      <c r="ALT1" s="30"/>
+      <c r="ALU1" s="30"/>
+      <c r="ALV1" s="30"/>
+      <c r="ALW1" s="30"/>
+      <c r="ALX1" s="30"/>
+      <c r="ALY1" s="30"/>
+      <c r="ALZ1" s="30"/>
+      <c r="AMA1" s="30"/>
+      <c r="AMB1" s="30"/>
+      <c r="AMC1" s="30"/>
+      <c r="AMD1" s="30"/>
+      <c r="AME1" s="30"/>
+      <c r="AMF1" s="30"/>
+      <c r="AMG1" s="30"/>
+      <c r="AMH1" s="30"/>
+      <c r="AMI1" s="30"/>
+      <c r="AMJ1" s="30"/>
+      <c r="AMK1" s="30"/>
+      <c r="AML1" s="30"/>
+      <c r="AMM1" s="30"/>
+      <c r="AMN1" s="30"/>
+      <c r="AMO1" s="30"/>
+    </row>
+    <row r="2" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B6" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B8" t="s">
+        <v>331</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>314</v>
+      </c>
+      <c r="B9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>315</v>
+      </c>
+      <c r="B10" t="s">
+        <v>333</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>316</v>
+      </c>
+      <c r="B11" t="s">
+        <v>334</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="E11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>317</v>
+      </c>
+      <c r="B12" t="s">
+        <v>335</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" t="s">
+        <v>359</v>
+      </c>
+      <c r="F12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>318</v>
+      </c>
+      <c r="B13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="E13" t="s">
+        <v>359</v>
+      </c>
+      <c r="F13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>319</v>
+      </c>
+      <c r="B14" t="s">
+        <v>337</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="E14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>320</v>
+      </c>
+      <c r="B15" t="s">
+        <v>338</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="E15" t="s">
+        <v>359</v>
+      </c>
+      <c r="F15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1029" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" t="s">
+        <v>339</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="E16" t="s">
+        <v>359</v>
+      </c>
+      <c r="F16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>322</v>
+      </c>
+      <c r="B17" t="s">
+        <v>340</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="E17" t="s">
+        <v>359</v>
+      </c>
+      <c r="F17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>323</v>
+      </c>
+      <c r="B18" t="s">
+        <v>341</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="E18" t="s">
+        <v>359</v>
+      </c>
+      <c r="F18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>324</v>
+      </c>
+      <c r="B19" t="s">
+        <v>342</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="E19" t="s">
+        <v>359</v>
+      </c>
+      <c r="F19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -2116,7 +4674,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -2139,8 +4697,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
@@ -2148,21 +4706,21 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="78" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.453125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2197,7 +4755,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -2223,7 +4781,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -2244,14 +4802,14 @@
       </c>
       <c r="H3" t="str">
         <f ca="1">TEXT(TODAY()+15,"mm/dd/yyyy")</f>
-        <v>11/16/2022</v>
+        <v>11/18/2022</v>
       </c>
       <c r="I3" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>11/26/2022</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>11/28/2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -2274,7 +4832,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -2285,7 +4843,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -2293,7 +4851,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -2316,7 +4874,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -2339,7 +4897,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -2358,7 +4916,7 @@
       <c r="F9" s="7"/>
       <c r="K9" s="14"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -2366,7 +4924,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -2374,7 +4932,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -2394,7 +4952,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>121</v>
       </c>
@@ -2414,7 +4972,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>224</v>
       </c>
@@ -2435,7 +4993,7 @@
       <c r="H14" s="23"/>
       <c r="I14" s="23"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>225</v>
       </c>
@@ -2456,7 +5014,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>226</v>
       </c>
@@ -2477,7 +5035,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>227</v>
       </c>
@@ -2504,31 +5062,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="4.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2566,7 +5124,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -2582,7 +5140,7 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2596,7 +5154,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -2610,7 +5168,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -2624,7 +5182,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -2638,7 +5196,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -2654,7 +5212,7 @@
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -2665,7 +5223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -2676,7 +5234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -2687,7 +5245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -2711,22 +5269,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212A931B-B5A0-4D20-AB7B-9542993AD90C}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="72.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="72.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2737,7 +5295,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -2752,100 +5310,4 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.453125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>229</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="23"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>234</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>235</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Creates testcase TC031-51 Signed-off-by: Sourabh kumar <sourabh@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A955453-190E-45C8-8296-DA99F734F2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B6B326-D1DE-4B97-9E25-8E18C33A82AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="666">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -1877,6 +1877,165 @@
   </si>
   <si>
     <t>A business entity such as a corporation, limited liability company, public limited company, sole proprietorship, or partnership that has products or services for sale is a firm. Law, accountancy and management consultancy partnerships are known as firms, and are rarely referred to as companies.</t>
+  </si>
+  <si>
+    <t>New Task 1</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>+5</t>
+  </si>
+  <si>
+    <t>Test Contact 1&lt;break&gt;Test Contact 4</t>
+  </si>
+  <si>
+    <t>New Call 1</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>New Meeting 1</t>
+  </si>
+  <si>
+    <t>This is Navatar Event</t>
+  </si>
+  <si>
+    <t>ATE_076</t>
+  </si>
+  <si>
+    <t>ATE_077</t>
+  </si>
+  <si>
+    <t>ATE_078</t>
+  </si>
+  <si>
+    <t>End_Day</t>
+  </si>
+  <si>
+    <t>11/28/2022</t>
+  </si>
+  <si>
+    <t>12/03/2022</t>
+  </si>
+  <si>
+    <t>ATE032</t>
+  </si>
+  <si>
+    <t>11/28/2022, 3:23 AM</t>
+  </si>
+  <si>
+    <t>11/28/2022, 3:33 AM</t>
+  </si>
+  <si>
+    <t>ATE_079</t>
+  </si>
+  <si>
+    <t>ATE_080</t>
+  </si>
+  <si>
+    <t>ATE_081</t>
+  </si>
+  <si>
+    <t>New Task 2</t>
+  </si>
+  <si>
+    <t>Test Contact 4&lt;break&gt;Test Account 1</t>
+  </si>
+  <si>
+    <t>New Call 2</t>
+  </si>
+  <si>
+    <t>New Meeting 2</t>
+  </si>
+  <si>
+    <t>12/04/2022</t>
+  </si>
+  <si>
+    <t>11/29/2022</t>
+  </si>
+  <si>
+    <t>ATE033</t>
+  </si>
+  <si>
+    <t>ATE_082</t>
+  </si>
+  <si>
+    <t>ATE_083</t>
+  </si>
+  <si>
+    <t>ATE_084</t>
+  </si>
+  <si>
+    <t>AccNew Task 2</t>
+  </si>
+  <si>
+    <t>Test Account 1&lt;break&gt;Navatar IntAccount 1</t>
+  </si>
+  <si>
+    <t>AccNew Call 2</t>
+  </si>
+  <si>
+    <t>NavTest Contact 10&lt;break&gt;Navatar IntAccount 1&lt;break&gt;Test Account 1</t>
+  </si>
+  <si>
+    <t>Event AccNew 2</t>
+  </si>
+  <si>
+    <t>NavTest Contact 10&lt;break&gt;Navatar IntAccount 1&lt;break&gt;Navatar IntAccount 2&lt;break&gt;Test Account 1&lt;break&gt;Nav Connection Deal1&lt;break&gt;Test Contact 4</t>
+  </si>
+  <si>
+    <t>ATE034</t>
+  </si>
+  <si>
+    <t>Navatar IntAccount 1</t>
+  </si>
+  <si>
+    <t>Navatar IntAccount 2</t>
+  </si>
+  <si>
+    <t>ATE035</t>
+  </si>
+  <si>
+    <t>ATE036</t>
+  </si>
+  <si>
+    <t>NavTest Contact 10</t>
+  </si>
+  <si>
+    <t>Nav Connection Deal1</t>
+  </si>
+  <si>
+    <t>11/29/2022, 4:52 AM</t>
+  </si>
+  <si>
+    <t>11/29/2022, 2:26 AM</t>
+  </si>
+  <si>
+    <t>11/29/2022, 5:52 AM</t>
+  </si>
+  <si>
+    <t>Followup New Task 2</t>
+  </si>
+  <si>
+    <t>ATE_085</t>
+  </si>
+  <si>
+    <t>12/10/2022</t>
+  </si>
+  <si>
+    <t>Test Contact 4&lt;break&gt;Test Account 1&lt;break&gt;CTest Account 12&lt;break&gt;Connection Deal 5</t>
+  </si>
+  <si>
+    <t>ATE037</t>
+  </si>
+  <si>
+    <t>ATE038</t>
+  </si>
+  <si>
+    <t>Tagged&lt;break&gt;Interactions&lt;break&gt;Connections&lt;break&gt;Deals</t>
   </si>
 </sst>
 </file>
@@ -2018,7 +2177,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2117,6 +2276,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2436,11 +2600,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2787,14 +2951,14 @@
     <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.88671875" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="24.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
@@ -2944,8 +3108,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -2957,10 +3121,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="B3" s="43"/>
+      <c r="B3" s="46"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -3020,16 +3184,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -3209,7 +3373,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3722,10 +3886,11 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N96"/>
+  <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3739,13 +3904,14 @@
     <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="4.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3779,15 +3945,18 @@
       <c r="K1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="42" t="s">
+        <v>624</v>
+      </c>
+      <c r="M1" s="28" t="s">
         <v>323</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="N1" s="28" t="s">
         <v>324</v>
       </c>
-      <c r="N1" s="28"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" s="28"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="29"/>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -3799,8 +3968,9 @@
       <c r="I2" s="29"/>
       <c r="J2" s="29"/>
       <c r="K2" s="29"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L2" s="29"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="28"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -3814,8 +3984,9 @@
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L3" s="42"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -3840,8 +4011,9 @@
       <c r="K4" s="14" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -3862,14 +4034,14 @@
       </c>
       <c r="H5" t="str">
         <f ca="1">TEXT(TODAY()+15,"mm/dd/yyyy")</f>
-        <v>12/12/2022</v>
+        <v>12/15/2022</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>12/22/2022</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>12/25/2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -3891,8 +4063,9 @@
       <c r="K6" s="14" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -3903,7 +4076,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -3911,7 +4084,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -3933,8 +4106,9 @@
       <c r="K9" s="14" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L9" s="14"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -3956,8 +4130,9 @@
       <c r="K10" s="14" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -3975,8 +4150,9 @@
       </c>
       <c r="F11" s="7"/>
       <c r="K11" s="14"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -3984,7 +4160,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -3992,7 +4168,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>115</v>
       </c>
@@ -4012,7 +4188,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -4032,7 +4208,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>221</v>
       </c>
@@ -4053,7 +4229,7 @@
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>222</v>
       </c>
@@ -4074,7 +4250,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>223</v>
       </c>
@@ -4095,7 +4271,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>224</v>
       </c>
@@ -4116,7 +4292,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -4130,8 +4306,9 @@
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
         <v>318</v>
       </c>
@@ -4153,16 +4330,19 @@
       <c r="G22" s="31"/>
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
+      <c r="J22" s="13" t="s">
+        <v>462</v>
+      </c>
       <c r="K22" s="31"/>
-      <c r="L22" s="31" t="s">
+      <c r="L22" s="31"/>
+      <c r="M22" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
         <v>341</v>
       </c>
@@ -4189,11 +4369,12 @@
       </c>
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
-      <c r="M23" t="s">
+      <c r="M23" s="31"/>
+      <c r="N23" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="31" t="s">
         <v>357</v>
       </c>
@@ -4222,8 +4403,9 @@
       </c>
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M24" s="31"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
         <v>375</v>
       </c>
@@ -4245,18 +4427,21 @@
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
+      <c r="J25" s="13" t="s">
+        <v>462</v>
+      </c>
       <c r="K25" s="31">
         <v>0</v>
       </c>
-      <c r="L25" s="31" t="s">
+      <c r="L25" s="31"/>
+      <c r="M25" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="40" t="s">
         <v>381</v>
       </c>
@@ -4278,18 +4463,21 @@
       <c r="G26" s="40"/>
       <c r="H26" s="40"/>
       <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
+      <c r="J26" s="13" t="s">
+        <v>462</v>
+      </c>
       <c r="K26" s="40">
         <v>0</v>
       </c>
-      <c r="L26" s="40" t="s">
+      <c r="L26" s="40"/>
+      <c r="M26" s="40" t="s">
         <v>325</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>503</v>
       </c>
@@ -4315,8 +4503,9 @@
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
-    </row>
-    <row r="28" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="N27" s="13"/>
+    </row>
+    <row r="28" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A28" s="31" t="s">
         <v>504</v>
       </c>
@@ -4342,8 +4531,9 @@
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
-    </row>
-    <row r="29" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="N28" s="13"/>
+    </row>
+    <row r="29" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A29" s="31" t="s">
         <v>505</v>
       </c>
@@ -4369,8 +4559,9 @@
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
-    </row>
-    <row r="30" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="N29" s="13"/>
+    </row>
+    <row r="30" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A30" s="31" t="s">
         <v>506</v>
       </c>
@@ -4396,8 +4587,9 @@
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
-    </row>
-    <row r="31" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="N30" s="13"/>
+    </row>
+    <row r="31" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
         <v>507</v>
       </c>
@@ -4423,8 +4615,9 @@
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
-    </row>
-    <row r="32" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="N31" s="13"/>
+    </row>
+    <row r="32" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" s="31" t="s">
         <v>508</v>
       </c>
@@ -4450,8 +4643,9 @@
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
-    </row>
-    <row r="33" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="N32" s="13"/>
+    </row>
+    <row r="33" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A33" s="31" t="s">
         <v>509</v>
       </c>
@@ -4477,8 +4671,9 @@
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
       <c r="M33" s="13"/>
-    </row>
-    <row r="34" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="N33" s="13"/>
+    </row>
+    <row r="34" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A34" s="31" t="s">
         <v>510</v>
       </c>
@@ -4504,8 +4699,9 @@
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
-    </row>
-    <row r="35" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="N34" s="13"/>
+    </row>
+    <row r="35" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
         <v>511</v>
       </c>
@@ -4531,8 +4727,9 @@
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
-    </row>
-    <row r="36" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="N35" s="13"/>
+    </row>
+    <row r="36" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
         <v>512</v>
       </c>
@@ -4558,8 +4755,9 @@
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
-    </row>
-    <row r="37" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N36" s="13"/>
+    </row>
+    <row r="37" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
         <v>513</v>
       </c>
@@ -4585,8 +4783,9 @@
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
       <c r="M37" s="13"/>
-    </row>
-    <row r="38" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N37" s="13"/>
+    </row>
+    <row r="38" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="s">
         <v>514</v>
       </c>
@@ -4612,8 +4811,9 @@
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
-    </row>
-    <row r="39" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N38" s="13"/>
+    </row>
+    <row r="39" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
         <v>515</v>
       </c>
@@ -4639,8 +4839,9 @@
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
       <c r="M39" s="13"/>
-    </row>
-    <row r="40" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N39" s="13"/>
+    </row>
+    <row r="40" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A40" s="31" t="s">
         <v>516</v>
       </c>
@@ -4666,8 +4867,9 @@
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
-    </row>
-    <row r="41" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N40" s="13"/>
+    </row>
+    <row r="41" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
         <v>517</v>
       </c>
@@ -4693,8 +4895,9 @@
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
       <c r="M41" s="13"/>
-    </row>
-    <row r="42" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N41" s="13"/>
+    </row>
+    <row r="42" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
         <v>518</v>
       </c>
@@ -4720,8 +4923,9 @@
       <c r="K42" s="13"/>
       <c r="L42" s="13"/>
       <c r="M42" s="13"/>
-    </row>
-    <row r="43" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N42" s="13"/>
+    </row>
+    <row r="43" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
         <v>519</v>
       </c>
@@ -4747,8 +4951,9 @@
       <c r="K43" s="13"/>
       <c r="L43" s="13"/>
       <c r="M43" s="13"/>
-    </row>
-    <row r="44" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N43" s="13"/>
+    </row>
+    <row r="44" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
         <v>520</v>
       </c>
@@ -4774,8 +4979,9 @@
       <c r="K44" s="13"/>
       <c r="L44" s="13"/>
       <c r="M44" s="13"/>
-    </row>
-    <row r="45" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N44" s="13"/>
+    </row>
+    <row r="45" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
         <v>521</v>
       </c>
@@ -4801,8 +5007,9 @@
       <c r="K45" s="13"/>
       <c r="L45" s="13"/>
       <c r="M45" s="13"/>
-    </row>
-    <row r="46" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N45" s="13"/>
+    </row>
+    <row r="46" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A46" s="31" t="s">
         <v>522</v>
       </c>
@@ -4828,8 +5035,9 @@
       <c r="K46" s="13"/>
       <c r="L46" s="13"/>
       <c r="M46" s="13"/>
-    </row>
-    <row r="47" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N46" s="13"/>
+    </row>
+    <row r="47" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="31" t="s">
         <v>523</v>
       </c>
@@ -4855,8 +5063,9 @@
       <c r="K47" s="13"/>
       <c r="L47" s="13"/>
       <c r="M47" s="13"/>
-    </row>
-    <row r="48" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N47" s="13"/>
+    </row>
+    <row r="48" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
         <v>524</v>
       </c>
@@ -4882,8 +5091,9 @@
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
       <c r="M48" s="13"/>
-    </row>
-    <row r="49" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N48" s="13"/>
+    </row>
+    <row r="49" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A49" s="31" t="s">
         <v>525</v>
       </c>
@@ -4909,8 +5119,9 @@
       <c r="K49" s="13"/>
       <c r="L49" s="13"/>
       <c r="M49" s="13"/>
-    </row>
-    <row r="50" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N49" s="13"/>
+    </row>
+    <row r="50" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A50" s="31" t="s">
         <v>526</v>
       </c>
@@ -4936,8 +5147,9 @@
       <c r="K50" s="13"/>
       <c r="L50" s="13"/>
       <c r="M50" s="13"/>
-    </row>
-    <row r="51" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N50" s="13"/>
+    </row>
+    <row r="51" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A51" s="31" t="s">
         <v>527</v>
       </c>
@@ -4963,8 +5175,9 @@
       <c r="K51" s="13"/>
       <c r="L51" s="13"/>
       <c r="M51" s="13"/>
-    </row>
-    <row r="52" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N51" s="13"/>
+    </row>
+    <row r="52" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A52" s="31" t="s">
         <v>528</v>
       </c>
@@ -4990,8 +5203,9 @@
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
       <c r="M52" s="13"/>
-    </row>
-    <row r="53" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N52" s="13"/>
+    </row>
+    <row r="53" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
         <v>529</v>
       </c>
@@ -5017,8 +5231,9 @@
       <c r="K53" s="13"/>
       <c r="L53" s="13"/>
       <c r="M53" s="13"/>
-    </row>
-    <row r="54" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N53" s="13"/>
+    </row>
+    <row r="54" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A54" s="31" t="s">
         <v>530</v>
       </c>
@@ -5044,8 +5259,9 @@
       <c r="K54" s="13"/>
       <c r="L54" s="13"/>
       <c r="M54" s="13"/>
-    </row>
-    <row r="55" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N54" s="13"/>
+    </row>
+    <row r="55" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="31" t="s">
         <v>531</v>
       </c>
@@ -5071,8 +5287,9 @@
       <c r="K55" s="13"/>
       <c r="L55" s="13"/>
       <c r="M55" s="13"/>
-    </row>
-    <row r="56" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N55" s="13"/>
+    </row>
+    <row r="56" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A56" s="31" t="s">
         <v>532</v>
       </c>
@@ -5098,8 +5315,9 @@
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
       <c r="M56" s="13"/>
-    </row>
-    <row r="57" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N56" s="13"/>
+    </row>
+    <row r="57" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A57" s="31" t="s">
         <v>533</v>
       </c>
@@ -5125,8 +5343,9 @@
       <c r="K57" s="13"/>
       <c r="L57" s="13"/>
       <c r="M57" s="13"/>
-    </row>
-    <row r="58" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N57" s="13"/>
+    </row>
+    <row r="58" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A58" s="31" t="s">
         <v>534</v>
       </c>
@@ -5152,8 +5371,9 @@
       <c r="K58" s="13"/>
       <c r="L58" s="13"/>
       <c r="M58" s="13"/>
-    </row>
-    <row r="59" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N58" s="13"/>
+    </row>
+    <row r="59" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A59" s="31" t="s">
         <v>535</v>
       </c>
@@ -5179,8 +5399,9 @@
       <c r="K59" s="13"/>
       <c r="L59" s="13"/>
       <c r="M59" s="13"/>
-    </row>
-    <row r="60" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N59" s="13"/>
+    </row>
+    <row r="60" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A60" s="31" t="s">
         <v>536</v>
       </c>
@@ -5206,8 +5427,9 @@
       <c r="K60" s="13"/>
       <c r="L60" s="13"/>
       <c r="M60" s="13"/>
-    </row>
-    <row r="61" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N60" s="13"/>
+    </row>
+    <row r="61" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A61" s="31" t="s">
         <v>537</v>
       </c>
@@ -5233,8 +5455,9 @@
       <c r="K61" s="13"/>
       <c r="L61" s="13"/>
       <c r="M61" s="13"/>
-    </row>
-    <row r="62" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N61" s="13"/>
+    </row>
+    <row r="62" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A62" s="31" t="s">
         <v>538</v>
       </c>
@@ -5260,8 +5483,9 @@
       <c r="K62" s="13"/>
       <c r="L62" s="13"/>
       <c r="M62" s="13"/>
-    </row>
-    <row r="63" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N62" s="13"/>
+    </row>
+    <row r="63" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A63" s="31" t="s">
         <v>539</v>
       </c>
@@ -5287,8 +5511,9 @@
       <c r="K63" s="13"/>
       <c r="L63" s="13"/>
       <c r="M63" s="13"/>
-    </row>
-    <row r="64" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N63" s="13"/>
+    </row>
+    <row r="64" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A64" s="31" t="s">
         <v>540</v>
       </c>
@@ -5314,8 +5539,9 @@
       <c r="K64" s="13"/>
       <c r="L64" s="13"/>
       <c r="M64" s="13"/>
-    </row>
-    <row r="65" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N64" s="13"/>
+    </row>
+    <row r="65" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A65" s="31" t="s">
         <v>541</v>
       </c>
@@ -5341,8 +5567,9 @@
       <c r="K65" s="13"/>
       <c r="L65" s="13"/>
       <c r="M65" s="13"/>
-    </row>
-    <row r="66" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N65" s="13"/>
+    </row>
+    <row r="66" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A66" s="31" t="s">
         <v>542</v>
       </c>
@@ -5368,8 +5595,9 @@
       <c r="K66" s="13"/>
       <c r="L66" s="13"/>
       <c r="M66" s="13"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N66" s="13"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="31" t="s">
         <v>543</v>
       </c>
@@ -5393,8 +5621,9 @@
       <c r="K67" s="13"/>
       <c r="L67" s="13"/>
       <c r="M67" s="13"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N67" s="13"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="31" t="s">
         <v>544</v>
       </c>
@@ -5418,8 +5647,9 @@
       <c r="K68" s="13"/>
       <c r="L68" s="13"/>
       <c r="M68" s="13"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N68" s="13"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="31" t="s">
         <v>545</v>
       </c>
@@ -5443,8 +5673,9 @@
       <c r="K69" s="13"/>
       <c r="L69" s="13"/>
       <c r="M69" s="13"/>
-    </row>
-    <row r="70" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N69" s="13"/>
+    </row>
+    <row r="70" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A70" s="31" t="s">
         <v>546</v>
       </c>
@@ -5470,8 +5701,9 @@
       <c r="K70" s="13"/>
       <c r="L70" s="13"/>
       <c r="M70" s="13"/>
-    </row>
-    <row r="71" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N70" s="13"/>
+    </row>
+    <row r="71" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A71" s="31" t="s">
         <v>547</v>
       </c>
@@ -5497,8 +5729,9 @@
       <c r="K71" s="13"/>
       <c r="L71" s="13"/>
       <c r="M71" s="13"/>
-    </row>
-    <row r="72" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N71" s="13"/>
+    </row>
+    <row r="72" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A72" s="31" t="s">
         <v>548</v>
       </c>
@@ -5524,8 +5757,9 @@
       <c r="K72" s="13"/>
       <c r="L72" s="13"/>
       <c r="M72" s="13"/>
-    </row>
-    <row r="73" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N72" s="13"/>
+    </row>
+    <row r="73" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A73" s="31" t="s">
         <v>549</v>
       </c>
@@ -5551,8 +5785,9 @@
       <c r="K73" s="13"/>
       <c r="L73" s="13"/>
       <c r="M73" s="13"/>
-    </row>
-    <row r="74" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N73" s="13"/>
+    </row>
+    <row r="74" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A74" s="31" t="s">
         <v>550</v>
       </c>
@@ -5578,8 +5813,9 @@
       <c r="K74" s="13"/>
       <c r="L74" s="13"/>
       <c r="M74" s="13"/>
-    </row>
-    <row r="75" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N74" s="13"/>
+    </row>
+    <row r="75" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A75" s="31" t="s">
         <v>551</v>
       </c>
@@ -5605,8 +5841,9 @@
       <c r="K75" s="13"/>
       <c r="L75" s="13"/>
       <c r="M75" s="13"/>
-    </row>
-    <row r="76" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N75" s="13"/>
+    </row>
+    <row r="76" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A76" s="31" t="s">
         <v>552</v>
       </c>
@@ -5632,8 +5869,9 @@
       <c r="K76" s="13"/>
       <c r="L76" s="13"/>
       <c r="M76" s="13"/>
-    </row>
-    <row r="77" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N76" s="13"/>
+    </row>
+    <row r="77" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A77" s="31" t="s">
         <v>553</v>
       </c>
@@ -5659,8 +5897,9 @@
       <c r="K77" s="13"/>
       <c r="L77" s="13"/>
       <c r="M77" s="13"/>
-    </row>
-    <row r="78" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N77" s="13"/>
+    </row>
+    <row r="78" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A78" s="31" t="s">
         <v>554</v>
       </c>
@@ -5686,8 +5925,9 @@
       <c r="K78" s="13"/>
       <c r="L78" s="13"/>
       <c r="M78" s="13"/>
-    </row>
-    <row r="79" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N78" s="13"/>
+    </row>
+    <row r="79" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A79" s="31" t="s">
         <v>555</v>
       </c>
@@ -5713,8 +5953,9 @@
       <c r="K79" s="13"/>
       <c r="L79" s="13"/>
       <c r="M79" s="13"/>
-    </row>
-    <row r="80" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N79" s="13"/>
+    </row>
+    <row r="80" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A80" s="31" t="s">
         <v>556</v>
       </c>
@@ -5740,8 +5981,9 @@
       <c r="K80" s="13"/>
       <c r="L80" s="13"/>
       <c r="M80" s="13"/>
-    </row>
-    <row r="81" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N80" s="13"/>
+    </row>
+    <row r="81" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A81" s="31" t="s">
         <v>557</v>
       </c>
@@ -5767,8 +6009,9 @@
       <c r="K81" s="13"/>
       <c r="L81" s="13"/>
       <c r="M81" s="13"/>
-    </row>
-    <row r="82" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N81" s="13"/>
+    </row>
+    <row r="82" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A82" s="31" t="s">
         <v>558</v>
       </c>
@@ -5794,8 +6037,9 @@
       <c r="K82" s="13"/>
       <c r="L82" s="13"/>
       <c r="M82" s="13"/>
-    </row>
-    <row r="83" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N82" s="13"/>
+    </row>
+    <row r="83" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A83" s="31" t="s">
         <v>559</v>
       </c>
@@ -5821,8 +6065,9 @@
       <c r="K83" s="13"/>
       <c r="L83" s="13"/>
       <c r="M83" s="13"/>
-    </row>
-    <row r="84" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N83" s="13"/>
+    </row>
+    <row r="84" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A84" s="31" t="s">
         <v>560</v>
       </c>
@@ -5848,8 +6093,9 @@
       <c r="K84" s="13"/>
       <c r="L84" s="13"/>
       <c r="M84" s="13"/>
-    </row>
-    <row r="85" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N84" s="13"/>
+    </row>
+    <row r="85" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A85" s="31" t="s">
         <v>561</v>
       </c>
@@ -5875,8 +6121,9 @@
       <c r="K85" s="13"/>
       <c r="L85" s="13"/>
       <c r="M85" s="13"/>
-    </row>
-    <row r="86" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N85" s="13"/>
+    </row>
+    <row r="86" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" s="31" t="s">
         <v>562</v>
       </c>
@@ -5902,8 +6149,9 @@
       <c r="K86" s="13"/>
       <c r="L86" s="13"/>
       <c r="M86" s="13"/>
-    </row>
-    <row r="87" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N86" s="13"/>
+    </row>
+    <row r="87" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A87" s="31" t="s">
         <v>563</v>
       </c>
@@ -5929,8 +6177,9 @@
       <c r="K87" s="13"/>
       <c r="L87" s="13"/>
       <c r="M87" s="13"/>
-    </row>
-    <row r="88" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N87" s="13"/>
+    </row>
+    <row r="88" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A88" s="31" t="s">
         <v>564</v>
       </c>
@@ -5956,8 +6205,9 @@
       <c r="K88" s="13"/>
       <c r="L88" s="13"/>
       <c r="M88" s="13"/>
-    </row>
-    <row r="89" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N88" s="13"/>
+    </row>
+    <row r="89" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A89" s="31" t="s">
         <v>565</v>
       </c>
@@ -5983,8 +6233,9 @@
       <c r="K89" s="13"/>
       <c r="L89" s="13"/>
       <c r="M89" s="13"/>
-    </row>
-    <row r="90" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N89" s="13"/>
+    </row>
+    <row r="90" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A90" s="31" t="s">
         <v>566</v>
       </c>
@@ -6010,8 +6261,9 @@
       <c r="K90" s="13"/>
       <c r="L90" s="13"/>
       <c r="M90" s="13"/>
-    </row>
-    <row r="91" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N90" s="13"/>
+    </row>
+    <row r="91" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A91" s="31" t="s">
         <v>567</v>
       </c>
@@ -6037,8 +6289,9 @@
       <c r="K91" s="13"/>
       <c r="L91" s="13"/>
       <c r="M91" s="13"/>
-    </row>
-    <row r="92" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N91" s="13"/>
+    </row>
+    <row r="92" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A92" s="31" t="s">
         <v>568</v>
       </c>
@@ -6064,8 +6317,9 @@
       <c r="K92" s="13"/>
       <c r="L92" s="13"/>
       <c r="M92" s="13"/>
-    </row>
-    <row r="93" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N92" s="13"/>
+    </row>
+    <row r="93" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A93" s="31" t="s">
         <v>569</v>
       </c>
@@ -6091,8 +6345,9 @@
       <c r="K93" s="13"/>
       <c r="L93" s="13"/>
       <c r="M93" s="13"/>
-    </row>
-    <row r="94" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N93" s="13"/>
+    </row>
+    <row r="94" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A94" s="31" t="s">
         <v>570</v>
       </c>
@@ -6118,8 +6373,9 @@
       <c r="K94" s="13"/>
       <c r="L94" s="13"/>
       <c r="M94" s="13"/>
-    </row>
-    <row r="95" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N94" s="13"/>
+    </row>
+    <row r="95" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A95" s="31" t="s">
         <v>571</v>
       </c>
@@ -6145,8 +6401,9 @@
       <c r="K95" s="13"/>
       <c r="L95" s="13"/>
       <c r="M95" s="13"/>
-    </row>
-    <row r="96" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="N95" s="13"/>
+    </row>
+    <row r="96" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A96" s="31" t="s">
         <v>572</v>
       </c>
@@ -6172,6 +6429,367 @@
       <c r="K96" s="13"/>
       <c r="L96" s="13"/>
       <c r="M96" s="13"/>
+      <c r="N96" s="13"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A97" s="31" t="s">
+        <v>621</v>
+      </c>
+      <c r="B97" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="C97" s="43" t="s">
+        <v>613</v>
+      </c>
+      <c r="D97" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="E97" s="13" t="s">
+        <v>616</v>
+      </c>
+      <c r="F97" s="13" t="s">
+        <v>626</v>
+      </c>
+      <c r="G97" s="13"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K97" s="44" t="s">
+        <v>615</v>
+      </c>
+      <c r="L97" s="44"/>
+      <c r="M97" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="N97" s="13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A98" s="31" t="s">
+        <v>622</v>
+      </c>
+      <c r="B98" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="C98" s="43" t="s">
+        <v>617</v>
+      </c>
+      <c r="D98" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="E98" s="13" t="s">
+        <v>616</v>
+      </c>
+      <c r="F98" s="13" t="s">
+        <v>625</v>
+      </c>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K98" s="13">
+        <v>0</v>
+      </c>
+      <c r="L98" s="13"/>
+      <c r="M98" s="13" t="s">
+        <v>618</v>
+      </c>
+      <c r="N98" s="13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A99" s="31" t="s">
+        <v>623</v>
+      </c>
+      <c r="B99" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C99" s="43" t="s">
+        <v>619</v>
+      </c>
+      <c r="D99" s="17" t="s">
+        <v>620</v>
+      </c>
+      <c r="E99" s="13" t="s">
+        <v>616</v>
+      </c>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="I99" s="13" t="s">
+        <v>629</v>
+      </c>
+      <c r="J99" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K99" s="13">
+        <v>0</v>
+      </c>
+      <c r="L99" s="13">
+        <v>0</v>
+      </c>
+      <c r="M99" s="13"/>
+      <c r="N99" s="13"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A100" s="31" t="s">
+        <v>630</v>
+      </c>
+      <c r="B100" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="C100" s="43" t="s">
+        <v>633</v>
+      </c>
+      <c r="D100" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="E100" s="43" t="s">
+        <v>634</v>
+      </c>
+      <c r="F100" s="13" t="s">
+        <v>637</v>
+      </c>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K100" s="44" t="s">
+        <v>615</v>
+      </c>
+      <c r="L100" s="13"/>
+      <c r="M100" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="N100" s="13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A101" s="31" t="s">
+        <v>631</v>
+      </c>
+      <c r="B101" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="C101" s="43" t="s">
+        <v>635</v>
+      </c>
+      <c r="D101" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="E101" s="43" t="s">
+        <v>634</v>
+      </c>
+      <c r="F101" s="13" t="s">
+        <v>638</v>
+      </c>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K101" s="13">
+        <v>0</v>
+      </c>
+      <c r="L101" s="13"/>
+      <c r="M101" s="13" t="s">
+        <v>618</v>
+      </c>
+      <c r="N101" s="13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A102" s="31" t="s">
+        <v>632</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C102" s="43" t="s">
+        <v>636</v>
+      </c>
+      <c r="D102" s="17" t="s">
+        <v>620</v>
+      </c>
+      <c r="E102" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="F102" s="13"/>
+      <c r="G102" s="13"/>
+      <c r="H102" s="13" t="s">
+        <v>657</v>
+      </c>
+      <c r="I102" s="13" t="s">
+        <v>638</v>
+      </c>
+      <c r="J102" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K102" s="13">
+        <v>0</v>
+      </c>
+      <c r="L102" s="13">
+        <v>0</v>
+      </c>
+      <c r="M102" s="13"/>
+      <c r="N102" s="13"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A103" s="31" t="s">
+        <v>640</v>
+      </c>
+      <c r="B103" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="C103" s="43" t="s">
+        <v>643</v>
+      </c>
+      <c r="D103" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="E103" s="43" t="s">
+        <v>644</v>
+      </c>
+      <c r="F103" s="13" t="s">
+        <v>638</v>
+      </c>
+      <c r="G103" s="13"/>
+      <c r="H103" s="13"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K103" s="13">
+        <v>0</v>
+      </c>
+      <c r="L103" s="13"/>
+      <c r="M103" s="43" t="s">
+        <v>614</v>
+      </c>
+      <c r="N103" s="13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A104" s="31" t="s">
+        <v>641</v>
+      </c>
+      <c r="B104" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="C104" s="43" t="s">
+        <v>645</v>
+      </c>
+      <c r="D104" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="E104" s="43" t="s">
+        <v>646</v>
+      </c>
+      <c r="F104" s="13" t="s">
+        <v>638</v>
+      </c>
+      <c r="G104" s="13"/>
+      <c r="H104" s="13"/>
+      <c r="I104" s="13"/>
+      <c r="J104" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K104" s="13">
+        <v>0</v>
+      </c>
+      <c r="L104" s="13"/>
+      <c r="M104" s="13" t="s">
+        <v>618</v>
+      </c>
+      <c r="N104" s="13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A105" s="31" t="s">
+        <v>642</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C105" s="43" t="s">
+        <v>647</v>
+      </c>
+      <c r="D105" s="17" t="s">
+        <v>620</v>
+      </c>
+      <c r="E105" s="43" t="s">
+        <v>648</v>
+      </c>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
+      <c r="H105" s="13" t="s">
+        <v>656</v>
+      </c>
+      <c r="I105" s="13" t="s">
+        <v>658</v>
+      </c>
+      <c r="J105" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K105" s="13">
+        <v>0</v>
+      </c>
+      <c r="L105" s="13">
+        <v>0</v>
+      </c>
+      <c r="M105" s="13"/>
+      <c r="N105" s="13"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A106" s="31" t="s">
+        <v>660</v>
+      </c>
+      <c r="B106" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>659</v>
+      </c>
+      <c r="D106" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="E106" s="13" t="s">
+        <v>662</v>
+      </c>
+      <c r="F106" t="s">
+        <v>661</v>
+      </c>
+      <c r="G106" s="13"/>
+      <c r="H106" s="13"/>
+      <c r="I106" s="13"/>
+      <c r="J106" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K106" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="L106" s="13"/>
+      <c r="M106" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="N106" s="13" t="s">
+        <v>326</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -6182,10 +6800,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AB52"/>
+  <dimension ref="A1:AB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6195,27 +6814,27 @@
     <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" customWidth="1"/>
-    <col min="18" max="18" width="19.5546875" customWidth="1"/>
-    <col min="19" max="21" width="17.33203125" customWidth="1"/>
-    <col min="22" max="22" width="48.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="33.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="61.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="40" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="69" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="19" max="21" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="48.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="33.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="61.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="40" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="69" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="35.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
@@ -6576,6 +7195,9 @@
       <c r="P23" t="s">
         <v>308</v>
       </c>
+      <c r="V23" t="s">
+        <v>665</v>
+      </c>
       <c r="AA23" t="s">
         <v>338</v>
       </c>
@@ -7291,6 +7913,21 @@
       <c r="L37">
         <v>0</v>
       </c>
+      <c r="Q37" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="R37" t="s">
+        <v>328</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>37</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -7384,6 +8021,12 @@
       <c r="E40">
         <v>40</v>
       </c>
+      <c r="F40" t="s">
+        <v>655</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
       <c r="H40" t="s">
         <v>447</v>
       </c>
@@ -7410,6 +8053,18 @@
       <c r="C41">
         <v>10</v>
       </c>
+      <c r="D41" t="s">
+        <v>284</v>
+      </c>
+      <c r="E41">
+        <v>49</v>
+      </c>
+      <c r="F41" t="s">
+        <v>428</v>
+      </c>
+      <c r="G41">
+        <v>31</v>
+      </c>
       <c r="H41" t="s">
         <v>448</v>
       </c>
@@ -7436,6 +8091,12 @@
       <c r="C42">
         <v>10</v>
       </c>
+      <c r="D42" t="s">
+        <v>284</v>
+      </c>
+      <c r="E42">
+        <v>51</v>
+      </c>
       <c r="H42" t="s">
         <v>449</v>
       </c>
@@ -7462,6 +8123,27 @@
       <c r="C43">
         <v>10</v>
       </c>
+      <c r="D43" t="s">
+        <v>284</v>
+      </c>
+      <c r="E43">
+        <v>52</v>
+      </c>
+      <c r="H43" t="s">
+        <v>280</v>
+      </c>
+      <c r="I43" t="s">
+        <v>328</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>64</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
@@ -7473,6 +8155,12 @@
       <c r="C44">
         <v>10</v>
       </c>
+      <c r="D44" t="s">
+        <v>654</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -7484,6 +8172,12 @@
       <c r="C45">
         <v>10</v>
       </c>
+      <c r="D45" t="s">
+        <v>284</v>
+      </c>
+      <c r="E45">
+        <v>53</v>
+      </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -7560,6 +8254,83 @@
       </c>
       <c r="C52">
         <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>627</v>
+      </c>
+      <c r="B53" t="s">
+        <v>346</v>
+      </c>
+      <c r="C53">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>639</v>
+      </c>
+      <c r="B54" t="s">
+        <v>346</v>
+      </c>
+      <c r="C54">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>649</v>
+      </c>
+      <c r="B55" t="s">
+        <v>346</v>
+      </c>
+      <c r="C55">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>652</v>
+      </c>
+      <c r="B56" t="s">
+        <v>650</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>653</v>
+      </c>
+      <c r="B57" t="s">
+        <v>651</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>663</v>
+      </c>
+      <c r="B58" t="s">
+        <v>346</v>
+      </c>
+      <c r="C58">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>664</v>
+      </c>
+      <c r="B59" t="s">
+        <v>395</v>
+      </c>
+      <c r="C59">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new sheet "CustomMetaData" in AcuityDataSheet file
Signed-off-by: NitinNavatar <ngarg@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7199A5-47D3-4D71-BA20-911360695582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
-    <sheet name="Firm" sheetId="1" r:id="rId1"/>
-    <sheet name="Research" sheetId="9" r:id="rId2"/>
-    <sheet name="Research Data" sheetId="12" r:id="rId3"/>
-    <sheet name="Contact" sheetId="2" r:id="rId4"/>
-    <sheet name="Deal" sheetId="3" r:id="rId5"/>
-    <sheet name="Deal Team" sheetId="7" r:id="rId6"/>
-    <sheet name="Activity Timeline" sheetId="5" r:id="rId7"/>
-    <sheet name="Acuity" sheetId="6" r:id="rId8"/>
-    <sheet name="Reports" sheetId="8" r:id="rId9"/>
-    <sheet name="Fund" sheetId="4" r:id="rId10"/>
-    <sheet name="Fundraisings" sheetId="10" r:id="rId11"/>
-    <sheet name="User" sheetId="13" r:id="rId12"/>
+    <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
+    <sheet name="Firm" sheetId="1" r:id="rId2"/>
+    <sheet name="Research" sheetId="9" r:id="rId3"/>
+    <sheet name="Research Data" sheetId="12" r:id="rId4"/>
+    <sheet name="Contact" sheetId="2" r:id="rId5"/>
+    <sheet name="Deal" sheetId="3" r:id="rId6"/>
+    <sheet name="Deal Team" sheetId="7" r:id="rId7"/>
+    <sheet name="Activity Timeline" sheetId="5" r:id="rId8"/>
+    <sheet name="Acuity" sheetId="6" r:id="rId9"/>
+    <sheet name="Reports" sheetId="8" r:id="rId10"/>
+    <sheet name="Fund" sheetId="4" r:id="rId11"/>
+    <sheet name="Fundraisings" sheetId="10" r:id="rId12"/>
+    <sheet name="User" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="743">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -2178,12 +2178,102 @@
   </si>
   <si>
     <t>ATE_Deal3</t>
+  </si>
+  <si>
+    <t>FieldName</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>New_Value</t>
+  </si>
+  <si>
+    <t>Cust_1</t>
+  </si>
+  <si>
+    <t>Research Acc Field2</t>
+  </si>
+  <si>
+    <t>navpeII__Fee_Comments__c</t>
+  </si>
+  <si>
+    <t>Cust_2</t>
+  </si>
+  <si>
+    <t>Research_Con_Field2</t>
+  </si>
+  <si>
+    <t>OwnerId</t>
+  </si>
+  <si>
+    <t>Cust_3</t>
+  </si>
+  <si>
+    <t>Research_Con_Field3</t>
+  </si>
+  <si>
+    <t>navpeII__Candidate_Notes__c</t>
+  </si>
+  <si>
+    <t>Cust_4</t>
+  </si>
+  <si>
+    <t>Research Deal Field2</t>
+  </si>
+  <si>
+    <t>navpeII__Source__c</t>
+  </si>
+  <si>
+    <t>Cust_5</t>
+  </si>
+  <si>
+    <t>Research Deal Field3</t>
+  </si>
+  <si>
+    <t>navpeII__Reason_for_Decline__c</t>
+  </si>
+  <si>
+    <t>Cust_6</t>
+  </si>
+  <si>
+    <t>Research Fund Field2</t>
+  </si>
+  <si>
+    <t>navpeII__Fund_Type__c</t>
+  </si>
+  <si>
+    <t>Cust_7</t>
+  </si>
+  <si>
+    <t>Research Fund Field3</t>
+  </si>
+  <si>
+    <t>navpeII__Investment_Category__c</t>
+  </si>
+  <si>
+    <t>Cust_8</t>
+  </si>
+  <si>
+    <t>Research Fundraising Field2</t>
+  </si>
+  <si>
+    <t>navpeII__Fund_Name__c</t>
+  </si>
+  <si>
+    <t>Cust_9</t>
+  </si>
+  <si>
+    <t>Research Fundraising Field3</t>
+  </si>
+  <si>
+    <t>Custom_Fundraising_LTA__c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2450,7 +2540,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2727,336 +2817,206 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="73.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="58.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>713</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>716</v>
+      </c>
+      <c r="B2" t="s">
+        <v>717</v>
+      </c>
+      <c r="D2" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>719</v>
+      </c>
+      <c r="B3" t="s">
+        <v>720</v>
+      </c>
+      <c r="C3" t="s">
+        <v>721</v>
+      </c>
+      <c r="D3" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>722</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>723</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>724</v>
+      </c>
+      <c r="D4" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>725</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>726</v>
+      </c>
+      <c r="D5" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>728</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>729</v>
+      </c>
+      <c r="D6" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>731</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>732</v>
+      </c>
+      <c r="D7" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>734</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>735</v>
+      </c>
+      <c r="D8" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>737</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>738</v>
+      </c>
+      <c r="D9" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>740</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C17" s="22"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="C18" s="22"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>278</v>
-      </c>
-      <c r="B21" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>283</v>
-      </c>
-      <c r="B22" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C29" s="27"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>295</v>
-      </c>
-      <c r="B30" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>310</v>
-      </c>
-      <c r="B31" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>316</v>
-      </c>
-      <c r="B32" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>376</v>
-      </c>
-      <c r="B33" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>381</v>
-      </c>
-      <c r="B34" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>667</v>
-      </c>
-      <c r="B35" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>668</v>
-      </c>
-      <c r="B36" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>669</v>
-      </c>
-      <c r="B37" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>676</v>
-      </c>
-      <c r="B38" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>711</v>
-      </c>
-      <c r="B39" t="s">
-        <v>710</v>
+        <v>741</v>
+      </c>
+      <c r="D10" t="s">
+        <v>742</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:C3"/>
-  </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="72.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3073,7 +3033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3087,7 +3047,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>225</v>
       </c>
@@ -3102,7 +3062,7 @@
       </c>
       <c r="E3" s="22"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>227</v>
       </c>
@@ -3113,7 +3073,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>229</v>
       </c>
@@ -3135,32 +3095,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -3204,7 +3164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24" t="s">
@@ -3215,7 +3175,7 @@
       <c r="F3" s="24"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>240</v>
       </c>
@@ -3243,7 +3203,7 @@
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>245</v>
       </c>
@@ -3263,7 +3223,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>247</v>
       </c>
@@ -3297,22 +3257,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF35A968-9FB9-4E9C-A1A3-7693EDA87B78}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -3323,7 +3282,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>664</v>
       </c>
@@ -3340,20 +3299,333 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="73.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="58.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="22"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="22"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>278</v>
+      </c>
+      <c r="B21" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>283</v>
+      </c>
+      <c r="B22" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="27"/>
+      <c r="B29" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="C29" s="27"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>295</v>
+      </c>
+      <c r="B30" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>310</v>
+      </c>
+      <c r="B31" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>316</v>
+      </c>
+      <c r="B32" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>376</v>
+      </c>
+      <c r="B33" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>381</v>
+      </c>
+      <c r="B34" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>667</v>
+      </c>
+      <c r="B35" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>668</v>
+      </c>
+      <c r="B36" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>669</v>
+      </c>
+      <c r="B37" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>676</v>
+      </c>
+      <c r="B38" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>711</v>
+      </c>
+      <c r="B39" t="s">
+        <v>710</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:C3"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3361,13 +3633,13 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
         <v>163</v>
       </c>
       <c r="B3" s="50"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -3375,7 +3647,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>166</v>
       </c>
@@ -3383,7 +3655,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -3391,7 +3663,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>170</v>
       </c>
@@ -3399,7 +3671,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -3415,29 +3687,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -3469,7 +3741,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
       <c r="B3" s="11"/>
       <c r="C3" s="23" t="s">
@@ -3483,7 +3755,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -3495,7 +3767,7 @@
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>269</v>
       </c>
@@ -3507,7 +3779,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>261</v>
       </c>
@@ -3519,7 +3791,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>262</v>
       </c>
@@ -3531,7 +3803,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>263</v>
       </c>
@@ -3543,7 +3815,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>264</v>
       </c>
@@ -3555,7 +3827,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="26"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>265</v>
       </c>
@@ -3567,7 +3839,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="26"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>266</v>
       </c>
@@ -3579,7 +3851,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="26"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>267</v>
       </c>
@@ -3591,7 +3863,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="26"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>268</v>
       </c>
@@ -3609,25 +3881,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B30" sqref="A30:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="45.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="117" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3656,7 +3928,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -3667,7 +3939,7 @@
       <c r="H2" s="29"/>
       <c r="I2" s="29"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -3680,7 +3952,7 @@
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3697,7 +3969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -3705,7 +3977,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -3713,7 +3985,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -3721,7 +3993,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -3741,7 +4013,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -3749,7 +4021,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -3757,7 +4029,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>182</v>
       </c>
@@ -3782,7 +4054,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>188</v>
       </c>
@@ -3797,7 +4069,7 @@
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>192</v>
       </c>
@@ -3812,7 +4084,7 @@
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>193</v>
       </c>
@@ -3835,7 +4107,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>194</v>
       </c>
@@ -3854,7 +4126,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>281</v>
       </c>
@@ -3862,7 +4134,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>286</v>
       </c>
@@ -3870,7 +4142,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>287</v>
       </c>
@@ -3878,7 +4150,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -3891,7 +4163,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>309</v>
       </c>
@@ -3899,7 +4171,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>312</v>
       </c>
@@ -3907,7 +4179,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>314</v>
       </c>
@@ -3915,7 +4187,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>380</v>
       </c>
@@ -3923,7 +4195,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>670</v>
       </c>
@@ -3934,7 +4206,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>671</v>
       </c>
@@ -3948,30 +4220,30 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="F8" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3997,7 +4269,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4011,7 +4283,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -4025,7 +4297,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>200</v>
       </c>
@@ -4049,7 +4321,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>202</v>
       </c>
@@ -4063,7 +4335,7 @@
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>208</v>
       </c>
@@ -4083,7 +4355,7 @@
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
@@ -4095,7 +4367,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>673</v>
       </c>
@@ -4103,7 +4375,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>675</v>
       </c>
@@ -4111,7 +4383,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>712</v>
       </c>
@@ -4125,24 +4397,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -4159,7 +4431,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -4182,8 +4454,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O114"/>
   <sheetViews>
@@ -4192,25 +4464,24 @@
       <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="24" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="58.77734375" style="34" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="58.7109375" style="34" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4255,7 +4526,7 @@
       </c>
       <c r="O1" s="28"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -4269,7 +4540,7 @@
       <c r="K2" s="29"/>
       <c r="L2" s="29"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -4285,7 +4556,7 @@
       <c r="K3" s="28"/>
       <c r="L3" s="42"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -4312,7 +4583,7 @@
       </c>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -4340,7 +4611,7 @@
         <v>01/02/2023</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -4364,7 +4635,7 @@
       </c>
       <c r="L6" s="14"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -4375,7 +4646,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -4383,7 +4654,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -4407,7 +4678,7 @@
       </c>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -4431,7 +4702,7 @@
       </c>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -4451,7 +4722,7 @@
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -4459,7 +4730,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -4467,7 +4738,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>115</v>
       </c>
@@ -4487,7 +4758,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -4507,7 +4778,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>221</v>
       </c>
@@ -4528,7 +4799,7 @@
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>222</v>
       </c>
@@ -4549,7 +4820,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>223</v>
       </c>
@@ -4570,7 +4841,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>224</v>
       </c>
@@ -4591,7 +4862,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -4607,7 +4878,7 @@
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>318</v>
       </c>
@@ -4641,7 +4912,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>341</v>
       </c>
@@ -4673,7 +4944,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>357</v>
       </c>
@@ -4708,7 +4979,7 @@
       </c>
       <c r="M24" s="31"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>372</v>
       </c>
@@ -4744,7 +5015,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
         <v>377</v>
       </c>
@@ -4780,7 +5051,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>499</v>
       </c>
@@ -4808,7 +5079,7 @@
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
     </row>
-    <row r="28" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>500</v>
       </c>
@@ -4836,7 +5107,7 @@
       <c r="M28" s="13"/>
       <c r="N28" s="13"/>
     </row>
-    <row r="29" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>501</v>
       </c>
@@ -4864,7 +5135,7 @@
       <c r="M29" s="13"/>
       <c r="N29" s="13"/>
     </row>
-    <row r="30" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>502</v>
       </c>
@@ -4892,7 +5163,7 @@
       <c r="M30" s="13"/>
       <c r="N30" s="13"/>
     </row>
-    <row r="31" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>503</v>
       </c>
@@ -4920,7 +5191,7 @@
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
     </row>
-    <row r="32" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>504</v>
       </c>
@@ -4948,7 +5219,7 @@
       <c r="M32" s="13"/>
       <c r="N32" s="13"/>
     </row>
-    <row r="33" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>505</v>
       </c>
@@ -4976,7 +5247,7 @@
       <c r="M33" s="13"/>
       <c r="N33" s="13"/>
     </row>
-    <row r="34" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>506</v>
       </c>
@@ -5004,7 +5275,7 @@
       <c r="M34" s="13"/>
       <c r="N34" s="13"/>
     </row>
-    <row r="35" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>507</v>
       </c>
@@ -5032,7 +5303,7 @@
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
     </row>
-    <row r="36" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>508</v>
       </c>
@@ -5060,7 +5331,7 @@
       <c r="M36" s="13"/>
       <c r="N36" s="13"/>
     </row>
-    <row r="37" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>509</v>
       </c>
@@ -5088,7 +5359,7 @@
       <c r="M37" s="13"/>
       <c r="N37" s="13"/>
     </row>
-    <row r="38" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>510</v>
       </c>
@@ -5116,7 +5387,7 @@
       <c r="M38" s="13"/>
       <c r="N38" s="13"/>
     </row>
-    <row r="39" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>511</v>
       </c>
@@ -5144,7 +5415,7 @@
       <c r="M39" s="13"/>
       <c r="N39" s="13"/>
     </row>
-    <row r="40" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>512</v>
       </c>
@@ -5172,7 +5443,7 @@
       <c r="M40" s="13"/>
       <c r="N40" s="13"/>
     </row>
-    <row r="41" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>513</v>
       </c>
@@ -5200,7 +5471,7 @@
       <c r="M41" s="13"/>
       <c r="N41" s="13"/>
     </row>
-    <row r="42" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>514</v>
       </c>
@@ -5228,7 +5499,7 @@
       <c r="M42" s="13"/>
       <c r="N42" s="13"/>
     </row>
-    <row r="43" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>515</v>
       </c>
@@ -5256,7 +5527,7 @@
       <c r="M43" s="13"/>
       <c r="N43" s="13"/>
     </row>
-    <row r="44" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>516</v>
       </c>
@@ -5284,7 +5555,7 @@
       <c r="M44" s="13"/>
       <c r="N44" s="13"/>
     </row>
-    <row r="45" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>517</v>
       </c>
@@ -5312,7 +5583,7 @@
       <c r="M45" s="13"/>
       <c r="N45" s="13"/>
     </row>
-    <row r="46" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
         <v>518</v>
       </c>
@@ -5340,7 +5611,7 @@
       <c r="M46" s="13"/>
       <c r="N46" s="13"/>
     </row>
-    <row r="47" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
         <v>519</v>
       </c>
@@ -5368,7 +5639,7 @@
       <c r="M47" s="13"/>
       <c r="N47" s="13"/>
     </row>
-    <row r="48" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
         <v>520</v>
       </c>
@@ -5396,7 +5667,7 @@
       <c r="M48" s="13"/>
       <c r="N48" s="13"/>
     </row>
-    <row r="49" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
         <v>521</v>
       </c>
@@ -5424,7 +5695,7 @@
       <c r="M49" s="13"/>
       <c r="N49" s="13"/>
     </row>
-    <row r="50" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>522</v>
       </c>
@@ -5452,7 +5723,7 @@
       <c r="M50" s="13"/>
       <c r="N50" s="13"/>
     </row>
-    <row r="51" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
         <v>523</v>
       </c>
@@ -5480,7 +5751,7 @@
       <c r="M51" s="13"/>
       <c r="N51" s="13"/>
     </row>
-    <row r="52" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
         <v>524</v>
       </c>
@@ -5508,7 +5779,7 @@
       <c r="M52" s="13"/>
       <c r="N52" s="13"/>
     </row>
-    <row r="53" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
         <v>525</v>
       </c>
@@ -5536,7 +5807,7 @@
       <c r="M53" s="13"/>
       <c r="N53" s="13"/>
     </row>
-    <row r="54" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
         <v>526</v>
       </c>
@@ -5564,7 +5835,7 @@
       <c r="M54" s="13"/>
       <c r="N54" s="13"/>
     </row>
-    <row r="55" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
         <v>527</v>
       </c>
@@ -5592,7 +5863,7 @@
       <c r="M55" s="13"/>
       <c r="N55" s="13"/>
     </row>
-    <row r="56" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
         <v>528</v>
       </c>
@@ -5620,7 +5891,7 @@
       <c r="M56" s="13"/>
       <c r="N56" s="13"/>
     </row>
-    <row r="57" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
         <v>529</v>
       </c>
@@ -5648,7 +5919,7 @@
       <c r="M57" s="13"/>
       <c r="N57" s="13"/>
     </row>
-    <row r="58" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="31" t="s">
         <v>530</v>
       </c>
@@ -5676,7 +5947,7 @@
       <c r="M58" s="13"/>
       <c r="N58" s="13"/>
     </row>
-    <row r="59" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="31" t="s">
         <v>531</v>
       </c>
@@ -5704,7 +5975,7 @@
       <c r="M59" s="13"/>
       <c r="N59" s="13"/>
     </row>
-    <row r="60" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="31" t="s">
         <v>532</v>
       </c>
@@ -5732,7 +6003,7 @@
       <c r="M60" s="13"/>
       <c r="N60" s="13"/>
     </row>
-    <row r="61" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="31" t="s">
         <v>533</v>
       </c>
@@ -5760,7 +6031,7 @@
       <c r="M61" s="13"/>
       <c r="N61" s="13"/>
     </row>
-    <row r="62" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
         <v>534</v>
       </c>
@@ -5788,7 +6059,7 @@
       <c r="M62" s="13"/>
       <c r="N62" s="13"/>
     </row>
-    <row r="63" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="31" t="s">
         <v>535</v>
       </c>
@@ -5816,7 +6087,7 @@
       <c r="M63" s="13"/>
       <c r="N63" s="13"/>
     </row>
-    <row r="64" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
         <v>536</v>
       </c>
@@ -5844,7 +6115,7 @@
       <c r="M64" s="13"/>
       <c r="N64" s="13"/>
     </row>
-    <row r="65" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="31" t="s">
         <v>537</v>
       </c>
@@ -5872,7 +6143,7 @@
       <c r="M65" s="13"/>
       <c r="N65" s="13"/>
     </row>
-    <row r="66" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="31" t="s">
         <v>538</v>
       </c>
@@ -5900,7 +6171,7 @@
       <c r="M66" s="13"/>
       <c r="N66" s="13"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="31" t="s">
         <v>539</v>
       </c>
@@ -5926,7 +6197,7 @@
       <c r="M67" s="13"/>
       <c r="N67" s="13"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="31" t="s">
         <v>540</v>
       </c>
@@ -5952,7 +6223,7 @@
       <c r="M68" s="13"/>
       <c r="N68" s="13"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="31" t="s">
         <v>541</v>
       </c>
@@ -5978,7 +6249,7 @@
       <c r="M69" s="13"/>
       <c r="N69" s="13"/>
     </row>
-    <row r="70" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="31" t="s">
         <v>542</v>
       </c>
@@ -6006,7 +6277,7 @@
       <c r="M70" s="13"/>
       <c r="N70" s="13"/>
     </row>
-    <row r="71" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="31" t="s">
         <v>543</v>
       </c>
@@ -6034,7 +6305,7 @@
       <c r="M71" s="13"/>
       <c r="N71" s="13"/>
     </row>
-    <row r="72" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="31" t="s">
         <v>544</v>
       </c>
@@ -6062,7 +6333,7 @@
       <c r="M72" s="13"/>
       <c r="N72" s="13"/>
     </row>
-    <row r="73" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="31" t="s">
         <v>545</v>
       </c>
@@ -6090,7 +6361,7 @@
       <c r="M73" s="13"/>
       <c r="N73" s="13"/>
     </row>
-    <row r="74" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" s="31" t="s">
         <v>546</v>
       </c>
@@ -6118,7 +6389,7 @@
       <c r="M74" s="13"/>
       <c r="N74" s="13"/>
     </row>
-    <row r="75" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="31" t="s">
         <v>547</v>
       </c>
@@ -6146,7 +6417,7 @@
       <c r="M75" s="13"/>
       <c r="N75" s="13"/>
     </row>
-    <row r="76" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="31" t="s">
         <v>548</v>
       </c>
@@ -6174,7 +6445,7 @@
       <c r="M76" s="13"/>
       <c r="N76" s="13"/>
     </row>
-    <row r="77" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="31" t="s">
         <v>549</v>
       </c>
@@ -6202,7 +6473,7 @@
       <c r="M77" s="13"/>
       <c r="N77" s="13"/>
     </row>
-    <row r="78" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="31" t="s">
         <v>550</v>
       </c>
@@ -6230,7 +6501,7 @@
       <c r="M78" s="13"/>
       <c r="N78" s="13"/>
     </row>
-    <row r="79" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="31" t="s">
         <v>551</v>
       </c>
@@ -6258,7 +6529,7 @@
       <c r="M79" s="13"/>
       <c r="N79" s="13"/>
     </row>
-    <row r="80" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="31" t="s">
         <v>552</v>
       </c>
@@ -6286,7 +6557,7 @@
       <c r="M80" s="13"/>
       <c r="N80" s="13"/>
     </row>
-    <row r="81" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="31" t="s">
         <v>553</v>
       </c>
@@ -6314,7 +6585,7 @@
       <c r="M81" s="13"/>
       <c r="N81" s="13"/>
     </row>
-    <row r="82" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" s="31" t="s">
         <v>554</v>
       </c>
@@ -6342,7 +6613,7 @@
       <c r="M82" s="13"/>
       <c r="N82" s="13"/>
     </row>
-    <row r="83" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="31" t="s">
         <v>555</v>
       </c>
@@ -6370,7 +6641,7 @@
       <c r="M83" s="13"/>
       <c r="N83" s="13"/>
     </row>
-    <row r="84" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" s="31" t="s">
         <v>556</v>
       </c>
@@ -6398,7 +6669,7 @@
       <c r="M84" s="13"/>
       <c r="N84" s="13"/>
     </row>
-    <row r="85" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" s="31" t="s">
         <v>557</v>
       </c>
@@ -6426,7 +6697,7 @@
       <c r="M85" s="13"/>
       <c r="N85" s="13"/>
     </row>
-    <row r="86" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="31" t="s">
         <v>558</v>
       </c>
@@ -6454,7 +6725,7 @@
       <c r="M86" s="13"/>
       <c r="N86" s="13"/>
     </row>
-    <row r="87" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="31" t="s">
         <v>559</v>
       </c>
@@ -6482,7 +6753,7 @@
       <c r="M87" s="13"/>
       <c r="N87" s="13"/>
     </row>
-    <row r="88" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="31" t="s">
         <v>560</v>
       </c>
@@ -6510,7 +6781,7 @@
       <c r="M88" s="13"/>
       <c r="N88" s="13"/>
     </row>
-    <row r="89" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="31" t="s">
         <v>561</v>
       </c>
@@ -6538,7 +6809,7 @@
       <c r="M89" s="13"/>
       <c r="N89" s="13"/>
     </row>
-    <row r="90" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="31" t="s">
         <v>562</v>
       </c>
@@ -6566,7 +6837,7 @@
       <c r="M90" s="13"/>
       <c r="N90" s="13"/>
     </row>
-    <row r="91" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="31" t="s">
         <v>563</v>
       </c>
@@ -6594,7 +6865,7 @@
       <c r="M91" s="13"/>
       <c r="N91" s="13"/>
     </row>
-    <row r="92" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="31" t="s">
         <v>564</v>
       </c>
@@ -6622,7 +6893,7 @@
       <c r="M92" s="13"/>
       <c r="N92" s="13"/>
     </row>
-    <row r="93" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="31" t="s">
         <v>565</v>
       </c>
@@ -6650,7 +6921,7 @@
       <c r="M93" s="13"/>
       <c r="N93" s="13"/>
     </row>
-    <row r="94" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="31" t="s">
         <v>566</v>
       </c>
@@ -6678,7 +6949,7 @@
       <c r="M94" s="13"/>
       <c r="N94" s="13"/>
     </row>
-    <row r="95" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="31" t="s">
         <v>567</v>
       </c>
@@ -6706,7 +6977,7 @@
       <c r="M95" s="13"/>
       <c r="N95" s="13"/>
     </row>
-    <row r="96" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="31" t="s">
         <v>568</v>
       </c>
@@ -6734,7 +7005,7 @@
       <c r="M96" s="13"/>
       <c r="N96" s="13"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="31" t="s">
         <v>617</v>
       </c>
@@ -6770,7 +7041,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="31" t="s">
         <v>618</v>
       </c>
@@ -6806,7 +7077,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="31" t="s">
         <v>619</v>
       </c>
@@ -6842,7 +7113,7 @@
       <c r="M99" s="13"/>
       <c r="N99" s="13"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="31" t="s">
         <v>626</v>
       </c>
@@ -6878,7 +7149,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="31" t="s">
         <v>627</v>
       </c>
@@ -6914,7 +7185,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="31" t="s">
         <v>628</v>
       </c>
@@ -6950,7 +7221,7 @@
       <c r="M102" s="13"/>
       <c r="N102" s="13"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="31" t="s">
         <v>636</v>
       </c>
@@ -6986,7 +7257,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="31" t="s">
         <v>637</v>
       </c>
@@ -7022,7 +7293,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="31" t="s">
         <v>638</v>
       </c>
@@ -7058,7 +7329,7 @@
       <c r="M105" s="13"/>
       <c r="N105" s="13"/>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="31" t="s">
         <v>656</v>
       </c>
@@ -7094,7 +7365,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="31" t="s">
         <v>697</v>
       </c>
@@ -7126,7 +7397,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="11"/>
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
@@ -7144,7 +7415,7 @@
       <c r="M112" s="11"/>
       <c r="N112" s="11"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="31" t="s">
         <v>679</v>
       </c>
@@ -7173,7 +7444,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="31" t="s">
         <v>682</v>
       </c>
@@ -7203,8 +7474,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7212,37 +7483,37 @@
       <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19.5546875" customWidth="1" collapsed="1"/>
-    <col min="19" max="21" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="48.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="33.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="61.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="19" max="21" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="48.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="33.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="61.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="40" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="26" max="26" width="69" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="35.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -7328,7 +7599,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -7353,7 +7624,7 @@
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -7367,7 +7638,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -7381,7 +7652,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -7395,7 +7666,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -7409,7 +7680,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -7434,7 +7705,7 @@
       <c r="T12" s="11"/>
       <c r="U12" s="11"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -7445,7 +7716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -7456,7 +7727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -7467,7 +7738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>126</v>
       </c>
@@ -7484,7 +7755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -7513,7 +7784,7 @@
       <c r="X21" s="11"/>
       <c r="Y21" s="11"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>293</v>
       </c>
@@ -7560,7 +7831,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>301</v>
       </c>
@@ -7610,7 +7881,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>330</v>
       </c>
@@ -7630,7 +7901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>345</v>
       </c>
@@ -7689,7 +7960,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>356</v>
       </c>
@@ -7748,7 +8019,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>366</v>
       </c>
@@ -7804,7 +8075,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>367</v>
       </c>
@@ -7857,7 +8128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>368</v>
       </c>
@@ -7910,7 +8181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>369</v>
       </c>
@@ -7963,7 +8234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>379</v>
       </c>
@@ -8016,7 +8287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>382</v>
       </c>
@@ -8069,7 +8340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>383</v>
       </c>
@@ -8122,7 +8393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>387</v>
       </c>
@@ -8175,7 +8446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>388</v>
       </c>
@@ -8228,7 +8499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>389</v>
       </c>
@@ -8281,7 +8552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>401</v>
       </c>
@@ -8334,7 +8605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>402</v>
       </c>
@@ -8387,7 +8658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>403</v>
       </c>
@@ -8425,7 +8696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>404</v>
       </c>
@@ -8463,7 +8734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>405</v>
       </c>
@@ -8501,7 +8772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>406</v>
       </c>
@@ -8539,7 +8810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>407</v>
       </c>
@@ -8577,7 +8848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>408</v>
       </c>
@@ -8615,7 +8886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>409</v>
       </c>
@@ -8653,7 +8924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>410</v>
       </c>
@@ -8676,7 +8947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>411</v>
       </c>
@@ -8699,7 +8970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>412</v>
       </c>
@@ -8722,7 +8993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>413</v>
       </c>
@@ -8745,7 +9016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>414</v>
       </c>
@@ -8768,7 +9039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>415</v>
       </c>
@@ -8785,7 +9056,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>416</v>
       </c>
@@ -8802,7 +9073,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>623</v>
       </c>
@@ -8819,7 +9090,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>635</v>
       </c>
@@ -8830,7 +9101,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>645</v>
       </c>
@@ -8841,7 +9112,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>648</v>
       </c>
@@ -8852,7 +9123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>649</v>
       </c>
@@ -8863,7 +9134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>659</v>
       </c>
@@ -8874,7 +9145,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>660</v>
       </c>
@@ -8885,7 +9156,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>686</v>
       </c>
@@ -8896,7 +9167,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>687</v>
       </c>
@@ -8907,7 +9178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>688</v>
       </c>
@@ -8918,7 +9189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>703</v>
       </c>
@@ -8929,7 +9200,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>704</v>
       </c>
@@ -8940,7 +9211,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>705</v>
       </c>
@@ -8951,7 +9222,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>706</v>
       </c>
@@ -8962,7 +9233,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>707</v>
       </c>
@@ -8978,47 +9249,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="72.109375" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add data to excel
Signed-off-by: ankur5579 <ankur@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD27F8CD-ACF2-406A-8076-C4BB23760663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1814DD93-90B5-4B10-A9E4-1353BB7F2FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Fund" sheetId="4" r:id="rId11"/>
     <sheet name="Fundraisings" sheetId="10" r:id="rId12"/>
     <sheet name="User" sheetId="13" r:id="rId13"/>
+    <sheet name="Test Custom Object" sheetId="16" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Activity Timeline'!$B$1:$B$114</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="814">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -2356,6 +2357,135 @@
   </si>
   <si>
     <t>Name&lt;break&gt;Department&lt;break&gt;Deals&lt;break&gt;Meetings and Calls&lt;break&gt;Emails</t>
+  </si>
+  <si>
+    <t>Meeting Notes Notification Reminder</t>
+  </si>
+  <si>
+    <t>Mutual Fund&lt;Break&gt;Sumo Kind Fund</t>
+  </si>
+  <si>
+    <t>Fund&lt;Break&gt;Fund</t>
+  </si>
+  <si>
+    <t>FC Fundraising&lt;Break&gt;Sumo Kind Fundraising</t>
+  </si>
+  <si>
+    <t>Acc 4&lt;Break&gt;Acc 12</t>
+  </si>
+  <si>
+    <t>Demo Deal&lt;Break&gt;Sumo Kind</t>
+  </si>
+  <si>
+    <t>Acc 7&lt;Break&gt;Sumo Kind</t>
+  </si>
+  <si>
+    <t>Deal Received&lt;Break&gt;NDA Signed</t>
+  </si>
+  <si>
+    <t>Test_Custom_Object_Name</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Test Custom Objects</t>
+  </si>
+  <si>
+    <t>Test Custom Object Name</t>
+  </si>
+  <si>
+    <t>Golden Ret&lt;Break&gt;Pothoscust&lt;Break&gt;custareca&lt;Break&gt;Custom Object 1.1&lt;Break&gt;Custom Object 1.2&lt;Break&gt;Custom Object 1.3</t>
+  </si>
+  <si>
+    <t>AMNNR_Fundraising1</t>
+  </si>
+  <si>
+    <t>AMNNR_Fund1</t>
+  </si>
+  <si>
+    <t>AMNNR_Deal1</t>
+  </si>
+  <si>
+    <t>AMNNR_CustomObjectRecord1</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity001</t>
+  </si>
+  <si>
+    <t>Task_Subject</t>
+  </si>
+  <si>
+    <t>Task_Status</t>
+  </si>
+  <si>
+    <t>Task_Due_Date</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity002</t>
+  </si>
+  <si>
+    <t>Send Invoice</t>
+  </si>
+  <si>
+    <t>Con 1&lt;break&gt;con 2&lt;break&gt;con 3&lt;break&gt;Sumo Logic&lt;break&gt;Houlihan Lokey&lt;break&gt;Vertica</t>
+  </si>
+  <si>
+    <t>Sumo Logic</t>
+  </si>
+  <si>
+    <t>This is to notify that @ con4, @con5 should be in loop</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity003</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity001</t>
+  </si>
+  <si>
+    <t>Con 1&lt;break&gt;con 2&lt;break&gt;+5</t>
+  </si>
+  <si>
+    <t>AMNNR_Record001</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity004</t>
+  </si>
+  <si>
+    <t>Send Letter</t>
+  </si>
+  <si>
+    <t>This is to check Con 2, Con 3, Logic should be the part of the deal kind</t>
+  </si>
+  <si>
+    <t>Vertica</t>
+  </si>
+  <si>
+    <t>con 2==Contact&lt;break&gt;con 3==Contact&lt;break&gt;Sumo Logic==Firm&lt;break&gt;Sumo Kind==Firm&lt;break&gt;Sumo Kind==Deal</t>
+  </si>
+  <si>
+    <t>AMNNR_Record002</t>
+  </si>
+  <si>
+    <t>This is to notify that Areca and Arrow should be in loop of vertica</t>
+  </si>
+  <si>
+    <t>con 2&lt;break&gt;con 3&lt;break&gt;+5</t>
+  </si>
+  <si>
+    <t>con 2&lt;break&gt;con 3&lt;break&gt;+6</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity002</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity003</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity005</t>
+  </si>
+  <si>
+    <t>areca</t>
   </si>
 </sst>
 </file>
@@ -2365,7 +2495,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2410,8 +2540,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2440,6 +2577,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -2511,7 +2654,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2586,10 +2729,29 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2880,14 +3042,14 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="26.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="26.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2901,7 +3063,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>698</v>
       </c>
@@ -2912,7 +3074,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>701</v>
       </c>
@@ -2926,7 +3088,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>704</v>
       </c>
@@ -2940,7 +3102,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>707</v>
       </c>
@@ -2951,7 +3113,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>710</v>
       </c>
@@ -2962,7 +3124,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>713</v>
       </c>
@@ -2973,7 +3135,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>716</v>
       </c>
@@ -2984,7 +3146,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>719</v>
       </c>
@@ -2995,7 +3157,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>722</v>
       </c>
@@ -3006,7 +3168,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>725</v>
       </c>
@@ -3023,7 +3185,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>726</v>
       </c>
@@ -3040,7 +3202,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>727</v>
       </c>
@@ -3057,7 +3219,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>734</v>
       </c>
@@ -3068,7 +3230,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>735</v>
       </c>
@@ -3085,7 +3247,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>736</v>
       </c>
@@ -3111,14 +3273,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="72.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="72.08984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3129,7 +3291,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -3148,22 +3310,23 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3180,7 +3343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3194,7 +3357,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>225</v>
       </c>
@@ -3209,7 +3372,7 @@
       </c>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>227</v>
       </c>
@@ -3220,7 +3383,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>229</v>
       </c>
@@ -3237,7 +3400,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -3246,7 +3409,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>744</v>
       </c>
@@ -3260,37 +3423,64 @@
         <v>18</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="46" t="s">
+        <v>771</v>
+      </c>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
+        <v>785</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>772</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>773</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>773</v>
+      </c>
+      <c r="E16" s="11"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:E15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.08984375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.90625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.6328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3334,7 +3524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
@@ -3345,7 +3535,7 @@
       <c r="F3" s="13"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>240</v>
       </c>
@@ -3373,7 +3563,7 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>245</v>
       </c>
@@ -3393,7 +3583,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>247</v>
       </c>
@@ -3421,7 +3611,52 @@
         <v>252</v>
       </c>
     </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="48" t="s">
+        <v>771</v>
+      </c>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>784</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>774</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>775</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>772</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:N10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3432,16 +3667,16 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="15.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3452,7 +3687,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>650</v>
       </c>
@@ -3464,26 +3699,110 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D62F989-B1EE-49D7-99A7-A4A6C00704A0}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>780</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>779</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="48" t="s">
+        <v>771</v>
+      </c>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>787</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>781</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>782</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>783</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.90625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.36328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.36328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3500,14 +3819,14 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3518,7 +3837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -3526,7 +3845,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -3534,7 +3853,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -3542,7 +3861,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -3550,7 +3869,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -3558,7 +3877,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -3566,7 +3885,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -3574,7 +3893,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -3582,7 +3901,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -3593,7 +3912,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>125</v>
       </c>
@@ -3601,7 +3920,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -3609,7 +3928,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>155</v>
       </c>
@@ -3620,7 +3939,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>156</v>
       </c>
@@ -3629,7 +3948,7 @@
       </c>
       <c r="C17" s="11"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>157</v>
       </c>
@@ -3638,7 +3957,7 @@
       </c>
       <c r="C18" s="11"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>158</v>
       </c>
@@ -3651,7 +3970,7 @@
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>159</v>
       </c>
@@ -3668,7 +3987,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>278</v>
       </c>
@@ -3676,7 +3995,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>283</v>
       </c>
@@ -3684,14 +4003,14 @@
         <v>282</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15"/>
       <c r="B29" s="15" t="s">
         <v>292</v>
       </c>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>295</v>
       </c>
@@ -3699,7 +4018,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>310</v>
       </c>
@@ -3707,7 +4026,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>316</v>
       </c>
@@ -3715,7 +4034,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>376</v>
       </c>
@@ -3723,7 +4042,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>381</v>
       </c>
@@ -3731,7 +4050,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>653</v>
       </c>
@@ -3739,7 +4058,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>654</v>
       </c>
@@ -3747,7 +4066,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>655</v>
       </c>
@@ -3755,7 +4074,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>662</v>
       </c>
@@ -3763,7 +4082,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>693</v>
       </c>
@@ -3771,7 +4090,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="15" t="s">
         <v>746</v>
@@ -3779,7 +4098,7 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>747</v>
       </c>
@@ -3790,9 +4109,41 @@
         <v>749</v>
       </c>
     </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="46" t="s">
+        <v>771</v>
+      </c>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>800</v>
+      </c>
+      <c r="B49" t="s">
+        <v>795</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>806</v>
+      </c>
+      <c r="B50" t="s">
+        <v>804</v>
+      </c>
+      <c r="C50" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A47:E47"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3808,13 +4159,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3822,13 +4173,13 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="B3" s="41"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="46"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -3836,7 +4187,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>166</v>
       </c>
@@ -3844,7 +4195,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -3852,7 +4203,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>170</v>
       </c>
@@ -3860,7 +4211,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -3884,21 +4235,21 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.90625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3930,7 +4281,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="12"/>
       <c r="B3" s="5"/>
       <c r="C3" s="12" t="s">
@@ -3944,7 +4295,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -3956,7 +4307,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>269</v>
       </c>
@@ -3968,7 +4319,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>261</v>
       </c>
@@ -3980,7 +4331,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>262</v>
       </c>
@@ -3992,7 +4343,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>263</v>
       </c>
@@ -4004,7 +4355,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>264</v>
       </c>
@@ -4016,7 +4367,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>265</v>
       </c>
@@ -4028,7 +4379,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>266</v>
       </c>
@@ -4040,7 +4391,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>267</v>
       </c>
@@ -4052,7 +4403,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>268</v>
       </c>
@@ -4074,21 +4425,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:I33"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="45.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="45.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.453125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="117" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4117,7 +4468,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -4128,7 +4479,7 @@
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4141,7 +4492,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4158,7 +4509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -4166,7 +4517,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -4174,7 +4525,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -4182,7 +4533,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -4202,7 +4553,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -4210,7 +4561,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -4218,7 +4569,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>182</v>
       </c>
@@ -4243,7 +4594,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>188</v>
       </c>
@@ -4258,7 +4609,7 @@
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>192</v>
       </c>
@@ -4273,7 +4624,7 @@
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>193</v>
       </c>
@@ -4296,7 +4647,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>194</v>
       </c>
@@ -4315,7 +4666,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>281</v>
       </c>
@@ -4323,7 +4674,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>286</v>
       </c>
@@ -4331,7 +4682,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>287</v>
       </c>
@@ -4339,7 +4690,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -4352,7 +4703,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>309</v>
       </c>
@@ -4360,7 +4711,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>312</v>
       </c>
@@ -4368,7 +4719,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>314</v>
       </c>
@@ -4376,7 +4727,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>380</v>
       </c>
@@ -4384,7 +4735,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>656</v>
       </c>
@@ -4395,7 +4746,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>657</v>
       </c>
@@ -4406,7 +4757,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -4419,7 +4770,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>751</v>
       </c>
@@ -4449,21 +4800,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.08984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4489,7 +4840,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4503,7 +4854,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -4517,7 +4868,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>200</v>
       </c>
@@ -4541,7 +4892,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>202</v>
       </c>
@@ -4555,7 +4906,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>208</v>
       </c>
@@ -4575,7 +4926,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
@@ -4587,7 +4938,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>659</v>
       </c>
@@ -4595,7 +4946,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>661</v>
       </c>
@@ -4603,7 +4954,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>694</v>
       </c>
@@ -4611,7 +4962,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
@@ -4623,7 +4974,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>756</v>
       </c>
@@ -4637,7 +4988,40 @@
         <v>759</v>
       </c>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="46" t="s">
+        <v>771</v>
+      </c>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
+        <v>786</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>776</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>777</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>778</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A22:H22"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4651,16 +5035,16 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4677,7 +5061,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -4703,31 +5087,35 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O114"/>
+  <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D111" sqref="D111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G124" sqref="G124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="58.6640625" style="20" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.44140625" style="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.08984375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.08984375" style="20" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.90625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.1796875" style="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4770,9 +5158,18 @@
       <c r="N1" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O1" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -4786,7 +5183,7 @@
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4802,7 +5199,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -4829,7 +5226,7 @@
       </c>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -4850,14 +5247,14 @@
       </c>
       <c r="H5" s="34" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>01/06/2023</v>
+        <v>01/07/2023</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>01/06/2023</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>01/07/2023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -4881,7 +5278,7 @@
       </c>
       <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -4892,7 +5289,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -4900,7 +5297,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -4924,7 +5321,7 @@
       </c>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -4948,7 +5345,7 @@
       </c>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -4968,7 +5365,7 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -4976,7 +5373,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -4984,7 +5381,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>115</v>
       </c>
@@ -5004,7 +5401,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -5024,7 +5421,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>221</v>
       </c>
@@ -5045,7 +5442,7 @@
       <c r="H16" s="35"/>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>222</v>
       </c>
@@ -5066,7 +5463,7 @@
       <c r="H17" s="35"/>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>223</v>
       </c>
@@ -5087,7 +5484,7 @@
       <c r="H18" s="35"/>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>224</v>
       </c>
@@ -5108,7 +5505,7 @@
       <c r="H19" s="35"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -5124,7 +5521,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
         <v>318</v>
       </c>
@@ -5158,7 +5555,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
         <v>341</v>
       </c>
@@ -5190,7 +5587,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
         <v>357</v>
       </c>
@@ -5225,7 +5622,7 @@
       </c>
       <c r="M24" s="17"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
         <v>372</v>
       </c>
@@ -5261,7 +5658,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="26" t="s">
         <v>377</v>
       </c>
@@ -5297,7 +5694,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>499</v>
       </c>
@@ -5325,7 +5722,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
         <v>500</v>
       </c>
@@ -5353,7 +5750,7 @@
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
         <v>501</v>
       </c>
@@ -5381,7 +5778,7 @@
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
         <v>502</v>
       </c>
@@ -5409,7 +5806,7 @@
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
     </row>
-    <row r="31" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
         <v>503</v>
       </c>
@@ -5437,7 +5834,7 @@
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
     </row>
-    <row r="32" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
         <v>504</v>
       </c>
@@ -5465,7 +5862,7 @@
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
     </row>
-    <row r="33" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
         <v>505</v>
       </c>
@@ -5493,7 +5890,7 @@
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
     </row>
-    <row r="34" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
         <v>506</v>
       </c>
@@ -5521,7 +5918,7 @@
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
     </row>
-    <row r="35" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
         <v>507</v>
       </c>
@@ -5549,7 +5946,7 @@
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
     </row>
-    <row r="36" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
         <v>508</v>
       </c>
@@ -5577,7 +5974,7 @@
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
     </row>
-    <row r="37" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
         <v>509</v>
       </c>
@@ -5605,7 +6002,7 @@
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
     </row>
-    <row r="38" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
         <v>510</v>
       </c>
@@ -5633,7 +6030,7 @@
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
     </row>
-    <row r="39" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
         <v>511</v>
       </c>
@@ -5661,7 +6058,7 @@
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
     </row>
-    <row r="40" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A40" s="17" t="s">
         <v>512</v>
       </c>
@@ -5689,7 +6086,7 @@
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
     </row>
-    <row r="41" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A41" s="17" t="s">
         <v>513</v>
       </c>
@@ -5717,7 +6114,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
     </row>
-    <row r="42" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A42" s="17" t="s">
         <v>514</v>
       </c>
@@ -5745,7 +6142,7 @@
       <c r="M42" s="7"/>
       <c r="N42" s="7"/>
     </row>
-    <row r="43" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
         <v>515</v>
       </c>
@@ -5773,7 +6170,7 @@
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
     </row>
-    <row r="44" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
         <v>516</v>
       </c>
@@ -5801,7 +6198,7 @@
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
     </row>
-    <row r="45" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
         <v>517</v>
       </c>
@@ -5829,7 +6226,7 @@
       <c r="M45" s="7"/>
       <c r="N45" s="7"/>
     </row>
-    <row r="46" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
         <v>518</v>
       </c>
@@ -5857,7 +6254,7 @@
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
     </row>
-    <row r="47" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
         <v>519</v>
       </c>
@@ -5885,7 +6282,7 @@
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
     </row>
-    <row r="48" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
         <v>520</v>
       </c>
@@ -5913,7 +6310,7 @@
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
     </row>
-    <row r="49" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
         <v>521</v>
       </c>
@@ -5941,7 +6338,7 @@
       <c r="M49" s="7"/>
       <c r="N49" s="7"/>
     </row>
-    <row r="50" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A50" s="17" t="s">
         <v>522</v>
       </c>
@@ -5969,7 +6366,7 @@
       <c r="M50" s="7"/>
       <c r="N50" s="7"/>
     </row>
-    <row r="51" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A51" s="17" t="s">
         <v>523</v>
       </c>
@@ -5997,7 +6394,7 @@
       <c r="M51" s="7"/>
       <c r="N51" s="7"/>
     </row>
-    <row r="52" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A52" s="17" t="s">
         <v>524</v>
       </c>
@@ -6025,7 +6422,7 @@
       <c r="M52" s="7"/>
       <c r="N52" s="7"/>
     </row>
-    <row r="53" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A53" s="17" t="s">
         <v>525</v>
       </c>
@@ -6053,7 +6450,7 @@
       <c r="M53" s="7"/>
       <c r="N53" s="7"/>
     </row>
-    <row r="54" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A54" s="17" t="s">
         <v>526</v>
       </c>
@@ -6081,7 +6478,7 @@
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
     </row>
-    <row r="55" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
         <v>527</v>
       </c>
@@ -6109,7 +6506,7 @@
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
     </row>
-    <row r="56" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A56" s="17" t="s">
         <v>528</v>
       </c>
@@ -6137,7 +6534,7 @@
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
     </row>
-    <row r="57" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>529</v>
       </c>
@@ -6165,7 +6562,7 @@
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
     </row>
-    <row r="58" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
         <v>530</v>
       </c>
@@ -6193,7 +6590,7 @@
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
     </row>
-    <row r="59" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>531</v>
       </c>
@@ -6221,7 +6618,7 @@
       <c r="M59" s="7"/>
       <c r="N59" s="7"/>
     </row>
-    <row r="60" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
         <v>532</v>
       </c>
@@ -6249,7 +6646,7 @@
       <c r="M60" s="7"/>
       <c r="N60" s="7"/>
     </row>
-    <row r="61" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A61" s="17" t="s">
         <v>533</v>
       </c>
@@ -6277,7 +6674,7 @@
       <c r="M61" s="7"/>
       <c r="N61" s="7"/>
     </row>
-    <row r="62" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A62" s="17" t="s">
         <v>534</v>
       </c>
@@ -6305,7 +6702,7 @@
       <c r="M62" s="7"/>
       <c r="N62" s="7"/>
     </row>
-    <row r="63" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A63" s="17" t="s">
         <v>535</v>
       </c>
@@ -6333,7 +6730,7 @@
       <c r="M63" s="7"/>
       <c r="N63" s="7"/>
     </row>
-    <row r="64" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A64" s="17" t="s">
         <v>536</v>
       </c>
@@ -6361,7 +6758,7 @@
       <c r="M64" s="7"/>
       <c r="N64" s="7"/>
     </row>
-    <row r="65" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A65" s="17" t="s">
         <v>537</v>
       </c>
@@ -6389,7 +6786,7 @@
       <c r="M65" s="7"/>
       <c r="N65" s="7"/>
     </row>
-    <row r="66" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A66" s="17" t="s">
         <v>538</v>
       </c>
@@ -6417,7 +6814,7 @@
       <c r="M66" s="7"/>
       <c r="N66" s="7"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" s="17" t="s">
         <v>539</v>
       </c>
@@ -6443,7 +6840,7 @@
       <c r="M67" s="7"/>
       <c r="N67" s="7"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" s="17" t="s">
         <v>540</v>
       </c>
@@ -6469,7 +6866,7 @@
       <c r="M68" s="7"/>
       <c r="N68" s="7"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" s="17" t="s">
         <v>541</v>
       </c>
@@ -6495,7 +6892,7 @@
       <c r="M69" s="7"/>
       <c r="N69" s="7"/>
     </row>
-    <row r="70" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A70" s="17" t="s">
         <v>542</v>
       </c>
@@ -6523,7 +6920,7 @@
       <c r="M70" s="7"/>
       <c r="N70" s="7"/>
     </row>
-    <row r="71" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A71" s="17" t="s">
         <v>543</v>
       </c>
@@ -6551,7 +6948,7 @@
       <c r="M71" s="7"/>
       <c r="N71" s="7"/>
     </row>
-    <row r="72" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A72" s="17" t="s">
         <v>544</v>
       </c>
@@ -6579,7 +6976,7 @@
       <c r="M72" s="7"/>
       <c r="N72" s="7"/>
     </row>
-    <row r="73" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A73" s="17" t="s">
         <v>545</v>
       </c>
@@ -6607,7 +7004,7 @@
       <c r="M73" s="7"/>
       <c r="N73" s="7"/>
     </row>
-    <row r="74" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A74" s="17" t="s">
         <v>546</v>
       </c>
@@ -6635,7 +7032,7 @@
       <c r="M74" s="7"/>
       <c r="N74" s="7"/>
     </row>
-    <row r="75" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
         <v>547</v>
       </c>
@@ -6663,7 +7060,7 @@
       <c r="M75" s="7"/>
       <c r="N75" s="7"/>
     </row>
-    <row r="76" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
         <v>548</v>
       </c>
@@ -6691,7 +7088,7 @@
       <c r="M76" s="7"/>
       <c r="N76" s="7"/>
     </row>
-    <row r="77" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A77" s="17" t="s">
         <v>549</v>
       </c>
@@ -6719,7 +7116,7 @@
       <c r="M77" s="7"/>
       <c r="N77" s="7"/>
     </row>
-    <row r="78" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A78" s="17" t="s">
         <v>550</v>
       </c>
@@ -6747,7 +7144,7 @@
       <c r="M78" s="7"/>
       <c r="N78" s="7"/>
     </row>
-    <row r="79" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A79" s="17" t="s">
         <v>551</v>
       </c>
@@ -6775,7 +7172,7 @@
       <c r="M79" s="7"/>
       <c r="N79" s="7"/>
     </row>
-    <row r="80" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A80" s="17" t="s">
         <v>552</v>
       </c>
@@ -6803,7 +7200,7 @@
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
     </row>
-    <row r="81" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A81" s="17" t="s">
         <v>553</v>
       </c>
@@ -6831,7 +7228,7 @@
       <c r="M81" s="7"/>
       <c r="N81" s="7"/>
     </row>
-    <row r="82" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
         <v>554</v>
       </c>
@@ -6859,7 +7256,7 @@
       <c r="M82" s="7"/>
       <c r="N82" s="7"/>
     </row>
-    <row r="83" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
         <v>555</v>
       </c>
@@ -6887,7 +7284,7 @@
       <c r="M83" s="7"/>
       <c r="N83" s="7"/>
     </row>
-    <row r="84" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A84" s="17" t="s">
         <v>556</v>
       </c>
@@ -6915,7 +7312,7 @@
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
     </row>
-    <row r="85" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A85" s="17" t="s">
         <v>557</v>
       </c>
@@ -6943,7 +7340,7 @@
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
     </row>
-    <row r="86" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A86" s="17" t="s">
         <v>558</v>
       </c>
@@ -6971,7 +7368,7 @@
       <c r="M86" s="7"/>
       <c r="N86" s="7"/>
     </row>
-    <row r="87" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A87" s="17" t="s">
         <v>559</v>
       </c>
@@ -6999,7 +7396,7 @@
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
     </row>
-    <row r="88" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A88" s="17" t="s">
         <v>560</v>
       </c>
@@ -7027,7 +7424,7 @@
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
     </row>
-    <row r="89" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A89" s="17" t="s">
         <v>561</v>
       </c>
@@ -7055,7 +7452,7 @@
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
     </row>
-    <row r="90" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A90" s="17" t="s">
         <v>562</v>
       </c>
@@ -7083,7 +7480,7 @@
       <c r="M90" s="7"/>
       <c r="N90" s="7"/>
     </row>
-    <row r="91" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A91" s="17" t="s">
         <v>563</v>
       </c>
@@ -7111,7 +7508,7 @@
       <c r="M91" s="7"/>
       <c r="N91" s="7"/>
     </row>
-    <row r="92" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A92" s="17" t="s">
         <v>564</v>
       </c>
@@ -7139,7 +7536,7 @@
       <c r="M92" s="7"/>
       <c r="N92" s="7"/>
     </row>
-    <row r="93" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A93" s="17" t="s">
         <v>565</v>
       </c>
@@ -7167,7 +7564,7 @@
       <c r="M93" s="7"/>
       <c r="N93" s="7"/>
     </row>
-    <row r="94" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A94" s="17" t="s">
         <v>566</v>
       </c>
@@ -7195,7 +7592,7 @@
       <c r="M94" s="7"/>
       <c r="N94" s="7"/>
     </row>
-    <row r="95" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A95" s="17" t="s">
         <v>567</v>
       </c>
@@ -7223,7 +7620,7 @@
       <c r="M95" s="7"/>
       <c r="N95" s="7"/>
     </row>
-    <row r="96" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A96" s="17" t="s">
         <v>568</v>
       </c>
@@ -7251,7 +7648,7 @@
       <c r="M96" s="7"/>
       <c r="N96" s="7"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A97" s="17" t="s">
         <v>612</v>
       </c>
@@ -7287,7 +7684,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A98" s="17" t="s">
         <v>613</v>
       </c>
@@ -7323,7 +7720,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A99" s="17" t="s">
         <v>614</v>
       </c>
@@ -7359,7 +7756,7 @@
       <c r="M99" s="7"/>
       <c r="N99" s="7"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A100" s="17" t="s">
         <v>617</v>
       </c>
@@ -7395,7 +7792,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A101" s="17" t="s">
         <v>618</v>
       </c>
@@ -7431,7 +7828,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A102" s="17" t="s">
         <v>619</v>
       </c>
@@ -7467,7 +7864,7 @@
       <c r="M102" s="7"/>
       <c r="N102" s="7"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A103" s="17" t="s">
         <v>625</v>
       </c>
@@ -7503,7 +7900,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A104" s="17" t="s">
         <v>626</v>
       </c>
@@ -7539,7 +7936,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A105" s="17" t="s">
         <v>627</v>
       </c>
@@ -7575,7 +7972,7 @@
       <c r="M105" s="7"/>
       <c r="N105" s="7"/>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A106" s="17" t="s">
         <v>642</v>
       </c>
@@ -7611,7 +8008,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A107" s="17" t="s">
         <v>681</v>
       </c>
@@ -7643,7 +8040,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A112" s="5"/>
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
@@ -7661,7 +8058,7 @@
       <c r="M112" s="5"/>
       <c r="N112" s="5"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A113" s="17" t="s">
         <v>665</v>
       </c>
@@ -7690,7 +8087,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A114" s="17" t="s">
         <v>668</v>
       </c>
@@ -7713,7 +8110,104 @@
         <v>606</v>
       </c>
     </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A119" s="47" t="s">
+        <v>771</v>
+      </c>
+      <c r="B119" s="47"/>
+      <c r="C119" s="47"/>
+      <c r="D119" s="47"/>
+      <c r="E119" s="47"/>
+      <c r="F119" s="47"/>
+      <c r="G119" s="47"/>
+      <c r="H119" s="47"/>
+      <c r="I119" s="47"/>
+      <c r="J119" s="47"/>
+      <c r="K119" s="47"/>
+      <c r="L119" s="47"/>
+      <c r="M119" s="47"/>
+      <c r="N119" s="47"/>
+      <c r="O119" s="47"/>
+      <c r="P119" s="47"/>
+      <c r="Q119" s="47"/>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>788</v>
+      </c>
+      <c r="B120" t="s">
+        <v>213</v>
+      </c>
+      <c r="M120" t="s">
+        <v>605</v>
+      </c>
+      <c r="N120" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>792</v>
+      </c>
+      <c r="C121" t="s">
+        <v>793</v>
+      </c>
+      <c r="E121" s="20" t="s">
+        <v>794</v>
+      </c>
+      <c r="M121" t="s">
+        <v>605</v>
+      </c>
+      <c r="N121" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>797</v>
+      </c>
+      <c r="D122" s="20" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>801</v>
+      </c>
+      <c r="C123" t="s">
+        <v>802</v>
+      </c>
+      <c r="D123" s="20" t="s">
+        <v>803</v>
+      </c>
+      <c r="E123" t="s">
+        <v>804</v>
+      </c>
+      <c r="G123" t="s">
+        <v>805</v>
+      </c>
+      <c r="M123" t="s">
+        <v>325</v>
+      </c>
+      <c r="N123" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>812</v>
+      </c>
+      <c r="D124" s="20" t="s">
+        <v>807</v>
+      </c>
+      <c r="G124" t="s">
+        <v>813</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A119:Q119"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7722,44 +8216,44 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AB67"/>
+  <dimension ref="A1:AB73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X23" sqref="X23"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.08984375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.36328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19.5546875" customWidth="1" collapsed="1"/>
-    <col min="19" max="21" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="48.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="33.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="61.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.36328125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="19" max="21" width="17.36328125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="48.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="33.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="61.6328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="40" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="26" max="26" width="69" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="21.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="35.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="21.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="35.08984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7845,7 +8339,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -7870,7 +8364,7 @@
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -7884,7 +8378,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -7898,7 +8392,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -7912,7 +8406,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -7926,7 +8420,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -7951,7 +8445,7 @@
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -7962,7 +8456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -7973,7 +8467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -7984,7 +8478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>126</v>
       </c>
@@ -8001,7 +8495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -8030,7 +8524,7 @@
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>293</v>
       </c>
@@ -8077,7 +8571,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>301</v>
       </c>
@@ -8130,7 +8624,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>330</v>
       </c>
@@ -8150,7 +8644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>345</v>
       </c>
@@ -8209,7 +8703,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>356</v>
       </c>
@@ -8268,7 +8762,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>366</v>
       </c>
@@ -8324,7 +8818,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>367</v>
       </c>
@@ -8377,7 +8871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>368</v>
       </c>
@@ -8430,7 +8924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>369</v>
       </c>
@@ -8483,7 +8977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>379</v>
       </c>
@@ -8536,7 +9030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>382</v>
       </c>
@@ -8589,7 +9083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>383</v>
       </c>
@@ -8642,7 +9136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>387</v>
       </c>
@@ -8695,7 +9189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>388</v>
       </c>
@@ -8748,7 +9242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>389</v>
       </c>
@@ -8801,7 +9295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>401</v>
       </c>
@@ -8854,7 +9348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>402</v>
       </c>
@@ -8907,7 +9401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>403</v>
       </c>
@@ -8945,7 +9439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>404</v>
       </c>
@@ -8983,7 +9477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>405</v>
       </c>
@@ -9021,7 +9515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>406</v>
       </c>
@@ -9059,7 +9553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>407</v>
       </c>
@@ -9097,7 +9591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>408</v>
       </c>
@@ -9135,7 +9629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>409</v>
       </c>
@@ -9173,7 +9667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>410</v>
       </c>
@@ -9196,7 +9690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>411</v>
       </c>
@@ -9219,7 +9713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>412</v>
       </c>
@@ -9242,7 +9736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>413</v>
       </c>
@@ -9265,7 +9759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>414</v>
       </c>
@@ -9288,7 +9782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>415</v>
       </c>
@@ -9305,7 +9799,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>416</v>
       </c>
@@ -9322,7 +9816,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>616</v>
       </c>
@@ -9339,7 +9833,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>624</v>
       </c>
@@ -9356,7 +9850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>634</v>
       </c>
@@ -9373,7 +9867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>637</v>
       </c>
@@ -9384,7 +9878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>638</v>
       </c>
@@ -9395,7 +9889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>645</v>
       </c>
@@ -9406,7 +9900,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>646</v>
       </c>
@@ -9417,7 +9911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>672</v>
       </c>
@@ -9428,7 +9922,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>673</v>
       </c>
@@ -9439,7 +9933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>674</v>
       </c>
@@ -9450,7 +9944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>685</v>
       </c>
@@ -9461,7 +9955,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>686</v>
       </c>
@@ -9472,7 +9966,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>687</v>
       </c>
@@ -9483,7 +9977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>688</v>
       </c>
@@ -9494,7 +9988,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>689</v>
       </c>
@@ -9505,7 +9999,66 @@
         <v>30</v>
       </c>
     </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A70" s="47" t="s">
+        <v>771</v>
+      </c>
+      <c r="B70" s="47"/>
+      <c r="C70" s="47"/>
+      <c r="D70" s="47"/>
+      <c r="E70" s="47"/>
+      <c r="F70" s="47"/>
+      <c r="G70" s="47"/>
+      <c r="H70" s="47"/>
+      <c r="I70" s="47"/>
+      <c r="J70" s="47"/>
+      <c r="K70" s="47"/>
+      <c r="L70" s="47"/>
+      <c r="M70" s="47"/>
+      <c r="N70" s="47"/>
+      <c r="O70" s="47"/>
+      <c r="P70" s="47"/>
+      <c r="Q70" s="47"/>
+      <c r="R70" s="47"/>
+      <c r="S70" s="47"/>
+      <c r="T70" s="47"/>
+      <c r="U70" s="47"/>
+      <c r="V70" s="47"/>
+      <c r="W70" s="47"/>
+      <c r="X70" s="47"/>
+      <c r="Y70" s="47"/>
+      <c r="Z70" s="47"/>
+      <c r="AA70" s="47"/>
+      <c r="AB70" s="47"/>
+    </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>798</v>
+      </c>
+      <c r="AA71" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>810</v>
+      </c>
+      <c r="AA72" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>811</v>
+      </c>
+      <c r="AA73" t="s">
+        <v>809</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A70:AB70"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes as per Module: Meeting Notes
Signed-off-by: ankur5579 <ankur@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1814DD93-90B5-4B10-A9E4-1353BB7F2FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8496D284-F132-4EA4-B070-9ACA1069B9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="919">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -2486,6 +2486,321 @@
   </si>
   <si>
     <t>areca</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>con 5&lt;break&gt;con 6&lt;break&gt;Sumo Logic&lt;break&gt;Vertica&lt;break&gt;Demo Deal&lt;break&gt;Mutual Fund</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity006</t>
+  </si>
+  <si>
+    <t>AMNNR_Con1</t>
+  </si>
+  <si>
+    <t>con 5</t>
+  </si>
+  <si>
+    <t>areca  moss fundraising should be tagged</t>
+  </si>
+  <si>
+    <t>con 5&lt;break&gt;con 6&lt;break&gt;+5</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity004</t>
+  </si>
+  <si>
+    <t>con 5&lt;break&gt;con 6&lt;break&gt;+10</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity005</t>
+  </si>
+  <si>
+    <t>All Records Select</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity007</t>
+  </si>
+  <si>
+    <t>Sales Meeting</t>
+  </si>
+  <si>
+    <t>Jhon&lt;break&gt;con 10&lt;break&gt;Sumo Logic</t>
+  </si>
+  <si>
+    <t>Golden Ret</t>
+  </si>
+  <si>
+    <t>Jhon&lt;break&gt;con 10&lt;break&gt;+2</t>
+  </si>
+  <si>
+    <t>Jhon&lt;break&gt;con 10&lt;break&gt;+3</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity008</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity009</t>
+  </si>
+  <si>
+    <t>Jhon</t>
+  </si>
+  <si>
+    <t>AMNNR_Con2</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity006</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity007</t>
+  </si>
+  <si>
+    <t>Marketing Strategy</t>
+  </si>
+  <si>
+    <t>We as an organization need to have certain strategy towards our marketing approch with Vertica and sumo logic Firm</t>
+  </si>
+  <si>
+    <t>Max&lt;break&gt;Jhon&lt;break&gt;con 11</t>
+  </si>
+  <si>
+    <t>Vertica&lt;break&gt;Sumo Logic</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;Vertica&lt;break&gt;Sumo Logic</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>keep in loop  con 4, con 5</t>
+  </si>
+  <si>
+    <t>Max&lt;break&gt;Jhon&lt;break&gt;+4</t>
+  </si>
+  <si>
+    <t>Max&lt;break&gt;Jhon&lt;break&gt;+6</t>
+  </si>
+  <si>
+    <t>con 4&lt;break&gt;con 5</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;con 4&lt;break&gt;con 5</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity010</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity011</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity012</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity008</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity009</t>
+  </si>
+  <si>
+    <t>AMNNR_Con3</t>
+  </si>
+  <si>
+    <t>Send Quote</t>
+  </si>
+  <si>
+    <t>unicorn</t>
+  </si>
+  <si>
+    <t>Maxtra&lt;break&gt;Martha&lt;break&gt;Jhon&lt;break&gt;con 11&lt;break&gt;Sumo Logic&lt;break&gt;Vertica</t>
+  </si>
+  <si>
+    <t>Martha</t>
+  </si>
+  <si>
+    <t>Palm areca</t>
+  </si>
+  <si>
+    <t>Martha&lt;break&gt;Jhon&lt;break&gt;+5</t>
+  </si>
+  <si>
+    <t>Martha&lt;break&gt;Jhon&lt;break&gt;+7</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;Palm&lt;break&gt;areca</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity013</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity014</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity010</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity011</t>
+  </si>
+  <si>
+    <t>AMNNR_Con4</t>
+  </si>
+  <si>
+    <t>Send Notice</t>
+  </si>
+  <si>
+    <t>Send Notice updated</t>
+  </si>
+  <si>
+    <t>Acc 3&lt;break&gt;Martha&lt;break&gt;Echo&lt;break&gt;Alexa&lt;break&gt;Green Pothos&lt;break&gt;areca</t>
+  </si>
+  <si>
+    <t>Acc 3</t>
+  </si>
+  <si>
+    <t>AMNNR_Record003</t>
+  </si>
+  <si>
+    <t>Martha&lt;break&gt;areca&lt;break&gt;+5</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity012</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity015</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity016</t>
+  </si>
+  <si>
+    <t>SSend Notice</t>
+  </si>
+  <si>
+    <t>echo alexa Green pothos areca</t>
+  </si>
+  <si>
+    <t>Acc 3&lt;break&gt;Martha</t>
+  </si>
+  <si>
+    <t>SSend Notice Follow up 1</t>
+  </si>
+  <si>
+    <t>SSend Notice Follow up 2</t>
+  </si>
+  <si>
+    <t>SSend Notice Follow up 3</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;Martha&lt;break&gt;+1</t>
+  </si>
+  <si>
+    <t>Martha&lt;break&gt;con 6&lt;break&gt;+5</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;con 6&lt;break&gt;con 7&lt;break&gt;con 8&lt;break&gt;Acc 4</t>
+  </si>
+  <si>
+    <t>con 6&lt;break&gt;con 7&lt;break&gt;con 8&lt;break&gt;Acc 4</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity017</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity018</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity019</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity020</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity021</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity013</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity014</t>
+  </si>
+  <si>
+    <t>Follow up task As Send Notice Updated for Con 6,Con 7, Con 8, Acc 4</t>
+  </si>
+  <si>
+    <t>Mutual Fund&lt;break&gt;FC Fundraising&lt;break&gt;Acc 1</t>
+  </si>
+  <si>
+    <t>Martha&lt;break&gt;con 6&lt;break&gt;+8</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity015</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity022</t>
+  </si>
+  <si>
+    <t>Task for the day</t>
+  </si>
+  <si>
+    <t>Follow up with Contacts Con 4, Con 5 about demo deal</t>
+  </si>
+  <si>
+    <t>Con 1&lt;break&gt;con 2&lt;break&gt;Acc 3&lt;break&gt;Maxtra</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity023</t>
+  </si>
+  <si>
+    <t>con 4&lt;break&gt;con 5&lt;break&gt;Demo Deal</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;con 4&lt;break&gt;con 5&lt;break&gt;Demo Deal</t>
+  </si>
+  <si>
+    <t>Con 1&lt;break&gt;con 2&lt;break&gt;+6</t>
+  </si>
+  <si>
+    <t>Maxtra&lt;break&gt;Demo Deal</t>
+  </si>
+  <si>
+    <t>Con 1&lt;break&gt;con 2&lt;break&gt;Acc 3&lt;break&gt;con 4&lt;break&gt;con 5</t>
+  </si>
+  <si>
+    <t>Con 1&lt;break&gt;con 2&lt;break&gt;+4</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity016</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity017</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity024</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity025</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity026</t>
+  </si>
+  <si>
+    <t>Task Test</t>
+  </si>
+  <si>
+    <t>Contact Invalid&lt;break&gt;Account Invalid</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity027</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity028</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity029</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity018</t>
   </si>
 </sst>
 </file>
@@ -3788,11 +4103,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4137,6 +4452,17 @@
         <v>804</v>
       </c>
       <c r="C50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>871</v>
+      </c>
+      <c r="B51" t="s">
+        <v>870</v>
+      </c>
+      <c r="C51" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4423,10 +4749,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4770,7 +5097,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>751</v>
       </c>
@@ -4787,7 +5114,55 @@
         <v>754</v>
       </c>
     </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="47" t="s">
+        <v>771</v>
+      </c>
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>817</v>
+      </c>
+      <c r="D37" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>834</v>
+      </c>
+      <c r="D38" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>853</v>
+      </c>
+      <c r="D39" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>866</v>
+      </c>
+      <c r="D40" t="s">
+        <v>857</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A36:I36"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
@@ -5087,11 +5462,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R124"/>
+  <dimension ref="A1:R148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G124" sqref="G124"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5247,11 +5622,11 @@
       </c>
       <c r="H5" s="34" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>01/07/2023</v>
+        <v>01/08/2023</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>01/07/2023</v>
+        <v>01/08/2023</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -8204,6 +8579,318 @@
         <v>813</v>
       </c>
     </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>816</v>
+      </c>
+      <c r="C125" t="s">
+        <v>814</v>
+      </c>
+      <c r="E125" t="s">
+        <v>815</v>
+      </c>
+      <c r="M125" t="s">
+        <v>609</v>
+      </c>
+      <c r="N125" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>825</v>
+      </c>
+      <c r="D126" s="20" t="s">
+        <v>819</v>
+      </c>
+      <c r="G126" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>831</v>
+      </c>
+      <c r="C127" t="s">
+        <v>826</v>
+      </c>
+      <c r="E127" t="s">
+        <v>827</v>
+      </c>
+      <c r="M127" t="s">
+        <v>609</v>
+      </c>
+      <c r="N127" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>832</v>
+      </c>
+      <c r="D128" s="20" t="s">
+        <v>828</v>
+      </c>
+      <c r="G128" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>848</v>
+      </c>
+      <c r="C129" t="s">
+        <v>837</v>
+      </c>
+      <c r="D129" s="20" t="s">
+        <v>838</v>
+      </c>
+      <c r="E129" t="s">
+        <v>839</v>
+      </c>
+      <c r="G129" t="s">
+        <v>840</v>
+      </c>
+      <c r="M129" t="s">
+        <v>605</v>
+      </c>
+      <c r="N129" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>849</v>
+      </c>
+      <c r="D130" s="20" t="s">
+        <v>843</v>
+      </c>
+      <c r="E130" t="s">
+        <v>841</v>
+      </c>
+      <c r="G130" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>850</v>
+      </c>
+      <c r="E131" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>862</v>
+      </c>
+      <c r="C132" t="s">
+        <v>854</v>
+      </c>
+      <c r="D132" s="20" t="s">
+        <v>855</v>
+      </c>
+      <c r="E132" t="s">
+        <v>856</v>
+      </c>
+      <c r="M132" t="s">
+        <v>325</v>
+      </c>
+      <c r="N132" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>863</v>
+      </c>
+      <c r="D133" s="20" t="s">
+        <v>858</v>
+      </c>
+      <c r="E133" t="s">
+        <v>861</v>
+      </c>
+      <c r="G133" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>874</v>
+      </c>
+      <c r="C134" t="s">
+        <v>867</v>
+      </c>
+      <c r="E134" t="s">
+        <v>869</v>
+      </c>
+      <c r="M134" t="s">
+        <v>325</v>
+      </c>
+      <c r="N134" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>875</v>
+      </c>
+      <c r="C135" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>886</v>
+      </c>
+      <c r="C136" t="s">
+        <v>876</v>
+      </c>
+      <c r="D136" s="20" t="s">
+        <v>877</v>
+      </c>
+      <c r="E136" t="s">
+        <v>878</v>
+      </c>
+      <c r="M136" t="s">
+        <v>325</v>
+      </c>
+      <c r="N136" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>887</v>
+      </c>
+      <c r="C137" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>888</v>
+      </c>
+      <c r="C138" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>889</v>
+      </c>
+      <c r="C139" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>890</v>
+      </c>
+      <c r="D140" s="20" t="s">
+        <v>893</v>
+      </c>
+      <c r="E140" t="s">
+        <v>884</v>
+      </c>
+      <c r="G140" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>897</v>
+      </c>
+      <c r="E141" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>901</v>
+      </c>
+      <c r="C142" t="s">
+        <v>898</v>
+      </c>
+      <c r="D142" s="20" t="s">
+        <v>899</v>
+      </c>
+      <c r="E142" t="s">
+        <v>900</v>
+      </c>
+      <c r="G142" t="s">
+        <v>902</v>
+      </c>
+      <c r="M142" t="s">
+        <v>325</v>
+      </c>
+      <c r="N142" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>910</v>
+      </c>
+      <c r="E143" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>911</v>
+      </c>
+      <c r="E144" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>912</v>
+      </c>
+      <c r="E145" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>915</v>
+      </c>
+      <c r="C146" t="s">
+        <v>913</v>
+      </c>
+      <c r="D146" s="20" t="s">
+        <v>899</v>
+      </c>
+      <c r="E146" t="s">
+        <v>900</v>
+      </c>
+      <c r="G146" t="s">
+        <v>902</v>
+      </c>
+      <c r="M146" t="s">
+        <v>325</v>
+      </c>
+      <c r="N146" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>916</v>
+      </c>
+      <c r="E147" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>917</v>
+      </c>
+      <c r="E148" t="s">
+        <v>914</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A119:Q119"/>
@@ -8216,11 +8903,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AB73"/>
+  <dimension ref="A1:AB88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10055,6 +10742,126 @@
         <v>809</v>
       </c>
     </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>821</v>
+      </c>
+      <c r="AA74" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>823</v>
+      </c>
+      <c r="AA75" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>835</v>
+      </c>
+      <c r="AA76" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>836</v>
+      </c>
+      <c r="AA77" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>851</v>
+      </c>
+      <c r="AA78" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>852</v>
+      </c>
+      <c r="AA79" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>864</v>
+      </c>
+      <c r="AA80" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>865</v>
+      </c>
+      <c r="AA81" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>873</v>
+      </c>
+      <c r="AA82" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>891</v>
+      </c>
+      <c r="AA83" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>892</v>
+      </c>
+      <c r="AA84" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>896</v>
+      </c>
+      <c r="AA85" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>908</v>
+      </c>
+      <c r="AA86" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>909</v>
+      </c>
+      <c r="AA87" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>918</v>
+      </c>
+      <c r="AA88" t="s">
+        <v>904</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A70:AB70"/>

</xml_diff>

<commit_message>
Changes as per Module Meeting Notes
Signed-off-by: ankur5579 <ankur@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8496D284-F132-4EA4-B070-9ACA1069B9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3558148A-ED62-478D-B00B-2C77B52A01F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16770" yWindow="1880" windowWidth="14400" windowHeight="7360" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="999">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -2801,6 +2801,246 @@
   </si>
   <si>
     <t>AMNNR_Acuity018</t>
+  </si>
+  <si>
+    <t>Task bulk contact</t>
+  </si>
+  <si>
+    <t>Max&lt;break&gt;Martha&lt;break&gt;Acc 3&lt;break&gt;Maxtra</t>
+  </si>
+  <si>
+    <t>Max&lt;break&gt;Martha&lt;break&gt;+3</t>
+  </si>
+  <si>
+    <t>Con 1, con 2, con 3, con 4, con 5, con 6, con 7, con 8, con 9, con 10, con 11, con 12, con 13, con 14, con 15, con 16, con 17, con 18, con 19, con 20, con 21, con 22, con 23, con 24, con 25, con 26, con 27, con 28, con 29, con 30, con 31, con 32, con 33, con 34, con 35, con 36, con 37, con 38, con 39, con 40, con 41, con 42, con 43, con 44, con 45, con 46, con 47, con 48, con 49, con 50</t>
+  </si>
+  <si>
+    <t>Con 1&lt;break&gt;con 2&lt;break&gt;con 3&lt;break&gt;con 4&lt;break&gt;con 5&lt;break&gt;con 6&lt;break&gt;con 7&lt;break&gt;con 8&lt;break&gt;con 9&lt;break&gt;con 10&lt;break&gt;con 11&lt;break&gt;con 12&lt;break&gt;con 13&lt;break&gt;con 14&lt;break&gt;con 15&lt;break&gt;con 16&lt;break&gt;con 17&lt;break&gt;con 18&lt;break&gt;con 19&lt;break&gt;con 20&lt;break&gt;con 21&lt;break&gt;con 22&lt;break&gt;con 23&lt;break&gt;con 24&lt;break&gt;con 25&lt;break&gt;con 26&lt;break&gt;con 27&lt;break&gt;con 28&lt;break&gt;con 29&lt;break&gt;con 30&lt;break&gt;con 31&lt;break&gt;con 32&lt;break&gt;con 33&lt;break&gt;con 34&lt;break&gt;con 35&lt;break&gt;con 36&lt;break&gt;con 37&lt;break&gt;con 38&lt;break&gt;con 39&lt;break&gt;con 40&lt;break&gt;con 41&lt;break&gt;con 42&lt;break&gt;con 43&lt;break&gt;con 44&lt;break&gt;con 45&lt;break&gt;con 46&lt;break&gt;con 47&lt;break&gt;con 48</t>
+  </si>
+  <si>
+    <t>Max&lt;break&gt;Martha&lt;break&gt;+51</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;Con 1&lt;break&gt;con 2&lt;break&gt;con 3&lt;break&gt;con 4&lt;break&gt;con 5&lt;break&gt;con 6&lt;break&gt;con 7&lt;break&gt;con 8&lt;break&gt;con 9&lt;break&gt;con 10&lt;break&gt;con 11&lt;break&gt;con 12&lt;break&gt;con 13&lt;break&gt;con 14&lt;break&gt;con 15&lt;break&gt;con 16&lt;break&gt;con 17&lt;break&gt;con 18&lt;break&gt;con 19&lt;break&gt;con 20&lt;break&gt;con 21&lt;break&gt;con 22&lt;break&gt;con 23&lt;break&gt;con 24&lt;break&gt;con 25&lt;break&gt;con 26&lt;break&gt;con 27&lt;break&gt;con 28&lt;break&gt;con 29&lt;break&gt;con 30&lt;break&gt;con 31&lt;break&gt;con 32&lt;break&gt;con 33&lt;break&gt;con 34&lt;break&gt;con 35&lt;break&gt;con 36&lt;break&gt;con 37&lt;break&gt;con 38&lt;break&gt;con 39&lt;break&gt;con 40&lt;break&gt;con 41&lt;break&gt;con 42&lt;break&gt;con 43&lt;break&gt;con 44&lt;break&gt;con 45&lt;break&gt;con 46&lt;break&gt;con 47&lt;break&gt;con 48</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity030</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity031</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity019</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity020</t>
+  </si>
+  <si>
+    <t>Task bulk Firm contact</t>
+  </si>
+  <si>
+    <t>Max&lt;break&gt;Martha&lt;break&gt;Vertica&lt;break&gt;Maxtra</t>
+  </si>
+  <si>
+    <t>Con 1, con 2, con 3, con 4, con 5, con 6, con 7, con 8, con 9, con 10, con 11, con 12, con 13, con 14, con 15, con 16, con 17, con 18, con 19, con 20, con 21, con 22, con 23, con 24, con 25, con 26, con 27, con 28, con 29, con 30, con 31, con 32, con 33, con 34, con 35, con 36, con 37, con 38, con 39, con 40, con 41, con 42, con 43, con 44, con 45, con 46, con 47, con 48, con 49, con 50, Acc 1, Acc 2, Acc 3, Acc 4, Acc 5, Acc 6, Acc 7, Acc 8, Acc 9, Acc 10, Acc 11, Acc 12, Acc 13</t>
+  </si>
+  <si>
+    <t>Con 1&lt;break&gt;con 2&lt;break&gt;con 3&lt;break&gt;con 4&lt;break&gt;con 5&lt;break&gt;con 6&lt;break&gt;con 7&lt;break&gt;con 8&lt;break&gt;con 9&lt;break&gt;con 10&lt;break&gt;con 11&lt;break&gt;con 12&lt;break&gt;con 13&lt;break&gt;con 14&lt;break&gt;con 15&lt;break&gt;con 16&lt;break&gt;con 17&lt;break&gt;con 18&lt;break&gt;con 19&lt;break&gt;con 20&lt;break&gt;con 21&lt;break&gt;con 22&lt;break&gt;con 23&lt;break&gt;con 24&lt;break&gt;con 25&lt;break&gt;con 26&lt;break&gt;con 27&lt;break&gt;con 28&lt;break&gt;con 29&lt;break&gt;con 30&lt;break&gt;con 31&lt;break&gt;con 32&lt;break&gt;con 33&lt;break&gt;con 34&lt;break&gt;con 35&lt;break&gt;con 36&lt;break&gt;con 37&lt;break&gt;con 38&lt;break&gt;con 39&lt;break&gt;con 40&lt;break&gt;con 41&lt;break&gt;con 42&lt;break&gt;con 43&lt;break&gt;con 44&lt;break&gt;con 45&lt;break&gt;con 46&lt;break&gt;con 47&lt;break&gt;con 48&lt;break&gt;Acc 1&lt;break&gt;Acc 2&lt;break&gt;Acc 3&lt;break&gt;Acc 4&lt;break&gt;Acc 5&lt;break&gt;Acc 6&lt;break&gt;Acc 7&lt;break&gt;Acc 8&lt;break&gt;Acc 9&lt;break&gt;Acc 10&lt;break&gt;Acc 11&lt;break&gt;Acc 12&lt;break&gt;Acc 13</t>
+  </si>
+  <si>
+    <t>Max&lt;break&gt;Martha&lt;break&gt;+64</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;Con 1&lt;break&gt;con 2&lt;break&gt;con 3&lt;break&gt;con 4&lt;break&gt;con 5&lt;break&gt;con 6&lt;break&gt;con 7&lt;break&gt;con 8&lt;break&gt;con 9&lt;break&gt;con 10&lt;break&gt;con 11&lt;break&gt;con 12&lt;break&gt;con 13&lt;break&gt;con 14&lt;break&gt;con 15&lt;break&gt;con 16&lt;break&gt;con 17&lt;break&gt;con 18&lt;break&gt;con 19&lt;break&gt;con 20&lt;break&gt;con 21&lt;break&gt;con 22&lt;break&gt;con 23&lt;break&gt;con 24&lt;break&gt;con 25&lt;break&gt;con 26&lt;break&gt;con 27&lt;break&gt;con 28&lt;break&gt;con 29&lt;break&gt;con 30&lt;break&gt;con 31&lt;break&gt;con 32&lt;break&gt;con 33&lt;break&gt;con 34&lt;break&gt;con 35&lt;break&gt;con 36&lt;break&gt;con 37&lt;break&gt;con 38&lt;break&gt;con 39&lt;break&gt;con 40&lt;break&gt;con 41&lt;break&gt;con 42&lt;break&gt;con 43&lt;break&gt;con 44&lt;break&gt;con 45&lt;break&gt;con 46&lt;break&gt;con 47&lt;break&gt;con 48&lt;break&gt;Acc 1&lt;break&gt;Acc 2&lt;break&gt;Acc 3&lt;break&gt;Acc 4&lt;break&gt;Acc 5&lt;break&gt;Acc 6&lt;break&gt;Acc 7&lt;break&gt;Acc 8&lt;break&gt;Acc 9&lt;break&gt;Acc 10&lt;break&gt;Acc 11&lt;break&gt;Acc 12&lt;break&gt;Acc 13</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity032</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity033</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity021</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity022</t>
+  </si>
+  <si>
+    <t>Task Custom Object</t>
+  </si>
+  <si>
+    <t>Send the quotation to Martha, jhon, con 11 and Custom Object 1.1 belonging to the Firm Nexus, Custom Object 1.2</t>
+  </si>
+  <si>
+    <t>Martha&lt;break&gt;Jhon&lt;break&gt;con 11&lt;break&gt;Sumo Logic&lt;break&gt;Vertica</t>
+  </si>
+  <si>
+    <t>Custom Object 1.1&lt;break&gt;Custom Object 1.2&lt;break&gt;Custom Object 1.3</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;Custom Object 1.1&lt;break&gt;Custom Object 1.2&lt;break&gt;Custom Object 1.3</t>
+  </si>
+  <si>
+    <t>con 11&lt;break&gt;Sumo Logic&lt;break&gt;Vertica&lt;break&gt;Custom Object 1.1&lt;break&gt;Custom Object 1.2&lt;break&gt;Custom Object 1.3</t>
+  </si>
+  <si>
+    <t>keep in loop  con 4, con 5 Acc 5, Custom Object 1.2, Custom object 1.3</t>
+  </si>
+  <si>
+    <t>con 4&lt;break&gt;con 5&lt;break&gt;Acc 5</t>
+  </si>
+  <si>
+    <t>Martha&lt;break&gt;Jhon&lt;break&gt;+10</t>
+  </si>
+  <si>
+    <t>con 11&lt;break&gt;Sumo Logic&lt;break&gt;Vertica&lt;break&gt;Custom Object 1.1&lt;break&gt;Custom Object 1.2&lt;break&gt;Custom Object 1.3&lt;break&gt;con 4&lt;break&gt;con 5&lt;break&gt;Acc 5</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;con 4&lt;break&gt;con 5&lt;break&gt;Acc 5</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity034</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity035</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity036</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity037</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity038</t>
+  </si>
+  <si>
+    <t>Task Demo</t>
+  </si>
+  <si>
+    <t>Follow up with Contacts con 4, con 5 about Demo Deal</t>
+  </si>
+  <si>
+    <t>Acc 3&lt;break&gt;con 4&lt;break&gt;con 5</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity039</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity040</t>
+  </si>
+  <si>
+    <t>Task Advance</t>
+  </si>
+  <si>
+    <t>Maxjonic&lt;break&gt;Maxtra&lt;break&gt;Con 1&lt;break&gt;con 2</t>
+  </si>
+  <si>
+    <t>Maxjonic</t>
+  </si>
+  <si>
+    <t>Intermediary</t>
+  </si>
+  <si>
+    <t>AMNNR_Record004</t>
+  </si>
+  <si>
+    <t>Maxjonic&lt;break&gt;Maxtra&lt;break&gt;con 4&lt;break&gt;con 5&lt;break&gt;Demo Deal</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity041</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity042</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity043</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity023</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity024</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity025</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity026</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity027</t>
+  </si>
+  <si>
+    <t>Task Advance Updated</t>
+  </si>
+  <si>
+    <t>Task TQW</t>
+  </si>
+  <si>
+    <t>Areca</t>
+  </si>
+  <si>
+    <t>Acc 12</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;areca</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>AMNNR_Record005</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sumo Kind</t>
+  </si>
+  <si>
+    <t>Sumo Kind==Firm&lt;break&gt;Sumo Kind==Deal&lt;break&gt;Sumo Kind==Contact&lt;break&gt;Sumo Kind Fund==Fund&lt;break&gt;Sumo Kind Fundraising==Fundraising</t>
+  </si>
+  <si>
+    <t>Acc 12==Firm&lt;break&gt;areca==Contact</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity044</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity045</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity046</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity047</t>
+  </si>
+  <si>
+    <t>&lt;break&gt;areca&lt;break&gt;+1</t>
+  </si>
+  <si>
+    <t>areca&lt;break&gt;Sumo Kind&lt;break&gt;+6</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity028</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity029</t>
+  </si>
+  <si>
+    <t>Task Demo 3</t>
+  </si>
+  <si>
+    <t>Acc 3&lt;break&gt;Maxtra&lt;break&gt;Con 1&lt;break&gt;con 2&lt;break&gt;Demo Deal</t>
+  </si>
+  <si>
+    <t>con 6&lt;break&gt;con 7</t>
+  </si>
+  <si>
+    <t>Acc 3&lt;break&gt;Maxtra&lt;break&gt;Demo Deal</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity048</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity049</t>
   </si>
 </sst>
 </file>
@@ -4103,11 +4343,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4464,6 +4704,28 @@
       </c>
       <c r="C51" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>965</v>
+      </c>
+      <c r="B52" t="s">
+        <v>963</v>
+      </c>
+      <c r="C52" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>981</v>
+      </c>
+      <c r="B53" t="s">
+        <v>978</v>
+      </c>
+      <c r="C53" t="s">
+        <v>980</v>
       </c>
     </row>
   </sheetData>
@@ -4753,7 +5015,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5462,11 +5724,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R148"/>
+  <dimension ref="A1:R168"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G146" sqref="G146"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5622,11 +5884,11 @@
       </c>
       <c r="H5" s="34" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>01/08/2023</v>
+        <v>01/09/2023</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>01/08/2023</v>
+        <v>01/09/2023</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -8891,6 +9153,274 @@
         <v>914</v>
       </c>
     </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>926</v>
+      </c>
+      <c r="C149" t="s">
+        <v>919</v>
+      </c>
+      <c r="E149" t="s">
+        <v>920</v>
+      </c>
+      <c r="M149" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="N149" s="7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>927</v>
+      </c>
+      <c r="D150" s="20" t="s">
+        <v>922</v>
+      </c>
+      <c r="E150" t="s">
+        <v>925</v>
+      </c>
+      <c r="G150" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>936</v>
+      </c>
+      <c r="C151" t="s">
+        <v>930</v>
+      </c>
+      <c r="E151" t="s">
+        <v>931</v>
+      </c>
+      <c r="M151" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="N151" s="7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>937</v>
+      </c>
+      <c r="D152" s="20" t="s">
+        <v>932</v>
+      </c>
+      <c r="E152" t="s">
+        <v>935</v>
+      </c>
+      <c r="G152" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>951</v>
+      </c>
+      <c r="C153" t="s">
+        <v>940</v>
+      </c>
+      <c r="D153" s="20" t="s">
+        <v>941</v>
+      </c>
+      <c r="E153" t="s">
+        <v>942</v>
+      </c>
+      <c r="G153" t="s">
+        <v>943</v>
+      </c>
+      <c r="M153" t="s">
+        <v>325</v>
+      </c>
+      <c r="N153" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>952</v>
+      </c>
+      <c r="D154" s="20" t="s">
+        <v>946</v>
+      </c>
+      <c r="E154" t="s">
+        <v>944</v>
+      </c>
+      <c r="G154" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>953</v>
+      </c>
+      <c r="E155" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>954</v>
+      </c>
+      <c r="E156" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>955</v>
+      </c>
+      <c r="E157" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>959</v>
+      </c>
+      <c r="C158" t="s">
+        <v>956</v>
+      </c>
+      <c r="D158" s="20" t="s">
+        <v>957</v>
+      </c>
+      <c r="E158" t="s">
+        <v>900</v>
+      </c>
+      <c r="G158" t="s">
+        <v>902</v>
+      </c>
+      <c r="M158" t="s">
+        <v>325</v>
+      </c>
+      <c r="N158" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>960</v>
+      </c>
+      <c r="E159" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>967</v>
+      </c>
+      <c r="E160" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>968</v>
+      </c>
+      <c r="C161" t="s">
+        <v>961</v>
+      </c>
+      <c r="D161" s="20" t="s">
+        <v>899</v>
+      </c>
+      <c r="E161" t="s">
+        <v>962</v>
+      </c>
+      <c r="G161" t="s">
+        <v>902</v>
+      </c>
+      <c r="M161" t="s">
+        <v>605</v>
+      </c>
+      <c r="N161" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>969</v>
+      </c>
+      <c r="E162" t="s">
+        <v>903</v>
+      </c>
+      <c r="M162" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>985</v>
+      </c>
+      <c r="C163" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>986</v>
+      </c>
+      <c r="C164" t="s">
+        <v>976</v>
+      </c>
+      <c r="D164" s="20" t="s">
+        <v>977</v>
+      </c>
+      <c r="E164" t="s">
+        <v>978</v>
+      </c>
+      <c r="G164" t="s">
+        <v>813</v>
+      </c>
+      <c r="M164" t="s">
+        <v>325</v>
+      </c>
+      <c r="N164" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>987</v>
+      </c>
+      <c r="D165" s="20" t="s">
+        <v>982</v>
+      </c>
+      <c r="E165" t="s">
+        <v>979</v>
+      </c>
+      <c r="G165" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>988</v>
+      </c>
+      <c r="E166" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>997</v>
+      </c>
+      <c r="C167" t="s">
+        <v>993</v>
+      </c>
+      <c r="E167" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>998</v>
+      </c>
+      <c r="E168" t="s">
+        <v>995</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A119:Q119"/>
@@ -8903,11 +9433,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AB88"/>
+  <dimension ref="A1:AB100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B88" sqref="B88"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10798,7 +11328,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>865</v>
       </c>
@@ -10806,7 +11336,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>873</v>
       </c>
@@ -10814,7 +11344,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>891</v>
       </c>
@@ -10822,7 +11352,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>892</v>
       </c>
@@ -10830,7 +11360,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>896</v>
       </c>
@@ -10838,7 +11368,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>908</v>
       </c>
@@ -10846,7 +11376,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>909</v>
       </c>
@@ -10854,12 +11384,117 @@
         <v>907</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>918</v>
       </c>
       <c r="AA88" t="s">
         <v>904</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>928</v>
+      </c>
+      <c r="AA89" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>929</v>
+      </c>
+      <c r="AA90" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>938</v>
+      </c>
+      <c r="AA91" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="92" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>939</v>
+      </c>
+      <c r="AA92" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>970</v>
+      </c>
+      <c r="AA93" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>971</v>
+      </c>
+      <c r="AA94" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>972</v>
+      </c>
+      <c r="AA95" t="s">
+        <v>904</v>
+      </c>
+      <c r="AB95" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>973</v>
+      </c>
+      <c r="AA96" t="s">
+        <v>907</v>
+      </c>
+      <c r="AB96" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>974</v>
+      </c>
+      <c r="AA97" t="s">
+        <v>904</v>
+      </c>
+      <c r="AB97" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="98" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>991</v>
+      </c>
+      <c r="AA98" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>992</v>
+      </c>
+      <c r="AA99" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AA100" t="s">
+        <v>907</v>
+      </c>
+      <c r="AB100" t="s">
+        <v>996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data to Datasheet
Signed-off-by: ankur5579 <ankur@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3558148A-ED62-478D-B00B-2C77B52A01F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469AC955-CC52-4B64-A4A6-228010535C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16770" yWindow="1880" windowWidth="14400" windowHeight="7360" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="999">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="1000">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -3041,6 +3041,9 @@
   </si>
   <si>
     <t>AMNNR_Activity049</t>
+  </si>
+  <si>
+    <t>AMNNR_Acuity030</t>
   </si>
 </sst>
 </file>
@@ -5728,7 +5731,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C170" sqref="C170"/>
+      <selection pane="bottomLeft" activeCell="A167" sqref="A167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9412,6 +9415,12 @@
       <c r="E167" t="s">
         <v>994</v>
       </c>
+      <c r="M167" t="s">
+        <v>325</v>
+      </c>
+      <c r="N167" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
@@ -9437,7 +9446,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
+      <selection pane="bottomLeft" activeCell="A98" sqref="A98:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11490,6 +11499,9 @@
       </c>
     </row>
     <row r="100" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>999</v>
+      </c>
       <c r="AA100" t="s">
         <v>907</v>
       </c>

</xml_diff>

<commit_message>
Changes as per Module RG Meeting Notes
Signed-off-by: ankur5579 <ankur@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2597AF-2D94-4770-8140-0CEDC90B9AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB430CD-906F-438B-9588-E4CE8687DF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="1099">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -3323,6 +3323,27 @@
   </si>
   <si>
     <t>TextBox</t>
+  </si>
+  <si>
+    <t>Task bulk contact Call Follow Up</t>
+  </si>
+  <si>
+    <t>con 15</t>
+  </si>
+  <si>
+    <t>AMNNR_Con5</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity055</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity056</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity057</t>
+  </si>
+  <si>
+    <t>AMNNR_Activity058</t>
   </si>
 </sst>
 </file>
@@ -3585,18 +3606,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3611,6 +3620,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4128,8 +4149,8 @@
   <dimension ref="A1:AB107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76:AB107"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6025,36 +6046,36 @@
       </c>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A76" s="49" t="s">
+      <c r="A76" s="54" t="s">
         <v>762</v>
       </c>
-      <c r="B76" s="49"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
-      <c r="E76" s="49"/>
-      <c r="F76" s="49"/>
-      <c r="G76" s="49"/>
-      <c r="H76" s="49"/>
-      <c r="I76" s="49"/>
-      <c r="J76" s="49"/>
-      <c r="K76" s="49"/>
-      <c r="L76" s="49"/>
-      <c r="M76" s="49"/>
-      <c r="N76" s="49"/>
-      <c r="O76" s="49"/>
-      <c r="P76" s="49"/>
-      <c r="Q76" s="49"/>
-      <c r="R76" s="49"/>
-      <c r="S76" s="49"/>
-      <c r="T76" s="49"/>
-      <c r="U76" s="49"/>
-      <c r="V76" s="49"/>
-      <c r="W76" s="49"/>
-      <c r="X76" s="49"/>
-      <c r="Y76" s="49"/>
-      <c r="Z76" s="49"/>
-      <c r="AA76" s="49"/>
-      <c r="AB76" s="49"/>
+      <c r="B76" s="54"/>
+      <c r="C76" s="54"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="54"/>
+      <c r="F76" s="54"/>
+      <c r="G76" s="54"/>
+      <c r="H76" s="54"/>
+      <c r="I76" s="54"/>
+      <c r="J76" s="54"/>
+      <c r="K76" s="54"/>
+      <c r="L76" s="54"/>
+      <c r="M76" s="54"/>
+      <c r="N76" s="54"/>
+      <c r="O76" s="54"/>
+      <c r="P76" s="54"/>
+      <c r="Q76" s="54"/>
+      <c r="R76" s="54"/>
+      <c r="S76" s="54"/>
+      <c r="T76" s="54"/>
+      <c r="U76" s="54"/>
+      <c r="V76" s="54"/>
+      <c r="W76" s="54"/>
+      <c r="X76" s="54"/>
+      <c r="Y76" s="54"/>
+      <c r="Z76" s="54"/>
+      <c r="AA76" s="54"/>
+      <c r="AB76" s="54"/>
     </row>
     <row r="77" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
@@ -6508,13 +6529,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="53" t="s">
         <v>762</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
@@ -6696,22 +6717,22 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="55" t="s">
         <v>762</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
@@ -6828,13 +6849,13 @@
       <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="55" t="s">
         <v>762</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
       <c r="F3" s="41"/>
       <c r="G3" s="43"/>
       <c r="H3" s="43"/>
@@ -6874,8 +6895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8FE239-7966-4B47-902D-BB193CC8E9D4}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6893,7 +6914,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -6914,7 +6935,7 @@
       <c r="G1" s="1" t="s">
         <v>1079</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="48" t="s">
         <v>771</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -6940,39 +6961,39 @@
         <v>762</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="52"/>
+      <c r="H3" s="48"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="49" t="s">
         <v>1084</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="50" t="s">
         <v>1085</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="50" t="s">
         <v>1086</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55" t="s">
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="51" t="s">
         <v>1087</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="50" t="s">
         <v>1088</v>
       </c>
-      <c r="H4" s="54" t="s">
+      <c r="H4" s="50" t="s">
         <v>1089</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="50" t="s">
         <v>1090</v>
       </c>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54" t="s">
+      <c r="J4" s="50"/>
+      <c r="K4" s="50" t="s">
         <v>1091</v>
       </c>
-      <c r="L4" s="54"/>
+      <c r="L4" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7014,11 +7035,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -7323,13 +7344,13 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="48" t="s">
+      <c r="A48" s="53" t="s">
         <v>762</v>
       </c>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
@@ -7431,10 +7452,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="53"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -7680,11 +7701,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8066,17 +8087,17 @@
       <c r="F35" s="3"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="54" t="s">
         <v>762</v>
       </c>
-      <c r="B37" s="49"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -8108,6 +8129,14 @@
       </c>
       <c r="D41" t="s">
         <v>848</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1093</v>
       </c>
     </row>
   </sheetData>
@@ -8330,16 +8359,16 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="53" t="s">
         <v>762</v>
       </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
@@ -8428,11 +8457,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R182"/>
+  <dimension ref="A1:R186"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E126" sqref="E126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H182" sqref="H182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8588,11 +8617,11 @@
       </c>
       <c r="H5" s="34" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>01/10/2023</v>
+        <v>01/12/2023</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>01/10/2023</v>
+        <v>01/12/2023</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -11642,25 +11671,25 @@
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A128" s="49" t="s">
+      <c r="A128" s="54" t="s">
         <v>762</v>
       </c>
-      <c r="B128" s="49"/>
-      <c r="C128" s="49"/>
-      <c r="D128" s="49"/>
-      <c r="E128" s="49"/>
-      <c r="F128" s="49"/>
-      <c r="G128" s="49"/>
-      <c r="H128" s="49"/>
-      <c r="I128" s="49"/>
-      <c r="J128" s="49"/>
-      <c r="K128" s="49"/>
-      <c r="L128" s="49"/>
-      <c r="M128" s="49"/>
-      <c r="N128" s="49"/>
-      <c r="O128" s="49"/>
-      <c r="P128" s="49"/>
-      <c r="Q128" s="49"/>
+      <c r="B128" s="54"/>
+      <c r="C128" s="54"/>
+      <c r="D128" s="54"/>
+      <c r="E128" s="54"/>
+      <c r="F128" s="54"/>
+      <c r="G128" s="54"/>
+      <c r="H128" s="54"/>
+      <c r="I128" s="54"/>
+      <c r="J128" s="54"/>
+      <c r="K128" s="54"/>
+      <c r="L128" s="54"/>
+      <c r="M128" s="54"/>
+      <c r="N128" s="54"/>
+      <c r="O128" s="54"/>
+      <c r="P128" s="54"/>
+      <c r="Q128" s="54"/>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
@@ -12395,6 +12424,32 @@
       </c>
       <c r="P182" t="s">
         <v>605</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C183" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E183" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>1098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CHanges as per module RG Meeting Notes Notification Reminder
Signed-off-by: ankur5579 <ankur@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0036AC-51A9-4388-B50C-115C06CD3BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8DEBC2-3684-4820-8C6C-D8B410CB1FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -20,10 +20,11 @@
     <sheet name="Acuity" sheetId="6" r:id="rId10"/>
     <sheet name="Reports" sheetId="8" r:id="rId11"/>
     <sheet name="Fund" sheetId="4" r:id="rId12"/>
-    <sheet name="Fundraisings" sheetId="10" r:id="rId13"/>
-    <sheet name="User" sheetId="13" r:id="rId14"/>
-    <sheet name="Test Custom Object" sheetId="16" r:id="rId15"/>
-    <sheet name="ListView" sheetId="18" r:id="rId16"/>
+    <sheet name="DetailPage" sheetId="19" r:id="rId13"/>
+    <sheet name="Fundraisings" sheetId="10" r:id="rId14"/>
+    <sheet name="User" sheetId="13" r:id="rId15"/>
+    <sheet name="Test Custom Object" sheetId="16" r:id="rId16"/>
+    <sheet name="ListView" sheetId="18" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Activity Timeline'!$B$1:$B$114</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="1250">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -3578,6 +3579,225 @@
   </si>
   <si>
     <t>RGAMNNR_Activity019</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity020</t>
+  </si>
+  <si>
+    <t>Task For Notification Check</t>
+  </si>
+  <si>
+    <t>con 3&lt;break&gt;Acc 12</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Con8</t>
+  </si>
+  <si>
+    <t>con 10</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Record007</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity021</t>
+  </si>
+  <si>
+    <t>Call For Notification Check</t>
+  </si>
+  <si>
+    <t>Event 2.0</t>
+  </si>
+  <si>
+    <t>Adding @Glomez @Jack in the loop</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity022</t>
+  </si>
+  <si>
+    <t>Marketing Webinar 2</t>
+  </si>
+  <si>
+    <t>Deal @sumo logic and @Max fund should be in loop</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity023</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity024</t>
+  </si>
+  <si>
+    <t>Mulesoft Connect</t>
+  </si>
+  <si>
+    <t>dealroom1.3+lomez@gmail.com,Dealroom1.3+James@gmail.com</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity025</t>
+  </si>
+  <si>
+    <t>Relive salesforce Live 1&lt;break&gt;Relive salesforce Live 2&lt;break&gt;Relive salesforce Live 3&lt;break&gt;Relive salesforce Live 4</t>
+  </si>
+  <si>
+    <t>dealroom1.3+con1@gmail.com,dealroom1.3+con2@gmail.com</t>
+  </si>
+  <si>
+    <t>Acc 11</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Record008</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity026</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity027</t>
+  </si>
+  <si>
+    <t>This event will have your Business circles talking +4</t>
+  </si>
+  <si>
+    <t>Dealroom1.3+Lomez@gmail.com,Dealroom1.3+Max@gmail.com,Dealroom1.3+James@gmail.com</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity028</t>
+  </si>
+  <si>
+    <t>updated</t>
+  </si>
+  <si>
+    <t>Relive salesforce Live 1</t>
+  </si>
+  <si>
+    <t>Acc 11, Con 1, con 2</t>
+  </si>
+  <si>
+    <t>SuggestedPopUpShouldNotThere</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity029</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity030</t>
+  </si>
+  <si>
+    <t>Webinar 1 all day</t>
+  </si>
+  <si>
+    <t>Dealroom1.3+James@gmail.com,Dealroom1.3+Lenis@gmail.com</t>
+  </si>
+  <si>
+    <t>Lenis</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Con9</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity031</t>
+  </si>
+  <si>
+    <t>Salesforce Event</t>
+  </si>
+  <si>
+    <t>Dealroom1.3+Litz@gmail.com,Dealroom1.3+Jhon@gmail.com</t>
+  </si>
+  <si>
+    <t>Salesforce Event Updated</t>
+  </si>
+  <si>
+    <t>Sumo Logic, Vertica, Demo Deal</t>
+  </si>
+  <si>
+    <t>James, Jhon, Litz</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity032</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity033</t>
+  </si>
+  <si>
+    <t>Outlook Private Event</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity034</t>
+  </si>
+  <si>
+    <t>Outlook Event Test</t>
+  </si>
+  <si>
+    <t>cont1.test@zxc.com,cont2+test@zxc.com;</t>
+  </si>
+  <si>
+    <t>Added the event in outlook to tag users and Contacts Con1</t>
+  </si>
+  <si>
+    <t>cont1 test</t>
+  </si>
+  <si>
+    <t>cont2+test</t>
+  </si>
+  <si>
+    <t>zxc.com</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Record009</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Record010</t>
+  </si>
+  <si>
+    <t>cont1.test@zxc.com</t>
+  </si>
+  <si>
+    <t>cont2+test@zxc.com</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity035</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Con10</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Con11</t>
+  </si>
+  <si>
+    <t>Outlook Event Test Firm</t>
+  </si>
+  <si>
+    <t>cont3.test@carlylegroup-ng.com,cont4+test@carlylegroup-ng.com;</t>
+  </si>
+  <si>
+    <t>cont3 test</t>
+  </si>
+  <si>
+    <t>carlylegroup-ng.com</t>
+  </si>
+  <si>
+    <t>cont4+test</t>
+  </si>
+  <si>
+    <t>cont3.test@carlylegroup-ng.com</t>
+  </si>
+  <si>
+    <t>cont4+test@carlylegroup-ng.com</t>
+  </si>
+  <si>
+    <t>Assign Multiple Associations</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Activity036</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Con12</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Con13</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Record011</t>
+  </si>
+  <si>
+    <t>RGAMNNR_Record012</t>
   </si>
 </sst>
 </file>
@@ -3855,6 +4075,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3867,7 +4088,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4385,7 +4605,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A114" sqref="A114"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6281,36 +6501,36 @@
       </c>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A76" s="54" t="s">
+      <c r="A76" s="55" t="s">
         <v>762</v>
       </c>
-      <c r="B76" s="54"/>
-      <c r="C76" s="54"/>
-      <c r="D76" s="54"/>
-      <c r="E76" s="54"/>
-      <c r="F76" s="54"/>
-      <c r="G76" s="54"/>
-      <c r="H76" s="54"/>
-      <c r="I76" s="54"/>
-      <c r="J76" s="54"/>
-      <c r="K76" s="54"/>
-      <c r="L76" s="54"/>
-      <c r="M76" s="54"/>
-      <c r="N76" s="54"/>
-      <c r="O76" s="54"/>
-      <c r="P76" s="54"/>
-      <c r="Q76" s="54"/>
-      <c r="R76" s="54"/>
-      <c r="S76" s="54"/>
-      <c r="T76" s="54"/>
-      <c r="U76" s="54"/>
-      <c r="V76" s="54"/>
-      <c r="W76" s="54"/>
-      <c r="X76" s="54"/>
-      <c r="Y76" s="54"/>
-      <c r="Z76" s="54"/>
-      <c r="AA76" s="54"/>
-      <c r="AB76" s="54"/>
+      <c r="B76" s="55"/>
+      <c r="C76" s="55"/>
+      <c r="D76" s="55"/>
+      <c r="E76" s="55"/>
+      <c r="F76" s="55"/>
+      <c r="G76" s="55"/>
+      <c r="H76" s="55"/>
+      <c r="I76" s="55"/>
+      <c r="J76" s="55"/>
+      <c r="K76" s="55"/>
+      <c r="L76" s="55"/>
+      <c r="M76" s="55"/>
+      <c r="N76" s="55"/>
+      <c r="O76" s="55"/>
+      <c r="P76" s="55"/>
+      <c r="Q76" s="55"/>
+      <c r="R76" s="55"/>
+      <c r="S76" s="55"/>
+      <c r="T76" s="55"/>
+      <c r="U76" s="55"/>
+      <c r="V76" s="55"/>
+      <c r="W76" s="55"/>
+      <c r="X76" s="55"/>
+      <c r="Y76" s="55"/>
+      <c r="Z76" s="55"/>
+      <c r="AA76" s="55"/>
+      <c r="AB76" s="55"/>
     </row>
     <row r="77" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
@@ -6573,36 +6793,36 @@
       </c>
     </row>
     <row r="111" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A111" s="54" t="s">
+      <c r="A111" s="55" t="s">
         <v>762</v>
       </c>
-      <c r="B111" s="54"/>
-      <c r="C111" s="54"/>
-      <c r="D111" s="54"/>
-      <c r="E111" s="54"/>
-      <c r="F111" s="54"/>
-      <c r="G111" s="54"/>
-      <c r="H111" s="54"/>
-      <c r="I111" s="54"/>
-      <c r="J111" s="54"/>
-      <c r="K111" s="54"/>
-      <c r="L111" s="54"/>
-      <c r="M111" s="54"/>
-      <c r="N111" s="54"/>
-      <c r="O111" s="54"/>
-      <c r="P111" s="54"/>
-      <c r="Q111" s="54"/>
-      <c r="R111" s="54"/>
-      <c r="S111" s="54"/>
-      <c r="T111" s="54"/>
-      <c r="U111" s="54"/>
-      <c r="V111" s="54"/>
-      <c r="W111" s="54"/>
-      <c r="X111" s="54"/>
-      <c r="Y111" s="54"/>
-      <c r="Z111" s="54"/>
-      <c r="AA111" s="54"/>
-      <c r="AB111" s="54"/>
+      <c r="B111" s="55"/>
+      <c r="C111" s="55"/>
+      <c r="D111" s="55"/>
+      <c r="E111" s="55"/>
+      <c r="F111" s="55"/>
+      <c r="G111" s="55"/>
+      <c r="H111" s="55"/>
+      <c r="I111" s="55"/>
+      <c r="J111" s="55"/>
+      <c r="K111" s="55"/>
+      <c r="L111" s="55"/>
+      <c r="M111" s="55"/>
+      <c r="N111" s="55"/>
+      <c r="O111" s="55"/>
+      <c r="P111" s="55"/>
+      <c r="Q111" s="55"/>
+      <c r="R111" s="55"/>
+      <c r="S111" s="55"/>
+      <c r="T111" s="55"/>
+      <c r="U111" s="55"/>
+      <c r="V111" s="55"/>
+      <c r="W111" s="55"/>
+      <c r="X111" s="55"/>
+      <c r="Y111" s="55"/>
+      <c r="Z111" s="55"/>
+      <c r="AA111" s="55"/>
+      <c r="AB111" s="55"/>
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
@@ -6813,13 +7033,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="54" t="s">
         <v>762</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
@@ -6845,6 +7065,110 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE83B363-17C2-4D92-A0C7-8E8D8E6A377D}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="53" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:F3"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
@@ -7001,22 +7325,22 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="56" t="s">
         <v>762</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
@@ -7051,7 +7375,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -7092,7 +7416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D62F989-B1EE-49D7-99A7-A4A6C00704A0}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -7133,13 +7457,13 @@
       <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>762</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
       <c r="F3" s="41"/>
       <c r="G3" s="43"/>
       <c r="H3" s="43"/>
@@ -7175,7 +7499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8FE239-7966-4B47-902D-BB193CC8E9D4}">
   <dimension ref="A1:L8"/>
   <sheetViews>
@@ -7331,11 +7655,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7363,11 +7687,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -7672,13 +7996,13 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="53" t="s">
+      <c r="A48" s="54" t="s">
         <v>762</v>
       </c>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="54"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
@@ -7747,13 +8071,13 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="53" t="s">
+      <c r="A59" s="54" t="s">
         <v>1099</v>
       </c>
-      <c r="B59" s="53"/>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
+      <c r="B59" s="54"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="54"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
@@ -7819,6 +8143,60 @@
       </c>
       <c r="C65" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B66" t="s">
+        <v>969</v>
+      </c>
+      <c r="C66" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1240</v>
       </c>
     </row>
   </sheetData>
@@ -7856,10 +8234,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="54"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -8105,11 +8483,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8491,17 +8869,17 @@
       <c r="F35" s="3"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="54" t="s">
+      <c r="A37" s="55" t="s">
         <v>762</v>
       </c>
-      <c r="B37" s="54"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="54"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -8544,17 +8922,17 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="54" t="s">
+      <c r="A44" s="55" t="s">
         <v>1107</v>
       </c>
-      <c r="B44" s="54"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="54"/>
+      <c r="B44" s="55"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
@@ -8610,6 +8988,54 @@
       </c>
       <c r="D51" t="s">
         <v>1172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1241</v>
       </c>
     </row>
   </sheetData>
@@ -8833,16 +9259,16 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="54" t="s">
         <v>762</v>
       </c>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
@@ -8931,32 +9357,35 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:U210"/>
+  <dimension ref="A1:U226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G207" sqref="G207"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C226" sqref="C226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.90625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.08984375" style="20" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.90625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.90625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="255.6328125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="255.6328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="255.6328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="18.1796875" style="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="8.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
@@ -9102,11 +9531,11 @@
       </c>
       <c r="H5" s="34" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>01/13/2023</v>
+        <v>01/14/2023</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>01/13/2023</v>
+        <v>01/14/2023</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -12156,25 +12585,25 @@
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A128" s="54" t="s">
+      <c r="A128" s="55" t="s">
         <v>762</v>
       </c>
-      <c r="B128" s="54"/>
-      <c r="C128" s="54"/>
-      <c r="D128" s="54"/>
-      <c r="E128" s="54"/>
-      <c r="F128" s="54"/>
-      <c r="G128" s="54"/>
-      <c r="H128" s="54"/>
-      <c r="I128" s="54"/>
-      <c r="J128" s="54"/>
-      <c r="K128" s="54"/>
-      <c r="L128" s="54"/>
-      <c r="M128" s="54"/>
-      <c r="N128" s="54"/>
-      <c r="O128" s="54"/>
-      <c r="P128" s="54"/>
-      <c r="Q128" s="54"/>
+      <c r="B128" s="55"/>
+      <c r="C128" s="55"/>
+      <c r="D128" s="55"/>
+      <c r="E128" s="55"/>
+      <c r="F128" s="55"/>
+      <c r="G128" s="55"/>
+      <c r="H128" s="55"/>
+      <c r="I128" s="55"/>
+      <c r="J128" s="55"/>
+      <c r="K128" s="55"/>
+      <c r="L128" s="55"/>
+      <c r="M128" s="55"/>
+      <c r="N128" s="55"/>
+      <c r="O128" s="55"/>
+      <c r="P128" s="55"/>
+      <c r="Q128" s="55"/>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
@@ -12938,25 +13367,25 @@
       </c>
     </row>
     <row r="190" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A190" s="54" t="s">
+      <c r="A190" s="55" t="s">
         <v>1099</v>
       </c>
-      <c r="B190" s="54"/>
-      <c r="C190" s="54"/>
-      <c r="D190" s="54"/>
-      <c r="E190" s="54"/>
-      <c r="F190" s="54"/>
-      <c r="G190" s="54"/>
-      <c r="H190" s="54"/>
-      <c r="I190" s="54"/>
-      <c r="J190" s="54"/>
-      <c r="K190" s="54"/>
-      <c r="L190" s="54"/>
-      <c r="M190" s="54"/>
-      <c r="N190" s="54"/>
-      <c r="O190" s="54"/>
-      <c r="P190" s="54"/>
-      <c r="Q190" s="54"/>
+      <c r="B190" s="55"/>
+      <c r="C190" s="55"/>
+      <c r="D190" s="55"/>
+      <c r="E190" s="55"/>
+      <c r="F190" s="55"/>
+      <c r="G190" s="55"/>
+      <c r="H190" s="55"/>
+      <c r="I190" s="55"/>
+      <c r="J190" s="55"/>
+      <c r="K190" s="55"/>
+      <c r="L190" s="55"/>
+      <c r="M190" s="55"/>
+      <c r="N190" s="55"/>
+      <c r="O190" s="55"/>
+      <c r="P190" s="55"/>
+      <c r="Q190" s="55"/>
     </row>
     <row r="191" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
@@ -12968,10 +13397,10 @@
       <c r="E191" t="s">
         <v>1102</v>
       </c>
-      <c r="R191" s="56">
+      <c r="R191" s="52">
         <v>0.75</v>
       </c>
-      <c r="S191" s="56">
+      <c r="S191" s="52">
         <v>0.77083333333333337</v>
       </c>
       <c r="T191" t="s">
@@ -13021,10 +13450,10 @@
       <c r="E195" t="s">
         <v>1102</v>
       </c>
-      <c r="R195" s="56">
+      <c r="R195" s="52">
         <v>0.75</v>
       </c>
-      <c r="S195" s="56">
+      <c r="S195" s="52">
         <v>0.77083333333333337</v>
       </c>
       <c r="T195" t="s">
@@ -13082,10 +13511,10 @@
       <c r="E200" s="45" t="s">
         <v>1149</v>
       </c>
-      <c r="R200" s="56">
+      <c r="R200" s="52">
         <v>0.75</v>
       </c>
-      <c r="S200" s="56">
+      <c r="S200" s="52">
         <v>0.77083333333333337</v>
       </c>
       <c r="T200" t="s">
@@ -13113,10 +13542,10 @@
       <c r="E202" t="s">
         <v>1156</v>
       </c>
-      <c r="R202" s="56">
+      <c r="R202" s="52">
         <v>0.75</v>
       </c>
-      <c r="S202" s="56">
+      <c r="S202" s="52">
         <v>0.77083333333333337</v>
       </c>
       <c r="T202" t="s">
@@ -13141,10 +13570,10 @@
       <c r="E204" s="20" t="s">
         <v>1161</v>
       </c>
-      <c r="R204" s="56">
+      <c r="R204" s="52">
         <v>0.75</v>
       </c>
-      <c r="S204" s="56">
+      <c r="S204" s="52">
         <v>0.77083333333333337</v>
       </c>
       <c r="T204" t="s">
@@ -13158,10 +13587,10 @@
       <c r="C205" t="s">
         <v>1164</v>
       </c>
-      <c r="R205" s="56">
+      <c r="R205" s="52">
         <v>0.75</v>
       </c>
-      <c r="S205" s="56">
+      <c r="S205" s="52">
         <v>0.77083333333333337</v>
       </c>
       <c r="T205" t="s">
@@ -13178,10 +13607,10 @@
       <c r="E206" t="s">
         <v>1114</v>
       </c>
-      <c r="R206" s="56">
+      <c r="R206" s="52">
         <v>0.75</v>
       </c>
-      <c r="S206" s="56">
+      <c r="S206" s="52">
         <v>0.77083333333333337</v>
       </c>
       <c r="T206" t="s">
@@ -13198,10 +13627,10 @@
       <c r="E207" t="s">
         <v>1169</v>
       </c>
-      <c r="R207" s="56">
+      <c r="R207" s="52">
         <v>0.75</v>
       </c>
-      <c r="S207" s="56">
+      <c r="S207" s="52">
         <v>0.77083333333333337</v>
       </c>
       <c r="T207" t="s">
@@ -13216,7 +13645,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>1176</v>
       </c>
@@ -13224,9 +13653,266 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B210" t="s">
+        <v>213</v>
+      </c>
       <c r="C210" t="s">
-        <v>984</v>
+        <v>1178</v>
+      </c>
+      <c r="E210" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="211" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B211" t="s">
+        <v>209</v>
+      </c>
+      <c r="C211" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E211" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="212" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C212" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D212" s="20" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="213" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C213" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E213" t="s">
+        <v>1149</v>
+      </c>
+      <c r="R213" s="52">
+        <v>0.75</v>
+      </c>
+      <c r="S213" s="52">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="T213" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="214" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D214" s="20" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="215" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C215" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E215" t="s">
+        <v>1193</v>
+      </c>
+      <c r="R215" s="52">
+        <v>0.75</v>
+      </c>
+      <c r="S215" s="52">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="T215" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="216" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C216" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E216" t="s">
+        <v>1196</v>
+      </c>
+      <c r="R216" s="52">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="S216" s="52">
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="217" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E217" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="218" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B218" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C218" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E218" t="s">
+        <v>1202</v>
+      </c>
+      <c r="R218" s="52">
+        <v>0.75</v>
+      </c>
+      <c r="S218" s="52">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="T218" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="219" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C219" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="220" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D220" s="20" t="s">
+        <v>1206</v>
+      </c>
+      <c r="G220" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="221" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C221" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E221" t="s">
+        <v>1211</v>
+      </c>
+      <c r="T221" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="222" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C222" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E222" t="s">
+        <v>1216</v>
+      </c>
+      <c r="R222" s="52">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="S222" s="52">
+        <v>0.875</v>
+      </c>
+      <c r="T222" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="223" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C223" t="s">
+        <v>1217</v>
+      </c>
+      <c r="E223" t="s">
+        <v>1156</v>
+      </c>
+      <c r="R223" s="52">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="S223" s="52">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="224" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C224" t="s">
+        <v>1222</v>
+      </c>
+      <c r="R224" s="52">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="S224" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="T224" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="225" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C225" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E225" t="s">
+        <v>1225</v>
+      </c>
+      <c r="R225" s="52">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="S225" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="T225" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="226" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C226" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E226" t="s">
+        <v>1238</v>
+      </c>
+      <c r="R226" s="52">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="S226" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="T226" t="s">
+        <v>1226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in Data as per Module Acuity Meeting Notes
Signed-off-by: ankur5579 <ankur@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -2381,7 +2381,7 @@
     <t>&lt;break&gt;Con 1&lt;break&gt;con 2&lt;break&gt;con 3&lt;break&gt;con 4&lt;break&gt;con 5&lt;break&gt;con 6&lt;break&gt;con 7&lt;break&gt;con 8&lt;break&gt;con 9&lt;break&gt;con 10&lt;break&gt;con 11&lt;break&gt;con 12&lt;break&gt;con 13&lt;break&gt;con 14&lt;break&gt;con 15&lt;break&gt;con 16&lt;break&gt;con 17&lt;break&gt;con 18&lt;break&gt;con 19&lt;break&gt;con 20&lt;break&gt;con 21&lt;break&gt;con 22&lt;break&gt;con 23&lt;break&gt;con 24&lt;break&gt;con 25&lt;break&gt;con 26&lt;break&gt;con 27&lt;break&gt;con 28&lt;break&gt;con 29&lt;break&gt;con 30&lt;break&gt;con 31&lt;break&gt;con 32&lt;break&gt;con 33&lt;break&gt;con 34&lt;break&gt;con 35&lt;break&gt;con 36&lt;break&gt;con 37&lt;break&gt;con 38&lt;break&gt;con 39&lt;break&gt;con 40&lt;break&gt;con 41&lt;break&gt;con 42&lt;break&gt;con 43&lt;break&gt;con 44&lt;break&gt;con 45&lt;break&gt;con 46&lt;break&gt;con 47&lt;break&gt;con 48&lt;break&gt;Acc 1&lt;break&gt;Acc 2&lt;break&gt;Acc 3&lt;break&gt;Acc 4&lt;break&gt;Acc 5&lt;break&gt;Acc 6&lt;break&gt;Acc 7&lt;break&gt;Acc 8&lt;break&gt;Acc 9&lt;break&gt;Acc 10&lt;break&gt;Acc 11</t>
   </si>
   <si>
-    <t>Con 1&lt;break&gt;con 2&lt;break&gt;con 3&lt;break&gt;con 4&lt;break&gt;con 5&lt;break&gt;con 6&lt;break&gt;con 7&lt;break&gt;con 8&lt;break&gt;con 9&lt;break&gt;con 10&lt;break&gt;con 11&lt;break&gt;con 12&lt;break&gt;con 13&lt;break&gt;con 14&lt;break&gt;con 15&lt;break&gt;con 16&lt;break&gt;con 17&lt;break&gt;con 18&lt;break&gt;con 19&lt;break&gt;con 20&lt;break&gt;con 21&lt;break&gt;con 22&lt;break&gt;con 23&lt;break&gt;con 24&lt;break&gt;con 25&lt;break&gt;con 26&lt;break&gt;con 27&lt;break&gt;con 28&lt;break&gt;con 29&lt;break&gt;con 30&lt;break&gt;con 31&lt;break&gt;con 32&lt;break&gt;con 33&lt;break&gt;con 34&lt;break&gt;con 35&lt;break&gt;con 36&lt;break&gt;con 37&lt;break&gt;con 38&lt;break&gt;con 39&lt;break&gt;con 40&lt;break&gt;con 41&lt;break&gt;con 42&lt;break&gt;con 43&lt;break&gt;con 44&lt;break&gt;con 45&lt;break&gt;con 46&lt;break&gt;con 47&lt;break&gt;con 48&lt;break&gt;Acc 1&lt;break&gt;Acc 2&lt;break&gt;Acc 3&lt;break&gt;Acc 4&lt;break&gt;Acc 5&lt;break&gt;Acc 6&lt;break&gt;Acc 7&lt;break&gt;Acc 8&lt;break&gt;Acc 9&lt;break&gt;Acc 10&lt;break&gt;Acc 11&lt;break&gt;Acc 12&lt;break&gt;Acc 13</t>
+    <t>Con 1&lt;break&gt;con 2&lt;break&gt;con 3&lt;break&gt;con 4&lt;break&gt;con 5&lt;break&gt;con 6&lt;break&gt;con 7&lt;break&gt;con 8&lt;break&gt;con 9&lt;break&gt;con 10&lt;break&gt;con 11&lt;break&gt;con 12&lt;break&gt;con 13&lt;break&gt;con 14&lt;break&gt;con 15&lt;break&gt;con 16&lt;break&gt;con 17&lt;break&gt;con 18&lt;break&gt;con 19&lt;break&gt;con 20&lt;break&gt;con 21&lt;break&gt;con 22&lt;break&gt;con 23&lt;break&gt;con 24&lt;break&gt;con 25&lt;break&gt;con 26&lt;break&gt;con 27&lt;break&gt;con 28&lt;break&gt;con 29&lt;break&gt;con 30&lt;break&gt;con 31&lt;break&gt;con 32&lt;break&gt;con 33&lt;break&gt;con 34&lt;break&gt;con 35&lt;break&gt;con 36&lt;break&gt;con 37&lt;break&gt;con 38&lt;break&gt;con 39&lt;break&gt;con 40&lt;break&gt;con 41&lt;break&gt;con 42&lt;break&gt;con 43&lt;break&gt;con 44&lt;break&gt;con 45&lt;break&gt;con 46&lt;break&gt;con 47&lt;break&gt;con 48&lt;break&gt;Acc 1&lt;break&gt;Acc 2&lt;break&gt;Acc 3&lt;break&gt;Acc 4&lt;break&gt;Acc 5&lt;break&gt;Acc 6&lt;break&gt;Acc 7&lt;break&gt;Acc 8&lt;break&gt;Acc 9&lt;break&gt;Acc 10&lt;break&gt;Acc 11</t>
   </si>
   <si>
     <t>AMNNR_Activity034</t>
@@ -3869,15 +3869,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="181" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="182" formatCode="h:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3924,7 +3924,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3938,7 +3967,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3946,22 +3983,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3975,32 +4013,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4016,7 +4045,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4028,44 +4057,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4110,13 +4103,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4128,13 +4115,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4146,7 +4133,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4164,43 +4223,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4212,79 +4265,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4361,11 +4348,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4388,34 +4401,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4455,144 +4442,144 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4662,8 +4649,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4672,7 +4659,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4682,20 +4669,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="181" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10175,7 +10162,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E166" sqref="E166"/>
+      <selection pane="bottomLeft" activeCell="I172" sqref="I172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -10341,11 +10328,11 @@
       </c>
       <c r="H5" s="27" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>02/03/2023</v>
+        <v>02/10/2023</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>02/03/2023</v>
+        <v>02/10/2023</v>
       </c>
     </row>
     <row r="6" ht="30" spans="1:11">

</xml_diff>

<commit_message>
Changes as per Module Acuity Meeting Notes and Changes Add Sheet named Label
Signed-off-by: ankur5579 <ankur@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -1,45 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\git\PE4.7Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\git\PE 4.7 Acuity\PE4.7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D0DAEA-D65A-4EF4-8A4C-FAE84F2EBAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990CCF88-B73C-4176-9F5A-6549288467A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
     <sheet name="Firm" sheetId="1" r:id="rId2"/>
-    <sheet name="Research" sheetId="9" r:id="rId3"/>
-    <sheet name="Research Data" sheetId="12" r:id="rId4"/>
-    <sheet name="Contact" sheetId="2" r:id="rId5"/>
-    <sheet name="Deal" sheetId="3" r:id="rId6"/>
-    <sheet name="Deal Team" sheetId="7" r:id="rId7"/>
-    <sheet name="Activity Timeline" sheetId="5" r:id="rId8"/>
-    <sheet name="Email" sheetId="17" r:id="rId9"/>
-    <sheet name="Acuity" sheetId="6" r:id="rId10"/>
-    <sheet name="Reports" sheetId="8" r:id="rId11"/>
-    <sheet name="Fund" sheetId="4" r:id="rId12"/>
-    <sheet name="Fundraisings" sheetId="10" r:id="rId13"/>
-    <sheet name="User" sheetId="13" r:id="rId14"/>
-    <sheet name="Test Custom Object" sheetId="16" r:id="rId15"/>
-    <sheet name="ListView" sheetId="18" r:id="rId16"/>
-    <sheet name="DetailPage" sheetId="19" r:id="rId17"/>
+    <sheet name="Labels" sheetId="20" r:id="rId3"/>
+    <sheet name="Research" sheetId="9" r:id="rId4"/>
+    <sheet name="Research Data" sheetId="12" r:id="rId5"/>
+    <sheet name="Contact" sheetId="2" r:id="rId6"/>
+    <sheet name="Deal" sheetId="3" r:id="rId7"/>
+    <sheet name="Deal Team" sheetId="7" r:id="rId8"/>
+    <sheet name="Activity Timeline" sheetId="5" r:id="rId9"/>
+    <sheet name="Email" sheetId="17" r:id="rId10"/>
+    <sheet name="Acuity" sheetId="6" r:id="rId11"/>
+    <sheet name="Reports" sheetId="8" r:id="rId12"/>
+    <sheet name="Fund" sheetId="4" r:id="rId13"/>
+    <sheet name="Fundraisings" sheetId="10" r:id="rId14"/>
+    <sheet name="User" sheetId="13" r:id="rId15"/>
+    <sheet name="Test Custom Object" sheetId="16" r:id="rId16"/>
+    <sheet name="ListView" sheetId="18" r:id="rId17"/>
+    <sheet name="DetailPage" sheetId="19" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Activity Timeline'!$B$1:$B$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Activity Timeline'!$B$1:$B$117</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="1293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="1311">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -3919,6 +3920,60 @@
   </si>
   <si>
     <t>Nav Institution Account 2_COMPANY</t>
+  </si>
+  <si>
+    <t>Acuity Meeting Notes</t>
+  </si>
+  <si>
+    <t>AMNNR_TaskLabel001</t>
+  </si>
+  <si>
+    <t>AMNNR_TaskLabel002</t>
+  </si>
+  <si>
+    <t>AMNNR_TaskLabel003</t>
+  </si>
+  <si>
+    <t>AMNNR_TaskLabel004</t>
+  </si>
+  <si>
+    <t>AMNNR_TaskLabel005</t>
+  </si>
+  <si>
+    <t>AMNNR_TaskLabel006</t>
+  </si>
+  <si>
+    <t>AMNNR_TaskLabel007</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>AMNNR_CallLabel001</t>
+  </si>
+  <si>
+    <t>AMNNR_CallLabel002</t>
+  </si>
+  <si>
+    <t>AMNNR_CallLabel003</t>
+  </si>
+  <si>
+    <t>AMNNR_CallLabel004</t>
+  </si>
+  <si>
+    <t>AMNNR_CallLabel005</t>
+  </si>
+  <si>
+    <t>Field_Label</t>
   </si>
 </sst>
 </file>
@@ -3928,12 +3983,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3978,6 +4040,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4084,22 +4152,22 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4111,56 +4179,56 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4200,8 +4268,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4210,8 +4278,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4496,11 +4568,11 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="26.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.90625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.08984375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="26.90625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -4719,6 +4791,126 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="8.90625" style="21"/>
+    <col min="2" max="2" width="73" style="21" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" style="21" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" style="21" customWidth="1"/>
+    <col min="7" max="7" width="30.453125" style="21" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>903</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>904</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>905</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>332</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24" t="s">
+        <v>907</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+    </row>
+    <row r="4" spans="1:7" ht="43.5">
+      <c r="A4" s="21" t="s">
+        <v>908</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>909</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>910</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>911</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>912</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.5">
+      <c r="A5" s="21" t="s">
+        <v>914</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>909</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>910</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>915</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.5">
+      <c r="A6" s="21" t="s">
+        <v>916</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>909</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>910</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>917</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>912</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AD117"/>
   <sheetViews>
@@ -4727,33 +4919,33 @@
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="16.08984375" customWidth="1"/>
+    <col min="10" max="10" width="13.08984375" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" customWidth="1"/>
-    <col min="16" max="17" width="17.44140625" customWidth="1"/>
-    <col min="18" max="18" width="19.5546875" customWidth="1"/>
-    <col min="19" max="21" width="17.44140625" customWidth="1"/>
-    <col min="22" max="22" width="48.88671875" customWidth="1"/>
-    <col min="23" max="23" width="33.5546875" customWidth="1"/>
-    <col min="24" max="24" width="61.5546875" customWidth="1"/>
+    <col min="14" max="14" width="13.90625" customWidth="1"/>
+    <col min="15" max="15" width="12.453125" customWidth="1"/>
+    <col min="16" max="17" width="17.453125" customWidth="1"/>
+    <col min="18" max="18" width="19.54296875" customWidth="1"/>
+    <col min="19" max="21" width="17.453125" customWidth="1"/>
+    <col min="22" max="22" width="48.90625" customWidth="1"/>
+    <col min="23" max="23" width="33.54296875" customWidth="1"/>
+    <col min="24" max="24" width="61.54296875" customWidth="1"/>
     <col min="25" max="25" width="40" customWidth="1"/>
     <col min="26" max="26" width="69" customWidth="1"/>
-    <col min="27" max="27" width="21.5546875" customWidth="1"/>
-    <col min="28" max="28" width="35.109375" customWidth="1"/>
+    <col min="27" max="27" width="21.54296875" customWidth="1"/>
+    <col min="28" max="28" width="35.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -5749,7 +5941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="28.8">
+    <row r="36" spans="1:22" ht="29">
       <c r="A36" t="s">
         <v>986</v>
       </c>
@@ -7083,7 +7275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -7091,11 +7283,11 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="81.44140625" customWidth="1"/>
-    <col min="3" max="3" width="72.109375" customWidth="1"/>
+    <col min="2" max="2" width="81.453125" customWidth="1"/>
+    <col min="3" max="3" width="72.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7125,7 +7317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -7134,13 +7326,13 @@
       <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.08984375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.54296875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7309,7 +7501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
@@ -7317,21 +7509,21 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.90625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.90625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.08984375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.453125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.08984375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.90625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.08984375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="17" customFormat="1">
@@ -7516,7 +7708,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -7524,10 +7716,10 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="15.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7557,7 +7749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -7565,12 +7757,12 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.90625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="14.90625" customWidth="1"/>
+    <col min="4" max="4" width="26.08984375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -7640,7 +7832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
@@ -7648,18 +7840,18 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.90625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="8" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="23.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.08984375" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.453125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.453125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.90625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.08984375" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="23.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -7714,7 +7906,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="28.8">
+    <row r="4" spans="1:12" ht="29">
       <c r="A4" s="6" t="s">
         <v>1166</v>
       </c>
@@ -7758,7 +7950,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="28.8">
+    <row r="8" spans="1:12" ht="29">
       <c r="A8" s="6" t="s">
         <v>1174</v>
       </c>
@@ -7794,7 +7986,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -7802,9 +7994,9 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -7905,16 +8097,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48:E48"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.90625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.453125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8459,17 +8651,153 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63144719-90C2-48AD-A268-7FC3CF13C51E}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="56" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="59" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="59" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B13" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="59" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B14" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="59" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B15" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1">
+      <c r="A16" s="59" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B16" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="59" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.54296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.90625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8534,7 +8862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
@@ -8542,18 +8870,18 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.90625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="20" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.08984375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.90625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.54296875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.453125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.90625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -8728,7 +9056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
@@ -8737,12 +9065,12 @@
       <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="45.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="45.453125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.54296875" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="117" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -9302,7 +9630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -9310,12 +9638,12 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.08984375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.08984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -9544,7 +9872,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -9552,11 +9880,11 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.08984375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7" customWidth="1" collapsed="1"/>
   </cols>
@@ -9601,7 +9929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V233"/>
@@ -9611,26 +9939,26 @@
       <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" style="26" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="23.08984375" style="21" customWidth="1"/>
+    <col min="5" max="5" width="26.90625" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="17.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.08984375" style="26" customWidth="1"/>
+    <col min="9" max="9" width="17.08984375" customWidth="1"/>
+    <col min="10" max="10" width="11.08984375" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" customWidth="1"/>
-    <col min="14" max="14" width="15.109375" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.88671875" customWidth="1"/>
-    <col min="17" max="17" width="14.109375" customWidth="1"/>
-    <col min="18" max="18" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.08984375" customWidth="1"/>
+    <col min="13" max="13" width="14.08984375" customWidth="1"/>
+    <col min="14" max="14" width="15.08984375" customWidth="1"/>
+    <col min="15" max="15" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.90625" customWidth="1"/>
+    <col min="17" max="17" width="14.08984375" customWidth="1"/>
+    <col min="18" max="18" width="22.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -9731,7 +10059,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="28.8">
+    <row r="4" spans="1:22" ht="29">
       <c r="A4" t="s">
         <v>352</v>
       </c>
@@ -9757,7 +10085,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="28.8">
+    <row r="5" spans="1:22" ht="29">
       <c r="A5" t="s">
         <v>360</v>
       </c>
@@ -9778,11 +10106,11 @@
       </c>
       <c r="H5" s="26" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>02/24/2023</v>
+        <v>02/25/2023</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>02/24/2023</v>
+        <v>02/25/2023</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -9808,7 +10136,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="28.8">
+    <row r="7" spans="1:22" ht="29">
       <c r="A7" t="s">
         <v>370</v>
       </c>
@@ -9819,7 +10147,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="28.8">
+    <row r="8" spans="1:22" ht="29">
       <c r="A8" t="s">
         <v>373</v>
       </c>
@@ -9827,7 +10155,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="28.8">
+    <row r="9" spans="1:22" ht="29">
       <c r="A9" t="s">
         <v>375</v>
       </c>
@@ -9850,7 +10178,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="28.8">
+    <row r="10" spans="1:22" ht="29">
       <c r="A10" t="s">
         <v>381</v>
       </c>
@@ -9873,7 +10201,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="28.8">
+    <row r="11" spans="1:22" ht="29">
       <c r="A11" t="s">
         <v>383</v>
       </c>
@@ -9907,7 +10235,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="28.8">
+    <row r="14" spans="1:22" ht="29">
       <c r="A14" t="s">
         <v>389</v>
       </c>
@@ -9927,7 +10255,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="28.8">
+    <row r="15" spans="1:22" ht="29">
       <c r="A15" t="s">
         <v>394</v>
       </c>
@@ -9989,7 +10317,7 @@
       <c r="H17" s="34"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:14" ht="28.8">
+    <row r="18" spans="1:14" ht="29">
       <c r="A18" s="13" t="s">
         <v>405</v>
       </c>
@@ -10010,7 +10338,7 @@
       <c r="H18" s="34"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:14" ht="28.8">
+    <row r="19" spans="1:14" ht="29">
       <c r="A19" s="13" t="s">
         <v>409</v>
       </c>
@@ -10148,7 +10476,7 @@
       </c>
       <c r="M24" s="36"/>
     </row>
-    <row r="25" spans="1:14" ht="43.2">
+    <row r="25" spans="1:14" ht="43.5">
       <c r="A25" s="36" t="s">
         <v>429</v>
       </c>
@@ -10184,7 +10512,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="43.2">
+    <row r="26" spans="1:14" ht="43.5">
       <c r="A26" s="40" t="s">
         <v>432</v>
       </c>
@@ -10220,7 +10548,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="360">
+    <row r="27" spans="1:14" ht="362.5">
       <c r="A27" s="36" t="s">
         <v>434</v>
       </c>
@@ -10248,7 +10576,7 @@
       <c r="M27" s="22"/>
       <c r="N27" s="22"/>
     </row>
-    <row r="28" spans="1:14" ht="360">
+    <row r="28" spans="1:14" ht="362.5">
       <c r="A28" s="36" t="s">
         <v>437</v>
       </c>
@@ -10276,7 +10604,7 @@
       <c r="M28" s="22"/>
       <c r="N28" s="22"/>
     </row>
-    <row r="29" spans="1:14" ht="360">
+    <row r="29" spans="1:14" ht="362.5">
       <c r="A29" s="36" t="s">
         <v>439</v>
       </c>
@@ -10304,7 +10632,7 @@
       <c r="M29" s="22"/>
       <c r="N29" s="22"/>
     </row>
-    <row r="30" spans="1:14" ht="360">
+    <row r="30" spans="1:14" ht="362.5">
       <c r="A30" s="36" t="s">
         <v>441</v>
       </c>
@@ -10332,7 +10660,7 @@
       <c r="M30" s="22"/>
       <c r="N30" s="22"/>
     </row>
-    <row r="31" spans="1:14" ht="360">
+    <row r="31" spans="1:14" ht="362.5">
       <c r="A31" s="36" t="s">
         <v>443</v>
       </c>
@@ -10360,7 +10688,7 @@
       <c r="M31" s="22"/>
       <c r="N31" s="22"/>
     </row>
-    <row r="32" spans="1:14" ht="360">
+    <row r="32" spans="1:14" ht="362.5">
       <c r="A32" s="36" t="s">
         <v>445</v>
       </c>
@@ -10388,7 +10716,7 @@
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
     </row>
-    <row r="33" spans="1:14" ht="360">
+    <row r="33" spans="1:14" ht="362.5">
       <c r="A33" s="36" t="s">
         <v>447</v>
       </c>
@@ -10416,7 +10744,7 @@
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
     </row>
-    <row r="34" spans="1:14" ht="360">
+    <row r="34" spans="1:14" ht="362.5">
       <c r="A34" s="36" t="s">
         <v>449</v>
       </c>
@@ -10444,7 +10772,7 @@
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
     </row>
-    <row r="35" spans="1:14" ht="360">
+    <row r="35" spans="1:14" ht="362.5">
       <c r="A35" s="36" t="s">
         <v>451</v>
       </c>
@@ -10472,7 +10800,7 @@
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
     </row>
-    <row r="36" spans="1:14" ht="360">
+    <row r="36" spans="1:14" ht="362.5">
       <c r="A36" s="36" t="s">
         <v>453</v>
       </c>
@@ -10500,7 +10828,7 @@
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
     </row>
-    <row r="37" spans="1:14" ht="187.2">
+    <row r="37" spans="1:14" ht="188.5">
       <c r="A37" s="36" t="s">
         <v>455</v>
       </c>
@@ -10528,7 +10856,7 @@
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
     </row>
-    <row r="38" spans="1:14" ht="187.2">
+    <row r="38" spans="1:14" ht="188.5">
       <c r="A38" s="36" t="s">
         <v>458</v>
       </c>
@@ -10556,7 +10884,7 @@
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
     </row>
-    <row r="39" spans="1:14" ht="187.2">
+    <row r="39" spans="1:14" ht="188.5">
       <c r="A39" s="36" t="s">
         <v>460</v>
       </c>
@@ -10584,7 +10912,7 @@
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
     </row>
-    <row r="40" spans="1:14" ht="187.2">
+    <row r="40" spans="1:14" ht="188.5">
       <c r="A40" s="36" t="s">
         <v>462</v>
       </c>
@@ -10612,7 +10940,7 @@
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
     </row>
-    <row r="41" spans="1:14" ht="187.2">
+    <row r="41" spans="1:14" ht="188.5">
       <c r="A41" s="36" t="s">
         <v>464</v>
       </c>
@@ -10640,7 +10968,7 @@
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
     </row>
-    <row r="42" spans="1:14" ht="187.2">
+    <row r="42" spans="1:14" ht="188.5">
       <c r="A42" s="36" t="s">
         <v>467</v>
       </c>
@@ -10668,7 +10996,7 @@
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
     </row>
-    <row r="43" spans="1:14" ht="187.2">
+    <row r="43" spans="1:14" ht="188.5">
       <c r="A43" s="36" t="s">
         <v>469</v>
       </c>
@@ -10696,7 +11024,7 @@
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
     </row>
-    <row r="44" spans="1:14" ht="187.2">
+    <row r="44" spans="1:14" ht="188.5">
       <c r="A44" s="36" t="s">
         <v>472</v>
       </c>
@@ -10724,7 +11052,7 @@
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
     </row>
-    <row r="45" spans="1:14" ht="187.2">
+    <row r="45" spans="1:14" ht="188.5">
       <c r="A45" s="36" t="s">
         <v>474</v>
       </c>
@@ -10752,7 +11080,7 @@
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
     </row>
-    <row r="46" spans="1:14" ht="187.2">
+    <row r="46" spans="1:14" ht="188.5">
       <c r="A46" s="36" t="s">
         <v>477</v>
       </c>
@@ -10780,7 +11108,7 @@
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
     </row>
-    <row r="47" spans="1:14" ht="187.2">
+    <row r="47" spans="1:14" ht="188.5">
       <c r="A47" s="36" t="s">
         <v>479</v>
       </c>
@@ -10808,7 +11136,7 @@
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
     </row>
-    <row r="48" spans="1:14" ht="187.2">
+    <row r="48" spans="1:14" ht="188.5">
       <c r="A48" s="36" t="s">
         <v>482</v>
       </c>
@@ -10836,7 +11164,7 @@
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
     </row>
-    <row r="49" spans="1:14" ht="187.2">
+    <row r="49" spans="1:14" ht="188.5">
       <c r="A49" s="36" t="s">
         <v>484</v>
       </c>
@@ -10864,7 +11192,7 @@
       <c r="M49" s="22"/>
       <c r="N49" s="22"/>
     </row>
-    <row r="50" spans="1:14" ht="187.2">
+    <row r="50" spans="1:14" ht="188.5">
       <c r="A50" s="36" t="s">
         <v>487</v>
       </c>
@@ -10892,7 +11220,7 @@
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
     </row>
-    <row r="51" spans="1:14" ht="187.2">
+    <row r="51" spans="1:14" ht="188.5">
       <c r="A51" s="36" t="s">
         <v>489</v>
       </c>
@@ -10920,7 +11248,7 @@
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
     </row>
-    <row r="52" spans="1:14" ht="187.2">
+    <row r="52" spans="1:14" ht="188.5">
       <c r="A52" s="36" t="s">
         <v>492</v>
       </c>
@@ -10948,7 +11276,7 @@
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
     </row>
-    <row r="53" spans="1:14" ht="187.2">
+    <row r="53" spans="1:14" ht="188.5">
       <c r="A53" s="36" t="s">
         <v>494</v>
       </c>
@@ -10976,7 +11304,7 @@
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
     </row>
-    <row r="54" spans="1:14" ht="187.2">
+    <row r="54" spans="1:14" ht="188.5">
       <c r="A54" s="36" t="s">
         <v>497</v>
       </c>
@@ -11004,7 +11332,7 @@
       <c r="M54" s="22"/>
       <c r="N54" s="22"/>
     </row>
-    <row r="55" spans="1:14" ht="187.2">
+    <row r="55" spans="1:14" ht="188.5">
       <c r="A55" s="36" t="s">
         <v>499</v>
       </c>
@@ -11032,7 +11360,7 @@
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
     </row>
-    <row r="56" spans="1:14" ht="187.2">
+    <row r="56" spans="1:14" ht="188.5">
       <c r="A56" s="36" t="s">
         <v>502</v>
       </c>
@@ -11060,7 +11388,7 @@
       <c r="M56" s="22"/>
       <c r="N56" s="22"/>
     </row>
-    <row r="57" spans="1:14" ht="187.2">
+    <row r="57" spans="1:14" ht="188.5">
       <c r="A57" s="36" t="s">
         <v>504</v>
       </c>
@@ -11088,7 +11416,7 @@
       <c r="M57" s="22"/>
       <c r="N57" s="22"/>
     </row>
-    <row r="58" spans="1:14" ht="187.2">
+    <row r="58" spans="1:14" ht="188.5">
       <c r="A58" s="36" t="s">
         <v>506</v>
       </c>
@@ -11116,7 +11444,7 @@
       <c r="M58" s="22"/>
       <c r="N58" s="22"/>
     </row>
-    <row r="59" spans="1:14" ht="187.2">
+    <row r="59" spans="1:14" ht="188.5">
       <c r="A59" s="36" t="s">
         <v>508</v>
       </c>
@@ -11144,7 +11472,7 @@
       <c r="M59" s="22"/>
       <c r="N59" s="22"/>
     </row>
-    <row r="60" spans="1:14" ht="187.2">
+    <row r="60" spans="1:14" ht="188.5">
       <c r="A60" s="36" t="s">
         <v>510</v>
       </c>
@@ -11172,7 +11500,7 @@
       <c r="M60" s="22"/>
       <c r="N60" s="22"/>
     </row>
-    <row r="61" spans="1:14" ht="187.2">
+    <row r="61" spans="1:14" ht="188.5">
       <c r="A61" s="36" t="s">
         <v>512</v>
       </c>
@@ -11200,7 +11528,7 @@
       <c r="M61" s="22"/>
       <c r="N61" s="22"/>
     </row>
-    <row r="62" spans="1:14" ht="187.2">
+    <row r="62" spans="1:14" ht="188.5">
       <c r="A62" s="36" t="s">
         <v>514</v>
       </c>
@@ -11228,7 +11556,7 @@
       <c r="M62" s="22"/>
       <c r="N62" s="22"/>
     </row>
-    <row r="63" spans="1:14" ht="187.2">
+    <row r="63" spans="1:14" ht="188.5">
       <c r="A63" s="36" t="s">
         <v>516</v>
       </c>
@@ -11256,7 +11584,7 @@
       <c r="M63" s="22"/>
       <c r="N63" s="22"/>
     </row>
-    <row r="64" spans="1:14" ht="187.2">
+    <row r="64" spans="1:14" ht="188.5">
       <c r="A64" s="36" t="s">
         <v>518</v>
       </c>
@@ -11284,7 +11612,7 @@
       <c r="M64" s="22"/>
       <c r="N64" s="22"/>
     </row>
-    <row r="65" spans="1:14" ht="187.2">
+    <row r="65" spans="1:14" ht="188.5">
       <c r="A65" s="36" t="s">
         <v>520</v>
       </c>
@@ -11312,7 +11640,7 @@
       <c r="M65" s="22"/>
       <c r="N65" s="22"/>
     </row>
-    <row r="66" spans="1:14" ht="187.2">
+    <row r="66" spans="1:14" ht="188.5">
       <c r="A66" s="36" t="s">
         <v>522</v>
       </c>
@@ -11418,7 +11746,7 @@
       <c r="M69" s="22"/>
       <c r="N69" s="22"/>
     </row>
-    <row r="70" spans="1:14" ht="187.2">
+    <row r="70" spans="1:14" ht="188.5">
       <c r="A70" s="36" t="s">
         <v>530</v>
       </c>
@@ -11446,7 +11774,7 @@
       <c r="M70" s="22"/>
       <c r="N70" s="22"/>
     </row>
-    <row r="71" spans="1:14" ht="187.2">
+    <row r="71" spans="1:14" ht="188.5">
       <c r="A71" s="36" t="s">
         <v>532</v>
       </c>
@@ -11474,7 +11802,7 @@
       <c r="M71" s="22"/>
       <c r="N71" s="22"/>
     </row>
-    <row r="72" spans="1:14" ht="187.2">
+    <row r="72" spans="1:14" ht="188.5">
       <c r="A72" s="36" t="s">
         <v>534</v>
       </c>
@@ -11502,7 +11830,7 @@
       <c r="M72" s="22"/>
       <c r="N72" s="22"/>
     </row>
-    <row r="73" spans="1:14" ht="187.2">
+    <row r="73" spans="1:14" ht="188.5">
       <c r="A73" s="36" t="s">
         <v>536</v>
       </c>
@@ -11530,7 +11858,7 @@
       <c r="M73" s="22"/>
       <c r="N73" s="22"/>
     </row>
-    <row r="74" spans="1:14" ht="187.2">
+    <row r="74" spans="1:14" ht="188.5">
       <c r="A74" s="36" t="s">
         <v>538</v>
       </c>
@@ -11558,7 +11886,7 @@
       <c r="M74" s="22"/>
       <c r="N74" s="22"/>
     </row>
-    <row r="75" spans="1:14" ht="187.2">
+    <row r="75" spans="1:14" ht="188.5">
       <c r="A75" s="36" t="s">
         <v>540</v>
       </c>
@@ -11586,7 +11914,7 @@
       <c r="M75" s="22"/>
       <c r="N75" s="22"/>
     </row>
-    <row r="76" spans="1:14" ht="187.2">
+    <row r="76" spans="1:14" ht="188.5">
       <c r="A76" s="36" t="s">
         <v>542</v>
       </c>
@@ -11614,7 +11942,7 @@
       <c r="M76" s="22"/>
       <c r="N76" s="22"/>
     </row>
-    <row r="77" spans="1:14" ht="187.2">
+    <row r="77" spans="1:14" ht="188.5">
       <c r="A77" s="36" t="s">
         <v>544</v>
       </c>
@@ -11642,7 +11970,7 @@
       <c r="M77" s="22"/>
       <c r="N77" s="22"/>
     </row>
-    <row r="78" spans="1:14" ht="187.2">
+    <row r="78" spans="1:14" ht="188.5">
       <c r="A78" s="36" t="s">
         <v>546</v>
       </c>
@@ -11670,7 +11998,7 @@
       <c r="M78" s="22"/>
       <c r="N78" s="22"/>
     </row>
-    <row r="79" spans="1:14" ht="187.2">
+    <row r="79" spans="1:14" ht="188.5">
       <c r="A79" s="36" t="s">
         <v>548</v>
       </c>
@@ -11698,7 +12026,7 @@
       <c r="M79" s="22"/>
       <c r="N79" s="22"/>
     </row>
-    <row r="80" spans="1:14" ht="187.2">
+    <row r="80" spans="1:14" ht="188.5">
       <c r="A80" s="36" t="s">
         <v>550</v>
       </c>
@@ -11726,7 +12054,7 @@
       <c r="M80" s="22"/>
       <c r="N80" s="22"/>
     </row>
-    <row r="81" spans="1:14" ht="187.2">
+    <row r="81" spans="1:14" ht="188.5">
       <c r="A81" s="36" t="s">
         <v>552</v>
       </c>
@@ -11754,7 +12082,7 @@
       <c r="M81" s="22"/>
       <c r="N81" s="22"/>
     </row>
-    <row r="82" spans="1:14" ht="187.2">
+    <row r="82" spans="1:14" ht="188.5">
       <c r="A82" s="36" t="s">
         <v>554</v>
       </c>
@@ -11782,7 +12110,7 @@
       <c r="M82" s="22"/>
       <c r="N82" s="22"/>
     </row>
-    <row r="83" spans="1:14" ht="187.2">
+    <row r="83" spans="1:14" ht="188.5">
       <c r="A83" s="36" t="s">
         <v>556</v>
       </c>
@@ -11810,7 +12138,7 @@
       <c r="M83" s="22"/>
       <c r="N83" s="22"/>
     </row>
-    <row r="84" spans="1:14" ht="187.2">
+    <row r="84" spans="1:14" ht="188.5">
       <c r="A84" s="36" t="s">
         <v>558</v>
       </c>
@@ -11838,7 +12166,7 @@
       <c r="M84" s="22"/>
       <c r="N84" s="22"/>
     </row>
-    <row r="85" spans="1:14" ht="187.2">
+    <row r="85" spans="1:14" ht="188.5">
       <c r="A85" s="36" t="s">
         <v>560</v>
       </c>
@@ -11866,7 +12194,7 @@
       <c r="M85" s="22"/>
       <c r="N85" s="22"/>
     </row>
-    <row r="86" spans="1:14" ht="187.2">
+    <row r="86" spans="1:14" ht="188.5">
       <c r="A86" s="36" t="s">
         <v>562</v>
       </c>
@@ -11894,7 +12222,7 @@
       <c r="M86" s="22"/>
       <c r="N86" s="22"/>
     </row>
-    <row r="87" spans="1:14" ht="187.2">
+    <row r="87" spans="1:14" ht="188.5">
       <c r="A87" s="36" t="s">
         <v>564</v>
       </c>
@@ -11922,7 +12250,7 @@
       <c r="M87" s="22"/>
       <c r="N87" s="22"/>
     </row>
-    <row r="88" spans="1:14" ht="187.2">
+    <row r="88" spans="1:14" ht="188.5">
       <c r="A88" s="36" t="s">
         <v>566</v>
       </c>
@@ -11950,7 +12278,7 @@
       <c r="M88" s="22"/>
       <c r="N88" s="22"/>
     </row>
-    <row r="89" spans="1:14" ht="187.2">
+    <row r="89" spans="1:14" ht="188.5">
       <c r="A89" s="36" t="s">
         <v>568</v>
       </c>
@@ -11978,7 +12306,7 @@
       <c r="M89" s="22"/>
       <c r="N89" s="22"/>
     </row>
-    <row r="90" spans="1:14" ht="187.2">
+    <row r="90" spans="1:14" ht="188.5">
       <c r="A90" s="36" t="s">
         <v>570</v>
       </c>
@@ -12006,7 +12334,7 @@
       <c r="M90" s="22"/>
       <c r="N90" s="22"/>
     </row>
-    <row r="91" spans="1:14" ht="187.2">
+    <row r="91" spans="1:14" ht="188.5">
       <c r="A91" s="36" t="s">
         <v>572</v>
       </c>
@@ -12034,7 +12362,7 @@
       <c r="M91" s="22"/>
       <c r="N91" s="22"/>
     </row>
-    <row r="92" spans="1:14" ht="187.2">
+    <row r="92" spans="1:14" ht="188.5">
       <c r="A92" s="36" t="s">
         <v>574</v>
       </c>
@@ -12062,7 +12390,7 @@
       <c r="M92" s="22"/>
       <c r="N92" s="22"/>
     </row>
-    <row r="93" spans="1:14" ht="187.2">
+    <row r="93" spans="1:14" ht="188.5">
       <c r="A93" s="36" t="s">
         <v>576</v>
       </c>
@@ -12090,7 +12418,7 @@
       <c r="M93" s="22"/>
       <c r="N93" s="22"/>
     </row>
-    <row r="94" spans="1:14" ht="187.2">
+    <row r="94" spans="1:14" ht="188.5">
       <c r="A94" s="36" t="s">
         <v>578</v>
       </c>
@@ -12118,7 +12446,7 @@
       <c r="M94" s="22"/>
       <c r="N94" s="22"/>
     </row>
-    <row r="95" spans="1:14" ht="187.2">
+    <row r="95" spans="1:14" ht="188.5">
       <c r="A95" s="36" t="s">
         <v>580</v>
       </c>
@@ -12146,7 +12474,7 @@
       <c r="M95" s="22"/>
       <c r="N95" s="22"/>
     </row>
-    <row r="96" spans="1:14" ht="187.2">
+    <row r="96" spans="1:14" ht="188.5">
       <c r="A96" s="36" t="s">
         <v>582</v>
       </c>
@@ -12677,7 +13005,7 @@
       <c r="M115" s="18"/>
       <c r="N115" s="18"/>
     </row>
-    <row r="116" spans="1:22" ht="28.8">
+    <row r="116" spans="1:22" ht="29">
       <c r="A116" t="s">
         <v>615</v>
       </c>
@@ -12707,7 +13035,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="117" spans="1:22" ht="28.8">
+    <row r="117" spans="1:22" ht="29">
       <c r="A117" t="s">
         <v>622</v>
       </c>
@@ -12737,7 +13065,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="118" spans="1:22" ht="28.8">
+    <row r="118" spans="1:22" ht="29">
       <c r="A118" t="s">
         <v>628</v>
       </c>
@@ -12767,7 +13095,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="119" spans="1:22" ht="28.8">
+    <row r="119" spans="1:22" ht="29">
       <c r="A119" t="s">
         <v>631</v>
       </c>
@@ -12800,7 +13128,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="120" spans="1:22" ht="28.8">
+    <row r="120" spans="1:22" ht="29">
       <c r="A120" t="s">
         <v>635</v>
       </c>
@@ -12830,7 +13158,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="121" spans="1:22" ht="28.8">
+    <row r="121" spans="1:22" ht="29">
       <c r="A121" t="s">
         <v>639</v>
       </c>
@@ -12860,7 +13188,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="122" spans="1:22" ht="28.8">
+    <row r="122" spans="1:22" ht="29">
       <c r="A122" t="s">
         <v>642</v>
       </c>
@@ -12915,7 +13243,7 @@
       <c r="N125" s="18"/>
       <c r="O125" s="18"/>
     </row>
-    <row r="126" spans="1:22" ht="43.2">
+    <row r="126" spans="1:22" ht="43.5">
       <c r="A126" t="s">
         <v>645</v>
       </c>
@@ -13045,7 +13373,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="137" spans="1:17" ht="57.6">
+    <row r="137" spans="1:17" ht="58">
       <c r="A137" t="s">
         <v>657</v>
       </c>
@@ -13062,7 +13390,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="138" spans="1:17" ht="43.2">
+    <row r="138" spans="1:17" ht="43.5">
       <c r="A138" t="s">
         <v>660</v>
       </c>
@@ -13308,7 +13636,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="43.2">
+    <row r="156" spans="1:14" ht="43.5">
       <c r="A156" t="s">
         <v>713</v>
       </c>
@@ -13578,7 +13906,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="177" spans="1:16" ht="43.2">
+    <row r="177" spans="1:16" ht="43.5">
       <c r="A177" t="s">
         <v>771</v>
       </c>
@@ -13916,7 +14244,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="206" spans="1:21" ht="57.6">
+    <row r="206" spans="1:21" ht="58">
       <c r="A206" t="s">
         <v>831</v>
       </c>
@@ -13927,7 +14255,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="207" spans="1:21" ht="43.2">
+    <row r="207" spans="1:21" ht="43.5">
       <c r="A207" t="s">
         <v>834</v>
       </c>
@@ -13947,7 +14275,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="208" spans="1:21" ht="57.6">
+    <row r="208" spans="1:21" ht="58">
       <c r="A208" t="s">
         <v>837</v>
       </c>
@@ -13986,7 +14314,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="43.2">
+    <row r="211" spans="1:20" ht="43.5">
       <c r="A211" t="s">
         <v>845</v>
       </c>
@@ -14107,7 +14435,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="28.8">
+    <row r="219" spans="1:20" ht="29">
       <c r="A219" t="s">
         <v>863</v>
       </c>
@@ -14138,7 +14466,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="43.2">
+    <row r="221" spans="1:20" ht="43.5">
       <c r="A221" t="s">
         <v>868</v>
       </c>
@@ -14359,124 +14687,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="21"/>
-    <col min="2" max="2" width="73" style="21" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" style="21" customWidth="1"/>
-    <col min="7" max="7" width="30.44140625" style="21" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="21"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="28.8">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>903</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>904</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>905</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>332</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>349</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24" t="s">
-        <v>907</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="1:7" ht="43.2">
-      <c r="A4" s="21" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>909</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>910</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>911</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>912</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="43.2">
-      <c r="A5" s="21" t="s">
-        <v>914</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>909</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>910</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>915</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="43.2">
-      <c r="A6" s="21" t="s">
-        <v>916</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>909</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>910</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>917</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>912</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Created a method to open record
Signed-off-by: sourabhnavatargroup <sourabhnavatargroup>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB22887-AB42-48A8-97A2-6F2774DA64BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A91FCF5-C18F-453C-9028-B5772010096F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Activity Timeline" sheetId="5" r:id="rId8"/>
     <sheet name="Email" sheetId="17" r:id="rId9"/>
     <sheet name="Acuity" sheetId="6" r:id="rId10"/>
-    <sheet name="Reports" sheetId="8" r:id="rId11"/>
-    <sheet name="Fund" sheetId="4" r:id="rId12"/>
-    <sheet name="Fundraisings" sheetId="10" r:id="rId13"/>
-    <sheet name="User" sheetId="13" r:id="rId14"/>
-    <sheet name="Test Custom Object" sheetId="16" r:id="rId15"/>
-    <sheet name="ListView" sheetId="18" r:id="rId16"/>
-    <sheet name="DetailPage" sheetId="19" r:id="rId17"/>
+    <sheet name="Themes" sheetId="20" r:id="rId11"/>
+    <sheet name="Reports" sheetId="8" r:id="rId12"/>
+    <sheet name="Fund" sheetId="4" r:id="rId13"/>
+    <sheet name="Fundraisings" sheetId="10" r:id="rId14"/>
+    <sheet name="User" sheetId="13" r:id="rId15"/>
+    <sheet name="Test Custom Object" sheetId="16" r:id="rId16"/>
+    <sheet name="ListView" sheetId="18" r:id="rId17"/>
+    <sheet name="DetailPage" sheetId="19" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Activity Timeline'!$B$1:$B$119</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="1370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="1374">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -4161,6 +4162,18 @@
   </si>
   <si>
     <t>PE Fundraising 1</t>
+  </si>
+  <si>
+    <t>Theme_Name</t>
+  </si>
+  <si>
+    <t>PE Theme 1</t>
+  </si>
+  <si>
+    <t>ATCE_Theme01</t>
+  </si>
+  <si>
+    <t>ATCE005</t>
   </si>
 </sst>
 </file>
@@ -4329,7 +4342,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4448,6 +4461,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4995,9 +5011,9 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AD127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W20" sqref="W20"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5428,6 +5444,14 @@
         <v>1365</v>
       </c>
     </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1373</v>
+      </c>
+      <c r="W23" t="s">
+        <v>275</v>
+      </c>
+    </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
@@ -7164,37 +7188,37 @@
       </c>
     </row>
     <row r="90" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A90" s="59" t="s">
+      <c r="A90" s="60" t="s">
         <v>655</v>
       </c>
-      <c r="B90" s="59"/>
-      <c r="C90" s="59"/>
-      <c r="D90" s="59"/>
-      <c r="E90" s="59"/>
-      <c r="F90" s="59"/>
-      <c r="G90" s="59"/>
-      <c r="H90" s="59"/>
-      <c r="I90" s="59"/>
-      <c r="J90" s="59"/>
-      <c r="K90" s="59"/>
-      <c r="L90" s="59"/>
-      <c r="M90" s="59"/>
-      <c r="N90" s="59"/>
-      <c r="O90" s="59"/>
-      <c r="P90" s="59"/>
-      <c r="Q90" s="59"/>
-      <c r="R90" s="59"/>
-      <c r="S90" s="59"/>
-      <c r="T90" s="59"/>
-      <c r="U90" s="59"/>
-      <c r="V90" s="59"/>
-      <c r="W90" s="59"/>
-      <c r="X90" s="59"/>
-      <c r="Y90" s="59"/>
-      <c r="Z90" s="59"/>
-      <c r="AA90" s="59"/>
-      <c r="AB90" s="59"/>
-      <c r="AC90" s="59"/>
+      <c r="B90" s="60"/>
+      <c r="C90" s="60"/>
+      <c r="D90" s="60"/>
+      <c r="E90" s="60"/>
+      <c r="F90" s="60"/>
+      <c r="G90" s="60"/>
+      <c r="H90" s="60"/>
+      <c r="I90" s="60"/>
+      <c r="J90" s="60"/>
+      <c r="K90" s="60"/>
+      <c r="L90" s="60"/>
+      <c r="M90" s="60"/>
+      <c r="N90" s="60"/>
+      <c r="O90" s="60"/>
+      <c r="P90" s="60"/>
+      <c r="Q90" s="60"/>
+      <c r="R90" s="60"/>
+      <c r="S90" s="60"/>
+      <c r="T90" s="60"/>
+      <c r="U90" s="60"/>
+      <c r="V90" s="60"/>
+      <c r="W90" s="60"/>
+      <c r="X90" s="60"/>
+      <c r="Y90" s="60"/>
+      <c r="Z90" s="60"/>
+      <c r="AA90" s="60"/>
+      <c r="AB90" s="60"/>
+      <c r="AC90" s="60"/>
     </row>
     <row r="91" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
@@ -7457,37 +7481,37 @@
       </c>
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A125" s="59" t="s">
+      <c r="A125" s="60" t="s">
         <v>655</v>
       </c>
-      <c r="B125" s="59"/>
-      <c r="C125" s="59"/>
-      <c r="D125" s="59"/>
-      <c r="E125" s="59"/>
-      <c r="F125" s="59"/>
-      <c r="G125" s="59"/>
-      <c r="H125" s="59"/>
-      <c r="I125" s="59"/>
-      <c r="J125" s="59"/>
-      <c r="K125" s="59"/>
-      <c r="L125" s="59"/>
-      <c r="M125" s="59"/>
-      <c r="N125" s="59"/>
-      <c r="O125" s="59"/>
-      <c r="P125" s="59"/>
-      <c r="Q125" s="59"/>
-      <c r="R125" s="59"/>
-      <c r="S125" s="59"/>
-      <c r="T125" s="59"/>
-      <c r="U125" s="59"/>
-      <c r="V125" s="59"/>
-      <c r="W125" s="59"/>
-      <c r="X125" s="59"/>
-      <c r="Y125" s="59"/>
-      <c r="Z125" s="59"/>
-      <c r="AA125" s="59"/>
-      <c r="AB125" s="59"/>
-      <c r="AC125" s="59"/>
+      <c r="B125" s="60"/>
+      <c r="C125" s="60"/>
+      <c r="D125" s="60"/>
+      <c r="E125" s="60"/>
+      <c r="F125" s="60"/>
+      <c r="G125" s="60"/>
+      <c r="H125" s="60"/>
+      <c r="I125" s="60"/>
+      <c r="J125" s="60"/>
+      <c r="K125" s="60"/>
+      <c r="L125" s="60"/>
+      <c r="M125" s="60"/>
+      <c r="N125" s="60"/>
+      <c r="O125" s="60"/>
+      <c r="P125" s="60"/>
+      <c r="Q125" s="60"/>
+      <c r="R125" s="60"/>
+      <c r="S125" s="60"/>
+      <c r="T125" s="60"/>
+      <c r="U125" s="60"/>
+      <c r="V125" s="60"/>
+      <c r="W125" s="60"/>
+      <c r="X125" s="60"/>
+      <c r="Y125" s="60"/>
+      <c r="Z125" s="60"/>
+      <c r="AA125" s="60"/>
+      <c r="AB125" s="60"/>
+      <c r="AC125" s="60"/>
     </row>
     <row r="126" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
@@ -7520,6 +7544,41 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F76B77E-E347-4FE8-8ADB-A4500466D553}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C2"/>
@@ -7563,14 +7622,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7739,13 +7798,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="59" t="s">
         <v>655</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
@@ -7770,7 +7829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:N15"/>
@@ -7930,22 +7989,22 @@
     </row>
     <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="61" t="s">
         <v>655</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="61"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -7972,22 +8031,22 @@
       <c r="N11" s="11"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="61" t="s">
         <v>1367</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="61"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -8007,7 +8066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:C2"/>
@@ -8049,7 +8108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:L4"/>
@@ -8091,13 +8150,13 @@
       <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="61" t="s">
         <v>655</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
       <c r="F3" s="41"/>
       <c r="G3" s="43"/>
       <c r="H3" s="43"/>
@@ -8133,7 +8192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:L8"/>
@@ -8288,7 +8347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F11"/>
@@ -8311,14 +8370,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>984</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -8431,11 +8490,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -8859,13 +8918,13 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="58" t="s">
+      <c r="A59" s="59" t="s">
         <v>655</v>
       </c>
-      <c r="B59" s="58"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
+      <c r="B59" s="59"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="59"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -8934,13 +8993,13 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="58" t="s">
+      <c r="A70" s="59" t="s">
         <v>984</v>
       </c>
-      <c r="B70" s="58"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
+      <c r="B70" s="59"/>
+      <c r="C70" s="59"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="59"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -9098,10 +9157,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="59" t="s">
         <v>163</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="59"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -9947,17 +10006,17 @@
       <c r="F54" s="3"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="60" t="s">
         <v>655</v>
       </c>
-      <c r="B56" s="59"/>
-      <c r="C56" s="59"/>
-      <c r="D56" s="59"/>
-      <c r="E56" s="59"/>
-      <c r="F56" s="59"/>
-      <c r="G56" s="59"/>
-      <c r="H56" s="59"/>
-      <c r="I56" s="59"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="60"/>
+      <c r="F56" s="60"/>
+      <c r="G56" s="60"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="60"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -10000,17 +10059,17 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="59" t="s">
+      <c r="A63" s="60" t="s">
         <v>992</v>
       </c>
-      <c r="B63" s="59"/>
-      <c r="C63" s="59"/>
-      <c r="D63" s="59"/>
-      <c r="E63" s="59"/>
-      <c r="F63" s="59"/>
-      <c r="G63" s="59"/>
-      <c r="H63" s="59"/>
-      <c r="I63" s="59"/>
+      <c r="B63" s="60"/>
+      <c r="C63" s="60"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="60"/>
+      <c r="F63" s="60"/>
+      <c r="G63" s="60"/>
+      <c r="H63" s="60"/>
+      <c r="I63" s="60"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -10358,16 +10417,16 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="58" t="s">
+      <c r="A27" s="59" t="s">
         <v>655</v>
       </c>
-      <c r="B27" s="58"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -13961,26 +14020,26 @@
       <c r="M134" s="8"/>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A137" s="59" t="s">
+      <c r="A137" s="60" t="s">
         <v>655</v>
       </c>
-      <c r="B137" s="59"/>
-      <c r="C137" s="59"/>
-      <c r="D137" s="59"/>
-      <c r="E137" s="59"/>
-      <c r="F137" s="59"/>
-      <c r="G137" s="59"/>
-      <c r="H137" s="59"/>
-      <c r="I137" s="59"/>
-      <c r="J137" s="59"/>
-      <c r="K137" s="59"/>
-      <c r="L137" s="59"/>
-      <c r="M137" s="59"/>
-      <c r="N137" s="59"/>
-      <c r="O137" s="59"/>
-      <c r="P137" s="59"/>
-      <c r="Q137" s="59"/>
-      <c r="R137" s="59"/>
+      <c r="B137" s="60"/>
+      <c r="C137" s="60"/>
+      <c r="D137" s="60"/>
+      <c r="E137" s="60"/>
+      <c r="F137" s="60"/>
+      <c r="G137" s="60"/>
+      <c r="H137" s="60"/>
+      <c r="I137" s="60"/>
+      <c r="J137" s="60"/>
+      <c r="K137" s="60"/>
+      <c r="L137" s="60"/>
+      <c r="M137" s="60"/>
+      <c r="N137" s="60"/>
+      <c r="O137" s="60"/>
+      <c r="P137" s="60"/>
+      <c r="Q137" s="60"/>
+      <c r="R137" s="60"/>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
@@ -14745,26 +14804,26 @@
       </c>
     </row>
     <row r="199" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A199" s="59" t="s">
+      <c r="A199" s="60" t="s">
         <v>984</v>
       </c>
-      <c r="B199" s="59"/>
-      <c r="C199" s="59"/>
-      <c r="D199" s="59"/>
-      <c r="E199" s="59"/>
-      <c r="F199" s="59"/>
-      <c r="G199" s="59"/>
-      <c r="H199" s="59"/>
-      <c r="I199" s="59"/>
-      <c r="J199" s="59"/>
-      <c r="K199" s="59"/>
-      <c r="L199" s="59"/>
-      <c r="M199" s="59"/>
-      <c r="N199" s="59"/>
-      <c r="O199" s="59"/>
-      <c r="P199" s="59"/>
-      <c r="Q199" s="59"/>
-      <c r="R199" s="59"/>
+      <c r="B199" s="60"/>
+      <c r="C199" s="60"/>
+      <c r="D199" s="60"/>
+      <c r="E199" s="60"/>
+      <c r="F199" s="60"/>
+      <c r="G199" s="60"/>
+      <c r="H199" s="60"/>
+      <c r="I199" s="60"/>
+      <c r="J199" s="60"/>
+      <c r="K199" s="60"/>
+      <c r="L199" s="60"/>
+      <c r="M199" s="60"/>
+      <c r="N199" s="60"/>
+      <c r="O199" s="60"/>
+      <c r="P199" s="60"/>
+      <c r="Q199" s="60"/>
+      <c r="R199" s="60"/>
     </row>
     <row r="200" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A200" t="s">

</xml_diff>

<commit_message>
updated method of UI of Connection page and Meeting & call page
Signed-off-by: sourabhnavatargroup <sourabhnavatargroup>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Satya Roopa\git\PE4.7Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6055A1-2946-4433-8204-4DE1D62E3F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E041866-5EF1-4A06-9F2D-386D13234CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2234" uniqueCount="1422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="1424">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -4321,6 +4321,12 @@
   </si>
   <si>
     <t>Test Account 1_COMPANY&lt;break&gt;Test Account 1_INSTITUTION&lt;break&gt;Test Account 1_ADVISOR&lt;break&gt;Test Account 1_LENDER&lt;break&gt;Test Account 1_INTERMEDIARY&lt;break&gt;Test Account 1_PORTFOLIOCOMPANY&lt;break&gt;Test Account 1_PRIVATEEQUITY&lt;break&gt;Connection Deal 1&lt;break&gt;PE Fund 1&lt;break&gt;PE Fundraising 1&lt;break&gt;PE Theme 1</t>
+  </si>
+  <si>
+    <t>MeetingAndCallsHeader</t>
+  </si>
+  <si>
+    <t>Type&lt;break&gt;Date&lt;break&gt;Subject&lt;break&gt;Details&lt;break&gt;Participants&lt;break&gt;Tags</t>
   </si>
 </sst>
 </file>
@@ -4331,12 +4337,19 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4519,26 +4532,26 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4550,45 +4563,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -4598,10 +4611,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -4622,7 +4635,7 @@
     <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4643,11 +4656,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4656,22 +4684,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5198,11 +5213,11 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:AE136"/>
+  <dimension ref="A1:AF136"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA19" sqref="AA19"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5232,11 +5247,12 @@
     <col min="26" max="26" width="61.5703125" customWidth="1" collapsed="1"/>
     <col min="27" max="27" width="40" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="69" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="35.140625" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="69" customWidth="1"/>
+    <col min="30" max="30" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="35.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:32">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5321,17 +5337,20 @@
       <c r="AB1" s="1" t="s">
         <v>1058</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="68" t="s">
+        <v>1422</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>1059</v>
       </c>
-      <c r="AE1" s="20" t="s">
+      <c r="AF1" s="20" t="s">
         <v>1060</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:32">
       <c r="A3" s="20"/>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
@@ -5358,7 +5377,7 @@
       <c r="V3" s="20"/>
       <c r="W3" s="20"/>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:32">
       <c r="A4" t="s">
         <v>1062</v>
       </c>
@@ -5372,7 +5391,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
         <v>1065</v>
       </c>
@@ -5386,7 +5405,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:32">
       <c r="A6" t="s">
         <v>1066</v>
       </c>
@@ -5400,7 +5419,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:32">
       <c r="A7" t="s">
         <v>1067</v>
       </c>
@@ -5414,7 +5433,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:32">
       <c r="A12" s="20"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
@@ -5441,7 +5460,7 @@
       <c r="V12" s="20"/>
       <c r="W12" s="20"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:32">
       <c r="A13" t="s">
         <v>1069</v>
       </c>
@@ -5452,7 +5471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:32">
       <c r="A14" t="s">
         <v>1070</v>
       </c>
@@ -5463,7 +5482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:32">
       <c r="A15" t="s">
         <v>1071</v>
       </c>
@@ -5474,7 +5493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:32">
       <c r="A16" t="s">
         <v>1072</v>
       </c>
@@ -5491,7 +5510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:29">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
@@ -5522,7 +5541,7 @@
       <c r="Z18" s="20"/>
       <c r="AA18" s="20"/>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:29">
       <c r="A19" s="60" t="s">
         <v>1075</v>
       </c>
@@ -5568,7 +5587,7 @@
       <c r="S19" s="23" t="s">
         <v>508</v>
       </c>
-      <c r="T19" s="66" t="s">
+      <c r="T19" s="62" t="s">
         <v>1086</v>
       </c>
       <c r="U19">
@@ -5595,8 +5614,11 @@
       <c r="AB19" t="s">
         <v>1082</v>
       </c>
-    </row>
-    <row r="20" spans="1:28">
+      <c r="AC19" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20" t="s">
         <v>1084</v>
       </c>
@@ -5625,7 +5647,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:29">
       <c r="A21" t="s">
         <v>1091</v>
       </c>
@@ -5648,7 +5670,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:29">
       <c r="A22" t="s">
         <v>1094</v>
       </c>
@@ -5668,7 +5690,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:29">
       <c r="A23" t="s">
         <v>1096</v>
       </c>
@@ -5688,7 +5710,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:29">
       <c r="A24" t="s">
         <v>1413</v>
       </c>
@@ -5705,7 +5727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:29">
       <c r="A25" t="s">
         <v>1414</v>
       </c>
@@ -5716,7 +5738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:29">
       <c r="A26" t="s">
         <v>1415</v>
       </c>
@@ -5727,7 +5749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:29">
       <c r="A27" t="s">
         <v>1416</v>
       </c>
@@ -5738,28 +5760,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:29">
       <c r="B28" s="60"/>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:29">
       <c r="B29" s="60"/>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:29">
       <c r="B30" s="60"/>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:29">
       <c r="B31" s="60"/>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:29">
       <c r="B32" s="60"/>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:32">
       <c r="B33" s="60"/>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:32">
       <c r="B34" s="60"/>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:32">
       <c r="A40" s="20"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
@@ -5790,7 +5812,7 @@
       <c r="Z40" s="20"/>
       <c r="AA40" s="20"/>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:32">
       <c r="A41" t="s">
         <v>1097</v>
       </c>
@@ -5836,11 +5858,11 @@
       <c r="AB41" t="s">
         <v>1082</v>
       </c>
-      <c r="AE41" t="s">
+      <c r="AF41" t="s">
         <v>1099</v>
       </c>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:32">
       <c r="A42" t="s">
         <v>1100</v>
       </c>
@@ -5886,14 +5908,14 @@
       <c r="Z42" t="s">
         <v>1089</v>
       </c>
-      <c r="AC42" t="s">
+      <c r="AD42" t="s">
         <v>1101</v>
       </c>
-      <c r="AD42" t="s">
+      <c r="AE42" t="s">
         <v>1102</v>
       </c>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:32">
       <c r="A43" t="s">
         <v>1103</v>
       </c>
@@ -5913,7 +5935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:32">
       <c r="A44" t="s">
         <v>1105</v>
       </c>
@@ -5965,14 +5987,14 @@
       <c r="W44">
         <v>0</v>
       </c>
-      <c r="AC44" t="s">
+      <c r="AD44" t="s">
         <v>1107</v>
       </c>
-      <c r="AD44" t="s">
+      <c r="AE44" t="s">
         <v>1108</v>
       </c>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:32">
       <c r="A45" t="s">
         <v>1109</v>
       </c>
@@ -6024,14 +6046,14 @@
       <c r="W45">
         <v>0</v>
       </c>
-      <c r="AC45" t="s">
+      <c r="AD45" t="s">
         <v>1110</v>
       </c>
-      <c r="AD45" t="s">
+      <c r="AE45" t="s">
         <v>1111</v>
       </c>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:32">
       <c r="A46" t="s">
         <v>1112</v>
       </c>
@@ -6083,11 +6105,11 @@
       <c r="W46">
         <v>0</v>
       </c>
-      <c r="AC46" t="s">
+      <c r="AD46" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:32">
       <c r="A47" t="s">
         <v>1116</v>
       </c>
@@ -6140,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:32">
       <c r="A48" t="s">
         <v>1120</v>
       </c>
@@ -7202,7 +7224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:30">
+    <row r="81" spans="1:31">
       <c r="A81" t="s">
         <v>1204</v>
       </c>
@@ -7213,7 +7235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:30">
+    <row r="82" spans="1:31">
       <c r="A82" t="s">
         <v>1206</v>
       </c>
@@ -7224,7 +7246,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:30">
+    <row r="83" spans="1:31">
       <c r="A83" t="s">
         <v>1207</v>
       </c>
@@ -7235,7 +7257,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:30">
+    <row r="84" spans="1:31">
       <c r="A84" t="s">
         <v>1208</v>
       </c>
@@ -7246,7 +7268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:30">
+    <row r="85" spans="1:31">
       <c r="A85" t="s">
         <v>1209</v>
       </c>
@@ -7257,7 +7279,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="86" spans="1:30">
+    <row r="86" spans="1:31">
       <c r="A86" t="s">
         <v>1210</v>
       </c>
@@ -7268,7 +7290,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:30">
+    <row r="88" spans="1:31">
       <c r="A88" s="20"/>
       <c r="B88" s="20"/>
       <c r="C88" s="20"/>
@@ -7301,8 +7323,9 @@
       <c r="AB88" s="20"/>
       <c r="AC88" s="20"/>
       <c r="AD88" s="20"/>
-    </row>
-    <row r="89" spans="1:30">
+      <c r="AE88" s="20"/>
+    </row>
+    <row r="89" spans="1:31">
       <c r="A89" t="s">
         <v>1211</v>
       </c>
@@ -7339,14 +7362,14 @@
       <c r="V89">
         <v>1</v>
       </c>
-      <c r="AC89" t="s">
+      <c r="AD89" t="s">
         <v>1216</v>
       </c>
-      <c r="AD89" t="s">
+      <c r="AE89" t="s">
         <v>1217</v>
       </c>
     </row>
-    <row r="90" spans="1:30">
+    <row r="90" spans="1:31">
       <c r="A90" t="s">
         <v>1218</v>
       </c>
@@ -7380,14 +7403,14 @@
       <c r="V90">
         <v>1</v>
       </c>
-      <c r="AC90" t="s">
+      <c r="AD90" t="s">
         <v>1221</v>
       </c>
-      <c r="AD90" t="s">
+      <c r="AE90" t="s">
         <v>1222</v>
       </c>
     </row>
-    <row r="91" spans="1:30">
+    <row r="91" spans="1:31">
       <c r="A91" t="s">
         <v>1223</v>
       </c>
@@ -7416,7 +7439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:30">
+    <row r="92" spans="1:31">
       <c r="A92" t="s">
         <v>1226</v>
       </c>
@@ -7433,7 +7456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:30">
+    <row r="93" spans="1:31">
       <c r="A93" t="s">
         <v>1228</v>
       </c>
@@ -7450,7 +7473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:30">
+    <row r="94" spans="1:31">
       <c r="A94" t="s">
         <v>1230</v>
       </c>
@@ -7467,7 +7490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:30">
+    <row r="95" spans="1:31">
       <c r="A95" t="s">
         <v>1232</v>
       </c>
@@ -7484,7 +7507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:30">
+    <row r="96" spans="1:31">
       <c r="A96" t="s">
         <v>1234</v>
       </c>
@@ -7495,356 +7518,358 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:30">
-      <c r="A99" s="64" t="s">
+    <row r="99" spans="1:31">
+      <c r="A99" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="B99" s="64"/>
-      <c r="C99" s="64"/>
-      <c r="D99" s="64"/>
-      <c r="E99" s="64"/>
-      <c r="F99" s="64"/>
-      <c r="G99" s="64"/>
-      <c r="H99" s="64"/>
-      <c r="I99" s="64"/>
-      <c r="J99" s="64"/>
-      <c r="K99" s="64"/>
-      <c r="L99" s="64"/>
-      <c r="M99" s="64"/>
-      <c r="N99" s="64"/>
-      <c r="O99" s="64"/>
-      <c r="P99" s="64"/>
-      <c r="Q99" s="64"/>
-      <c r="R99" s="64"/>
-      <c r="S99" s="64"/>
-      <c r="T99" s="64"/>
-      <c r="U99" s="64"/>
-      <c r="V99" s="64"/>
-      <c r="W99" s="64"/>
-      <c r="X99" s="64"/>
-      <c r="Y99" s="64"/>
-      <c r="Z99" s="64"/>
-      <c r="AA99" s="64"/>
-      <c r="AB99" s="64"/>
-      <c r="AC99" s="64"/>
-      <c r="AD99" s="64"/>
-    </row>
-    <row r="100" spans="1:30">
+      <c r="B99" s="71"/>
+      <c r="C99" s="71"/>
+      <c r="D99" s="71"/>
+      <c r="E99" s="71"/>
+      <c r="F99" s="71"/>
+      <c r="G99" s="71"/>
+      <c r="H99" s="71"/>
+      <c r="I99" s="71"/>
+      <c r="J99" s="71"/>
+      <c r="K99" s="71"/>
+      <c r="L99" s="71"/>
+      <c r="M99" s="71"/>
+      <c r="N99" s="71"/>
+      <c r="O99" s="71"/>
+      <c r="P99" s="71"/>
+      <c r="Q99" s="71"/>
+      <c r="R99" s="71"/>
+      <c r="S99" s="71"/>
+      <c r="T99" s="71"/>
+      <c r="U99" s="71"/>
+      <c r="V99" s="71"/>
+      <c r="W99" s="71"/>
+      <c r="X99" s="71"/>
+      <c r="Y99" s="71"/>
+      <c r="Z99" s="71"/>
+      <c r="AA99" s="71"/>
+      <c r="AB99" s="71"/>
+      <c r="AC99" s="71"/>
+      <c r="AD99" s="71"/>
+      <c r="AE99" s="71"/>
+    </row>
+    <row r="100" spans="1:31">
       <c r="A100" t="s">
         <v>1235</v>
       </c>
-      <c r="AC100" t="s">
+      <c r="AD100" t="s">
         <v>1236</v>
       </c>
     </row>
-    <row r="101" spans="1:30">
+    <row r="101" spans="1:31">
       <c r="A101" t="s">
         <v>1237</v>
       </c>
-      <c r="AC101" t="s">
+      <c r="AD101" t="s">
         <v>1238</v>
       </c>
     </row>
-    <row r="102" spans="1:30">
+    <row r="102" spans="1:31">
       <c r="A102" t="s">
         <v>1239</v>
       </c>
-      <c r="AC102" t="s">
+      <c r="AD102" t="s">
         <v>1240</v>
       </c>
     </row>
-    <row r="103" spans="1:30">
+    <row r="103" spans="1:31">
       <c r="A103" t="s">
         <v>1241</v>
       </c>
-      <c r="AC103" t="s">
+      <c r="AD103" t="s">
         <v>1242</v>
       </c>
     </row>
-    <row r="104" spans="1:30">
+    <row r="104" spans="1:31">
       <c r="A104" t="s">
         <v>1243</v>
       </c>
-      <c r="AC104" t="s">
+      <c r="AD104" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="105" spans="1:30">
+    <row r="105" spans="1:31">
       <c r="A105" t="s">
         <v>1245</v>
       </c>
-      <c r="AC105" t="s">
+      <c r="AD105" t="s">
         <v>1246</v>
       </c>
     </row>
-    <row r="106" spans="1:30">
+    <row r="106" spans="1:31">
       <c r="A106" t="s">
         <v>1247</v>
       </c>
-      <c r="AC106" t="s">
+      <c r="AD106" t="s">
         <v>1248</v>
       </c>
     </row>
-    <row r="107" spans="1:30">
+    <row r="107" spans="1:31">
       <c r="A107" t="s">
         <v>1249</v>
       </c>
-      <c r="AC107" t="s">
+      <c r="AD107" t="s">
         <v>1250</v>
       </c>
     </row>
-    <row r="108" spans="1:30">
+    <row r="108" spans="1:31">
       <c r="A108" t="s">
         <v>1251</v>
       </c>
-      <c r="AC108" t="s">
+      <c r="AD108" t="s">
         <v>1252</v>
       </c>
     </row>
-    <row r="109" spans="1:30">
+    <row r="109" spans="1:31">
       <c r="A109" t="s">
         <v>1253</v>
       </c>
-      <c r="AC109" t="s">
+      <c r="AD109" t="s">
         <v>1254</v>
       </c>
     </row>
-    <row r="110" spans="1:30">
+    <row r="110" spans="1:31">
       <c r="A110" t="s">
         <v>1255</v>
       </c>
-      <c r="AC110" t="s">
+      <c r="AD110" t="s">
         <v>1256</v>
       </c>
     </row>
-    <row r="111" spans="1:30">
+    <row r="111" spans="1:31">
       <c r="A111" t="s">
         <v>1257</v>
       </c>
-      <c r="AC111" t="s">
+      <c r="AD111" t="s">
         <v>1258</v>
       </c>
     </row>
-    <row r="112" spans="1:30">
+    <row r="112" spans="1:31">
       <c r="A112" t="s">
         <v>1259</v>
       </c>
-      <c r="AC112" t="s">
+      <c r="AD112" t="s">
         <v>1260</v>
       </c>
     </row>
-    <row r="113" spans="1:30">
+    <row r="113" spans="1:31">
       <c r="A113" t="s">
         <v>1261</v>
       </c>
-      <c r="AC113" t="s">
+      <c r="AD113" t="s">
         <v>1262</v>
       </c>
     </row>
-    <row r="114" spans="1:30">
+    <row r="114" spans="1:31">
       <c r="A114" t="s">
         <v>1263</v>
       </c>
-      <c r="AC114" t="s">
+      <c r="AD114" t="s">
         <v>1264</v>
       </c>
     </row>
-    <row r="115" spans="1:30">
+    <row r="115" spans="1:31">
       <c r="A115" t="s">
         <v>1265</v>
       </c>
-      <c r="AC115" t="s">
+      <c r="AD115" t="s">
         <v>1266</v>
       </c>
     </row>
-    <row r="116" spans="1:30">
+    <row r="116" spans="1:31">
       <c r="A116" t="s">
         <v>1267</v>
       </c>
-      <c r="AC116" t="s">
+      <c r="AD116" t="s">
         <v>1268</v>
       </c>
     </row>
-    <row r="117" spans="1:30">
+    <row r="117" spans="1:31">
       <c r="A117" t="s">
         <v>1269</v>
       </c>
-      <c r="AC117" t="s">
+      <c r="AD117" t="s">
         <v>1266</v>
       </c>
     </row>
-    <row r="118" spans="1:30">
+    <row r="118" spans="1:31">
       <c r="A118" t="s">
         <v>1270</v>
       </c>
-      <c r="AC118" t="s">
+      <c r="AD118" t="s">
         <v>1271</v>
       </c>
     </row>
-    <row r="119" spans="1:30">
+    <row r="119" spans="1:31">
       <c r="A119" t="s">
         <v>1272</v>
       </c>
-      <c r="AC119" t="s">
+      <c r="AD119" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="120" spans="1:30">
+    <row r="120" spans="1:31">
       <c r="A120" t="s">
         <v>1274</v>
       </c>
-      <c r="AC120" t="s">
+      <c r="AD120" t="s">
         <v>1271</v>
       </c>
     </row>
-    <row r="121" spans="1:30">
+    <row r="121" spans="1:31">
       <c r="A121" t="s">
         <v>1275</v>
       </c>
-      <c r="AC121" t="s">
+      <c r="AD121" t="s">
         <v>1276</v>
       </c>
     </row>
-    <row r="122" spans="1:30">
+    <row r="122" spans="1:31">
       <c r="A122" t="s">
         <v>1277</v>
       </c>
-      <c r="AC122" t="s">
+      <c r="AD122" t="s">
         <v>1256</v>
       </c>
     </row>
-    <row r="123" spans="1:30">
+    <row r="123" spans="1:31">
       <c r="A123" t="s">
         <v>1278</v>
       </c>
-      <c r="AC123" t="s">
+      <c r="AD123" t="s">
         <v>1279</v>
       </c>
     </row>
-    <row r="124" spans="1:30">
+    <row r="124" spans="1:31">
       <c r="A124" t="s">
         <v>1280</v>
       </c>
-      <c r="AC124" t="s">
+      <c r="AD124" t="s">
         <v>1266</v>
       </c>
-      <c r="AD124" t="s">
+      <c r="AE124" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="125" spans="1:30">
+    <row r="125" spans="1:31">
       <c r="A125" t="s">
         <v>1281</v>
       </c>
-      <c r="AC125" t="s">
+      <c r="AD125" t="s">
         <v>1268</v>
       </c>
-      <c r="AD125" t="s">
+      <c r="AE125" t="s">
         <v>1282</v>
       </c>
     </row>
-    <row r="126" spans="1:30">
+    <row r="126" spans="1:31">
       <c r="A126" t="s">
         <v>1283</v>
       </c>
-      <c r="AC126" t="s">
+      <c r="AD126" t="s">
         <v>1266</v>
       </c>
-      <c r="AD126" t="s">
+      <c r="AE126" t="s">
         <v>1284</v>
       </c>
     </row>
-    <row r="127" spans="1:30">
+    <row r="127" spans="1:31">
       <c r="A127" t="s">
         <v>1285</v>
       </c>
-      <c r="AC127" t="s">
+      <c r="AD127" t="s">
         <v>1286</v>
       </c>
     </row>
-    <row r="128" spans="1:30">
+    <row r="128" spans="1:31">
       <c r="A128" t="s">
         <v>1287</v>
       </c>
-      <c r="AC128" t="s">
+      <c r="AD128" t="s">
         <v>1288</v>
       </c>
     </row>
-    <row r="129" spans="1:30">
+    <row r="129" spans="1:31">
       <c r="A129" t="s">
         <v>1289</v>
       </c>
-      <c r="AC129" t="s">
+      <c r="AD129" t="s">
         <v>1268</v>
       </c>
-      <c r="AD129" t="s">
+      <c r="AE129" t="s">
         <v>1290</v>
       </c>
     </row>
-    <row r="130" spans="1:30">
+    <row r="130" spans="1:31">
       <c r="A130" t="s">
         <v>1291</v>
       </c>
-      <c r="AC130" t="s">
+      <c r="AD130" t="s">
         <v>1292</v>
       </c>
     </row>
-    <row r="134" spans="1:30">
-      <c r="A134" s="64" t="s">
+    <row r="134" spans="1:31">
+      <c r="A134" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="B134" s="64"/>
-      <c r="C134" s="64"/>
-      <c r="D134" s="64"/>
-      <c r="E134" s="64"/>
-      <c r="F134" s="64"/>
-      <c r="G134" s="64"/>
-      <c r="H134" s="64"/>
-      <c r="I134" s="64"/>
-      <c r="J134" s="64"/>
-      <c r="K134" s="64"/>
-      <c r="L134" s="64"/>
-      <c r="M134" s="64"/>
-      <c r="N134" s="64"/>
-      <c r="O134" s="64"/>
-      <c r="P134" s="64"/>
-      <c r="Q134" s="64"/>
-      <c r="R134" s="64"/>
-      <c r="S134" s="64"/>
-      <c r="T134" s="64"/>
-      <c r="U134" s="64"/>
-      <c r="V134" s="64"/>
-      <c r="W134" s="64"/>
-      <c r="X134" s="64"/>
-      <c r="Y134" s="64"/>
-      <c r="Z134" s="64"/>
-      <c r="AA134" s="64"/>
-      <c r="AB134" s="64"/>
-      <c r="AC134" s="64"/>
-      <c r="AD134" s="64"/>
-    </row>
-    <row r="135" spans="1:30">
+      <c r="B134" s="71"/>
+      <c r="C134" s="71"/>
+      <c r="D134" s="71"/>
+      <c r="E134" s="71"/>
+      <c r="F134" s="71"/>
+      <c r="G134" s="71"/>
+      <c r="H134" s="71"/>
+      <c r="I134" s="71"/>
+      <c r="J134" s="71"/>
+      <c r="K134" s="71"/>
+      <c r="L134" s="71"/>
+      <c r="M134" s="71"/>
+      <c r="N134" s="71"/>
+      <c r="O134" s="71"/>
+      <c r="P134" s="71"/>
+      <c r="Q134" s="71"/>
+      <c r="R134" s="71"/>
+      <c r="S134" s="71"/>
+      <c r="T134" s="71"/>
+      <c r="U134" s="71"/>
+      <c r="V134" s="71"/>
+      <c r="W134" s="71"/>
+      <c r="X134" s="71"/>
+      <c r="Y134" s="71"/>
+      <c r="Z134" s="71"/>
+      <c r="AA134" s="71"/>
+      <c r="AB134" s="71"/>
+      <c r="AC134" s="71"/>
+      <c r="AD134" s="71"/>
+      <c r="AE134" s="71"/>
+    </row>
+    <row r="135" spans="1:31">
       <c r="A135" t="s">
         <v>1293</v>
       </c>
-      <c r="AC135" t="s">
+      <c r="AD135" t="s">
         <v>1294</v>
       </c>
     </row>
-    <row r="136" spans="1:30">
+    <row r="136" spans="1:31">
       <c r="A136" t="s">
         <v>1295</v>
       </c>
-      <c r="AC136" t="s">
+      <c r="AD136" t="s">
         <v>1271</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A99:AD99"/>
-    <mergeCell ref="A134:AD134"/>
+    <mergeCell ref="A99:AE99"/>
+    <mergeCell ref="A134:AE134"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D91" r:id="rId1" tooltip="frank" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
   </hyperlinks>
@@ -8107,13 +8132,13 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="15" t="s">
@@ -8298,22 +8323,22 @@
     </row>
     <row r="9" spans="1:14" ht="19.5" customHeight="1"/>
     <row r="10" spans="1:14">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
-      <c r="N10" s="65"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="15" t="s">
@@ -8340,22 +8365,22 @@
       <c r="N11" s="15"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="72" t="s">
         <v>1347</v>
       </c>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="65"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="72"/>
+      <c r="K14" s="72"/>
+      <c r="L14" s="72"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="72"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
@@ -8456,13 +8481,13 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
       <c r="F3" s="13"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -8676,12 +8701,12 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="70" t="s">
         <v>1378</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
@@ -8810,14 +8835,14 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="69" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -8930,11 +8955,11 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -9358,13 +9383,13 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="63" t="s">
+      <c r="A59" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="B59" s="63"/>
-      <c r="C59" s="63"/>
-      <c r="D59" s="63"/>
-      <c r="E59" s="63"/>
+      <c r="B59" s="70"/>
+      <c r="C59" s="70"/>
+      <c r="D59" s="70"/>
+      <c r="E59" s="70"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
@@ -9433,13 +9458,13 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="63" t="s">
+      <c r="A70" s="70" t="s">
         <v>168</v>
       </c>
-      <c r="B70" s="63"/>
-      <c r="C70" s="63"/>
-      <c r="D70" s="63"/>
-      <c r="E70" s="63"/>
+      <c r="B70" s="70"/>
+      <c r="C70" s="70"/>
+      <c r="D70" s="70"/>
+      <c r="E70" s="70"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
@@ -9596,10 +9621,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="70" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="63"/>
+      <c r="B3" s="70"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
@@ -9849,9 +9874,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -10488,17 +10513,17 @@
       <c r="F54" s="2"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="64" t="s">
+      <c r="A56" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="B56" s="64"/>
-      <c r="C56" s="64"/>
-      <c r="D56" s="64"/>
-      <c r="E56" s="64"/>
-      <c r="F56" s="64"/>
-      <c r="G56" s="64"/>
-      <c r="H56" s="64"/>
-      <c r="I56" s="64"/>
+      <c r="B56" s="71"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="71"/>
+      <c r="E56" s="71"/>
+      <c r="F56" s="71"/>
+      <c r="G56" s="71"/>
+      <c r="H56" s="71"/>
+      <c r="I56" s="71"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
@@ -10563,17 +10588,17 @@
       </c>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="64" t="s">
+      <c r="A65" s="71" t="s">
         <v>347</v>
       </c>
-      <c r="B65" s="64"/>
-      <c r="C65" s="64"/>
-      <c r="D65" s="64"/>
-      <c r="E65" s="64"/>
-      <c r="F65" s="64"/>
-      <c r="G65" s="64"/>
-      <c r="H65" s="64"/>
-      <c r="I65" s="64"/>
+      <c r="B65" s="71"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="71"/>
+      <c r="E65" s="71"/>
+      <c r="F65" s="71"/>
+      <c r="G65" s="71"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="71"/>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
@@ -10925,16 +10950,16 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="63" t="s">
+      <c r="A27" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="15" t="s">
@@ -11025,9 +11050,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -11073,10 +11098,10 @@
       <c r="E1" s="24" t="s">
         <v>424</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="65" t="s">
         <v>1418</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="65" t="s">
         <v>1419</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -11212,11 +11237,11 @@
       </c>
       <c r="J5" s="28" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>03/18/2023</v>
+        <v>03/19/2023</v>
       </c>
       <c r="K5" s="27" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>03/18/2023</v>
+        <v>03/19/2023</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="30">
@@ -11517,19 +11542,13 @@
       <c r="E23" s="23" t="s">
         <v>1411</v>
       </c>
-      <c r="F23" s="71" t="s">
-        <v>1420</v>
-      </c>
-      <c r="G23" s="71" t="s">
-        <v>1421</v>
-      </c>
       <c r="H23" t="s">
         <v>1412</v>
       </c>
       <c r="I23" s="30"/>
       <c r="J23" s="36"/>
       <c r="K23" s="30"/>
-      <c r="L23" s="72" t="s">
+      <c r="L23" s="66" t="s">
         <v>508</v>
       </c>
       <c r="M23" s="34">
@@ -11559,8 +11578,12 @@
       <c r="E24" s="23" t="s">
         <v>1411</v>
       </c>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
+      <c r="F24" s="67" t="s">
+        <v>1420</v>
+      </c>
+      <c r="G24" s="67" t="s">
+        <v>1421</v>
+      </c>
       <c r="H24" t="s">
         <v>1412</v>
       </c>
@@ -11663,7 +11686,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="60">
+    <row r="33" spans="1:16" ht="75">
       <c r="A33" s="34" t="s">
         <v>516</v>
       </c>
@@ -11716,8 +11739,8 @@
       <c r="E34" s="55" t="s">
         <v>529</v>
       </c>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
       <c r="H34" s="27" t="s">
         <v>530</v>
       </c>
@@ -11754,8 +11777,8 @@
       <c r="E35" s="57" t="s">
         <v>529</v>
       </c>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
       <c r="H35" s="27" t="s">
         <v>530</v>
       </c>
@@ -13886,8 +13909,8 @@
       <c r="E106" s="58" t="s">
         <v>685</v>
       </c>
-      <c r="F106" s="69"/>
-      <c r="G106" s="69"/>
+      <c r="F106" s="64"/>
+      <c r="G106" s="64"/>
       <c r="H106" s="27" t="s">
         <v>686</v>
       </c>
@@ -13924,8 +13947,8 @@
       <c r="E107" s="58" t="s">
         <v>685</v>
       </c>
-      <c r="F107" s="69"/>
-      <c r="G107" s="69"/>
+      <c r="F107" s="64"/>
+      <c r="G107" s="64"/>
       <c r="H107" s="27" t="s">
         <v>690</v>
       </c>
@@ -14000,8 +14023,8 @@
       <c r="E109" s="58" t="s">
         <v>697</v>
       </c>
-      <c r="F109" s="69"/>
-      <c r="G109" s="69"/>
+      <c r="F109" s="64"/>
+      <c r="G109" s="64"/>
       <c r="H109" s="27" t="s">
         <v>686</v>
       </c>
@@ -14038,8 +14061,8 @@
       <c r="E110" s="58" t="s">
         <v>697</v>
       </c>
-      <c r="F110" s="69"/>
-      <c r="G110" s="69"/>
+      <c r="F110" s="64"/>
+      <c r="G110" s="64"/>
       <c r="H110" s="27" t="s">
         <v>690</v>
       </c>
@@ -14114,8 +14137,8 @@
       <c r="E112" s="58" t="s">
         <v>704</v>
       </c>
-      <c r="F112" s="69"/>
-      <c r="G112" s="69"/>
+      <c r="F112" s="64"/>
+      <c r="G112" s="64"/>
       <c r="H112" s="27" t="s">
         <v>690</v>
       </c>
@@ -14152,8 +14175,8 @@
       <c r="E113" s="58" t="s">
         <v>707</v>
       </c>
-      <c r="F113" s="69"/>
-      <c r="G113" s="69"/>
+      <c r="F113" s="64"/>
+      <c r="G113" s="64"/>
       <c r="H113" s="27" t="s">
         <v>690</v>
       </c>
@@ -14228,8 +14251,8 @@
       <c r="E115" s="58" t="s">
         <v>713</v>
       </c>
-      <c r="F115" s="69"/>
-      <c r="G115" s="69"/>
+      <c r="F115" s="64"/>
+      <c r="G115" s="64"/>
       <c r="H115" s="27" t="s">
         <v>714</v>
       </c>
@@ -14266,8 +14289,8 @@
       <c r="E116" s="59" t="s">
         <v>717</v>
       </c>
-      <c r="F116" s="69"/>
-      <c r="G116" s="69"/>
+      <c r="F116" s="64"/>
+      <c r="G116" s="64"/>
       <c r="J116" s="28">
         <v>44601</v>
       </c>
@@ -14721,27 +14744,27 @@
       <c r="J143" s="27"/>
     </row>
     <row r="146" spans="1:19">
-      <c r="A146" s="64" t="s">
+      <c r="A146" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="B146" s="64"/>
-      <c r="C146" s="64"/>
-      <c r="D146" s="64"/>
-      <c r="E146" s="64"/>
-      <c r="F146" s="64"/>
-      <c r="G146" s="64"/>
-      <c r="H146" s="64"/>
-      <c r="I146" s="64"/>
-      <c r="J146" s="64"/>
-      <c r="K146" s="64"/>
-      <c r="L146" s="64"/>
-      <c r="M146" s="64"/>
-      <c r="N146" s="64"/>
-      <c r="O146" s="64"/>
-      <c r="P146" s="64"/>
-      <c r="Q146" s="64"/>
-      <c r="R146" s="64"/>
-      <c r="S146" s="64"/>
+      <c r="B146" s="71"/>
+      <c r="C146" s="71"/>
+      <c r="D146" s="71"/>
+      <c r="E146" s="71"/>
+      <c r="F146" s="71"/>
+      <c r="G146" s="71"/>
+      <c r="H146" s="71"/>
+      <c r="I146" s="71"/>
+      <c r="J146" s="71"/>
+      <c r="K146" s="71"/>
+      <c r="L146" s="71"/>
+      <c r="M146" s="71"/>
+      <c r="N146" s="71"/>
+      <c r="O146" s="71"/>
+      <c r="P146" s="71"/>
+      <c r="Q146" s="71"/>
+      <c r="R146" s="71"/>
+      <c r="S146" s="71"/>
     </row>
     <row r="147" spans="1:19">
       <c r="A147" s="27" t="s">
@@ -15526,27 +15549,27 @@
       </c>
     </row>
     <row r="208" spans="1:19">
-      <c r="A208" s="64" t="s">
+      <c r="A208" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="B208" s="64"/>
-      <c r="C208" s="64"/>
-      <c r="D208" s="64"/>
-      <c r="E208" s="64"/>
-      <c r="F208" s="64"/>
-      <c r="G208" s="64"/>
-      <c r="H208" s="64"/>
-      <c r="I208" s="64"/>
-      <c r="J208" s="64"/>
-      <c r="K208" s="64"/>
-      <c r="L208" s="64"/>
-      <c r="M208" s="64"/>
-      <c r="N208" s="64"/>
-      <c r="O208" s="64"/>
-      <c r="P208" s="64"/>
-      <c r="Q208" s="64"/>
-      <c r="R208" s="64"/>
-      <c r="S208" s="64"/>
+      <c r="B208" s="71"/>
+      <c r="C208" s="71"/>
+      <c r="D208" s="71"/>
+      <c r="E208" s="71"/>
+      <c r="F208" s="71"/>
+      <c r="G208" s="71"/>
+      <c r="H208" s="71"/>
+      <c r="I208" s="71"/>
+      <c r="J208" s="71"/>
+      <c r="K208" s="71"/>
+      <c r="L208" s="71"/>
+      <c r="M208" s="71"/>
+      <c r="N208" s="71"/>
+      <c r="O208" s="71"/>
+      <c r="P208" s="71"/>
+      <c r="Q208" s="71"/>
+      <c r="R208" s="71"/>
+      <c r="S208" s="71"/>
     </row>
     <row r="209" spans="1:23" ht="30">
       <c r="A209" s="27" t="s">
@@ -16085,7 +16108,7 @@
     <mergeCell ref="A146:S146"/>
     <mergeCell ref="A208:S208"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E127" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
     <hyperlink ref="E129" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>

</xml_diff>

<commit_message>
Created method infoMessageOfAcuitySection Creatd testcase TC029-TC034
Signed-off-by: sourabhnavatargroup <sourabhnavatargroup>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Satya Roopa\git\PE4.7Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA43EFB6-B8F6-4ADF-90A2-477CEC31BD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D8F5E9-1B49-4300-AA93-57F3CA112CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="1425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="1424">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -3315,9 +3315,6 @@
   </si>
   <si>
     <t>Managing Director</t>
-  </si>
-  <si>
-    <t>Tagged&lt;break&gt;Interactions&lt;break&gt;Contacts&lt;break&gt;Fundraisings</t>
   </si>
   <si>
     <t>Firms&lt;break&gt;People&lt;break&gt;Funds&lt;break&gt;Themes&lt;break&gt;Clips</t>
@@ -4326,10 +4323,10 @@
     <t>Type&lt;break&gt;Date&lt;break&gt;Subject&lt;break&gt;Details&lt;break&gt;Participants&lt;break&gt;Tags</t>
   </si>
   <si>
-    <t>02/23/2023</t>
-  </si>
-  <si>
     <t>ATCE010</t>
+  </si>
+  <si>
+    <t>Tagged&lt;break&gt;Interactions&lt;break&gt;Contacts</t>
   </si>
 </sst>
 </file>
@@ -4545,7 +4542,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4686,6 +4683,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5226,9 +5224,9 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AF136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomLeft" activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5287,7 +5285,7 @@
         <v>216</v>
       </c>
       <c r="I1" s="61" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1041</v>
@@ -5347,7 +5345,7 @@
         <v>1058</v>
       </c>
       <c r="AC1" s="68" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>424</v>
@@ -5573,7 +5571,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="60" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -5582,7 +5580,7 @@
         <v>275</v>
       </c>
       <c r="K19" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -5624,7 +5622,7 @@
         <v>1082</v>
       </c>
       <c r="AC19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="20" spans="1:29">
@@ -5647,7 +5645,7 @@
         <v>295</v>
       </c>
       <c r="K20" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -5659,21 +5657,21 @@
         <v>0</v>
       </c>
       <c r="X20" t="s">
+        <v>1423</v>
+      </c>
+      <c r="Y20" t="s">
         <v>1087</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>1088</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AB20" t="s">
         <v>1089</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>1090</v>
       </c>
     </row>
     <row r="21" spans="1:29">
       <c r="A21" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B21" s="60" t="s">
         <v>106</v>
@@ -5691,7 +5689,7 @@
         <v>290</v>
       </c>
       <c r="K21" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -5703,15 +5701,15 @@
         <v>0</v>
       </c>
       <c r="X21" t="s">
+        <v>1091</v>
+      </c>
+      <c r="Y21" t="s">
         <v>1092</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="22" spans="1:29">
       <c r="A22" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B22" s="60" t="s">
         <v>110</v>
@@ -5729,7 +5727,7 @@
         <v>285</v>
       </c>
       <c r="K22" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -5741,12 +5739,12 @@
         <v>0</v>
       </c>
       <c r="X22" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="23" spans="1:29">
       <c r="A23" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B23" s="60" t="s">
         <v>112</v>
@@ -5764,7 +5762,7 @@
         <v>280</v>
       </c>
       <c r="K23" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -5781,7 +5779,7 @@
     </row>
     <row r="24" spans="1:29">
       <c r="A24" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="B24" s="60" t="s">
         <v>114</v>
@@ -5799,7 +5797,7 @@
         <v>300</v>
       </c>
       <c r="K24" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -5813,7 +5811,7 @@
     </row>
     <row r="25" spans="1:29">
       <c r="A25" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="B25" s="60" t="s">
         <v>116</v>
@@ -5831,7 +5829,7 @@
         <v>305</v>
       </c>
       <c r="K25" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -5845,7 +5843,7 @@
     </row>
     <row r="26" spans="1:29">
       <c r="A26" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="B26" s="60" t="s">
         <v>118</v>
@@ -5856,7 +5854,7 @@
     </row>
     <row r="27" spans="1:29">
       <c r="A27" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="B27" s="60" t="s">
         <v>122</v>
@@ -5867,7 +5865,7 @@
     </row>
     <row r="28" spans="1:29">
       <c r="A28" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="B28" s="69" t="s">
         <v>98</v>
@@ -5927,7 +5925,7 @@
     </row>
     <row r="41" spans="1:32">
       <c r="A41" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="J41" t="s">
         <v>312</v>
@@ -5960,7 +5958,7 @@
         <v>1080</v>
       </c>
       <c r="Y41" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="Z41" t="s">
         <v>1082</v>
@@ -5972,12 +5970,12 @@
         <v>1082</v>
       </c>
       <c r="AF41" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="42" spans="1:32">
       <c r="A42" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B42" t="s">
         <v>104</v>
@@ -6016,27 +6014,27 @@
         <v>1079</v>
       </c>
       <c r="X42" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="Z42" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="AD42" t="s">
+        <v>1100</v>
+      </c>
+      <c r="AE42" t="s">
         <v>1101</v>
-      </c>
-      <c r="AE42" t="s">
-        <v>1102</v>
       </c>
     </row>
     <row r="43" spans="1:32">
       <c r="A43" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="J43" t="s">
         <v>282</v>
       </c>
       <c r="K43" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L43">
         <v>0</v>
@@ -6050,7 +6048,7 @@
     </row>
     <row r="44" spans="1:32">
       <c r="A44" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B44" t="s">
         <v>132</v>
@@ -6065,7 +6063,7 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -6101,15 +6099,15 @@
         <v>0</v>
       </c>
       <c r="AD44" t="s">
+        <v>1106</v>
+      </c>
+      <c r="AE44" t="s">
         <v>1107</v>
-      </c>
-      <c r="AE44" t="s">
-        <v>1108</v>
       </c>
     </row>
     <row r="45" spans="1:32">
       <c r="A45" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B45" t="s">
         <v>104</v>
@@ -6160,15 +6158,15 @@
         <v>0</v>
       </c>
       <c r="AD45" t="s">
+        <v>1109</v>
+      </c>
+      <c r="AE45" t="s">
         <v>1110</v>
-      </c>
-      <c r="AE45" t="s">
-        <v>1111</v>
       </c>
     </row>
     <row r="46" spans="1:32">
       <c r="A46" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B46" t="s">
         <v>132</v>
@@ -6177,22 +6175,22 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="G46">
         <v>1</v>
       </c>
       <c r="J46" t="s">
+        <v>1113</v>
+      </c>
+      <c r="K46" t="s">
         <v>1114</v>
-      </c>
-      <c r="K46" t="s">
-        <v>1115</v>
       </c>
       <c r="L46">
         <v>0</v>
@@ -6224,7 +6222,7 @@
     </row>
     <row r="47" spans="1:32">
       <c r="A47" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B47" t="s">
         <v>135</v>
@@ -6233,19 +6231,19 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="K47" t="s">
         <v>1076</v>
@@ -6277,7 +6275,7 @@
     </row>
     <row r="48" spans="1:32">
       <c r="A48" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B48" t="s">
         <v>137</v>
@@ -6292,16 +6290,16 @@
         <v>3</v>
       </c>
       <c r="F48" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="G48">
         <v>30</v>
       </c>
       <c r="J48" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="K48" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="L48">
         <v>0</v>
@@ -6316,7 +6314,7 @@
         <v>585</v>
       </c>
       <c r="T48" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="U48">
         <v>0</v>
@@ -6330,10 +6328,10 @@
     </row>
     <row r="49" spans="1:23">
       <c r="A49" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B49" t="s">
         <v>1124</v>
-      </c>
-      <c r="B49" t="s">
-        <v>1125</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -6345,7 +6343,7 @@
         <v>2</v>
       </c>
       <c r="F49" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="G49">
         <v>30</v>
@@ -6354,7 +6352,7 @@
         <v>310</v>
       </c>
       <c r="K49" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -6369,7 +6367,7 @@
         <v>590</v>
       </c>
       <c r="T49" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="U49">
         <v>0</v>
@@ -6383,7 +6381,7 @@
     </row>
     <row r="50" spans="1:23">
       <c r="A50" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B50" t="s">
         <v>132</v>
@@ -6398,7 +6396,7 @@
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="G50">
         <v>10</v>
@@ -6436,7 +6434,7 @@
     </row>
     <row r="51" spans="1:23">
       <c r="A51" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B51" t="s">
         <v>102</v>
@@ -6475,7 +6473,7 @@
         <v>565</v>
       </c>
       <c r="T51" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="U51">
         <v>0</v>
@@ -6489,7 +6487,7 @@
     </row>
     <row r="52" spans="1:23">
       <c r="A52" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B52" t="s">
         <v>132</v>
@@ -6498,13 +6496,13 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E52">
         <v>46</v>
       </c>
       <c r="F52" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="G52">
         <v>10</v>
@@ -6513,7 +6511,7 @@
         <v>282</v>
       </c>
       <c r="K52" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L52">
         <v>0</v>
@@ -6542,7 +6540,7 @@
     </row>
     <row r="53" spans="1:23">
       <c r="A53" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B53" t="s">
         <v>102</v>
@@ -6551,22 +6549,22 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="E53">
         <v>46</v>
       </c>
       <c r="F53" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="G53">
         <v>10</v>
       </c>
       <c r="J53" t="s">
+        <v>1136</v>
+      </c>
+      <c r="K53" t="s">
         <v>1137</v>
-      </c>
-      <c r="K53" t="s">
-        <v>1138</v>
       </c>
       <c r="L53">
         <v>0</v>
@@ -6595,7 +6593,7 @@
     </row>
     <row r="54" spans="1:23">
       <c r="A54" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B54" t="s">
         <v>104</v>
@@ -6610,13 +6608,13 @@
         <v>46</v>
       </c>
       <c r="F54" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="G54">
         <v>10</v>
       </c>
       <c r="J54" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K54" t="s">
         <v>1086</v>
@@ -6648,7 +6646,7 @@
     </row>
     <row r="55" spans="1:23" ht="30">
       <c r="A55" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B55" t="s">
         <v>102</v>
@@ -6657,22 +6655,22 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E55">
         <v>44</v>
       </c>
       <c r="F55" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G55">
         <v>8</v>
       </c>
       <c r="J55" t="s">
+        <v>1144</v>
+      </c>
+      <c r="K55" s="22" t="s">
         <v>1145</v>
-      </c>
-      <c r="K55" s="22" t="s">
-        <v>1146</v>
       </c>
       <c r="L55">
         <v>0</v>
@@ -6687,7 +6685,7 @@
         <v>570</v>
       </c>
       <c r="T55" s="22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="U55">
         <v>0</v>
@@ -6701,7 +6699,7 @@
     </row>
     <row r="56" spans="1:23">
       <c r="A56" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B56" t="s">
         <v>132</v>
@@ -6710,22 +6708,22 @@
         <v>63</v>
       </c>
       <c r="D56" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="E56">
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G56">
         <v>8</v>
       </c>
       <c r="J56" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="K56" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="L56">
         <v>0</v>
@@ -6754,7 +6752,7 @@
     </row>
     <row r="57" spans="1:23">
       <c r="A57" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B57" t="s">
         <v>141</v>
@@ -6763,19 +6761,19 @@
         <v>46</v>
       </c>
       <c r="D57" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="E57">
         <v>43</v>
       </c>
       <c r="F57" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G57">
         <v>8</v>
       </c>
       <c r="J57" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="K57" t="s">
         <v>1073</v>
@@ -6793,7 +6791,7 @@
         <v>565</v>
       </c>
       <c r="T57" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="U57">
         <v>0</v>
@@ -6807,31 +6805,31 @@
     </row>
     <row r="58" spans="1:23">
       <c r="A58" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B58" t="s">
         <v>1155</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1156</v>
       </c>
       <c r="C58">
         <v>30</v>
       </c>
       <c r="D58" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="E58">
         <v>42</v>
       </c>
       <c r="F58" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="G58">
         <v>8</v>
       </c>
       <c r="J58" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="K58" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="L58">
         <v>0</v>
@@ -6845,10 +6843,10 @@
     </row>
     <row r="59" spans="1:23">
       <c r="A59" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B59" t="s">
         <v>1160</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1161</v>
       </c>
       <c r="C59">
         <v>30</v>
@@ -6860,13 +6858,13 @@
         <v>40</v>
       </c>
       <c r="F59" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="G59">
         <v>1</v>
       </c>
       <c r="J59" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="K59" t="s">
         <v>1086</v>
@@ -6883,10 +6881,10 @@
     </row>
     <row r="60" spans="1:23">
       <c r="A60" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B60" t="s">
         <v>1164</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1165</v>
       </c>
       <c r="C60">
         <v>10</v>
@@ -6898,16 +6896,16 @@
         <v>49</v>
       </c>
       <c r="F60" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="G60">
         <v>31</v>
       </c>
       <c r="J60" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="K60" s="22" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="L60">
         <v>0</v>
@@ -6921,10 +6919,10 @@
     </row>
     <row r="61" spans="1:23">
       <c r="A61" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B61" t="s">
         <v>1167</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1168</v>
       </c>
       <c r="C61">
         <v>10</v>
@@ -6936,16 +6934,16 @@
         <v>51</v>
       </c>
       <c r="F61" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="G61">
         <v>30</v>
       </c>
       <c r="J61" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="K61" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="L61">
         <v>0</v>
@@ -6959,10 +6957,10 @@
     </row>
     <row r="62" spans="1:23">
       <c r="A62" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B62" t="s">
         <v>1170</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1171</v>
       </c>
       <c r="C62">
         <v>10</v>
@@ -6997,22 +6995,22 @@
     </row>
     <row r="63" spans="1:23">
       <c r="A63" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B63" t="s">
         <v>1172</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1173</v>
       </c>
       <c r="C63">
         <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="E63">
         <v>2</v>
       </c>
       <c r="F63" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="G63">
         <v>1</v>
@@ -7035,10 +7033,10 @@
     </row>
     <row r="64" spans="1:23">
       <c r="A64" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B64" t="s">
         <v>1176</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1177</v>
       </c>
       <c r="C64">
         <v>10</v>
@@ -7050,16 +7048,16 @@
         <v>53</v>
       </c>
       <c r="F64" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="G64">
         <v>1</v>
       </c>
       <c r="J64" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="K64" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L64">
         <v>0</v>
@@ -7073,16 +7071,16 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B65" t="s">
         <v>1179</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1180</v>
       </c>
       <c r="C65">
         <v>8</v>
       </c>
       <c r="D65" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E65">
         <v>42</v>
@@ -7096,22 +7094,22 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B66" t="s">
         <v>1182</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1183</v>
       </c>
       <c r="C66">
         <v>8</v>
       </c>
       <c r="D66" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="G66">
         <v>10</v>
@@ -7119,7 +7117,7 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="B67" t="s">
         <v>104</v>
@@ -7128,13 +7126,13 @@
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="E67">
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="G67">
         <v>10</v>
@@ -7142,10 +7140,10 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B68" t="s">
         <v>1187</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1188</v>
       </c>
       <c r="C68">
         <v>2</v>
@@ -7157,7 +7155,7 @@
         <v>54</v>
       </c>
       <c r="F68" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="G68">
         <v>10</v>
@@ -7165,7 +7163,7 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B69" t="s">
         <v>135</v>
@@ -7174,13 +7172,13 @@
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E69">
         <v>44</v>
       </c>
       <c r="F69" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="G69">
         <v>10</v>
@@ -7188,7 +7186,7 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B70" t="s">
         <v>137</v>
@@ -7197,7 +7195,7 @@
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E70">
         <v>43</v>
@@ -7205,16 +7203,16 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B71" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="E71">
         <v>42</v>
@@ -7222,7 +7220,7 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B72" t="s">
         <v>132</v>
@@ -7239,7 +7237,7 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B73" t="s">
         <v>132</v>
@@ -7256,7 +7254,7 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B74" t="s">
         <v>132</v>
@@ -7273,10 +7271,10 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B75" t="s">
         <v>1195</v>
-      </c>
-      <c r="B75" t="s">
-        <v>1196</v>
       </c>
       <c r="C75">
         <v>3</v>
@@ -7284,10 +7282,10 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B76" t="s">
         <v>1197</v>
-      </c>
-      <c r="B76" t="s">
-        <v>1198</v>
       </c>
       <c r="C76">
         <v>2</v>
@@ -7295,7 +7293,7 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B77" t="s">
         <v>132</v>
@@ -7306,10 +7304,10 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B78" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C78">
         <v>31</v>
@@ -7317,7 +7315,7 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B79" t="s">
         <v>139</v>
@@ -7328,10 +7326,10 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B80" t="s">
         <v>1202</v>
-      </c>
-      <c r="B80" t="s">
-        <v>1203</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -7339,10 +7337,10 @@
     </row>
     <row r="81" spans="1:31">
       <c r="A81" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B81" t="s">
         <v>1204</v>
-      </c>
-      <c r="B81" t="s">
-        <v>1205</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -7350,7 +7348,7 @@
     </row>
     <row r="82" spans="1:31">
       <c r="A82" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B82" t="s">
         <v>132</v>
@@ -7361,10 +7359,10 @@
     </row>
     <row r="83" spans="1:31">
       <c r="A83" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B83" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C83">
         <v>31</v>
@@ -7372,10 +7370,10 @@
     </row>
     <row r="84" spans="1:31">
       <c r="A84" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B84" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C84">
         <v>31</v>
@@ -7383,7 +7381,7 @@
     </row>
     <row r="85" spans="1:31">
       <c r="A85" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B85" t="s">
         <v>132</v>
@@ -7394,10 +7392,10 @@
     </row>
     <row r="86" spans="1:31">
       <c r="A86" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B86" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C86">
         <v>30</v>
@@ -7440,22 +7438,22 @@
     </row>
     <row r="89" spans="1:31">
       <c r="A89" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B89" t="s">
         <v>1211</v>
-      </c>
-      <c r="B89" t="s">
-        <v>1212</v>
       </c>
       <c r="C89">
         <v>5</v>
       </c>
       <c r="D89" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="E89">
         <v>5</v>
       </c>
       <c r="J89" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="L89">
         <v>0</v>
@@ -7467,7 +7465,7 @@
         <v>0</v>
       </c>
       <c r="S89" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="U89">
         <v>0</v>
@@ -7476,15 +7474,15 @@
         <v>1</v>
       </c>
       <c r="AD89" t="s">
+        <v>1215</v>
+      </c>
+      <c r="AE89" t="s">
         <v>1216</v>
-      </c>
-      <c r="AE89" t="s">
-        <v>1217</v>
       </c>
     </row>
     <row r="90" spans="1:31">
       <c r="A90" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B90" t="s">
         <v>149</v>
@@ -7493,13 +7491,13 @@
         <v>1</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="E90">
         <v>1</v>
       </c>
       <c r="J90" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="L90">
         <v>1</v>
@@ -7508,7 +7506,7 @@
         <v>1</v>
       </c>
       <c r="S90" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U90">
         <v>0</v>
@@ -7517,30 +7515,30 @@
         <v>1</v>
       </c>
       <c r="AD90" t="s">
+        <v>1220</v>
+      </c>
+      <c r="AE90" t="s">
         <v>1221</v>
-      </c>
-      <c r="AE90" t="s">
-        <v>1222</v>
       </c>
     </row>
     <row r="91" spans="1:31">
       <c r="A91" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B91" t="s">
         <v>1223</v>
-      </c>
-      <c r="B91" t="s">
-        <v>1224</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="E91">
         <v>1</v>
       </c>
       <c r="J91" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="L91">
         <v>0</v>
@@ -7554,16 +7552,16 @@
     </row>
     <row r="92" spans="1:31">
       <c r="A92" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B92" t="s">
         <v>1226</v>
-      </c>
-      <c r="B92" t="s">
-        <v>1227</v>
       </c>
       <c r="C92">
         <v>5</v>
       </c>
       <c r="D92" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="E92">
         <v>8</v>
@@ -7571,16 +7569,16 @@
     </row>
     <row r="93" spans="1:31">
       <c r="A93" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B93" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="C93">
         <v>8</v>
       </c>
       <c r="D93" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="E93">
         <v>3</v>
@@ -7588,16 +7586,16 @@
     </row>
     <row r="94" spans="1:31">
       <c r="A94" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B94" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C94">
         <v>4</v>
       </c>
       <c r="D94" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="E94">
         <v>3</v>
@@ -7605,7 +7603,7 @@
     </row>
     <row r="95" spans="1:31">
       <c r="A95" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B95" t="s">
         <v>329</v>
@@ -7614,7 +7612,7 @@
         <v>3</v>
       </c>
       <c r="D95" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="E95">
         <v>3</v>
@@ -7622,7 +7620,7 @@
     </row>
     <row r="96" spans="1:31">
       <c r="A96" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B96" t="s">
         <v>410</v>
@@ -7632,238 +7630,238 @@
       </c>
     </row>
     <row r="99" spans="1:31">
-      <c r="A99" s="72" t="s">
+      <c r="A99" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="B99" s="72"/>
-      <c r="C99" s="72"/>
-      <c r="D99" s="72"/>
-      <c r="E99" s="72"/>
-      <c r="F99" s="72"/>
-      <c r="G99" s="72"/>
-      <c r="H99" s="72"/>
-      <c r="I99" s="72"/>
-      <c r="J99" s="72"/>
-      <c r="K99" s="72"/>
-      <c r="L99" s="72"/>
-      <c r="M99" s="72"/>
-      <c r="N99" s="72"/>
-      <c r="O99" s="72"/>
-      <c r="P99" s="72"/>
-      <c r="Q99" s="72"/>
-      <c r="R99" s="72"/>
-      <c r="S99" s="72"/>
-      <c r="T99" s="72"/>
-      <c r="U99" s="72"/>
-      <c r="V99" s="72"/>
-      <c r="W99" s="72"/>
-      <c r="X99" s="72"/>
-      <c r="Y99" s="72"/>
-      <c r="Z99" s="72"/>
-      <c r="AA99" s="72"/>
-      <c r="AB99" s="72"/>
-      <c r="AC99" s="72"/>
-      <c r="AD99" s="72"/>
-      <c r="AE99" s="72"/>
+      <c r="B99" s="73"/>
+      <c r="C99" s="73"/>
+      <c r="D99" s="73"/>
+      <c r="E99" s="73"/>
+      <c r="F99" s="73"/>
+      <c r="G99" s="73"/>
+      <c r="H99" s="73"/>
+      <c r="I99" s="73"/>
+      <c r="J99" s="73"/>
+      <c r="K99" s="73"/>
+      <c r="L99" s="73"/>
+      <c r="M99" s="73"/>
+      <c r="N99" s="73"/>
+      <c r="O99" s="73"/>
+      <c r="P99" s="73"/>
+      <c r="Q99" s="73"/>
+      <c r="R99" s="73"/>
+      <c r="S99" s="73"/>
+      <c r="T99" s="73"/>
+      <c r="U99" s="73"/>
+      <c r="V99" s="73"/>
+      <c r="W99" s="73"/>
+      <c r="X99" s="73"/>
+      <c r="Y99" s="73"/>
+      <c r="Z99" s="73"/>
+      <c r="AA99" s="73"/>
+      <c r="AB99" s="73"/>
+      <c r="AC99" s="73"/>
+      <c r="AD99" s="73"/>
+      <c r="AE99" s="73"/>
     </row>
     <row r="100" spans="1:31">
       <c r="A100" t="s">
+        <v>1234</v>
+      </c>
+      <c r="AD100" t="s">
         <v>1235</v>
-      </c>
-      <c r="AD100" t="s">
-        <v>1236</v>
       </c>
     </row>
     <row r="101" spans="1:31">
       <c r="A101" t="s">
+        <v>1236</v>
+      </c>
+      <c r="AD101" t="s">
         <v>1237</v>
-      </c>
-      <c r="AD101" t="s">
-        <v>1238</v>
       </c>
     </row>
     <row r="102" spans="1:31">
       <c r="A102" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AD102" t="s">
         <v>1239</v>
-      </c>
-      <c r="AD102" t="s">
-        <v>1240</v>
       </c>
     </row>
     <row r="103" spans="1:31">
       <c r="A103" t="s">
+        <v>1240</v>
+      </c>
+      <c r="AD103" t="s">
         <v>1241</v>
-      </c>
-      <c r="AD103" t="s">
-        <v>1242</v>
       </c>
     </row>
     <row r="104" spans="1:31">
       <c r="A104" t="s">
+        <v>1242</v>
+      </c>
+      <c r="AD104" t="s">
         <v>1243</v>
-      </c>
-      <c r="AD104" t="s">
-        <v>1244</v>
       </c>
     </row>
     <row r="105" spans="1:31">
       <c r="A105" t="s">
+        <v>1244</v>
+      </c>
+      <c r="AD105" t="s">
         <v>1245</v>
-      </c>
-      <c r="AD105" t="s">
-        <v>1246</v>
       </c>
     </row>
     <row r="106" spans="1:31">
       <c r="A106" t="s">
+        <v>1246</v>
+      </c>
+      <c r="AD106" t="s">
         <v>1247</v>
-      </c>
-      <c r="AD106" t="s">
-        <v>1248</v>
       </c>
     </row>
     <row r="107" spans="1:31">
       <c r="A107" t="s">
+        <v>1248</v>
+      </c>
+      <c r="AD107" t="s">
         <v>1249</v>
-      </c>
-      <c r="AD107" t="s">
-        <v>1250</v>
       </c>
     </row>
     <row r="108" spans="1:31">
       <c r="A108" t="s">
+        <v>1250</v>
+      </c>
+      <c r="AD108" t="s">
         <v>1251</v>
-      </c>
-      <c r="AD108" t="s">
-        <v>1252</v>
       </c>
     </row>
     <row r="109" spans="1:31">
       <c r="A109" t="s">
+        <v>1252</v>
+      </c>
+      <c r="AD109" t="s">
         <v>1253</v>
-      </c>
-      <c r="AD109" t="s">
-        <v>1254</v>
       </c>
     </row>
     <row r="110" spans="1:31">
       <c r="A110" t="s">
+        <v>1254</v>
+      </c>
+      <c r="AD110" t="s">
         <v>1255</v>
-      </c>
-      <c r="AD110" t="s">
-        <v>1256</v>
       </c>
     </row>
     <row r="111" spans="1:31">
       <c r="A111" t="s">
+        <v>1256</v>
+      </c>
+      <c r="AD111" t="s">
         <v>1257</v>
-      </c>
-      <c r="AD111" t="s">
-        <v>1258</v>
       </c>
     </row>
     <row r="112" spans="1:31">
       <c r="A112" t="s">
+        <v>1258</v>
+      </c>
+      <c r="AD112" t="s">
         <v>1259</v>
-      </c>
-      <c r="AD112" t="s">
-        <v>1260</v>
       </c>
     </row>
     <row r="113" spans="1:31">
       <c r="A113" t="s">
+        <v>1260</v>
+      </c>
+      <c r="AD113" t="s">
         <v>1261</v>
-      </c>
-      <c r="AD113" t="s">
-        <v>1262</v>
       </c>
     </row>
     <row r="114" spans="1:31">
       <c r="A114" t="s">
+        <v>1262</v>
+      </c>
+      <c r="AD114" t="s">
         <v>1263</v>
-      </c>
-      <c r="AD114" t="s">
-        <v>1264</v>
       </c>
     </row>
     <row r="115" spans="1:31">
       <c r="A115" t="s">
+        <v>1264</v>
+      </c>
+      <c r="AD115" t="s">
         <v>1265</v>
-      </c>
-      <c r="AD115" t="s">
-        <v>1266</v>
       </c>
     </row>
     <row r="116" spans="1:31">
       <c r="A116" t="s">
+        <v>1266</v>
+      </c>
+      <c r="AD116" t="s">
         <v>1267</v>
-      </c>
-      <c r="AD116" t="s">
-        <v>1268</v>
       </c>
     </row>
     <row r="117" spans="1:31">
       <c r="A117" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="AD117" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="118" spans="1:31">
       <c r="A118" t="s">
+        <v>1269</v>
+      </c>
+      <c r="AD118" t="s">
         <v>1270</v>
-      </c>
-      <c r="AD118" t="s">
-        <v>1271</v>
       </c>
     </row>
     <row r="119" spans="1:31">
       <c r="A119" t="s">
+        <v>1271</v>
+      </c>
+      <c r="AD119" t="s">
         <v>1272</v>
-      </c>
-      <c r="AD119" t="s">
-        <v>1273</v>
       </c>
     </row>
     <row r="120" spans="1:31">
       <c r="A120" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="AD120" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="121" spans="1:31">
       <c r="A121" t="s">
+        <v>1274</v>
+      </c>
+      <c r="AD121" t="s">
         <v>1275</v>
-      </c>
-      <c r="AD121" t="s">
-        <v>1276</v>
       </c>
     </row>
     <row r="122" spans="1:31">
       <c r="A122" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="AD122" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="123" spans="1:31">
       <c r="A123" t="s">
+        <v>1277</v>
+      </c>
+      <c r="AD123" t="s">
         <v>1278</v>
-      </c>
-      <c r="AD123" t="s">
-        <v>1279</v>
       </c>
     </row>
     <row r="124" spans="1:31">
       <c r="A124" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="AD124" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="AE124" t="s">
         <v>843</v>
@@ -7871,110 +7869,110 @@
     </row>
     <row r="125" spans="1:31">
       <c r="A125" t="s">
+        <v>1280</v>
+      </c>
+      <c r="AD125" t="s">
+        <v>1267</v>
+      </c>
+      <c r="AE125" t="s">
         <v>1281</v>
-      </c>
-      <c r="AD125" t="s">
-        <v>1268</v>
-      </c>
-      <c r="AE125" t="s">
-        <v>1282</v>
       </c>
     </row>
     <row r="126" spans="1:31">
       <c r="A126" t="s">
+        <v>1282</v>
+      </c>
+      <c r="AD126" t="s">
+        <v>1265</v>
+      </c>
+      <c r="AE126" t="s">
         <v>1283</v>
-      </c>
-      <c r="AD126" t="s">
-        <v>1266</v>
-      </c>
-      <c r="AE126" t="s">
-        <v>1284</v>
       </c>
     </row>
     <row r="127" spans="1:31">
       <c r="A127" t="s">
+        <v>1284</v>
+      </c>
+      <c r="AD127" t="s">
         <v>1285</v>
-      </c>
-      <c r="AD127" t="s">
-        <v>1286</v>
       </c>
     </row>
     <row r="128" spans="1:31">
       <c r="A128" t="s">
+        <v>1286</v>
+      </c>
+      <c r="AD128" t="s">
         <v>1287</v>
-      </c>
-      <c r="AD128" t="s">
-        <v>1288</v>
       </c>
     </row>
     <row r="129" spans="1:31">
       <c r="A129" t="s">
+        <v>1288</v>
+      </c>
+      <c r="AD129" t="s">
+        <v>1267</v>
+      </c>
+      <c r="AE129" t="s">
         <v>1289</v>
-      </c>
-      <c r="AD129" t="s">
-        <v>1268</v>
-      </c>
-      <c r="AE129" t="s">
-        <v>1290</v>
       </c>
     </row>
     <row r="130" spans="1:31">
       <c r="A130" t="s">
+        <v>1290</v>
+      </c>
+      <c r="AD130" t="s">
         <v>1291</v>
       </c>
-      <c r="AD130" t="s">
-        <v>1292</v>
-      </c>
     </row>
     <row r="134" spans="1:31">
-      <c r="A134" s="72" t="s">
+      <c r="A134" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="B134" s="72"/>
-      <c r="C134" s="72"/>
-      <c r="D134" s="72"/>
-      <c r="E134" s="72"/>
-      <c r="F134" s="72"/>
-      <c r="G134" s="72"/>
-      <c r="H134" s="72"/>
-      <c r="I134" s="72"/>
-      <c r="J134" s="72"/>
-      <c r="K134" s="72"/>
-      <c r="L134" s="72"/>
-      <c r="M134" s="72"/>
-      <c r="N134" s="72"/>
-      <c r="O134" s="72"/>
-      <c r="P134" s="72"/>
-      <c r="Q134" s="72"/>
-      <c r="R134" s="72"/>
-      <c r="S134" s="72"/>
-      <c r="T134" s="72"/>
-      <c r="U134" s="72"/>
-      <c r="V134" s="72"/>
-      <c r="W134" s="72"/>
-      <c r="X134" s="72"/>
-      <c r="Y134" s="72"/>
-      <c r="Z134" s="72"/>
-      <c r="AA134" s="72"/>
-      <c r="AB134" s="72"/>
-      <c r="AC134" s="72"/>
-      <c r="AD134" s="72"/>
-      <c r="AE134" s="72"/>
+      <c r="B134" s="73"/>
+      <c r="C134" s="73"/>
+      <c r="D134" s="73"/>
+      <c r="E134" s="73"/>
+      <c r="F134" s="73"/>
+      <c r="G134" s="73"/>
+      <c r="H134" s="73"/>
+      <c r="I134" s="73"/>
+      <c r="J134" s="73"/>
+      <c r="K134" s="73"/>
+      <c r="L134" s="73"/>
+      <c r="M134" s="73"/>
+      <c r="N134" s="73"/>
+      <c r="O134" s="73"/>
+      <c r="P134" s="73"/>
+      <c r="Q134" s="73"/>
+      <c r="R134" s="73"/>
+      <c r="S134" s="73"/>
+      <c r="T134" s="73"/>
+      <c r="U134" s="73"/>
+      <c r="V134" s="73"/>
+      <c r="W134" s="73"/>
+      <c r="X134" s="73"/>
+      <c r="Y134" s="73"/>
+      <c r="Z134" s="73"/>
+      <c r="AA134" s="73"/>
+      <c r="AB134" s="73"/>
+      <c r="AC134" s="73"/>
+      <c r="AD134" s="73"/>
+      <c r="AE134" s="73"/>
     </row>
     <row r="135" spans="1:31">
       <c r="A135" t="s">
+        <v>1292</v>
+      </c>
+      <c r="AD135" t="s">
         <v>1293</v>
-      </c>
-      <c r="AD135" t="s">
-        <v>1294</v>
       </c>
     </row>
     <row r="136" spans="1:31">
       <c r="A136" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="AD136" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
   </sheetData>
@@ -8010,15 +8008,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B2" t="s">
         <v>1297</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1298</v>
       </c>
     </row>
   </sheetData>
@@ -8047,7 +8045,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>439</v>
@@ -8055,13 +8053,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B2" t="s">
         <v>1300</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1301</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1302</v>
       </c>
     </row>
   </sheetData>
@@ -8076,7 +8074,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8092,13 +8090,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1303</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1304</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1305</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>52</v>
@@ -8106,7 +8104,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B2" t="s">
         <v>449</v>
@@ -8120,10 +8118,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="15" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>1307</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>1308</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>216</v>
@@ -8135,30 +8133,30 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="15" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
       <c r="E4" s="15" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="15" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>1311</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>1312</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
+        <v>1312</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>1313</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>1313</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>1314</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -8166,16 +8164,16 @@
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
       <c r="D7" s="20" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B8" t="s">
         <v>1316</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1317</v>
       </c>
       <c r="C8" t="s">
         <v>216</v>
@@ -8195,10 +8193,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B13" t="s">
         <v>1318</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1319</v>
       </c>
       <c r="C13" t="s">
         <v>216</v>
@@ -8218,10 +8216,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B16" t="s">
         <v>1318</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1319</v>
       </c>
       <c r="C16" t="s">
         <v>216</v>
@@ -8232,10 +8230,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B17" t="s">
         <v>1320</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1321</v>
       </c>
       <c r="C17" t="s">
         <v>216</v>
@@ -8245,26 +8243,26 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="15" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>1322</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="C20" s="15" t="s">
         <v>1323</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>1324</v>
-      </c>
       <c r="D20" s="15" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="E20" s="15"/>
     </row>
@@ -8281,8 +8279,8 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8308,25 +8306,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>1325</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>1326</v>
-      </c>
       <c r="D1" s="19" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>517</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>421</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>423</v>
@@ -8335,10 +8333,10 @@
         <v>373</v>
       </c>
       <c r="K1" s="19" t="s">
+        <v>1328</v>
+      </c>
+      <c r="L1" s="19" t="s">
         <v>1329</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>1330</v>
       </c>
       <c r="M1" s="19" t="s">
         <v>423</v>
@@ -8360,16 +8358,16 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="15" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>1331</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="C4" s="15" t="s">
         <v>1332</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>1333</v>
-      </c>
       <c r="D4" s="15" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -8377,10 +8375,10 @@
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K4" s="15" t="s">
         <v>1334</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>1335</v>
       </c>
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
@@ -8388,7 +8386,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="15" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -8403,18 +8401,18 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
       <c r="N5" s="15" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="15" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>1338</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="C6" s="15" t="s">
         <v>1339</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>1340</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -8423,48 +8421,48 @@
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15" t="s">
+        <v>1340</v>
+      </c>
+      <c r="K6" s="15" t="s">
         <v>1341</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>1342</v>
       </c>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
       <c r="N6" s="15" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="19.5" customHeight="1"/>
     <row r="10" spans="1:14">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="74" t="s">
         <v>152</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="15" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>1344</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="C11" s="15" t="s">
         <v>1345</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>1346</v>
-      </c>
       <c r="D11" s="15" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -8478,29 +8476,29 @@
       <c r="N11" s="15"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="73" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
+      <c r="A14" s="74" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B15" t="s">
         <v>1348</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1349</v>
       </c>
     </row>
   </sheetData>
@@ -8533,18 +8531,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>1350</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>1351</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B2" t="s">
         <v>1352</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1353</v>
       </c>
       <c r="C2" t="s">
         <v>565</v>
@@ -8577,10 +8575,10 @@
         <v>1055</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>1354</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>1355</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>52</v>
@@ -8594,13 +8592,13 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="74" t="s">
         <v>152</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
       <c r="F3" s="13"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -8611,16 +8609,16 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="15" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>1356</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="C4" s="15" t="s">
         <v>1357</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>1358</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>1359</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="16"/>
@@ -8670,31 +8668,31 @@
         <v>1055</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1360</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>1361</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="1" t="s">
         <v>1362</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1363</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>1354</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>1364</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1365</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>1366</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>1367</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -8713,31 +8711,31 @@
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" s="8" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>1368</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>1369</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>1370</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="10" t="s">
+        <v>1370</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>1371</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>1372</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>1373</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>1374</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="L4" s="9"/>
     </row>
@@ -8757,31 +8755,31 @@
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" s="8" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>1369</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>1370</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="10" t="s">
+        <v>1370</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>1371</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>1372</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>1373</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>1374</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="L8" s="9"/>
     </row>
@@ -8810,20 +8808,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="72" t="s">
         <v>1377</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="71" t="s">
-        <v>1378</v>
-      </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>422</v>
@@ -8831,7 +8829,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="B5" t="s">
         <v>423</v>
@@ -8839,7 +8837,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B6" t="s">
         <v>424</v>
@@ -8847,39 +8845,39 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>1382</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>1383</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B8" t="s">
         <v>1384</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1385</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B9" t="s">
         <v>1386</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1387</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B10" t="s">
         <v>1388</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1389</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="B13" t="s">
         <v>422</v>
@@ -8887,7 +8885,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="B14" t="s">
         <v>423</v>
@@ -8895,7 +8893,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="B15" t="s">
         <v>424</v>
@@ -8903,7 +8901,7 @@
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="B16" t="s">
         <v>374</v>
@@ -8911,10 +8909,10 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="B17" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
   </sheetData>
@@ -8948,14 +8946,14 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -8970,7 +8968,7 @@
         <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -8978,7 +8976,7 @@
         <v>172</v>
       </c>
       <c r="B6" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -8986,7 +8984,7 @@
         <v>174</v>
       </c>
       <c r="B7" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -8994,7 +8992,7 @@
         <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -9002,7 +9000,7 @@
         <v>176</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -9010,7 +9008,7 @@
         <v>177</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -9018,7 +9016,7 @@
         <v>178</v>
       </c>
       <c r="B11" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
   </sheetData>
@@ -9068,11 +9066,11 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -9496,13 +9494,13 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="71" t="s">
+      <c r="A59" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="B59" s="71"/>
-      <c r="C59" s="71"/>
-      <c r="D59" s="71"/>
-      <c r="E59" s="71"/>
+      <c r="B59" s="72"/>
+      <c r="C59" s="72"/>
+      <c r="D59" s="72"/>
+      <c r="E59" s="72"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
@@ -9571,13 +9569,13 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="71" t="s">
+      <c r="A70" s="72" t="s">
         <v>168</v>
       </c>
-      <c r="B70" s="71"/>
-      <c r="C70" s="71"/>
-      <c r="D70" s="71"/>
-      <c r="E70" s="71"/>
+      <c r="B70" s="72"/>
+      <c r="C70" s="72"/>
+      <c r="D70" s="72"/>
+      <c r="E70" s="72"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
@@ -9734,10 +9732,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="71"/>
+      <c r="B3" s="72"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
@@ -9989,7 +9987,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -10284,10 +10282,10 @@
         <v>98</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="G21" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -10318,10 +10316,10 @@
         <v>102</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="G23" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -10352,10 +10350,10 @@
         <v>114</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="G25" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -10386,10 +10384,10 @@
         <v>110</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="G27" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -10420,10 +10418,10 @@
         <v>106</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="G29" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -10454,10 +10452,10 @@
         <v>118</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="G31" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -10488,10 +10486,10 @@
         <v>122</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="G33" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -10626,17 +10624,17 @@
       <c r="F54" s="2"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="72" t="s">
+      <c r="A56" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="B56" s="72"/>
-      <c r="C56" s="72"/>
-      <c r="D56" s="72"/>
-      <c r="E56" s="72"/>
-      <c r="F56" s="72"/>
-      <c r="G56" s="72"/>
-      <c r="H56" s="72"/>
-      <c r="I56" s="72"/>
+      <c r="B56" s="73"/>
+      <c r="C56" s="73"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="73"/>
+      <c r="F56" s="73"/>
+      <c r="G56" s="73"/>
+      <c r="H56" s="73"/>
+      <c r="I56" s="73"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
@@ -10701,17 +10699,17 @@
       </c>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="72" t="s">
+      <c r="A65" s="73" t="s">
         <v>347</v>
       </c>
-      <c r="B65" s="72"/>
-      <c r="C65" s="72"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="72"/>
-      <c r="H65" s="72"/>
-      <c r="I65" s="72"/>
+      <c r="B65" s="73"/>
+      <c r="C65" s="73"/>
+      <c r="D65" s="73"/>
+      <c r="E65" s="73"/>
+      <c r="F65" s="73"/>
+      <c r="G65" s="73"/>
+      <c r="H65" s="73"/>
+      <c r="I65" s="73"/>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
@@ -10844,7 +10842,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -11063,16 +11063,16 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="71"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="15" t="s">
@@ -11163,9 +11163,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X244"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -11212,10 +11212,10 @@
         <v>424</v>
       </c>
       <c r="F1" s="65" t="s">
+        <v>1416</v>
+      </c>
+      <c r="G1" s="65" t="s">
         <v>1417</v>
-      </c>
-      <c r="G1" s="65" t="s">
-        <v>1418</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>425</v>
@@ -11350,11 +11350,11 @@
       </c>
       <c r="J5" s="28" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>03/20/2023</v>
+        <v>03/25/2023</v>
       </c>
       <c r="K5" s="27" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>03/20/2023</v>
+        <v>03/25/2023</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="30">
@@ -11641,7 +11641,7 @@
     </row>
     <row r="23" spans="1:24">
       <c r="A23" s="34" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>493</v>
@@ -11653,10 +11653,10 @@
         <v>505</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>1411</v>
-      </c>
-      <c r="H23" t="s">
-        <v>1423</v>
+        <v>1410</v>
+      </c>
+      <c r="H23" s="70">
+        <v>44980</v>
       </c>
       <c r="I23" s="30"/>
       <c r="J23" s="36"/>
@@ -11677,7 +11677,7 @@
     </row>
     <row r="24" spans="1:24">
       <c r="A24" s="34" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="B24" s="34" t="s">
         <v>488</v>
@@ -11689,16 +11689,16 @@
         <v>505</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="F24" s="67" t="s">
+        <v>1418</v>
+      </c>
+      <c r="G24" s="67" t="s">
         <v>1419</v>
       </c>
-      <c r="G24" s="67" t="s">
-        <v>1420</v>
-      </c>
-      <c r="H24" t="s">
-        <v>1423</v>
+      <c r="H24" s="70">
+        <v>44980</v>
       </c>
       <c r="I24" s="30"/>
       <c r="J24" s="36"/>
@@ -14857,27 +14857,27 @@
       <c r="J143" s="27"/>
     </row>
     <row r="146" spans="1:19">
-      <c r="A146" s="72" t="s">
+      <c r="A146" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="B146" s="72"/>
-      <c r="C146" s="72"/>
-      <c r="D146" s="72"/>
-      <c r="E146" s="72"/>
-      <c r="F146" s="72"/>
-      <c r="G146" s="72"/>
-      <c r="H146" s="72"/>
-      <c r="I146" s="72"/>
-      <c r="J146" s="72"/>
-      <c r="K146" s="72"/>
-      <c r="L146" s="72"/>
-      <c r="M146" s="72"/>
-      <c r="N146" s="72"/>
-      <c r="O146" s="72"/>
-      <c r="P146" s="72"/>
-      <c r="Q146" s="72"/>
-      <c r="R146" s="72"/>
-      <c r="S146" s="72"/>
+      <c r="B146" s="73"/>
+      <c r="C146" s="73"/>
+      <c r="D146" s="73"/>
+      <c r="E146" s="73"/>
+      <c r="F146" s="73"/>
+      <c r="G146" s="73"/>
+      <c r="H146" s="73"/>
+      <c r="I146" s="73"/>
+      <c r="J146" s="73"/>
+      <c r="K146" s="73"/>
+      <c r="L146" s="73"/>
+      <c r="M146" s="73"/>
+      <c r="N146" s="73"/>
+      <c r="O146" s="73"/>
+      <c r="P146" s="73"/>
+      <c r="Q146" s="73"/>
+      <c r="R146" s="73"/>
+      <c r="S146" s="73"/>
     </row>
     <row r="147" spans="1:19">
       <c r="A147" s="27" t="s">
@@ -15662,27 +15662,27 @@
       </c>
     </row>
     <row r="208" spans="1:19">
-      <c r="A208" s="72" t="s">
+      <c r="A208" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="B208" s="72"/>
-      <c r="C208" s="72"/>
-      <c r="D208" s="72"/>
-      <c r="E208" s="72"/>
-      <c r="F208" s="72"/>
-      <c r="G208" s="72"/>
-      <c r="H208" s="72"/>
-      <c r="I208" s="72"/>
-      <c r="J208" s="72"/>
-      <c r="K208" s="72"/>
-      <c r="L208" s="72"/>
-      <c r="M208" s="72"/>
-      <c r="N208" s="72"/>
-      <c r="O208" s="72"/>
-      <c r="P208" s="72"/>
-      <c r="Q208" s="72"/>
-      <c r="R208" s="72"/>
-      <c r="S208" s="72"/>
+      <c r="B208" s="73"/>
+      <c r="C208" s="73"/>
+      <c r="D208" s="73"/>
+      <c r="E208" s="73"/>
+      <c r="F208" s="73"/>
+      <c r="G208" s="73"/>
+      <c r="H208" s="73"/>
+      <c r="I208" s="73"/>
+      <c r="J208" s="73"/>
+      <c r="K208" s="73"/>
+      <c r="L208" s="73"/>
+      <c r="M208" s="73"/>
+      <c r="N208" s="73"/>
+      <c r="O208" s="73"/>
+      <c r="P208" s="73"/>
+      <c r="Q208" s="73"/>
+      <c r="R208" s="73"/>
+      <c r="S208" s="73"/>
     </row>
     <row r="209" spans="1:23" ht="30">
       <c r="A209" s="27" t="s">
@@ -16233,7 +16233,7 @@
     <hyperlink ref="E244" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated method and created testcase of Acuity Task call and Event
Signed-off-by: Sourabh kumar <sourabh@navatargroup.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\git\PE4.7Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9339E9F8-56EC-48C1-943F-9AD8D8B799E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC663065-FD18-4282-A76D-DC5C24FFED59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2584" uniqueCount="1509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2604" uniqueCount="1520">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -4571,6 +4571,39 @@
   </si>
   <si>
     <t>Test Account 1_INSTITUTION&lt;break&gt;Test Account 1_INTERMEDIARY&lt;break&gt;Test Account 2_INSTITUTION</t>
+  </si>
+  <si>
+    <t>ParticipantRecord</t>
+  </si>
+  <si>
+    <t>ParticipantRecordObject</t>
+  </si>
+  <si>
+    <t>TagsRecord</t>
+  </si>
+  <si>
+    <t>TagsObject</t>
+  </si>
+  <si>
+    <t>Test Contact 1_COMPANY&lt;break&gt;Test Contact 1_ADVISOR</t>
+  </si>
+  <si>
+    <t>Contact&lt;break&gt;Contact</t>
+  </si>
+  <si>
+    <t>Test Account 1_COMPANY&lt;break&gt;Connection Deal 1&lt;break&gt;PE Fund 1&lt;break&gt;PE Fundraising 1&lt;break&gt;PE Theme 1</t>
+  </si>
+  <si>
+    <t>Firm&lt;break&gt;Deal&lt;break&gt;Fund&lt;break&gt;Fundraising&lt;break&gt;Theme</t>
+  </si>
+  <si>
+    <t>2/23/2023</t>
+  </si>
+  <si>
+    <t>Followup Task 1</t>
+  </si>
+  <si>
+    <t>ATCE_027</t>
   </si>
 </sst>
 </file>
@@ -4880,7 +4913,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5023,8 +5056,19 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5040,7 +5084,6 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5569,11 +5612,11 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:AF158"/>
+  <dimension ref="A1:AJ158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE23" sqref="AE23"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -5604,10 +5647,14 @@
     <col min="28" max="29" width="69" customWidth="1" collapsed="1"/>
     <col min="30" max="30" width="21.5546875" customWidth="1" collapsed="1"/>
     <col min="31" max="31" width="35.109375" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="68.21875" customWidth="1"/>
+    <col min="32" max="32" width="68.21875" style="18" customWidth="1"/>
+    <col min="33" max="33" width="38.88671875" customWidth="1"/>
+    <col min="34" max="34" width="32.88671875" customWidth="1"/>
+    <col min="35" max="35" width="49.5546875" style="18" customWidth="1"/>
+    <col min="36" max="36" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5701,11 +5748,23 @@
       <c r="AE1" s="1" t="s">
         <v>1055</v>
       </c>
-      <c r="AF1" s="17" t="s">
+      <c r="AF1" s="71" t="s">
         <v>1056</v>
       </c>
-    </row>
-    <row r="3" spans="1:32">
+      <c r="AG1" s="1" t="s">
+        <v>1509</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>1510</v>
+      </c>
+      <c r="AI1" s="20" t="s">
+        <v>1511</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -5732,7 +5791,7 @@
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:36">
       <c r="A4" t="s">
         <v>1058</v>
       </c>
@@ -5746,7 +5805,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:36">
       <c r="A5" t="s">
         <v>1061</v>
       </c>
@@ -5760,7 +5819,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:36">
       <c r="A6" t="s">
         <v>1062</v>
       </c>
@@ -5774,7 +5833,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:36">
       <c r="A7" t="s">
         <v>1063</v>
       </c>
@@ -5788,7 +5847,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:36">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -5815,7 +5874,7 @@
       <c r="V12" s="16"/>
       <c r="W12" s="16"/>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:36">
       <c r="A13" t="s">
         <v>1065</v>
       </c>
@@ -5826,7 +5885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:36">
       <c r="A14" t="s">
         <v>1066</v>
       </c>
@@ -5837,7 +5896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:36">
       <c r="A15" t="s">
         <v>1067</v>
       </c>
@@ -5848,7 +5907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:36">
       <c r="A16" t="s">
         <v>1068</v>
       </c>
@@ -5865,7 +5924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:36">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -5896,7 +5955,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="16"/>
     </row>
-    <row r="19" spans="1:32" ht="15">
+    <row r="19" spans="1:36" ht="43.8">
       <c r="A19" s="69" t="s">
         <v>1071</v>
       </c>
@@ -5972,11 +6031,23 @@
       <c r="AC19" t="s">
         <v>1412</v>
       </c>
-      <c r="AF19" s="69" t="s">
+      <c r="AF19" s="72" t="s">
         <v>1502</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" ht="15">
+      <c r="AG19" t="s">
+        <v>1513</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>1514</v>
+      </c>
+      <c r="AI19" s="18" t="s">
+        <v>1515</v>
+      </c>
+      <c r="AJ19" s="18" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" ht="43.8">
       <c r="A20" t="s">
         <v>1080</v>
       </c>
@@ -6046,11 +6117,11 @@
       <c r="AB20" t="s">
         <v>1085</v>
       </c>
-      <c r="AF20" s="70" t="s">
+      <c r="AF20" s="73" t="s">
         <v>1503</v>
       </c>
     </row>
-    <row r="21" spans="1:32" ht="15">
+    <row r="21" spans="1:36" ht="43.8">
       <c r="A21" t="s">
         <v>1086</v>
       </c>
@@ -6108,11 +6179,11 @@
       <c r="Y21" t="s">
         <v>1088</v>
       </c>
-      <c r="AF21" s="70" t="s">
+      <c r="AF21" s="73" t="s">
         <v>1504</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:36" ht="28.8">
       <c r="A22" t="s">
         <v>1089</v>
       </c>
@@ -6146,11 +6217,11 @@
       <c r="X22" t="s">
         <v>1090</v>
       </c>
-      <c r="AF22" s="70" t="s">
+      <c r="AF22" s="73" t="s">
         <v>1505</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:36" ht="28.8">
       <c r="A23" t="s">
         <v>1091</v>
       </c>
@@ -6184,11 +6255,11 @@
       <c r="X23" t="s">
         <v>219</v>
       </c>
-      <c r="AF23" s="77" t="s">
+      <c r="AF23" s="74" t="s">
         <v>1508</v>
       </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:36">
       <c r="A24" t="s">
         <v>1402</v>
       </c>
@@ -6220,7 +6291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:36">
       <c r="A25" t="s">
         <v>1403</v>
       </c>
@@ -6252,7 +6323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:32">
+    <row r="26" spans="1:36">
       <c r="A26" t="s">
         <v>1404</v>
       </c>
@@ -6284,7 +6355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:32">
+    <row r="27" spans="1:36">
       <c r="A27" t="s">
         <v>1405</v>
       </c>
@@ -6316,7 +6387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:32">
+    <row r="28" spans="1:36">
       <c r="A28" t="s">
         <v>1413</v>
       </c>
@@ -6348,7 +6419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:32">
+    <row r="29" spans="1:36">
       <c r="A29" t="s">
         <v>1459</v>
       </c>
@@ -6380,7 +6451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:32">
+    <row r="30" spans="1:36">
       <c r="A30" t="s">
         <v>1460</v>
       </c>
@@ -6412,7 +6483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:32">
+    <row r="31" spans="1:36">
       <c r="A31" t="s">
         <v>1461</v>
       </c>
@@ -6444,7 +6515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:32">
+    <row r="32" spans="1:36">
       <c r="A32" t="s">
         <v>1462</v>
       </c>
@@ -6791,7 +6862,7 @@
       <c r="Z62" s="16"/>
       <c r="AA62" s="16"/>
     </row>
-    <row r="63" spans="1:32">
+    <row r="63" spans="1:32" ht="57.6">
       <c r="A63" t="s">
         <v>1092</v>
       </c>
@@ -6837,7 +6908,7 @@
       <c r="AB63" t="s">
         <v>1078</v>
       </c>
-      <c r="AF63" t="s">
+      <c r="AF63" s="18" t="s">
         <v>1094</v>
       </c>
     </row>
@@ -8498,39 +8569,39 @@
       </c>
     </row>
     <row r="121" spans="1:31">
-      <c r="A121" s="74" t="s">
+      <c r="A121" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="B121" s="74"/>
-      <c r="C121" s="74"/>
-      <c r="D121" s="74"/>
-      <c r="E121" s="74"/>
-      <c r="F121" s="74"/>
-      <c r="G121" s="74"/>
-      <c r="H121" s="74"/>
-      <c r="I121" s="74"/>
-      <c r="J121" s="74"/>
-      <c r="K121" s="74"/>
-      <c r="L121" s="74"/>
-      <c r="M121" s="74"/>
-      <c r="N121" s="74"/>
-      <c r="O121" s="74"/>
-      <c r="P121" s="74"/>
-      <c r="Q121" s="74"/>
-      <c r="R121" s="74"/>
-      <c r="S121" s="74"/>
-      <c r="T121" s="74"/>
-      <c r="U121" s="74"/>
-      <c r="V121" s="74"/>
-      <c r="W121" s="74"/>
-      <c r="X121" s="74"/>
-      <c r="Y121" s="74"/>
-      <c r="Z121" s="74"/>
-      <c r="AA121" s="74"/>
-      <c r="AB121" s="74"/>
-      <c r="AC121" s="74"/>
-      <c r="AD121" s="74"/>
-      <c r="AE121" s="74"/>
+      <c r="B121" s="77"/>
+      <c r="C121" s="77"/>
+      <c r="D121" s="77"/>
+      <c r="E121" s="77"/>
+      <c r="F121" s="77"/>
+      <c r="G121" s="77"/>
+      <c r="H121" s="77"/>
+      <c r="I121" s="77"/>
+      <c r="J121" s="77"/>
+      <c r="K121" s="77"/>
+      <c r="L121" s="77"/>
+      <c r="M121" s="77"/>
+      <c r="N121" s="77"/>
+      <c r="O121" s="77"/>
+      <c r="P121" s="77"/>
+      <c r="Q121" s="77"/>
+      <c r="R121" s="77"/>
+      <c r="S121" s="77"/>
+      <c r="T121" s="77"/>
+      <c r="U121" s="77"/>
+      <c r="V121" s="77"/>
+      <c r="W121" s="77"/>
+      <c r="X121" s="77"/>
+      <c r="Y121" s="77"/>
+      <c r="Z121" s="77"/>
+      <c r="AA121" s="77"/>
+      <c r="AB121" s="77"/>
+      <c r="AC121" s="77"/>
+      <c r="AD121" s="77"/>
+      <c r="AE121" s="77"/>
     </row>
     <row r="122" spans="1:31">
       <c r="A122" t="s">
@@ -8793,39 +8864,39 @@
       </c>
     </row>
     <row r="156" spans="1:31">
-      <c r="A156" s="74" t="s">
+      <c r="A156" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="B156" s="74"/>
-      <c r="C156" s="74"/>
-      <c r="D156" s="74"/>
-      <c r="E156" s="74"/>
-      <c r="F156" s="74"/>
-      <c r="G156" s="74"/>
-      <c r="H156" s="74"/>
-      <c r="I156" s="74"/>
-      <c r="J156" s="74"/>
-      <c r="K156" s="74"/>
-      <c r="L156" s="74"/>
-      <c r="M156" s="74"/>
-      <c r="N156" s="74"/>
-      <c r="O156" s="74"/>
-      <c r="P156" s="74"/>
-      <c r="Q156" s="74"/>
-      <c r="R156" s="74"/>
-      <c r="S156" s="74"/>
-      <c r="T156" s="74"/>
-      <c r="U156" s="74"/>
-      <c r="V156" s="74"/>
-      <c r="W156" s="74"/>
-      <c r="X156" s="74"/>
-      <c r="Y156" s="74"/>
-      <c r="Z156" s="74"/>
-      <c r="AA156" s="74"/>
-      <c r="AB156" s="74"/>
-      <c r="AC156" s="74"/>
-      <c r="AD156" s="74"/>
-      <c r="AE156" s="74"/>
+      <c r="B156" s="77"/>
+      <c r="C156" s="77"/>
+      <c r="D156" s="77"/>
+      <c r="E156" s="77"/>
+      <c r="F156" s="77"/>
+      <c r="G156" s="77"/>
+      <c r="H156" s="77"/>
+      <c r="I156" s="77"/>
+      <c r="J156" s="77"/>
+      <c r="K156" s="77"/>
+      <c r="L156" s="77"/>
+      <c r="M156" s="77"/>
+      <c r="N156" s="77"/>
+      <c r="O156" s="77"/>
+      <c r="P156" s="77"/>
+      <c r="Q156" s="77"/>
+      <c r="R156" s="77"/>
+      <c r="S156" s="77"/>
+      <c r="T156" s="77"/>
+      <c r="U156" s="77"/>
+      <c r="V156" s="77"/>
+      <c r="W156" s="77"/>
+      <c r="X156" s="77"/>
+      <c r="Y156" s="77"/>
+      <c r="Z156" s="77"/>
+      <c r="AA156" s="77"/>
+      <c r="AB156" s="77"/>
+      <c r="AC156" s="77"/>
+      <c r="AD156" s="77"/>
+      <c r="AE156" s="77"/>
     </row>
     <row r="157" spans="1:31">
       <c r="A157" t="s">
@@ -9125,13 +9196,13 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="76" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
@@ -9315,22 +9386,22 @@
     </row>
     <row r="9" spans="1:14" ht="19.5" customHeight="1"/>
     <row r="10" spans="1:14">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
@@ -9347,22 +9418,22 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="79" t="s">
         <v>1338</v>
       </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="76"/>
-      <c r="L14" s="76"/>
-      <c r="M14" s="76"/>
-      <c r="N14" s="76"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="79"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
@@ -9465,13 +9536,13 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
       <c r="F3" s="62"/>
       <c r="G3" s="63"/>
       <c r="H3" s="63"/>
@@ -9680,12 +9751,12 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="76" t="s">
         <v>1368</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
@@ -9814,14 +9885,14 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="75" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -9934,11 +10005,11 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -10362,13 +10433,13 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="73" t="s">
+      <c r="A59" s="76" t="s">
         <v>152</v>
       </c>
-      <c r="B59" s="73"/>
-      <c r="C59" s="73"/>
-      <c r="D59" s="73"/>
-      <c r="E59" s="73"/>
+      <c r="B59" s="76"/>
+      <c r="C59" s="76"/>
+      <c r="D59" s="76"/>
+      <c r="E59" s="76"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
@@ -10448,13 +10519,13 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="73" t="s">
+      <c r="A70" s="76" t="s">
         <v>168</v>
       </c>
-      <c r="B70" s="73"/>
-      <c r="C70" s="73"/>
-      <c r="D70" s="73"/>
-      <c r="E70" s="73"/>
+      <c r="B70" s="76"/>
+      <c r="C70" s="76"/>
+      <c r="D70" s="76"/>
+      <c r="E70" s="76"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
@@ -10611,10 +10682,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="76" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="73"/>
+      <c r="B3" s="76"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
@@ -10865,8 +10936,8 @@
   <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -11503,17 +11574,17 @@
       <c r="F54" s="2"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="74" t="s">
+      <c r="A56" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="B56" s="74"/>
-      <c r="C56" s="74"/>
-      <c r="D56" s="74"/>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-      <c r="G56" s="74"/>
-      <c r="H56" s="74"/>
-      <c r="I56" s="74"/>
+      <c r="B56" s="77"/>
+      <c r="C56" s="77"/>
+      <c r="D56" s="77"/>
+      <c r="E56" s="77"/>
+      <c r="F56" s="77"/>
+      <c r="G56" s="77"/>
+      <c r="H56" s="77"/>
+      <c r="I56" s="77"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
@@ -11578,17 +11649,17 @@
       </c>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="74" t="s">
+      <c r="A65" s="77" t="s">
         <v>346</v>
       </c>
-      <c r="B65" s="74"/>
-      <c r="C65" s="74"/>
-      <c r="D65" s="74"/>
-      <c r="E65" s="74"/>
-      <c r="F65" s="74"/>
-      <c r="G65" s="74"/>
-      <c r="H65" s="74"/>
-      <c r="I65" s="74"/>
+      <c r="B65" s="77"/>
+      <c r="C65" s="77"/>
+      <c r="D65" s="77"/>
+      <c r="E65" s="77"/>
+      <c r="F65" s="77"/>
+      <c r="G65" s="77"/>
+      <c r="H65" s="77"/>
+      <c r="I65" s="77"/>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
@@ -11883,7 +11954,7 @@
       <c r="B12" s="68" t="s">
         <v>1499</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="70" t="s">
         <v>1506</v>
       </c>
     </row>
@@ -11964,16 +12035,16 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="73" t="s">
+      <c r="A27" s="76" t="s">
         <v>152</v>
       </c>
-      <c r="B27" s="73"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="76"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="76"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
@@ -12061,9 +12132,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X266"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -12250,11 +12321,11 @@
       </c>
       <c r="J5" s="23" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>04/05/2023</v>
+        <v>04/06/2023</v>
       </c>
       <c r="K5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>04/05/2023</v>
+        <v>04/06/2023</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="28.8">
@@ -12561,8 +12632,8 @@
       <c r="G23" s="59" t="s">
         <v>1410</v>
       </c>
-      <c r="H23" s="67">
-        <v>44987</v>
+      <c r="H23" s="67" t="s">
+        <v>1517</v>
       </c>
       <c r="I23" s="19"/>
       <c r="J23" s="28"/>
@@ -12603,8 +12674,8 @@
       <c r="G24" s="59" t="s">
         <v>1410</v>
       </c>
-      <c r="H24" s="67">
-        <v>44987</v>
+      <c r="H24" s="67" t="s">
+        <v>1517</v>
       </c>
       <c r="I24" s="19"/>
       <c r="J24" s="28"/>
@@ -13552,6 +13623,38 @@
       <c r="N48" s="19"/>
       <c r="O48" s="19"/>
       <c r="P48" s="19"/>
+    </row>
+    <row r="49" spans="1:16" s="26" customFormat="1">
+      <c r="A49" s="26" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>489</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>1518</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>501</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>1401</v>
+      </c>
+      <c r="F49" s="26" t="s">
+        <v>1409</v>
+      </c>
+      <c r="G49" s="26" t="s">
+        <v>1410</v>
+      </c>
+      <c r="M49" s="26" t="s">
+        <v>714</v>
+      </c>
+      <c r="O49" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="P49" s="26" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="52" spans="1:16">
       <c r="A52" s="16"/>
@@ -16683,27 +16786,27 @@
       <c r="J165"/>
     </row>
     <row r="168" spans="1:20">
-      <c r="A168" s="74" t="s">
+      <c r="A168" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="B168" s="74"/>
-      <c r="C168" s="74"/>
-      <c r="D168" s="74"/>
-      <c r="E168" s="74"/>
-      <c r="F168" s="74"/>
-      <c r="G168" s="74"/>
-      <c r="H168" s="74"/>
-      <c r="I168" s="74"/>
-      <c r="J168" s="74"/>
-      <c r="K168" s="74"/>
-      <c r="L168" s="74"/>
-      <c r="M168" s="74"/>
-      <c r="N168" s="74"/>
-      <c r="O168" s="74"/>
-      <c r="P168" s="74"/>
-      <c r="Q168" s="74"/>
-      <c r="R168" s="74"/>
-      <c r="S168" s="74"/>
+      <c r="B168" s="77"/>
+      <c r="C168" s="77"/>
+      <c r="D168" s="77"/>
+      <c r="E168" s="77"/>
+      <c r="F168" s="77"/>
+      <c r="G168" s="77"/>
+      <c r="H168" s="77"/>
+      <c r="I168" s="77"/>
+      <c r="J168" s="77"/>
+      <c r="K168" s="77"/>
+      <c r="L168" s="77"/>
+      <c r="M168" s="77"/>
+      <c r="N168" s="77"/>
+      <c r="O168" s="77"/>
+      <c r="P168" s="77"/>
+      <c r="Q168" s="77"/>
+      <c r="R168" s="77"/>
+      <c r="S168" s="77"/>
     </row>
     <row r="169" spans="1:20">
       <c r="A169" t="s">
@@ -17488,27 +17591,27 @@
       </c>
     </row>
     <row r="230" spans="1:23">
-      <c r="A230" s="74" t="s">
+      <c r="A230" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="B230" s="74"/>
-      <c r="C230" s="74"/>
-      <c r="D230" s="74"/>
-      <c r="E230" s="74"/>
-      <c r="F230" s="74"/>
-      <c r="G230" s="74"/>
-      <c r="H230" s="74"/>
-      <c r="I230" s="74"/>
-      <c r="J230" s="74"/>
-      <c r="K230" s="74"/>
-      <c r="L230" s="74"/>
-      <c r="M230" s="74"/>
-      <c r="N230" s="74"/>
-      <c r="O230" s="74"/>
-      <c r="P230" s="74"/>
-      <c r="Q230" s="74"/>
-      <c r="R230" s="74"/>
-      <c r="S230" s="74"/>
+      <c r="B230" s="77"/>
+      <c r="C230" s="77"/>
+      <c r="D230" s="77"/>
+      <c r="E230" s="77"/>
+      <c r="F230" s="77"/>
+      <c r="G230" s="77"/>
+      <c r="H230" s="77"/>
+      <c r="I230" s="77"/>
+      <c r="J230" s="77"/>
+      <c r="K230" s="77"/>
+      <c r="L230" s="77"/>
+      <c r="M230" s="77"/>
+      <c r="N230" s="77"/>
+      <c r="O230" s="77"/>
+      <c r="P230" s="77"/>
+      <c r="Q230" s="77"/>
+      <c r="R230" s="77"/>
+      <c r="S230" s="77"/>
     </row>
     <row r="231" spans="1:23" ht="28.8">
       <c r="A231" t="s">

</xml_diff>

<commit_message>
Added Deal and email missing point  of contact and fundrasing sheet of acuity data sheet
Signed-off-by: raviNavatar <106242727+raviNavatar@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\File merge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Kumar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535A7E07-00CE-4583-80F3-B5D00A0F5BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11280" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -38,7 +39,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Activity Timeline'!$B$1:$B$166</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4584" uniqueCount="2659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4587" uniqueCount="2660">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -8062,20 +8063,30 @@
   <si>
     <t>Firms&lt;break&gt;Contacts&lt;break&gt;Themes&lt;break&gt;Clips</t>
   </si>
+  <si>
+    <t>Parent_Institution</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="57">
+  <fonts count="58">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8607,29 +8618,29 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="37" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="38" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8641,45 +8652,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="37" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="38" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="38" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -8696,7 +8707,7 @@
     <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -8717,58 +8728,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8776,27 +8788,26 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8805,37 +8816,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="53" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="53" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="54" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="3" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="3" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -8844,22 +8856,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="3"/>
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 2" xfId="4"/>
-    <cellStyle name="Normal 2 3" xfId="6"/>
-    <cellStyle name="Normal 3" xfId="5"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -9131,7 +9142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L40"/>
   <sheetViews>
@@ -9139,11 +9150,11 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="26.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="26.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -9399,7 +9410,7 @@
         <v>2238</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" ht="15">
       <c r="A25" t="s">
         <v>2239</v>
       </c>
@@ -9413,7 +9424,7 @@
         <v>2241</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" ht="15">
       <c r="A26" t="s">
         <v>2242</v>
       </c>
@@ -9544,11 +9555,11 @@
       </c>
     </row>
     <row r="35" spans="1:12" s="16" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A35" s="116" t="s">
+      <c r="A35" s="117" t="s">
         <v>2267</v>
       </c>
-      <c r="B35" s="116"/>
-      <c r="C35" s="116"/>
+      <c r="B35" s="117"/>
+      <c r="C35" s="117"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" t="s">
@@ -9606,7 +9617,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" ht="15">
       <c r="A40" t="s">
         <v>2281</v>
       </c>
@@ -9624,14 +9635,14 @@
   <mergeCells count="1">
     <mergeCell ref="A35:C35"/>
   </mergeCells>
-  <phoneticPr fontId="52" type="noConversion"/>
+  <phoneticPr fontId="53" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -9639,19 +9650,19 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="18" collapsed="1"/>
+    <col min="1" max="1" width="8.88671875" style="18" collapsed="1"/>
     <col min="2" max="2" width="73" style="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.42578125" style="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" style="18" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.42578125" style="18" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.5703125" style="18" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.42578125" style="18" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="8.85546875" style="18" collapsed="1"/>
+    <col min="3" max="3" width="16.44140625" style="18" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.109375" style="18" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.44140625" style="18" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.5546875" style="18" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.44140625" style="18" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="8.88671875" style="18" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" ht="28.8">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -9684,7 +9695,7 @@
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
     </row>
-    <row r="4" spans="1:7" ht="45">
+    <row r="4" spans="1:7" ht="43.2">
       <c r="A4" s="18" t="s">
         <v>1007</v>
       </c>
@@ -9704,7 +9715,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="43.2">
       <c r="A5" s="18" t="s">
         <v>1013</v>
       </c>
@@ -9721,7 +9732,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45">
+    <row r="6" spans="1:7" ht="43.2">
       <c r="A6" s="18" t="s">
         <v>1015</v>
       </c>
@@ -9740,62 +9751,62 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4"/>
-    <hyperlink ref="B5" r:id="rId5"/>
-    <hyperlink ref="B6" r:id="rId6"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AL249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+    <sheetView topLeftCell="X1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA19" sqref="AA19"/>
+      <selection pane="bottomLeft" activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.109375" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="26" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.44140625" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="16" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="48.85546875" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="61.5703125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="25.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="48.88671875" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="33.5546875" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="61.5546875" customWidth="1" collapsed="1"/>
     <col min="27" max="27" width="40" customWidth="1" collapsed="1"/>
     <col min="28" max="29" width="69" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="68.28515625" style="18" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="38.85546875" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="49.5703125" style="18" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="63.42578125" style="18" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="63.7109375" style="18" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="21.5546875" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="35.109375" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="68.33203125" style="18" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="38.88671875" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="32.88671875" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="49.5546875" style="18" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="28.33203125" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="63.44140625" style="18" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="63.6640625" style="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
@@ -10105,7 +10116,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="16"/>
     </row>
-    <row r="19" spans="1:38" ht="105">
+    <row r="19" spans="1:38" ht="101.4">
       <c r="A19" s="67" t="s">
         <v>1055</v>
       </c>
@@ -10203,7 +10214,7 @@
         <v>2138</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="45">
+    <row r="20" spans="1:38" ht="43.8">
       <c r="A20" t="s">
         <v>1063</v>
       </c>
@@ -10277,7 +10288,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="45">
+    <row r="21" spans="1:38" ht="43.8">
       <c r="A21" t="s">
         <v>1068</v>
       </c>
@@ -10345,7 +10356,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="45">
+    <row r="22" spans="1:38" ht="29.4">
       <c r="A22" t="s">
         <v>1070</v>
       </c>
@@ -10410,7 +10421,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="30">
+    <row r="23" spans="1:38" ht="29.4">
       <c r="A23" t="s">
         <v>1072</v>
       </c>
@@ -10475,7 +10486,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" ht="15">
       <c r="A24" t="s">
         <v>1381</v>
       </c>
@@ -10534,7 +10545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" ht="15">
       <c r="A25" t="s">
         <v>1382</v>
       </c>
@@ -10593,7 +10604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" ht="15">
       <c r="A26" t="s">
         <v>1383</v>
       </c>
@@ -10652,7 +10663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" ht="15">
       <c r="A27" t="s">
         <v>1384</v>
       </c>
@@ -12699,7 +12710,7 @@
       <c r="Z144" s="16"/>
       <c r="AA144" s="16"/>
     </row>
-    <row r="145" spans="1:32" ht="60">
+    <row r="145" spans="1:32" ht="57.6">
       <c r="A145" t="s">
         <v>1073</v>
       </c>
@@ -13420,7 +13431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:32" ht="30">
+    <row r="159" spans="1:32">
       <c r="A159" t="s">
         <v>1118</v>
       </c>
@@ -14509,39 +14520,39 @@
       </c>
     </row>
     <row r="212" spans="1:31">
-      <c r="A212" s="118" t="s">
+      <c r="A212" s="119" t="s">
         <v>144</v>
       </c>
-      <c r="B212" s="118"/>
-      <c r="C212" s="118"/>
-      <c r="D212" s="118"/>
-      <c r="E212" s="118"/>
-      <c r="F212" s="118"/>
-      <c r="G212" s="118"/>
-      <c r="H212" s="118"/>
-      <c r="I212" s="118"/>
-      <c r="J212" s="118"/>
-      <c r="K212" s="118"/>
-      <c r="L212" s="118"/>
-      <c r="M212" s="118"/>
-      <c r="N212" s="118"/>
-      <c r="O212" s="118"/>
-      <c r="P212" s="118"/>
-      <c r="Q212" s="118"/>
-      <c r="R212" s="118"/>
-      <c r="S212" s="118"/>
-      <c r="T212" s="118"/>
-      <c r="U212" s="118"/>
-      <c r="V212" s="118"/>
-      <c r="W212" s="118"/>
-      <c r="X212" s="118"/>
-      <c r="Y212" s="118"/>
-      <c r="Z212" s="118"/>
-      <c r="AA212" s="118"/>
-      <c r="AB212" s="118"/>
-      <c r="AC212" s="118"/>
-      <c r="AD212" s="118"/>
-      <c r="AE212" s="118"/>
+      <c r="B212" s="119"/>
+      <c r="C212" s="119"/>
+      <c r="D212" s="119"/>
+      <c r="E212" s="119"/>
+      <c r="F212" s="119"/>
+      <c r="G212" s="119"/>
+      <c r="H212" s="119"/>
+      <c r="I212" s="119"/>
+      <c r="J212" s="119"/>
+      <c r="K212" s="119"/>
+      <c r="L212" s="119"/>
+      <c r="M212" s="119"/>
+      <c r="N212" s="119"/>
+      <c r="O212" s="119"/>
+      <c r="P212" s="119"/>
+      <c r="Q212" s="119"/>
+      <c r="R212" s="119"/>
+      <c r="S212" s="119"/>
+      <c r="T212" s="119"/>
+      <c r="U212" s="119"/>
+      <c r="V212" s="119"/>
+      <c r="W212" s="119"/>
+      <c r="X212" s="119"/>
+      <c r="Y212" s="119"/>
+      <c r="Z212" s="119"/>
+      <c r="AA212" s="119"/>
+      <c r="AB212" s="119"/>
+      <c r="AC212" s="119"/>
+      <c r="AD212" s="119"/>
+      <c r="AE212" s="119"/>
     </row>
     <row r="213" spans="1:31">
       <c r="A213" t="s">
@@ -14804,39 +14815,39 @@
       </c>
     </row>
     <row r="247" spans="1:31">
-      <c r="A247" s="118" t="s">
+      <c r="A247" s="119" t="s">
         <v>144</v>
       </c>
-      <c r="B247" s="118"/>
-      <c r="C247" s="118"/>
-      <c r="D247" s="118"/>
-      <c r="E247" s="118"/>
-      <c r="F247" s="118"/>
-      <c r="G247" s="118"/>
-      <c r="H247" s="118"/>
-      <c r="I247" s="118"/>
-      <c r="J247" s="118"/>
-      <c r="K247" s="118"/>
-      <c r="L247" s="118"/>
-      <c r="M247" s="118"/>
-      <c r="N247" s="118"/>
-      <c r="O247" s="118"/>
-      <c r="P247" s="118"/>
-      <c r="Q247" s="118"/>
-      <c r="R247" s="118"/>
-      <c r="S247" s="118"/>
-      <c r="T247" s="118"/>
-      <c r="U247" s="118"/>
-      <c r="V247" s="118"/>
-      <c r="W247" s="118"/>
-      <c r="X247" s="118"/>
-      <c r="Y247" s="118"/>
-      <c r="Z247" s="118"/>
-      <c r="AA247" s="118"/>
-      <c r="AB247" s="118"/>
-      <c r="AC247" s="118"/>
-      <c r="AD247" s="118"/>
-      <c r="AE247" s="118"/>
+      <c r="B247" s="119"/>
+      <c r="C247" s="119"/>
+      <c r="D247" s="119"/>
+      <c r="E247" s="119"/>
+      <c r="F247" s="119"/>
+      <c r="G247" s="119"/>
+      <c r="H247" s="119"/>
+      <c r="I247" s="119"/>
+      <c r="J247" s="119"/>
+      <c r="K247" s="119"/>
+      <c r="L247" s="119"/>
+      <c r="M247" s="119"/>
+      <c r="N247" s="119"/>
+      <c r="O247" s="119"/>
+      <c r="P247" s="119"/>
+      <c r="Q247" s="119"/>
+      <c r="R247" s="119"/>
+      <c r="S247" s="119"/>
+      <c r="T247" s="119"/>
+      <c r="U247" s="119"/>
+      <c r="V247" s="119"/>
+      <c r="W247" s="119"/>
+      <c r="X247" s="119"/>
+      <c r="Y247" s="119"/>
+      <c r="Z247" s="119"/>
+      <c r="AA247" s="119"/>
+      <c r="AB247" s="119"/>
+      <c r="AC247" s="119"/>
+      <c r="AD247" s="119"/>
+      <c r="AE247" s="119"/>
     </row>
     <row r="248" spans="1:31">
       <c r="A248" t="s">
@@ -14859,10 +14870,10 @@
     <mergeCell ref="A212:AE212"/>
     <mergeCell ref="A247:AE247"/>
   </mergeCells>
-  <phoneticPr fontId="43" type="noConversion"/>
+  <phoneticPr fontId="44" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D61" r:id="rId1" tooltip="Test Contact 2_INSTITUTION" display="https://navatar-c--tr4sb6.sandbox.lightning.force.com/003DN000001U5JiYAK"/>
-    <hyperlink ref="D195" r:id="rId2" tooltip="frank"/>
+    <hyperlink ref="D61" r:id="rId1" tooltip="Test Contact 2_INSTITUTION" display="https://navatar-c--tr4sb6.sandbox.lightning.force.com/003DN000001U5JiYAK" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="D195" r:id="rId2" tooltip="frank" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId3"/>
@@ -14870,17 +14881,17 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -14919,7 +14930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -14927,11 +14938,11 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="72.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="72.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -14962,7 +14973,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:G33"/>
   <sheetViews>
@@ -14971,12 +14982,12 @@
       <selection pane="bottomLeft" activeCell="A25" sqref="A25:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="28.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -15179,13 +15190,13 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="117" t="s">
+      <c r="A19" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="117"/>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="87" t="s">
@@ -15219,11 +15230,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" s="16" customFormat="1">
-      <c r="A25" s="116" t="s">
+      <c r="A25" s="117" t="s">
         <v>2284</v>
       </c>
-      <c r="B25" s="116"/>
-      <c r="C25" s="116"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="117"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
@@ -15300,33 +15311,34 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="42.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="6" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="12" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="6.33203125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.88671875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="26" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="39.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.33203125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="39.44140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="15" customFormat="1">
+    <row r="1" spans="1:15" s="15" customFormat="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -15369,8 +15381,11 @@
       <c r="N1" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" s="16" customFormat="1">
+      <c r="O1" s="15" t="s">
+        <v>2461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="16" customFormat="1">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
@@ -15381,7 +15396,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="12" t="s">
         <v>1303</v>
       </c>
@@ -15409,7 +15424,7 @@
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="12" t="s">
         <v>1308</v>
       </c>
@@ -15429,7 +15444,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="12" t="s">
         <v>1310</v>
       </c>
@@ -15457,26 +15472,26 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="19.5" customHeight="1"/>
-    <row r="10" spans="1:14">
-      <c r="A10" s="119" t="s">
+    <row r="9" spans="1:15" ht="19.5" customHeight="1"/>
+    <row r="10" spans="1:15">
+      <c r="A10" s="120" t="s">
         <v>144</v>
       </c>
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="119"/>
-      <c r="N10" s="119"/>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="B10" s="120"/>
+      <c r="C10" s="120"/>
+      <c r="D10" s="120"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="M10" s="120"/>
+      <c r="N10" s="120"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="87" t="s">
         <v>1316</v>
       </c>
@@ -15502,7 +15517,7 @@
       <c r="M11" s="87"/>
       <c r="N11" s="87"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" s="87" t="s">
         <v>2053</v>
       </c>
@@ -15510,7 +15525,7 @@
         <v>1846</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" s="87" t="s">
         <v>2054</v>
       </c>
@@ -15518,23 +15533,23 @@
         <v>2055</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="120" t="s">
+    <row r="16" spans="1:15">
+      <c r="A16" s="121" t="s">
         <v>1317</v>
       </c>
-      <c r="B16" s="120"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
-      <c r="G16" s="120"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="120"/>
-      <c r="J16" s="120"/>
-      <c r="K16" s="120"/>
-      <c r="L16" s="120"/>
-      <c r="M16" s="120"/>
-      <c r="N16" s="120"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="121"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="121"/>
+      <c r="L16" s="121"/>
+      <c r="M16" s="121"/>
+      <c r="N16" s="121"/>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
@@ -15605,11 +15620,11 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="16" customFormat="1">
-      <c r="A25" s="116" t="s">
+      <c r="A25" s="117" t="s">
         <v>2284</v>
       </c>
-      <c r="B25" s="116"/>
-      <c r="C25" s="116"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="117"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="12" t="s">
@@ -15767,26 +15782,26 @@
     <mergeCell ref="A16:N16"/>
     <mergeCell ref="A25:C25"/>
   </mergeCells>
-  <phoneticPr fontId="50" type="noConversion"/>
+  <phoneticPr fontId="51" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="44.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="15" customFormat="1">
@@ -15854,13 +15869,13 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="52" type="noConversion"/>
+  <phoneticPr fontId="53" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -15868,11 +15883,11 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -15921,7 +15936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -15929,11 +15944,11 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="3" width="14.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -15961,13 +15976,13 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="119" t="s">
+      <c r="A3" s="120" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="119"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
       <c r="F3" s="61"/>
       <c r="G3" s="62"/>
       <c r="H3" s="62"/>
@@ -16000,7 +16015,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:L8"/>
   <sheetViews>
@@ -16008,18 +16023,18 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="8" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.88671875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="23.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -16074,7 +16089,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="45">
+    <row r="4" spans="1:12" ht="28.8">
       <c r="A4" s="7" t="s">
         <v>1337</v>
       </c>
@@ -16118,7 +16133,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="45">
+    <row r="8" spans="1:12" ht="28.8">
       <c r="A8" s="7" t="s">
         <v>1345</v>
       </c>
@@ -16155,23 +16170,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16187,15 +16204,18 @@
       <c r="E1" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="116" t="s">
+      <c r="F1" s="1" t="s">
+        <v>2659</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="116"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -16206,7 +16226,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -16214,7 +16234,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -16222,7 +16242,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -16230,7 +16250,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -16238,7 +16258,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -16246,7 +16266,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -16254,7 +16274,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -16262,7 +16282,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -16270,7 +16290,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -16281,7 +16301,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -16289,7 +16309,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -16297,7 +16317,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" s="12" t="s">
         <v>69</v>
       </c>
@@ -16669,13 +16689,13 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="117" t="s">
+      <c r="A64" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="117"/>
-      <c r="C64" s="117"/>
-      <c r="D64" s="117"/>
-      <c r="E64" s="117"/>
+      <c r="B64" s="118"/>
+      <c r="C64" s="118"/>
+      <c r="D64" s="118"/>
+      <c r="E64" s="118"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
@@ -16754,7 +16774,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="120">
+    <row r="73" spans="1:3" ht="100.8">
       <c r="A73" s="87" t="s">
         <v>1450</v>
       </c>
@@ -16847,13 +16867,13 @@
       <c r="C82" s="87"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="117" t="s">
+      <c r="A85" s="118" t="s">
         <v>160</v>
       </c>
-      <c r="B85" s="117"/>
-      <c r="C85" s="117"/>
-      <c r="D85" s="117"/>
-      <c r="E85" s="117"/>
+      <c r="B85" s="118"/>
+      <c r="C85" s="118"/>
+      <c r="D85" s="118"/>
+      <c r="E85" s="118"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
@@ -16976,11 +16996,11 @@
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="116" t="s">
+      <c r="A101" s="117" t="s">
         <v>2284</v>
       </c>
-      <c r="B101" s="116"/>
-      <c r="C101" s="116"/>
+      <c r="B101" s="117"/>
+      <c r="C101" s="117"/>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
@@ -17051,7 +17071,7 @@
         <v>2290</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15.75" thickBot="1">
+    <row r="108" spans="1:6" ht="15" thickBot="1">
       <c r="A108" t="s">
         <v>2299</v>
       </c>
@@ -17150,7 +17170,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" ht="15">
       <c r="A117" t="s">
         <v>2317</v>
       </c>
@@ -17215,11 +17235,11 @@
       </c>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="116" t="s">
+      <c r="A125" s="117" t="s">
         <v>2267</v>
       </c>
-      <c r="B125" s="116"/>
-      <c r="C125" s="116"/>
+      <c r="B125" s="117"/>
+      <c r="C125" s="117"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
@@ -17251,24 +17271,24 @@
     <mergeCell ref="A101:C101"/>
     <mergeCell ref="A125:C125"/>
   </mergeCells>
-  <phoneticPr fontId="50" type="noConversion"/>
+  <phoneticPr fontId="51" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -17280,12 +17300,12 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="118" t="s">
         <v>1347</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
@@ -17408,7 +17428,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F26"/>
   <sheetViews>
@@ -17416,9 +17436,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -17430,14 +17450,14 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="117" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -17504,12 +17524,12 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="118" t="s">
         <v>1347</v>
       </c>
-      <c r="B13" s="117"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="117"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="118"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="87" t="s">
@@ -17615,24 +17635,24 @@
     <mergeCell ref="A13:D13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B9" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="113"/>
+    <col min="1" max="16384" width="8.88671875" style="113"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -17710,7 +17730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -17718,10 +17738,10 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -17733,10 +17753,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="118" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="117"/>
+      <c r="B3" s="118"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
@@ -17787,26 +17807,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="20" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.88671875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17982,27 +18002,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96:XFD140"/>
+      <selection pane="bottomLeft" activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="45.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="45.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.5546875" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="117" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18030,8 +18051,11 @@
       <c r="I1" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -18042,7 +18066,7 @@
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -18055,7 +18079,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -18072,7 +18096,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>225</v>
       </c>
@@ -18080,7 +18104,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>227</v>
       </c>
@@ -18088,7 +18112,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>228</v>
       </c>
@@ -18096,7 +18120,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>229</v>
       </c>
@@ -18116,7 +18140,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>234</v>
       </c>
@@ -18124,7 +18148,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>236</v>
       </c>
@@ -18132,7 +18156,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>238</v>
       </c>
@@ -18157,7 +18181,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" s="12" t="s">
         <v>245</v>
       </c>
@@ -18172,7 +18196,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" s="12" t="s">
         <v>247</v>
       </c>
@@ -18187,7 +18211,7 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" s="12" t="s">
         <v>249</v>
       </c>
@@ -18210,7 +18234,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" s="12" t="s">
         <v>255</v>
       </c>
@@ -18229,7 +18253,7 @@
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>259</v>
       </c>
@@ -18768,17 +18792,17 @@
       <c r="F56" s="2"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="118" t="s">
+      <c r="A58" s="119" t="s">
         <v>144</v>
       </c>
-      <c r="B58" s="118"/>
-      <c r="C58" s="118"/>
-      <c r="D58" s="118"/>
-      <c r="E58" s="118"/>
-      <c r="F58" s="118"/>
-      <c r="G58" s="118"/>
-      <c r="H58" s="118"/>
-      <c r="I58" s="118"/>
+      <c r="B58" s="119"/>
+      <c r="C58" s="119"/>
+      <c r="D58" s="119"/>
+      <c r="E58" s="119"/>
+      <c r="F58" s="119"/>
+      <c r="G58" s="119"/>
+      <c r="H58" s="119"/>
+      <c r="I58" s="119"/>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
@@ -18998,17 +19022,17 @@
       <c r="I76" s="87"/>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="118" t="s">
+      <c r="A80" s="119" t="s">
         <v>338</v>
       </c>
-      <c r="B80" s="118"/>
-      <c r="C80" s="118"/>
-      <c r="D80" s="118"/>
-      <c r="E80" s="118"/>
-      <c r="F80" s="118"/>
-      <c r="G80" s="118"/>
-      <c r="H80" s="118"/>
-      <c r="I80" s="118"/>
+      <c r="B80" s="119"/>
+      <c r="C80" s="119"/>
+      <c r="D80" s="119"/>
+      <c r="E80" s="119"/>
+      <c r="F80" s="119"/>
+      <c r="G80" s="119"/>
+      <c r="H80" s="119"/>
+      <c r="I80" s="119"/>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
@@ -19115,11 +19139,11 @@
       </c>
     </row>
     <row r="96" spans="1:8" s="16" customFormat="1">
-      <c r="A96" s="116" t="s">
+      <c r="A96" s="117" t="s">
         <v>2284</v>
       </c>
-      <c r="B96" s="116"/>
-      <c r="C96" s="116"/>
+      <c r="B96" s="117"/>
+      <c r="C96" s="117"/>
       <c r="H96"/>
     </row>
     <row r="97" spans="1:9">
@@ -19225,7 +19249,7 @@
       </c>
       <c r="H102" s="106"/>
     </row>
-    <row r="103" spans="1:9" ht="15.75" thickBot="1">
+    <row r="103" spans="1:9" ht="15" thickBot="1">
       <c r="A103" t="s">
         <v>2351</v>
       </c>
@@ -19328,7 +19352,7 @@
         <v>2369</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" ht="15">
       <c r="A109" t="s">
         <v>2370</v>
       </c>
@@ -19607,11 +19631,11 @@
       </c>
     </row>
     <row r="130" spans="1:7">
-      <c r="A130" s="116" t="s">
+      <c r="A130" s="117" t="s">
         <v>2267</v>
       </c>
-      <c r="B130" s="116"/>
-      <c r="C130" s="116"/>
+      <c r="B130" s="117"/>
+      <c r="C130" s="117"/>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
@@ -19656,7 +19680,7 @@
       </c>
       <c r="G133" s="2"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" ht="15">
       <c r="A134" t="s">
         <v>2430</v>
       </c>
@@ -19667,7 +19691,7 @@
         <v>2432</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" ht="15">
       <c r="A135" t="s">
         <v>2433</v>
       </c>
@@ -19747,44 +19771,44 @@
     <mergeCell ref="A96:C96"/>
     <mergeCell ref="A130:C130"/>
   </mergeCells>
-  <phoneticPr fontId="50" type="noConversion"/>
+  <phoneticPr fontId="51" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1"/>
-    <hyperlink ref="F8" r:id="rId2"/>
-    <hyperlink ref="F52" r:id="rId3"/>
-    <hyperlink ref="F53" r:id="rId4"/>
-    <hyperlink ref="F21" r:id="rId5"/>
-    <hyperlink ref="F23" r:id="rId6"/>
-    <hyperlink ref="F25" r:id="rId7"/>
-    <hyperlink ref="F27" r:id="rId8"/>
-    <hyperlink ref="F29" r:id="rId9"/>
-    <hyperlink ref="F31" r:id="rId10"/>
-    <hyperlink ref="F33" r:id="rId11"/>
-    <hyperlink ref="F36" r:id="rId12"/>
-    <hyperlink ref="F37" r:id="rId13"/>
-    <hyperlink ref="F38" r:id="rId14"/>
-    <hyperlink ref="F39" r:id="rId15"/>
-    <hyperlink ref="F54" r:id="rId16"/>
-    <hyperlink ref="F55" r:id="rId17"/>
-    <hyperlink ref="F103" r:id="rId18"/>
-    <hyperlink ref="E118" r:id="rId19" display="https://navatar61--tr2sb9.sandbox.lightning.force.com/lightning/r/Account/0013C00000nE0TTQA0/view"/>
-    <hyperlink ref="F115" r:id="rId20"/>
-    <hyperlink ref="F116" r:id="rId21"/>
-    <hyperlink ref="F118" r:id="rId22"/>
-    <hyperlink ref="E133" r:id="rId23" display="https://navatar61--tr2sb9.sandbox.lightning.force.com/lightning/r/Account/0013C00000nE0TTQA0/view"/>
-    <hyperlink ref="F110" r:id="rId24"/>
-    <hyperlink ref="F97" r:id="rId25"/>
-    <hyperlink ref="F102" r:id="rId26"/>
-    <hyperlink ref="C131" r:id="rId27" tooltip="mathews" display="https://navatar-2f--tr2sb21.sandbox.lightning.force.com/lightning/r/0033C00000eoImAQAU/view?0.tour=&amp;0.isdtp=p1&amp;0.sfdcIFrameOrigin=https%3A%2F%2Fnavatar-2f--tr2sb21.sandbox.lightning.force.com&amp;0.sfdcIFrameHost=web&amp;0.nonce=6a99e809d878f09a6802118218964c2278c719e9cd1270e5c5a0b3ce1d0ed811&amp;0.ltn_app_id=06m3x000001WCRqAAO&amp;0.clc=0"/>
-    <hyperlink ref="C132" r:id="rId28" tooltip="fernando" display="https://navatar-2f--tr2sb21.sandbox.lightning.force.com/lightning/r/0033C00000eoIneQAE/view?0.tour=&amp;0.isdtp=p1&amp;0.sfdcIFrameOrigin=https%3A%2F%2Fnavatar-2f--tr2sb21.sandbox.lightning.force.com&amp;0.sfdcIFrameHost=web&amp;0.nonce=6a99e809d878f09a6802118218964c2278c719e9cd1270e5c5a0b3ce1d0ed811&amp;0.ltn_app_id=06m3x000001WCRqAAO&amp;0.clc=0"/>
-    <hyperlink ref="C133" r:id="rId29" tooltip="stephan" display="https://navatar-2f--tr2sb21.sandbox.lightning.force.com/lightning/r/0033C00000eoImBQAU/view?0.tour=&amp;0.isdtp=p1&amp;0.sfdcIFrameOrigin=https%3A%2F%2Fnavatar-2f--tr2sb21.sandbox.lightning.force.com&amp;0.sfdcIFrameHost=web&amp;0.nonce=6a99e809d878f09a6802118218964c2278c719e9cd1270e5c5a0b3ce1d0ed811&amp;0.ltn_app_id=06m3x000001WCRqAAO&amp;0.clc=0"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="F52" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="F53" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="F21" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="F23" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="F25" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="F27" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="F29" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="F31" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="F33" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="F36" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="F37" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="F38" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="F39" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
+    <hyperlink ref="F54" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="F55" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
+    <hyperlink ref="F103" r:id="rId18" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
+    <hyperlink ref="E118" r:id="rId19" display="https://navatar61--tr2sb9.sandbox.lightning.force.com/lightning/r/Account/0013C00000nE0TTQA0/view" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="F115" r:id="rId20" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="F116" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
+    <hyperlink ref="F118" r:id="rId22" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
+    <hyperlink ref="E133" r:id="rId23" display="https://navatar61--tr2sb9.sandbox.lightning.force.com/lightning/r/Account/0013C00000nE0TTQA0/view" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
+    <hyperlink ref="F110" r:id="rId24" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
+    <hyperlink ref="F97" r:id="rId25" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
+    <hyperlink ref="F102" r:id="rId26" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
+    <hyperlink ref="C131" r:id="rId27" tooltip="mathews" display="https://navatar-2f--tr2sb21.sandbox.lightning.force.com/lightning/r/0033C00000eoImAQAU/view?0.tour=&amp;0.isdtp=p1&amp;0.sfdcIFrameOrigin=https%3A%2F%2Fnavatar-2f--tr2sb21.sandbox.lightning.force.com&amp;0.sfdcIFrameHost=web&amp;0.nonce=6a99e809d878f09a6802118218964c2278c719e9cd1270e5c5a0b3ce1d0ed811&amp;0.ltn_app_id=06m3x000001WCRqAAO&amp;0.clc=0" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
+    <hyperlink ref="C132" r:id="rId28" tooltip="fernando" display="https://navatar-2f--tr2sb21.sandbox.lightning.force.com/lightning/r/0033C00000eoIneQAE/view?0.tour=&amp;0.isdtp=p1&amp;0.sfdcIFrameOrigin=https%3A%2F%2Fnavatar-2f--tr2sb21.sandbox.lightning.force.com&amp;0.sfdcIFrameHost=web&amp;0.nonce=6a99e809d878f09a6802118218964c2278c719e9cd1270e5c5a0b3ce1d0ed811&amp;0.ltn_app_id=06m3x000001WCRqAAO&amp;0.clc=0" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
+    <hyperlink ref="C133" r:id="rId29" tooltip="stephan" display="https://navatar-2f--tr2sb21.sandbox.lightning.force.com/lightning/r/0033C00000eoImBQAU/view?0.tour=&amp;0.isdtp=p1&amp;0.sfdcIFrameOrigin=https%3A%2F%2Fnavatar-2f--tr2sb21.sandbox.lightning.force.com&amp;0.sfdcIFrameHost=web&amp;0.nonce=6a99e809d878f09a6802118218964c2278c719e9cd1270e5c5a0b3ce1d0ed811&amp;0.ltn_app_id=06m3x000001WCRqAAO&amp;0.clc=0" xr:uid="{00000000-0004-0000-0400-00001C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H44"/>
   <sheetViews>
@@ -19793,15 +19817,15 @@
       <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -20100,16 +20124,16 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="117" t="s">
+      <c r="A29" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="117"/>
-      <c r="C29" s="117"/>
-      <c r="D29" s="117"/>
-      <c r="E29" s="117"/>
-      <c r="F29" s="117"/>
-      <c r="G29" s="117"/>
-      <c r="H29" s="117"/>
+      <c r="B29" s="118"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="118"/>
+      <c r="E29" s="118"/>
+      <c r="F29" s="118"/>
+      <c r="G29" s="118"/>
+      <c r="H29" s="118"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="87" t="s">
@@ -20214,23 +20238,23 @@
   <mergeCells count="1">
     <mergeCell ref="A29:H29"/>
   </mergeCells>
-  <phoneticPr fontId="41" type="noConversion"/>
+  <phoneticPr fontId="42" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMP35"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="113" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="8.85546875" style="113"/>
+    <col min="1" max="1" width="14.88671875" style="113" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="8.88671875" style="113"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1030">
@@ -21882,7 +21906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F41"/>
   <sheetViews>
@@ -21890,11 +21914,11 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7" customWidth="1" collapsed="1"/>
   </cols>
@@ -21993,45 +22017,45 @@
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="116" t="s">
         <v>1378</v>
       </c>
-      <c r="B10" s="121" t="s">
+      <c r="B10" s="116" t="s">
         <v>2095</v>
       </c>
-      <c r="C10" s="121" t="s">
+      <c r="C10" s="116" t="s">
         <v>2093</v>
       </c>
-      <c r="D10" s="121" t="s">
+      <c r="D10" s="116" t="s">
         <v>496</v>
       </c>
-      <c r="E10" s="121" t="s">
+      <c r="E10" s="116" t="s">
         <v>2097</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="116" t="s">
         <v>1379</v>
       </c>
-      <c r="B11" s="121" t="s">
+      <c r="B11" s="116" t="s">
         <v>2095</v>
       </c>
-      <c r="C11" s="121" t="s">
+      <c r="C11" s="116" t="s">
         <v>2094</v>
       </c>
-      <c r="D11" s="121" t="s">
+      <c r="D11" s="116" t="s">
         <v>511</v>
       </c>
-      <c r="E11" s="121" t="s">
+      <c r="E11" s="116" t="s">
         <v>2097</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="16" customFormat="1">
-      <c r="A14" s="116" t="s">
+      <c r="A14" s="117" t="s">
         <v>2284</v>
       </c>
-      <c r="B14" s="116"/>
-      <c r="C14" s="116"/>
+      <c r="B14" s="117"/>
+      <c r="C14" s="117"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
@@ -22405,7 +22429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AE449"/>
   <sheetViews>
@@ -22414,33 +22438,33 @@
       <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="60.7109375" style="18" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="56.5703125" style="18" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="71.7109375" style="18" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.140625" style="23" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="4.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="49.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="9.140625" collapsed="1"/>
-    <col min="24" max="24" width="7.28515625" customWidth="1" collapsed="1"/>
-    <col min="25" max="16384" width="9.140625" collapsed="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="60.6640625" style="18" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="56.5546875" style="18" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="71.6640625" style="18" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.109375" style="23" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="4.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="8.109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23.6640625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="22.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="49.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="9.109375" collapsed="1"/>
+    <col min="24" max="24" width="7.33203125" customWidth="1" collapsed="1"/>
+    <col min="25" max="16384" width="9.109375" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -22572,7 +22596,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:31" ht="30">
+    <row r="4" spans="1:31" ht="28.8">
       <c r="A4" t="s">
         <v>431</v>
       </c>
@@ -22598,7 +22622,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="45">
+    <row r="5" spans="1:31" ht="28.8">
       <c r="A5" t="s">
         <v>439</v>
       </c>
@@ -22619,14 +22643,14 @@
       </c>
       <c r="J5" s="23" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>07/16/2023</v>
+        <v>08/05/2023</v>
       </c>
       <c r="K5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>07/16/2023</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" ht="30">
+        <v>08/05/2023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="28.8">
       <c r="A6" t="s">
         <v>444</v>
       </c>
@@ -22668,7 +22692,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="30">
+    <row r="9" spans="1:31" ht="28.8">
       <c r="A9" t="s">
         <v>454</v>
       </c>
@@ -22691,7 +22715,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="30">
+    <row r="10" spans="1:31" ht="28.8">
       <c r="A10" t="s">
         <v>460</v>
       </c>
@@ -22714,7 +22738,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="30">
+    <row r="11" spans="1:31" ht="28.8">
       <c r="A11" t="s">
         <v>462</v>
       </c>
@@ -22834,7 +22858,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:24" ht="45">
+    <row r="18" spans="1:24" ht="28.8">
       <c r="A18" s="12" t="s">
         <v>484</v>
       </c>
@@ -22857,7 +22881,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:24" ht="45">
+    <row r="19" spans="1:24" ht="28.8">
       <c r="A19" s="12" t="s">
         <v>488</v>
       </c>
@@ -22908,7 +22932,7 @@
       <c r="W22" s="16"/>
       <c r="X22" s="16"/>
     </row>
-    <row r="23" spans="1:24" ht="180">
+    <row r="23" spans="1:24" ht="144">
       <c r="A23" s="26" t="s">
         <v>1378</v>
       </c>
@@ -22950,7 +22974,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="180">
+    <row r="24" spans="1:24" ht="144">
       <c r="A24" s="26" t="s">
         <v>1379</v>
       </c>
@@ -22988,7 +23012,7 @@
       <c r="O24" s="19"/>
       <c r="P24" s="19"/>
     </row>
-    <row r="25" spans="1:24" ht="180">
+    <row r="25" spans="1:24" ht="144">
       <c r="A25" s="26" t="s">
         <v>1396</v>
       </c>
@@ -23030,7 +23054,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="180">
+    <row r="26" spans="1:24" ht="144">
       <c r="A26" s="26" t="s">
         <v>1397</v>
       </c>
@@ -23068,7 +23092,7 @@
       <c r="O26" s="19"/>
       <c r="P26" s="19"/>
     </row>
-    <row r="27" spans="1:24" ht="180">
+    <row r="27" spans="1:24" ht="158.4">
       <c r="A27" s="26" t="s">
         <v>1398</v>
       </c>
@@ -23110,7 +23134,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="180">
+    <row r="28" spans="1:24" ht="158.4">
       <c r="A28" s="26" t="s">
         <v>1399</v>
       </c>
@@ -23148,7 +23172,7 @@
       <c r="O28" s="19"/>
       <c r="P28" s="19"/>
     </row>
-    <row r="29" spans="1:24" ht="180">
+    <row r="29" spans="1:24" ht="158.4">
       <c r="A29" s="26" t="s">
         <v>1400</v>
       </c>
@@ -23190,7 +23214,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="180">
+    <row r="30" spans="1:24" ht="158.4">
       <c r="A30" s="26" t="s">
         <v>1401</v>
       </c>
@@ -23228,7 +23252,7 @@
       <c r="O30" s="19"/>
       <c r="P30" s="19"/>
     </row>
-    <row r="31" spans="1:24" ht="180">
+    <row r="31" spans="1:24" ht="158.4">
       <c r="A31" s="26" t="s">
         <v>1402</v>
       </c>
@@ -23270,7 +23294,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="180">
+    <row r="32" spans="1:24" ht="158.4">
       <c r="A32" s="26" t="s">
         <v>1403</v>
       </c>
@@ -23308,7 +23332,7 @@
       <c r="O32" s="19"/>
       <c r="P32" s="19"/>
     </row>
-    <row r="33" spans="1:16" ht="180">
+    <row r="33" spans="1:16" ht="158.4">
       <c r="A33" s="26" t="s">
         <v>1404</v>
       </c>
@@ -23350,7 +23374,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="180">
+    <row r="34" spans="1:16" ht="158.4">
       <c r="A34" s="26" t="s">
         <v>1405</v>
       </c>
@@ -23388,7 +23412,7 @@
       <c r="O34" s="19"/>
       <c r="P34" s="19"/>
     </row>
-    <row r="35" spans="1:16" ht="180">
+    <row r="35" spans="1:16" ht="144">
       <c r="A35" s="26" t="s">
         <v>1406</v>
       </c>
@@ -23430,7 +23454,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="180">
+    <row r="36" spans="1:16" ht="144">
       <c r="A36" s="26" t="s">
         <v>1407</v>
       </c>
@@ -23468,7 +23492,7 @@
       <c r="O36" s="19"/>
       <c r="P36" s="19"/>
     </row>
-    <row r="37" spans="1:16" ht="180">
+    <row r="37" spans="1:16" ht="158.4">
       <c r="A37" s="26" t="s">
         <v>1408</v>
       </c>
@@ -23510,7 +23534,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="180">
+    <row r="38" spans="1:16" ht="158.4">
       <c r="A38" s="26" t="s">
         <v>1409</v>
       </c>
@@ -23548,7 +23572,7 @@
       <c r="O38" s="19"/>
       <c r="P38" s="19"/>
     </row>
-    <row r="39" spans="1:16" ht="180">
+    <row r="39" spans="1:16" ht="158.4">
       <c r="A39" s="26" t="s">
         <v>1410</v>
       </c>
@@ -23590,7 +23614,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="180">
+    <row r="40" spans="1:16" ht="158.4">
       <c r="A40" s="26" t="s">
         <v>1411</v>
       </c>
@@ -23628,7 +23652,7 @@
       <c r="O40" s="19"/>
       <c r="P40" s="19"/>
     </row>
-    <row r="41" spans="1:16" ht="180">
+    <row r="41" spans="1:16" ht="144">
       <c r="A41" s="26" t="s">
         <v>1412</v>
       </c>
@@ -23670,7 +23694,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="180">
+    <row r="42" spans="1:16" ht="144">
       <c r="A42" s="26" t="s">
         <v>1413</v>
       </c>
@@ -23708,7 +23732,7 @@
       <c r="O42" s="19"/>
       <c r="P42" s="19"/>
     </row>
-    <row r="43" spans="1:16" ht="180">
+    <row r="43" spans="1:16" ht="144">
       <c r="A43" s="26" t="s">
         <v>1414</v>
       </c>
@@ -23750,7 +23774,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="180">
+    <row r="44" spans="1:16" ht="144">
       <c r="A44" s="26" t="s">
         <v>1415</v>
       </c>
@@ -23788,7 +23812,7 @@
       <c r="O44" s="19"/>
       <c r="P44" s="19"/>
     </row>
-    <row r="45" spans="1:16" ht="180">
+    <row r="45" spans="1:16" ht="144">
       <c r="A45" s="26" t="s">
         <v>1416</v>
       </c>
@@ -23830,7 +23854,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="180">
+    <row r="46" spans="1:16" ht="144">
       <c r="A46" s="26" t="s">
         <v>1417</v>
       </c>
@@ -23868,7 +23892,7 @@
       <c r="O46" s="19"/>
       <c r="P46" s="19"/>
     </row>
-    <row r="47" spans="1:16" ht="180">
+    <row r="47" spans="1:16" ht="144">
       <c r="A47" s="26" t="s">
         <v>1418</v>
       </c>
@@ -23910,7 +23934,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="180">
+    <row r="48" spans="1:16" ht="144">
       <c r="A48" s="26" t="s">
         <v>1419</v>
       </c>
@@ -23948,7 +23972,7 @@
       <c r="O48" s="19"/>
       <c r="P48" s="19"/>
     </row>
-    <row r="49" spans="1:16" s="26" customFormat="1" ht="90">
+    <row r="49" spans="1:16" s="26" customFormat="1" ht="86.4">
       <c r="A49" s="26" t="s">
         <v>1490</v>
       </c>
@@ -23986,7 +24010,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="26" customFormat="1" ht="180">
+    <row r="50" spans="1:16" s="26" customFormat="1" ht="144">
       <c r="A50" s="26" t="s">
         <v>1493</v>
       </c>
@@ -24018,7 +24042,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="26" customFormat="1" ht="180">
+    <row r="51" spans="1:16" s="26" customFormat="1" ht="144">
       <c r="A51" s="26" t="s">
         <v>1494</v>
       </c>
@@ -24118,7 +24142,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="26" customFormat="1" ht="165">
+    <row r="54" spans="1:16" s="26" customFormat="1" ht="144">
       <c r="A54" s="26" t="s">
         <v>1556</v>
       </c>
@@ -24150,7 +24174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="26" customFormat="1" ht="150">
+    <row r="55" spans="1:16" s="26" customFormat="1" ht="129.6">
       <c r="A55" s="26" t="s">
         <v>1557</v>
       </c>
@@ -24182,7 +24206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="26" customFormat="1" ht="90">
+    <row r="56" spans="1:16" s="26" customFormat="1" ht="72">
       <c r="A56" s="26" t="s">
         <v>1582</v>
       </c>
@@ -24224,7 +24248,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="26" customFormat="1" ht="90">
+    <row r="57" spans="1:16" s="26" customFormat="1" ht="72">
       <c r="A57" s="26" t="s">
         <v>1583</v>
       </c>
@@ -24262,7 +24286,7 @@
       <c r="O57" s="19"/>
       <c r="P57" s="19"/>
     </row>
-    <row r="58" spans="1:16" s="26" customFormat="1" ht="165">
+    <row r="58" spans="1:16" s="26" customFormat="1" ht="158.4">
       <c r="A58" s="26" t="s">
         <v>1586</v>
       </c>
@@ -24301,7 +24325,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="45" customFormat="1" ht="30">
+    <row r="59" spans="1:16" s="45" customFormat="1" ht="28.8">
       <c r="A59" s="26" t="s">
         <v>2102</v>
       </c>
@@ -24338,7 +24362,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="45" customFormat="1" ht="30">
+    <row r="60" spans="1:16" s="45" customFormat="1" ht="28.8">
       <c r="A60" s="26" t="s">
         <v>2103</v>
       </c>
@@ -24369,7 +24393,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="45" customFormat="1" ht="30">
+    <row r="61" spans="1:16" s="45" customFormat="1" ht="28.8">
       <c r="A61" s="26" t="s">
         <v>2126</v>
       </c>
@@ -24406,7 +24430,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="62" spans="1:16" s="45" customFormat="1" ht="30">
+    <row r="62" spans="1:16" s="45" customFormat="1" ht="28.8">
       <c r="A62" s="26" t="s">
         <v>2127</v>
       </c>
@@ -24485,7 +24509,7 @@
       <c r="M68" s="16"/>
       <c r="N68" s="16"/>
     </row>
-    <row r="69" spans="1:16" ht="30">
+    <row r="69" spans="1:16" ht="28.8">
       <c r="A69" s="26" t="s">
         <v>491</v>
       </c>
@@ -24521,7 +24545,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="45">
+    <row r="70" spans="1:16" ht="43.2">
       <c r="A70" s="26" t="s">
         <v>499</v>
       </c>
@@ -24555,7 +24579,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="75">
+    <row r="71" spans="1:16" ht="72">
       <c r="A71" s="26" t="s">
         <v>504</v>
       </c>
@@ -24592,7 +24616,7 @@
       </c>
       <c r="O71" s="26"/>
     </row>
-    <row r="72" spans="1:16" ht="30">
+    <row r="72" spans="1:16" ht="28.8">
       <c r="A72" s="26" t="s">
         <v>514</v>
       </c>
@@ -24630,7 +24654,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="30">
+    <row r="73" spans="1:16" ht="28.8">
       <c r="A73" s="27" t="s">
         <v>519</v>
       </c>
@@ -26982,7 +27006,7 @@
       <c r="O149" s="19"/>
       <c r="P149" s="19"/>
     </row>
-    <row r="150" spans="1:23" ht="30">
+    <row r="150" spans="1:23" ht="28.8">
       <c r="A150" s="26" t="s">
         <v>690</v>
       </c>
@@ -27018,7 +27042,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="30">
+    <row r="151" spans="1:23" ht="28.8">
       <c r="A151" s="26" t="s">
         <v>693</v>
       </c>
@@ -27054,7 +27078,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="75">
+    <row r="152" spans="1:23" ht="57.6">
       <c r="A152" s="26" t="s">
         <v>696</v>
       </c>
@@ -27092,7 +27116,7 @@
       <c r="O152" s="19"/>
       <c r="P152" s="19"/>
     </row>
-    <row r="153" spans="1:23" ht="45">
+    <row r="153" spans="1:23" ht="43.2">
       <c r="A153" s="26" t="s">
         <v>699</v>
       </c>
@@ -27128,7 +27152,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="75">
+    <row r="154" spans="1:23" ht="57.6">
       <c r="A154" s="26" t="s">
         <v>703</v>
       </c>
@@ -27191,7 +27215,7 @@
       <c r="V157" s="16"/>
       <c r="W157" s="16"/>
     </row>
-    <row r="158" spans="1:23" ht="90">
+    <row r="158" spans="1:23" ht="72">
       <c r="A158" t="s">
         <v>708</v>
       </c>
@@ -27220,7 +27244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="90">
+    <row r="159" spans="1:23" ht="72">
       <c r="A159" t="s">
         <v>712</v>
       </c>
@@ -27263,7 +27287,7 @@
       <c r="O164" s="16"/>
       <c r="P164" s="16"/>
     </row>
-    <row r="165" spans="1:24" ht="30">
+    <row r="165" spans="1:24" ht="28.8">
       <c r="A165" t="s">
         <v>716</v>
       </c>
@@ -27325,7 +27349,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="167" spans="1:24" ht="30">
+    <row r="167" spans="1:24" ht="28.8">
       <c r="A167" t="s">
         <v>724</v>
       </c>
@@ -27358,7 +27382,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="168" spans="1:24" ht="30">
+    <row r="168" spans="1:24" ht="28.8">
       <c r="A168" t="s">
         <v>727</v>
       </c>
@@ -27394,7 +27418,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="169" spans="1:24" ht="45">
+    <row r="169" spans="1:24" ht="28.8">
       <c r="A169" t="s">
         <v>731</v>
       </c>
@@ -27427,7 +27451,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="170" spans="1:24" ht="30">
+    <row r="170" spans="1:24" ht="28.8">
       <c r="A170" t="s">
         <v>734</v>
       </c>
@@ -27460,7 +27484,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="171" spans="1:24" ht="30">
+    <row r="171" spans="1:24" ht="28.8">
       <c r="A171" t="s">
         <v>736</v>
       </c>
@@ -27617,7 +27641,7 @@
       <c r="P177" s="16"/>
       <c r="Q177" s="16"/>
     </row>
-    <row r="178" spans="1:20" ht="45">
+    <row r="178" spans="1:20" ht="43.2">
       <c r="A178" t="s">
         <v>739</v>
       </c>
@@ -27714,27 +27738,27 @@
       <c r="J184"/>
     </row>
     <row r="187" spans="1:20">
-      <c r="A187" s="118" t="s">
+      <c r="A187" s="119" t="s">
         <v>144</v>
       </c>
-      <c r="B187" s="118"/>
-      <c r="C187" s="118"/>
-      <c r="D187" s="118"/>
-      <c r="E187" s="118"/>
-      <c r="F187" s="118"/>
-      <c r="G187" s="118"/>
-      <c r="H187" s="118"/>
-      <c r="I187" s="118"/>
-      <c r="J187" s="118"/>
-      <c r="K187" s="118"/>
-      <c r="L187" s="118"/>
-      <c r="M187" s="118"/>
-      <c r="N187" s="118"/>
-      <c r="O187" s="118"/>
-      <c r="P187" s="118"/>
-      <c r="Q187" s="118"/>
-      <c r="R187" s="118"/>
-      <c r="S187" s="118"/>
+      <c r="B187" s="119"/>
+      <c r="C187" s="119"/>
+      <c r="D187" s="119"/>
+      <c r="E187" s="119"/>
+      <c r="F187" s="119"/>
+      <c r="G187" s="119"/>
+      <c r="H187" s="119"/>
+      <c r="I187" s="119"/>
+      <c r="J187" s="119"/>
+      <c r="K187" s="119"/>
+      <c r="L187" s="119"/>
+      <c r="M187" s="119"/>
+      <c r="N187" s="119"/>
+      <c r="O187" s="119"/>
+      <c r="P187" s="119"/>
+      <c r="Q187" s="119"/>
+      <c r="R187" s="119"/>
+      <c r="S187" s="119"/>
     </row>
     <row r="188" spans="1:20">
       <c r="A188" t="s">
@@ -27750,7 +27774,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="30">
+    <row r="189" spans="1:20" ht="28.8">
       <c r="A189" t="s">
         <v>751</v>
       </c>
@@ -27775,7 +27799,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="14.45" customHeight="1">
+    <row r="191" spans="1:20" ht="14.4" customHeight="1">
       <c r="A191" t="s">
         <v>756</v>
       </c>
@@ -27798,7 +27822,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="14.45" customHeight="1">
+    <row r="192" spans="1:20" ht="14.4" customHeight="1">
       <c r="A192" t="s">
         <v>760</v>
       </c>
@@ -27809,7 +27833,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="193" spans="1:16" ht="30">
+    <row r="193" spans="1:16" ht="28.8">
       <c r="A193" t="s">
         <v>763</v>
       </c>
@@ -27826,7 +27850,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="194" spans="1:16" ht="14.45" customHeight="1">
+    <row r="194" spans="1:16" ht="14.4" customHeight="1">
       <c r="A194" t="s">
         <v>766</v>
       </c>
@@ -27865,7 +27889,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="197" spans="1:16" ht="14.45" customHeight="1">
+    <row r="197" spans="1:16" ht="14.4" customHeight="1">
       <c r="A197" t="s">
         <v>774</v>
       </c>
@@ -27910,7 +27934,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="200" spans="1:16" ht="30">
+    <row r="200" spans="1:16" ht="28.8">
       <c r="A200" t="s">
         <v>785</v>
       </c>
@@ -27944,7 +27968,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="202" spans="1:16" ht="30">
+    <row r="202" spans="1:16" ht="28.8">
       <c r="A202" t="s">
         <v>792</v>
       </c>
@@ -27969,7 +27993,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="204" spans="1:16" ht="14.45" customHeight="1">
+    <row r="204" spans="1:16" ht="14.4" customHeight="1">
       <c r="A204" t="s">
         <v>797</v>
       </c>
@@ -28038,7 +28062,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="14.45" customHeight="1">
+    <row r="210" spans="1:16" ht="14.4" customHeight="1">
       <c r="A210" t="s">
         <v>814</v>
       </c>
@@ -28088,7 +28112,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="14.45" customHeight="1">
+    <row r="214" spans="1:16" ht="14.4" customHeight="1">
       <c r="A214" t="s">
         <v>826</v>
       </c>
@@ -28144,7 +28168,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="218" spans="1:16" ht="14.45" customHeight="1">
+    <row r="218" spans="1:16" ht="14.4" customHeight="1">
       <c r="A218" t="s">
         <v>834</v>
       </c>
@@ -28175,7 +28199,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="220" spans="1:16" ht="14.45" customHeight="1">
+    <row r="220" spans="1:16" ht="14.4" customHeight="1">
       <c r="A220" t="s">
         <v>841</v>
       </c>
@@ -28189,7 +28213,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="221" spans="1:16" ht="14.45" customHeight="1">
+    <row r="221" spans="1:16" ht="14.4" customHeight="1">
       <c r="A221" t="s">
         <v>845</v>
       </c>
@@ -28212,7 +28236,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="14.45" customHeight="1">
+    <row r="222" spans="1:16" ht="14.4" customHeight="1">
       <c r="A222" t="s">
         <v>850</v>
       </c>
@@ -28226,7 +28250,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="30">
+    <row r="223" spans="1:16" ht="28.8">
       <c r="A223" t="s">
         <v>854</v>
       </c>
@@ -28234,7 +28258,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="224" spans="1:16" ht="45">
+    <row r="224" spans="1:16" ht="43.2">
       <c r="A224" t="s">
         <v>856</v>
       </c>
@@ -28250,7 +28274,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="226" spans="1:16" ht="14.45" customHeight="1">
+    <row r="226" spans="1:16" ht="14.4" customHeight="1">
       <c r="A226" t="s">
         <v>860</v>
       </c>
@@ -29536,7 +29560,7 @@
       <c r="AD269" s="87"/>
       <c r="AE269" s="87"/>
     </row>
-    <row r="270" spans="1:31" ht="90">
+    <row r="270" spans="1:31" ht="86.4">
       <c r="A270" s="87" t="s">
         <v>1714</v>
       </c>
@@ -30787,7 +30811,7 @@
         <v>1799</v>
       </c>
     </row>
-    <row r="301" spans="1:31" ht="75">
+    <row r="301" spans="1:31" ht="57.6">
       <c r="A301" s="87" t="s">
         <v>1800</v>
       </c>
@@ -31647,7 +31671,7 @@
         <v>1662</v>
       </c>
     </row>
-    <row r="321" spans="1:31" ht="30">
+    <row r="321" spans="1:31" ht="28.8">
       <c r="A321" s="87" t="s">
         <v>1859</v>
       </c>
@@ -31915,7 +31939,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="327" spans="1:31" ht="45">
+    <row r="327" spans="1:31" ht="28.8">
       <c r="A327" s="87" t="s">
         <v>1876</v>
       </c>
@@ -32007,7 +32031,7 @@
         <v>1882</v>
       </c>
     </row>
-    <row r="329" spans="1:31" ht="60">
+    <row r="329" spans="1:31" ht="43.2">
       <c r="A329" s="87" t="s">
         <v>1883</v>
       </c>
@@ -32475,7 +32499,7 @@
       <c r="AD340" s="87"/>
       <c r="AE340" s="87"/>
     </row>
-    <row r="341" spans="1:31" ht="105">
+    <row r="341" spans="1:31" ht="100.8">
       <c r="A341" s="87" t="s">
         <v>1916</v>
       </c>
@@ -33621,7 +33645,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="371" spans="1:31" ht="75">
+    <row r="371" spans="1:31" ht="72">
       <c r="A371" s="87" t="s">
         <v>1990</v>
       </c>
@@ -34384,29 +34408,29 @@
       </c>
     </row>
     <row r="413" spans="1:22">
-      <c r="A413" s="118" t="s">
+      <c r="A413" s="119" t="s">
         <v>160</v>
       </c>
-      <c r="B413" s="118"/>
-      <c r="C413" s="118"/>
-      <c r="D413" s="118"/>
-      <c r="E413" s="118"/>
-      <c r="F413" s="118"/>
-      <c r="G413" s="118"/>
-      <c r="H413" s="118"/>
-      <c r="I413" s="118"/>
-      <c r="J413" s="118"/>
-      <c r="K413" s="118"/>
-      <c r="L413" s="118"/>
-      <c r="M413" s="118"/>
-      <c r="N413" s="118"/>
-      <c r="O413" s="118"/>
-      <c r="P413" s="118"/>
-      <c r="Q413" s="118"/>
-      <c r="R413" s="118"/>
-      <c r="S413" s="118"/>
-    </row>
-    <row r="414" spans="1:22" ht="30">
+      <c r="B413" s="119"/>
+      <c r="C413" s="119"/>
+      <c r="D413" s="119"/>
+      <c r="E413" s="119"/>
+      <c r="F413" s="119"/>
+      <c r="G413" s="119"/>
+      <c r="H413" s="119"/>
+      <c r="I413" s="119"/>
+      <c r="J413" s="119"/>
+      <c r="K413" s="119"/>
+      <c r="L413" s="119"/>
+      <c r="M413" s="119"/>
+      <c r="N413" s="119"/>
+      <c r="O413" s="119"/>
+      <c r="P413" s="119"/>
+      <c r="Q413" s="119"/>
+      <c r="R413" s="119"/>
+      <c r="S413" s="119"/>
+    </row>
+    <row r="414" spans="1:22" ht="28.8">
       <c r="A414" t="s">
         <v>908</v>
       </c>
@@ -34451,7 +34475,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="417" spans="1:23" ht="30">
+    <row r="417" spans="1:23" ht="28.8">
       <c r="A417" t="s">
         <v>919</v>
       </c>
@@ -34459,7 +34483,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="418" spans="1:23" ht="30">
+    <row r="418" spans="1:23" ht="28.8">
       <c r="A418" t="s">
         <v>921</v>
       </c>
@@ -34786,7 +34810,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="441" spans="1:22" ht="30">
+    <row r="441" spans="1:22" ht="28.8">
       <c r="A441" t="s">
         <v>976</v>
       </c>
@@ -34916,7 +34940,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="449" spans="1:22" ht="30">
+    <row r="449" spans="1:22">
       <c r="A449" t="s">
         <v>999</v>
       </c>
@@ -34943,18 +34967,18 @@
     <mergeCell ref="A187:S187"/>
     <mergeCell ref="A413:S413"/>
   </mergeCells>
-  <phoneticPr fontId="41" type="noConversion"/>
+  <phoneticPr fontId="42" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E449" r:id="rId1"/>
-    <hyperlink ref="E423" r:id="rId2"/>
-    <hyperlink ref="E165" r:id="rId3"/>
-    <hyperlink ref="E167" r:id="rId4"/>
-    <hyperlink ref="E168" r:id="rId5"/>
-    <hyperlink ref="E170" r:id="rId6"/>
-    <hyperlink ref="E171" r:id="rId7"/>
-    <hyperlink ref="E169" r:id="rId8"/>
-    <hyperlink ref="E172" r:id="rId9" display="mailto:1investorportal+testingcompanycon1@gmail.com"/>
-    <hyperlink ref="E174" r:id="rId10"/>
+    <hyperlink ref="E449" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="E423" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="E165" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="E167" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="E168" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="E170" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="E171" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="E169" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="E172" r:id="rId9" display="mailto:1investorportal+testingcompanycon1@gmail.com" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="E174" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>

<commit_message>
Added data sheet and removed unused module
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Kumar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Kumar\git\PE4.7Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535A7E07-00CE-4583-80F3-B5D00A0F5BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D59C352-E962-4CC9-AAEB-0DEE4D86865D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4587" uniqueCount="2660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4619" uniqueCount="2671">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -8066,6 +8066,39 @@
   <si>
     <t>Parent_Institution</t>
   </si>
+  <si>
+    <t>ATCE_041</t>
+  </si>
+  <si>
+    <t>Call to Verify External Tab</t>
+  </si>
+  <si>
+    <t>This is Navatar Activity to verify external tab</t>
+  </si>
+  <si>
+    <t>Test Contact 1_ADVISOR&lt;break&gt;Test Contact 1_COMPANY&lt;break&gt;Test Contact 1_INSTITUTION&lt;break&gt;Test Contact 1_INTERMEDIARY&lt;break&gt;Test Contact 1_LENDER&lt;break&gt;Test Contact 1_PORTFOLIOCOMPANY&lt;break&gt;Test Contact 1_PRIVATEEQUITY&lt;break&gt;Test Contact 2_ADVISOR&lt;break&gt;Test Contact 2_COMPANY&lt;break&gt;Test Contact 2_INSTITUTION&lt;break&gt;Test Contact 2_INTERMEDIARY&lt;break&gt;Test Contact 2_LENDER&lt;break&gt;Test Contact 2_PORTFOLIOCOMPANY&lt;break&gt;Test Contact 2_PRIVATEEQUITY</t>
+  </si>
+  <si>
+    <t>RGATE_011</t>
+  </si>
+  <si>
+    <t>RG Event To Verify External Tab</t>
+  </si>
+  <si>
+    <t>andrewmeslow@statefarm-ng.com,josephsmith@truistfinancialcorp-ng.com</t>
+  </si>
+  <si>
+    <t>External_ContactName</t>
+  </si>
+  <si>
+    <t>External_FirmName</t>
+  </si>
+  <si>
+    <t>External_Title</t>
+  </si>
+  <si>
+    <t>External_MeetingAndCallCount</t>
+  </si>
 </sst>
 </file>
 
@@ -8074,7 +8107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="58">
+  <fonts count="59">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8479,6 +8512,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -8625,7 +8666,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8861,6 +8902,19 @@
     </xf>
     <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -9765,11 +9819,11 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:AL249"/>
+  <dimension ref="A1:AP249"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z19" sqref="Z19"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AL15" sqref="AL15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -9807,9 +9861,13 @@
     <col min="36" max="36" width="28.33203125" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="63.44140625" style="18" customWidth="1" collapsed="1"/>
     <col min="38" max="38" width="63.6640625" style="18" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="26.109375" customWidth="1"/>
+    <col min="40" max="40" width="19.44140625" customWidth="1"/>
+    <col min="41" max="41" width="19" customWidth="1"/>
+    <col min="42" max="42" width="31.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:42">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9924,8 +9982,20 @@
       <c r="AL1" s="20" t="s">
         <v>2137</v>
       </c>
-    </row>
-    <row r="3" spans="1:38">
+      <c r="AM1" s="125" t="s">
+        <v>2667</v>
+      </c>
+      <c r="AN1" s="126" t="s">
+        <v>2668</v>
+      </c>
+      <c r="AO1" s="126" t="s">
+        <v>2669</v>
+      </c>
+      <c r="AP1" s="126" t="s">
+        <v>2670</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -9952,7 +10022,7 @@
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:42">
       <c r="A4" t="s">
         <v>1042</v>
       </c>
@@ -9966,7 +10036,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:42">
       <c r="A5" t="s">
         <v>1045</v>
       </c>
@@ -9980,7 +10050,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:42">
       <c r="A6" t="s">
         <v>1046</v>
       </c>
@@ -9994,7 +10064,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:42">
       <c r="A7" t="s">
         <v>1047</v>
       </c>
@@ -10008,7 +10078,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:42">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -10035,7 +10105,7 @@
       <c r="V12" s="16"/>
       <c r="W12" s="16"/>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:42">
       <c r="A13" t="s">
         <v>1049</v>
       </c>
@@ -10046,7 +10116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:42">
       <c r="A14" t="s">
         <v>1050</v>
       </c>
@@ -10057,7 +10127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:42">
       <c r="A15" t="s">
         <v>1051</v>
       </c>
@@ -10068,7 +10138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:42">
       <c r="A16" t="s">
         <v>1052</v>
       </c>
@@ -10085,7 +10155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:42">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -10116,7 +10186,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="16"/>
     </row>
-    <row r="19" spans="1:38" ht="101.4">
+    <row r="19" spans="1:42" ht="101.4">
       <c r="A19" s="67" t="s">
         <v>1055</v>
       </c>
@@ -10213,8 +10283,20 @@
       <c r="AL19" s="18" t="s">
         <v>2138</v>
       </c>
-    </row>
-    <row r="20" spans="1:38" ht="43.8">
+      <c r="AM19" t="s">
+        <v>1558</v>
+      </c>
+      <c r="AN19" s="18" t="s">
+        <v>1544</v>
+      </c>
+      <c r="AO19" s="18" t="s">
+        <v>1065</v>
+      </c>
+      <c r="AP19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" ht="43.8">
       <c r="A20" t="s">
         <v>1063</v>
       </c>
@@ -10287,8 +10369,20 @@
       <c r="AF20" s="71" t="s">
         <v>1475</v>
       </c>
-    </row>
-    <row r="21" spans="1:38" ht="43.8">
+      <c r="AM20" t="s">
+        <v>289</v>
+      </c>
+      <c r="AN20" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO20" t="s">
+        <v>1122</v>
+      </c>
+      <c r="AP20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" ht="43.8">
       <c r="A21" t="s">
         <v>1068</v>
       </c>
@@ -10355,8 +10449,20 @@
       <c r="AF21" s="71" t="s">
         <v>1476</v>
       </c>
-    </row>
-    <row r="22" spans="1:38" ht="29.4">
+      <c r="AM21" t="s">
+        <v>294</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>112</v>
+      </c>
+      <c r="AO21" t="s">
+        <v>1122</v>
+      </c>
+      <c r="AP21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" ht="29.4">
       <c r="A22" t="s">
         <v>1070</v>
       </c>
@@ -10420,8 +10526,20 @@
       <c r="AF22" s="71" t="s">
         <v>1477</v>
       </c>
-    </row>
-    <row r="23" spans="1:38" ht="29.4">
+      <c r="AM22" t="s">
+        <v>274</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>96</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>1122</v>
+      </c>
+      <c r="AP22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" ht="29.4">
       <c r="A23" t="s">
         <v>1072</v>
       </c>
@@ -10485,8 +10603,20 @@
       <c r="AF23" s="72" t="s">
         <v>1480</v>
       </c>
-    </row>
-    <row r="24" spans="1:38" ht="15">
+      <c r="AM23" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN23" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO23" s="18" t="s">
+        <v>1065</v>
+      </c>
+      <c r="AP23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" ht="15">
       <c r="A24" t="s">
         <v>1381</v>
       </c>
@@ -10545,7 +10675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="15">
+    <row r="25" spans="1:42" ht="15">
       <c r="A25" t="s">
         <v>1382</v>
       </c>
@@ -10604,7 +10734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="15">
+    <row r="26" spans="1:42" ht="15">
       <c r="A26" t="s">
         <v>1383</v>
       </c>
@@ -10663,7 +10793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:38" ht="15">
+    <row r="27" spans="1:42" ht="15">
       <c r="A27" t="s">
         <v>1384</v>
       </c>
@@ -10708,7 +10838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:42">
       <c r="A28" t="s">
         <v>1392</v>
       </c>
@@ -10746,7 +10876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:42">
       <c r="A29" t="s">
         <v>1432</v>
       </c>
@@ -10784,7 +10914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:42">
       <c r="A30" t="s">
         <v>1433</v>
       </c>
@@ -10822,7 +10952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:42">
       <c r="A31" t="s">
         <v>1434</v>
       </c>
@@ -10860,7 +10990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:42">
       <c r="A32" t="s">
         <v>1435</v>
       </c>
@@ -18006,9 +18136,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F134" sqref="F134"/>
+      <selection pane="bottomLeft" activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -22434,8 +22564,8 @@
   <dimension ref="A1:AE449"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A485" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A175" sqref="A175:XFD175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -22643,11 +22773,11 @@
       </c>
       <c r="J5" s="23" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>08/05/2023</v>
+        <v>08/26/2023</v>
       </c>
       <c r="K5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>08/05/2023</v>
+        <v>08/26/2023</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="28.8">
@@ -24461,11 +24591,29 @@
         <v>512</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="45" customFormat="1">
+    <row r="63" spans="1:16" s="45" customFormat="1" ht="129.6">
+      <c r="A63" s="26" t="s">
+        <v>2660</v>
+      </c>
+      <c r="B63" s="45" t="s">
+        <v>476</v>
+      </c>
+      <c r="C63" s="45" t="s">
+        <v>2661</v>
+      </c>
+      <c r="D63" s="45" t="s">
+        <v>2662</v>
+      </c>
+      <c r="E63" s="45" t="s">
+        <v>2663</v>
+      </c>
       <c r="H63" s="18"/>
       <c r="J63" s="18"/>
       <c r="K63" s="18"/>
-      <c r="L63" s="95"/>
+      <c r="L63" s="122"/>
+      <c r="M63" s="26" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="64" spans="1:16" s="45" customFormat="1">
       <c r="H64" s="18"/>
@@ -27615,10 +27763,30 @@
       </c>
     </row>
     <row r="175" spans="1:24">
-      <c r="E175" s="22"/>
-      <c r="F175" s="99"/>
+      <c r="A175" s="123" t="s">
+        <v>2664</v>
+      </c>
+      <c r="B175" t="s">
+        <v>505</v>
+      </c>
+      <c r="C175" t="s">
+        <v>2665</v>
+      </c>
+      <c r="D175" t="s">
+        <v>2196</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>2666</v>
+      </c>
+      <c r="F175" s="124"/>
       <c r="G175" s="22"/>
       <c r="J175"/>
+      <c r="M175" s="39" t="s">
+        <v>2222</v>
+      </c>
+      <c r="N175" s="39" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="177" spans="1:20">
       <c r="A177" s="16"/>
@@ -34979,8 +35147,9 @@
     <hyperlink ref="E169" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
     <hyperlink ref="E172" r:id="rId9" display="mailto:1investorportal+testingcompanycon1@gmail.com" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
     <hyperlink ref="E174" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="E175" r:id="rId11" xr:uid="{62530BAC-6D7C-4660-A174-FDA56055997C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merge All Interaction Data Sheet
Signed-off-by: raviNavatar <106242727+raviNavatar@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Kumar\git\PE4.7Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D59C352-E962-4CC9-AAEB-0DEE4D86865D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA9EFC8-31A2-44F6-B386-758D621A400A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4619" uniqueCount="2671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4701" uniqueCount="2705">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -8099,6 +8099,108 @@
   <si>
     <t>External_MeetingAndCallCount</t>
   </si>
+  <si>
+    <t>AllIntraction</t>
+  </si>
+  <si>
+    <t>AI_001</t>
+  </si>
+  <si>
+    <t>DanInteract Task1</t>
+  </si>
+  <si>
+    <t>This is task 1 to test All Interactions page</t>
+  </si>
+  <si>
+    <t>Dan CompContact1&lt;break&gt;Dan FS1&lt;break&gt;Dan Advisor2&lt;break&gt;DanSellSideDeal 1&lt;break&gt;DanInteract FundR 1&lt;break&gt;Dan Theme 1&lt;break&gt;DanInteract Fund 1</t>
+  </si>
+  <si>
+    <t>10/04/2023</t>
+  </si>
+  <si>
+    <t>AI_002</t>
+  </si>
+  <si>
+    <t>DanInteract Task2</t>
+  </si>
+  <si>
+    <t>Dan CompContact2&lt;break&gt;Dan FSContact1&lt;break&gt;Dan Comp1&lt;break&gt;DanAdvSrvDeal 1&lt;break&gt;DanInteract FundR 2&lt;break&gt;Dan Theme 2&lt;break&gt;DanInteract Fund 2</t>
+  </si>
+  <si>
+    <t>AI_003</t>
+  </si>
+  <si>
+    <t>DanInteract TaskEmail3</t>
+  </si>
+  <si>
+    <t>This is task 3 to test All Interactions page</t>
+  </si>
+  <si>
+    <t>Dan Comp2&lt;break&gt;Dan StrgCorpContact1&lt;break&gt;Dan StrgCorpContact2&lt;break&gt;DanBuySideDeal 2&lt;break&gt;DanInteract FundR 3&lt;break&gt;Dan Theme 3&lt;break&gt;DanInteract Fund 3</t>
+  </si>
+  <si>
+    <t>AI_004</t>
+  </si>
+  <si>
+    <t>DanInteract TaskEmail4</t>
+  </si>
+  <si>
+    <t>This is task 4 to test All Interactions page</t>
+  </si>
+  <si>
+    <t>Dan FSContact1&lt;break&gt;Dan FSContact2&lt;break&gt;Dan FSContact3&lt;break&gt;Dan FS3&lt;break&gt;DanCapRaiseDeal 1&lt;break&gt;DanInteract FundR 4&lt;break&gt;Dan Theme 4&lt;break&gt;DanInteract Fund 4</t>
+  </si>
+  <si>
+    <t>AI_005</t>
+  </si>
+  <si>
+    <t>DanInteract TaskCall5</t>
+  </si>
+  <si>
+    <t>This is task 5 to test All Interactions page</t>
+  </si>
+  <si>
+    <t>Dan FSContact10&lt;break&gt;Dan FS4&lt;break&gt;Dan FS5&lt;break&gt;DanPitchDeal 1&lt;break&gt;DanInteract FundR 5&lt;break&gt;Dan FS3&lt;break&gt;Dan StrgCorp4&lt;break&gt;Dan Theme 5&lt;break&gt;DanInteract Fund 5</t>
+  </si>
+  <si>
+    <t>AI_006</t>
+  </si>
+  <si>
+    <t>DanInteract TaskCall6</t>
+  </si>
+  <si>
+    <t>This is task 6 to test All Interactions page</t>
+  </si>
+  <si>
+    <t>Dan FSContact6&lt;break&gt;Dan FS6&lt;break&gt;Dan FS3&lt;break&gt;DanPitchDeal 1&lt;break&gt;DanInteract FundR 6&lt;break&gt;Dan Theme 6&lt;break&gt;DanInteract Fund 6</t>
+  </si>
+  <si>
+    <t>07/12023</t>
+  </si>
+  <si>
+    <t>AI_007</t>
+  </si>
+  <si>
+    <t>DanInteractTaskNewTab</t>
+  </si>
+  <si>
+    <t>This is new tab task</t>
+  </si>
+  <si>
+    <t>Dan Theme 6&lt;break&gt;Dan AdvCont2</t>
+  </si>
+  <si>
+    <t>AI_008</t>
+  </si>
+  <si>
+    <t>DanInteract TaskDeal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is task 7 to test All Interactions page. </t>
+  </si>
+  <si>
+    <t>DanAdvSrvDeal 1&lt;break&gt;DanBuySideDeal 5&lt;break&gt;DanCapRaiseDeal 5&lt;break&gt;DanPitchDeal 5</t>
+  </si>
 </sst>
 </file>
 
@@ -8107,12 +8209,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="59">
+  <fonts count="61">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8520,6 +8629,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -8659,29 +8774,29 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="38" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="39" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8693,45 +8808,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="38" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="39" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="39" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -8748,7 +8863,7 @@
     <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -8769,58 +8884,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8828,27 +8944,26 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="52" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8857,38 +8972,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="54" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="54" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="55" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="3" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="3" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -8897,25 +9025,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9609,11 +9742,11 @@
       </c>
     </row>
     <row r="35" spans="1:12" s="16" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A35" s="117" t="s">
+      <c r="A35" s="122" t="s">
         <v>2267</v>
       </c>
-      <c r="B35" s="117"/>
-      <c r="C35" s="117"/>
+      <c r="B35" s="122"/>
+      <c r="C35" s="122"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" t="s">
@@ -9689,7 +9822,7 @@
   <mergeCells count="1">
     <mergeCell ref="A35:C35"/>
   </mergeCells>
-  <phoneticPr fontId="53" type="noConversion"/>
+  <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -9819,11 +9952,11 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:AP249"/>
+  <dimension ref="A1:AP260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL15" sqref="AL15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F260" sqref="F260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -9982,16 +10115,16 @@
       <c r="AL1" s="20" t="s">
         <v>2137</v>
       </c>
-      <c r="AM1" s="125" t="s">
+      <c r="AM1" s="120" t="s">
         <v>2667</v>
       </c>
-      <c r="AN1" s="126" t="s">
+      <c r="AN1" s="121" t="s">
         <v>2668</v>
       </c>
-      <c r="AO1" s="126" t="s">
+      <c r="AO1" s="121" t="s">
         <v>2669</v>
       </c>
-      <c r="AP1" s="126" t="s">
+      <c r="AP1" s="121" t="s">
         <v>2670</v>
       </c>
     </row>
@@ -14650,39 +14783,39 @@
       </c>
     </row>
     <row r="212" spans="1:31">
-      <c r="A212" s="119" t="s">
+      <c r="A212" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="B212" s="119"/>
-      <c r="C212" s="119"/>
-      <c r="D212" s="119"/>
-      <c r="E212" s="119"/>
-      <c r="F212" s="119"/>
-      <c r="G212" s="119"/>
-      <c r="H212" s="119"/>
-      <c r="I212" s="119"/>
-      <c r="J212" s="119"/>
-      <c r="K212" s="119"/>
-      <c r="L212" s="119"/>
-      <c r="M212" s="119"/>
-      <c r="N212" s="119"/>
-      <c r="O212" s="119"/>
-      <c r="P212" s="119"/>
-      <c r="Q212" s="119"/>
-      <c r="R212" s="119"/>
-      <c r="S212" s="119"/>
-      <c r="T212" s="119"/>
-      <c r="U212" s="119"/>
-      <c r="V212" s="119"/>
-      <c r="W212" s="119"/>
-      <c r="X212" s="119"/>
-      <c r="Y212" s="119"/>
-      <c r="Z212" s="119"/>
-      <c r="AA212" s="119"/>
-      <c r="AB212" s="119"/>
-      <c r="AC212" s="119"/>
-      <c r="AD212" s="119"/>
-      <c r="AE212" s="119"/>
+      <c r="B212" s="124"/>
+      <c r="C212" s="124"/>
+      <c r="D212" s="124"/>
+      <c r="E212" s="124"/>
+      <c r="F212" s="124"/>
+      <c r="G212" s="124"/>
+      <c r="H212" s="124"/>
+      <c r="I212" s="124"/>
+      <c r="J212" s="124"/>
+      <c r="K212" s="124"/>
+      <c r="L212" s="124"/>
+      <c r="M212" s="124"/>
+      <c r="N212" s="124"/>
+      <c r="O212" s="124"/>
+      <c r="P212" s="124"/>
+      <c r="Q212" s="124"/>
+      <c r="R212" s="124"/>
+      <c r="S212" s="124"/>
+      <c r="T212" s="124"/>
+      <c r="U212" s="124"/>
+      <c r="V212" s="124"/>
+      <c r="W212" s="124"/>
+      <c r="X212" s="124"/>
+      <c r="Y212" s="124"/>
+      <c r="Z212" s="124"/>
+      <c r="AA212" s="124"/>
+      <c r="AB212" s="124"/>
+      <c r="AC212" s="124"/>
+      <c r="AD212" s="124"/>
+      <c r="AE212" s="124"/>
     </row>
     <row r="213" spans="1:31">
       <c r="A213" t="s">
@@ -14917,7 +15050,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="241" spans="1:31">
+    <row r="241" spans="1:38">
       <c r="A241" t="s">
         <v>1261</v>
       </c>
@@ -14925,7 +15058,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="242" spans="1:31">
+    <row r="242" spans="1:38">
       <c r="A242" t="s">
         <v>1263</v>
       </c>
@@ -14936,7 +15069,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="243" spans="1:31">
+    <row r="243" spans="1:38">
       <c r="A243" t="s">
         <v>1265</v>
       </c>
@@ -14944,42 +15077,42 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="247" spans="1:31">
-      <c r="A247" s="119" t="s">
+    <row r="247" spans="1:38">
+      <c r="A247" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="B247" s="119"/>
-      <c r="C247" s="119"/>
-      <c r="D247" s="119"/>
-      <c r="E247" s="119"/>
-      <c r="F247" s="119"/>
-      <c r="G247" s="119"/>
-      <c r="H247" s="119"/>
-      <c r="I247" s="119"/>
-      <c r="J247" s="119"/>
-      <c r="K247" s="119"/>
-      <c r="L247" s="119"/>
-      <c r="M247" s="119"/>
-      <c r="N247" s="119"/>
-      <c r="O247" s="119"/>
-      <c r="P247" s="119"/>
-      <c r="Q247" s="119"/>
-      <c r="R247" s="119"/>
-      <c r="S247" s="119"/>
-      <c r="T247" s="119"/>
-      <c r="U247" s="119"/>
-      <c r="V247" s="119"/>
-      <c r="W247" s="119"/>
-      <c r="X247" s="119"/>
-      <c r="Y247" s="119"/>
-      <c r="Z247" s="119"/>
-      <c r="AA247" s="119"/>
-      <c r="AB247" s="119"/>
-      <c r="AC247" s="119"/>
-      <c r="AD247" s="119"/>
-      <c r="AE247" s="119"/>
-    </row>
-    <row r="248" spans="1:31">
+      <c r="B247" s="124"/>
+      <c r="C247" s="124"/>
+      <c r="D247" s="124"/>
+      <c r="E247" s="124"/>
+      <c r="F247" s="124"/>
+      <c r="G247" s="124"/>
+      <c r="H247" s="124"/>
+      <c r="I247" s="124"/>
+      <c r="J247" s="124"/>
+      <c r="K247" s="124"/>
+      <c r="L247" s="124"/>
+      <c r="M247" s="124"/>
+      <c r="N247" s="124"/>
+      <c r="O247" s="124"/>
+      <c r="P247" s="124"/>
+      <c r="Q247" s="124"/>
+      <c r="R247" s="124"/>
+      <c r="S247" s="124"/>
+      <c r="T247" s="124"/>
+      <c r="U247" s="124"/>
+      <c r="V247" s="124"/>
+      <c r="W247" s="124"/>
+      <c r="X247" s="124"/>
+      <c r="Y247" s="124"/>
+      <c r="Z247" s="124"/>
+      <c r="AA247" s="124"/>
+      <c r="AB247" s="124"/>
+      <c r="AC247" s="124"/>
+      <c r="AD247" s="124"/>
+      <c r="AE247" s="124"/>
+    </row>
+    <row r="248" spans="1:38">
       <c r="A248" t="s">
         <v>1267</v>
       </c>
@@ -14987,20 +15120,417 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="249" spans="1:31">
+    <row r="249" spans="1:38">
       <c r="A249" t="s">
         <v>1269</v>
       </c>
       <c r="AD249" t="s">
         <v>1245</v>
       </c>
+    </row>
+    <row r="251" spans="1:38">
+      <c r="A251" s="16"/>
+      <c r="B251" s="16"/>
+      <c r="C251" s="16"/>
+      <c r="D251" s="16"/>
+      <c r="E251" s="127" t="s">
+        <v>2671</v>
+      </c>
+      <c r="F251" s="21"/>
+      <c r="G251" s="21"/>
+      <c r="H251" s="16"/>
+      <c r="I251" s="16"/>
+      <c r="J251" s="33"/>
+      <c r="K251" s="16"/>
+      <c r="L251" s="16"/>
+      <c r="M251" s="16"/>
+      <c r="N251" s="16"/>
+      <c r="O251" s="16"/>
+      <c r="P251" s="16"/>
+      <c r="Q251" s="16"/>
+      <c r="R251" s="16"/>
+      <c r="S251" s="16"/>
+      <c r="T251" s="16"/>
+      <c r="U251" s="16"/>
+      <c r="V251" s="16"/>
+      <c r="W251" s="16"/>
+      <c r="X251" s="16"/>
+      <c r="AF251"/>
+      <c r="AI251"/>
+      <c r="AK251"/>
+      <c r="AL251"/>
+    </row>
+    <row r="252" spans="1:38" ht="244.8">
+      <c r="A252" s="26" t="s">
+        <v>2672</v>
+      </c>
+      <c r="B252" s="26" t="s">
+        <v>481</v>
+      </c>
+      <c r="C252" s="26" t="s">
+        <v>2673</v>
+      </c>
+      <c r="D252" s="26" t="s">
+        <v>2674</v>
+      </c>
+      <c r="E252" s="128" t="s">
+        <v>2675</v>
+      </c>
+      <c r="F252" s="128"/>
+      <c r="G252" s="128" t="s">
+        <v>2675</v>
+      </c>
+      <c r="H252" t="s">
+        <v>2676</v>
+      </c>
+      <c r="I252" s="19"/>
+      <c r="J252" s="28"/>
+      <c r="K252" s="19"/>
+      <c r="L252" s="129" t="s">
+        <v>496</v>
+      </c>
+      <c r="M252" s="26">
+        <v>0</v>
+      </c>
+      <c r="N252" s="19"/>
+      <c r="O252" s="130" t="s">
+        <v>675</v>
+      </c>
+      <c r="P252" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF252"/>
+      <c r="AI252"/>
+      <c r="AK252"/>
+      <c r="AL252"/>
+    </row>
+    <row r="253" spans="1:38" ht="244.8">
+      <c r="A253" s="131" t="s">
+        <v>2677</v>
+      </c>
+      <c r="B253" s="26" t="s">
+        <v>481</v>
+      </c>
+      <c r="C253" s="26" t="s">
+        <v>2678</v>
+      </c>
+      <c r="D253" s="26" t="s">
+        <v>2674</v>
+      </c>
+      <c r="E253" s="128" t="s">
+        <v>2679</v>
+      </c>
+      <c r="F253" s="128"/>
+      <c r="G253" s="128" t="s">
+        <v>2679</v>
+      </c>
+      <c r="H253" t="s">
+        <v>2676</v>
+      </c>
+      <c r="I253" s="19"/>
+      <c r="J253" s="28"/>
+      <c r="K253" s="19"/>
+      <c r="L253" s="129" t="s">
+        <v>511</v>
+      </c>
+      <c r="M253" s="26">
+        <v>0</v>
+      </c>
+      <c r="N253" s="19"/>
+      <c r="O253" s="130" t="s">
+        <v>497</v>
+      </c>
+      <c r="P253" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF253"/>
+      <c r="AI253"/>
+      <c r="AK253"/>
+      <c r="AL253"/>
+    </row>
+    <row r="254" spans="1:38" ht="259.2">
+      <c r="A254" s="131" t="s">
+        <v>2680</v>
+      </c>
+      <c r="B254" s="26" t="s">
+        <v>481</v>
+      </c>
+      <c r="C254" s="131" t="s">
+        <v>2681</v>
+      </c>
+      <c r="D254" s="131" t="s">
+        <v>2682</v>
+      </c>
+      <c r="E254" s="128" t="s">
+        <v>2683</v>
+      </c>
+      <c r="F254" s="128"/>
+      <c r="G254" s="128" t="s">
+        <v>2683</v>
+      </c>
+      <c r="H254" t="s">
+        <v>2676</v>
+      </c>
+      <c r="I254" s="19"/>
+      <c r="J254" s="28"/>
+      <c r="K254" s="19"/>
+      <c r="L254" s="129" t="s">
+        <v>496</v>
+      </c>
+      <c r="M254" s="26">
+        <v>0</v>
+      </c>
+      <c r="N254" s="19"/>
+      <c r="O254" s="130" t="s">
+        <v>497</v>
+      </c>
+      <c r="P254" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF254"/>
+      <c r="AI254"/>
+      <c r="AK254"/>
+      <c r="AL254"/>
+    </row>
+    <row r="255" spans="1:38" ht="259.2">
+      <c r="A255" s="131" t="s">
+        <v>2684</v>
+      </c>
+      <c r="B255" s="26" t="s">
+        <v>481</v>
+      </c>
+      <c r="C255" s="26" t="s">
+        <v>2685</v>
+      </c>
+      <c r="D255" s="131" t="s">
+        <v>2686</v>
+      </c>
+      <c r="E255" s="128" t="s">
+        <v>2687</v>
+      </c>
+      <c r="F255" s="128"/>
+      <c r="G255" s="128" t="s">
+        <v>2687</v>
+      </c>
+      <c r="H255" t="s">
+        <v>2676</v>
+      </c>
+      <c r="I255" s="19"/>
+      <c r="J255" s="28"/>
+      <c r="K255" s="19"/>
+      <c r="L255" s="129" t="s">
+        <v>496</v>
+      </c>
+      <c r="M255" s="26">
+        <v>0</v>
+      </c>
+      <c r="N255" s="19"/>
+      <c r="O255" s="130" t="s">
+        <v>497</v>
+      </c>
+      <c r="P255" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF255"/>
+      <c r="AI255"/>
+      <c r="AK255"/>
+      <c r="AL255"/>
+    </row>
+    <row r="256" spans="1:38" ht="288">
+      <c r="A256" s="131" t="s">
+        <v>2688</v>
+      </c>
+      <c r="B256" s="26" t="s">
+        <v>481</v>
+      </c>
+      <c r="C256" s="26" t="s">
+        <v>2689</v>
+      </c>
+      <c r="D256" s="131" t="s">
+        <v>2690</v>
+      </c>
+      <c r="E256" s="128" t="s">
+        <v>2691</v>
+      </c>
+      <c r="F256" s="128"/>
+      <c r="G256" s="128" t="s">
+        <v>2691</v>
+      </c>
+      <c r="H256" t="s">
+        <v>2676</v>
+      </c>
+      <c r="I256" s="19"/>
+      <c r="J256" s="28"/>
+      <c r="K256" s="19"/>
+      <c r="L256" s="129" t="s">
+        <v>496</v>
+      </c>
+      <c r="M256" s="26">
+        <v>0</v>
+      </c>
+      <c r="N256" s="19"/>
+      <c r="O256" s="130" t="s">
+        <v>497</v>
+      </c>
+      <c r="P256" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF256"/>
+      <c r="AI256"/>
+      <c r="AK256"/>
+      <c r="AL256"/>
+    </row>
+    <row r="257" spans="1:38" ht="216">
+      <c r="A257" s="132" t="s">
+        <v>2692</v>
+      </c>
+      <c r="B257" s="27" t="s">
+        <v>481</v>
+      </c>
+      <c r="C257" s="27" t="s">
+        <v>2693</v>
+      </c>
+      <c r="D257" s="132" t="s">
+        <v>2694</v>
+      </c>
+      <c r="E257" s="128" t="s">
+        <v>2695</v>
+      </c>
+      <c r="F257" s="128"/>
+      <c r="G257" s="128" t="s">
+        <v>2695</v>
+      </c>
+      <c r="H257" t="s">
+        <v>2676</v>
+      </c>
+      <c r="I257" s="133"/>
+      <c r="J257" s="134"/>
+      <c r="K257" s="133"/>
+      <c r="L257" s="135" t="s">
+        <v>511</v>
+      </c>
+      <c r="M257" s="27">
+        <v>0</v>
+      </c>
+      <c r="N257" s="133"/>
+      <c r="O257" s="130" t="s">
+        <v>497</v>
+      </c>
+      <c r="P257" s="133" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF257"/>
+      <c r="AI257"/>
+      <c r="AK257"/>
+      <c r="AL257"/>
+    </row>
+    <row r="258" spans="1:38">
+      <c r="E258" s="18"/>
+      <c r="F258" s="18"/>
+      <c r="G258" s="18"/>
+      <c r="H258" s="136" t="s">
+        <v>2696</v>
+      </c>
+      <c r="J258" s="23"/>
+      <c r="AF258"/>
+      <c r="AI258"/>
+      <c r="AK258"/>
+      <c r="AL258"/>
+    </row>
+    <row r="259" spans="1:38" ht="43.2">
+      <c r="A259" s="131" t="s">
+        <v>2697</v>
+      </c>
+      <c r="B259" s="26" t="s">
+        <v>481</v>
+      </c>
+      <c r="C259" s="131" t="s">
+        <v>2698</v>
+      </c>
+      <c r="D259" s="131" t="s">
+        <v>2699</v>
+      </c>
+      <c r="E259" s="137" t="s">
+        <v>2700</v>
+      </c>
+      <c r="F259" s="137"/>
+      <c r="G259" s="137" t="s">
+        <v>2700</v>
+      </c>
+      <c r="H259" t="s">
+        <v>2676</v>
+      </c>
+      <c r="I259" s="19"/>
+      <c r="J259" s="28"/>
+      <c r="K259" s="19"/>
+      <c r="L259" s="129" t="s">
+        <v>496</v>
+      </c>
+      <c r="M259" s="26">
+        <v>0</v>
+      </c>
+      <c r="N259" s="19"/>
+      <c r="O259" s="138" t="s">
+        <v>675</v>
+      </c>
+      <c r="P259" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF259"/>
+      <c r="AI259"/>
+      <c r="AK259"/>
+      <c r="AL259"/>
+    </row>
+    <row r="260" spans="1:38" ht="144">
+      <c r="A260" s="131" t="s">
+        <v>2701</v>
+      </c>
+      <c r="B260" s="26" t="s">
+        <v>481</v>
+      </c>
+      <c r="C260" s="129" t="s">
+        <v>2702</v>
+      </c>
+      <c r="D260" s="19" t="s">
+        <v>2703</v>
+      </c>
+      <c r="E260" s="137" t="s">
+        <v>2704</v>
+      </c>
+      <c r="F260" s="48"/>
+      <c r="G260" s="137" t="s">
+        <v>2704</v>
+      </c>
+      <c r="H260" t="s">
+        <v>2676</v>
+      </c>
+      <c r="I260" s="19"/>
+      <c r="J260" s="28"/>
+      <c r="K260" s="19"/>
+      <c r="L260" s="129" t="s">
+        <v>496</v>
+      </c>
+      <c r="M260" s="26">
+        <v>0</v>
+      </c>
+      <c r="N260" s="19"/>
+      <c r="O260" s="138" t="s">
+        <v>497</v>
+      </c>
+      <c r="P260" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF260"/>
+      <c r="AI260"/>
+      <c r="AK260"/>
+      <c r="AL260"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A212:AE212"/>
     <mergeCell ref="A247:AE247"/>
   </mergeCells>
-  <phoneticPr fontId="44" type="noConversion"/>
+  <phoneticPr fontId="45" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D61" r:id="rId1" tooltip="Test Contact 2_INSTITUTION" display="https://navatar-c--tr4sb6.sandbox.lightning.force.com/003DN000001U5JiYAK" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
     <hyperlink ref="D195" r:id="rId2" tooltip="frank" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
@@ -15320,13 +15850,13 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="118" t="s">
+      <c r="A19" s="123" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="118"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="118"/>
-      <c r="E19" s="118"/>
+      <c r="B19" s="123"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="87" t="s">
@@ -15360,11 +15890,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" s="16" customFormat="1">
-      <c r="A25" s="117" t="s">
+      <c r="A25" s="122" t="s">
         <v>2284</v>
       </c>
-      <c r="B25" s="117"/>
-      <c r="C25" s="117"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="122"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
@@ -15604,22 +16134,22 @@
     </row>
     <row r="9" spans="1:15" ht="19.5" customHeight="1"/>
     <row r="10" spans="1:15">
-      <c r="A10" s="120" t="s">
+      <c r="A10" s="125" t="s">
         <v>144</v>
       </c>
-      <c r="B10" s="120"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="120"/>
-      <c r="K10" s="120"/>
-      <c r="L10" s="120"/>
-      <c r="M10" s="120"/>
-      <c r="N10" s="120"/>
+      <c r="B10" s="125"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="125"/>
+      <c r="F10" s="125"/>
+      <c r="G10" s="125"/>
+      <c r="H10" s="125"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="125"/>
+      <c r="K10" s="125"/>
+      <c r="L10" s="125"/>
+      <c r="M10" s="125"/>
+      <c r="N10" s="125"/>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="87" t="s">
@@ -15664,22 +16194,22 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="121" t="s">
+      <c r="A16" s="126" t="s">
         <v>1317</v>
       </c>
-      <c r="B16" s="121"/>
-      <c r="C16" s="121"/>
-      <c r="D16" s="121"/>
-      <c r="E16" s="121"/>
-      <c r="F16" s="121"/>
-      <c r="G16" s="121"/>
-      <c r="H16" s="121"/>
-      <c r="I16" s="121"/>
-      <c r="J16" s="121"/>
-      <c r="K16" s="121"/>
-      <c r="L16" s="121"/>
-      <c r="M16" s="121"/>
-      <c r="N16" s="121"/>
+      <c r="B16" s="126"/>
+      <c r="C16" s="126"/>
+      <c r="D16" s="126"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="126"/>
+      <c r="G16" s="126"/>
+      <c r="H16" s="126"/>
+      <c r="I16" s="126"/>
+      <c r="J16" s="126"/>
+      <c r="K16" s="126"/>
+      <c r="L16" s="126"/>
+      <c r="M16" s="126"/>
+      <c r="N16" s="126"/>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
@@ -15750,11 +16280,11 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="16" customFormat="1">
-      <c r="A25" s="117" t="s">
+      <c r="A25" s="122" t="s">
         <v>2284</v>
       </c>
-      <c r="B25" s="117"/>
-      <c r="C25" s="117"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="122"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="12" t="s">
@@ -15912,7 +16442,7 @@
     <mergeCell ref="A16:N16"/>
     <mergeCell ref="A25:C25"/>
   </mergeCells>
-  <phoneticPr fontId="51" type="noConversion"/>
+  <phoneticPr fontId="52" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -15999,7 +16529,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="53" type="noConversion"/>
+  <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16106,13 +16636,13 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="125" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="120"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
       <c r="F3" s="61"/>
       <c r="G3" s="62"/>
       <c r="H3" s="62"/>
@@ -16339,11 +16869,11 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="122" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -16819,13 +17349,13 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="118" t="s">
+      <c r="A64" s="123" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="118"/>
-      <c r="C64" s="118"/>
-      <c r="D64" s="118"/>
-      <c r="E64" s="118"/>
+      <c r="B64" s="123"/>
+      <c r="C64" s="123"/>
+      <c r="D64" s="123"/>
+      <c r="E64" s="123"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
@@ -16997,13 +17527,13 @@
       <c r="C82" s="87"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="118" t="s">
+      <c r="A85" s="123" t="s">
         <v>160</v>
       </c>
-      <c r="B85" s="118"/>
-      <c r="C85" s="118"/>
-      <c r="D85" s="118"/>
-      <c r="E85" s="118"/>
+      <c r="B85" s="123"/>
+      <c r="C85" s="123"/>
+      <c r="D85" s="123"/>
+      <c r="E85" s="123"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
@@ -17126,11 +17656,11 @@
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="117" t="s">
+      <c r="A101" s="122" t="s">
         <v>2284</v>
       </c>
-      <c r="B101" s="117"/>
-      <c r="C101" s="117"/>
+      <c r="B101" s="122"/>
+      <c r="C101" s="122"/>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
@@ -17365,11 +17895,11 @@
       </c>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="117" t="s">
+      <c r="A125" s="122" t="s">
         <v>2267</v>
       </c>
-      <c r="B125" s="117"/>
-      <c r="C125" s="117"/>
+      <c r="B125" s="122"/>
+      <c r="C125" s="122"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
@@ -17401,7 +17931,7 @@
     <mergeCell ref="A101:C101"/>
     <mergeCell ref="A125:C125"/>
   </mergeCells>
-  <phoneticPr fontId="51" type="noConversion"/>
+  <phoneticPr fontId="52" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300"/>
 </worksheet>
@@ -17430,12 +17960,12 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="123" t="s">
         <v>1347</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
@@ -17580,14 +18110,14 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="122" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -17654,12 +18184,12 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="118" t="s">
+      <c r="A13" s="123" t="s">
         <v>1347</v>
       </c>
-      <c r="B13" s="118"/>
-      <c r="C13" s="118"/>
-      <c r="D13" s="118"/>
+      <c r="B13" s="123"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="123"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="87" t="s">
@@ -17883,10 +18413,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="123" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="118"/>
+      <c r="B3" s="123"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
@@ -18922,17 +19452,17 @@
       <c r="F56" s="2"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="119" t="s">
+      <c r="A58" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="B58" s="119"/>
-      <c r="C58" s="119"/>
-      <c r="D58" s="119"/>
-      <c r="E58" s="119"/>
-      <c r="F58" s="119"/>
-      <c r="G58" s="119"/>
-      <c r="H58" s="119"/>
-      <c r="I58" s="119"/>
+      <c r="B58" s="124"/>
+      <c r="C58" s="124"/>
+      <c r="D58" s="124"/>
+      <c r="E58" s="124"/>
+      <c r="F58" s="124"/>
+      <c r="G58" s="124"/>
+      <c r="H58" s="124"/>
+      <c r="I58" s="124"/>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
@@ -19152,17 +19682,17 @@
       <c r="I76" s="87"/>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="119" t="s">
+      <c r="A80" s="124" t="s">
         <v>338</v>
       </c>
-      <c r="B80" s="119"/>
-      <c r="C80" s="119"/>
-      <c r="D80" s="119"/>
-      <c r="E80" s="119"/>
-      <c r="F80" s="119"/>
-      <c r="G80" s="119"/>
-      <c r="H80" s="119"/>
-      <c r="I80" s="119"/>
+      <c r="B80" s="124"/>
+      <c r="C80" s="124"/>
+      <c r="D80" s="124"/>
+      <c r="E80" s="124"/>
+      <c r="F80" s="124"/>
+      <c r="G80" s="124"/>
+      <c r="H80" s="124"/>
+      <c r="I80" s="124"/>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
@@ -19269,11 +19799,11 @@
       </c>
     </row>
     <row r="96" spans="1:8" s="16" customFormat="1">
-      <c r="A96" s="117" t="s">
+      <c r="A96" s="122" t="s">
         <v>2284</v>
       </c>
-      <c r="B96" s="117"/>
-      <c r="C96" s="117"/>
+      <c r="B96" s="122"/>
+      <c r="C96" s="122"/>
       <c r="H96"/>
     </row>
     <row r="97" spans="1:9">
@@ -19761,11 +20291,11 @@
       </c>
     </row>
     <row r="130" spans="1:7">
-      <c r="A130" s="117" t="s">
+      <c r="A130" s="122" t="s">
         <v>2267</v>
       </c>
-      <c r="B130" s="117"/>
-      <c r="C130" s="117"/>
+      <c r="B130" s="122"/>
+      <c r="C130" s="122"/>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
@@ -19901,7 +20431,7 @@
     <mergeCell ref="A96:C96"/>
     <mergeCell ref="A130:C130"/>
   </mergeCells>
-  <phoneticPr fontId="51" type="noConversion"/>
+  <phoneticPr fontId="52" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
     <hyperlink ref="F8" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
@@ -20254,16 +20784,16 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="118" t="s">
+      <c r="A29" s="123" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="118"/>
-      <c r="C29" s="118"/>
-      <c r="D29" s="118"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="118"/>
-      <c r="H29" s="118"/>
+      <c r="B29" s="123"/>
+      <c r="C29" s="123"/>
+      <c r="D29" s="123"/>
+      <c r="E29" s="123"/>
+      <c r="F29" s="123"/>
+      <c r="G29" s="123"/>
+      <c r="H29" s="123"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="87" t="s">
@@ -20368,7 +20898,7 @@
   <mergeCells count="1">
     <mergeCell ref="A29:H29"/>
   </mergeCells>
-  <phoneticPr fontId="42" type="noConversion"/>
+  <phoneticPr fontId="43" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -22181,11 +22711,11 @@
       </c>
     </row>
     <row r="14" spans="1:6" s="16" customFormat="1">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="122" t="s">
         <v>2284</v>
       </c>
-      <c r="B14" s="117"/>
-      <c r="C14" s="117"/>
+      <c r="B14" s="122"/>
+      <c r="C14" s="122"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
@@ -22773,11 +23303,11 @@
       </c>
       <c r="J5" s="23" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>08/26/2023</v>
+        <v>10/29/2023</v>
       </c>
       <c r="K5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>08/26/2023</v>
+        <v>10/29/2023</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="28.8">
@@ -24610,7 +25140,7 @@
       <c r="H63" s="18"/>
       <c r="J63" s="18"/>
       <c r="K63" s="18"/>
-      <c r="L63" s="122"/>
+      <c r="L63" s="117"/>
       <c r="M63" s="26" t="s">
         <v>706</v>
       </c>
@@ -27763,7 +28293,7 @@
       </c>
     </row>
     <row r="175" spans="1:24">
-      <c r="A175" s="123" t="s">
+      <c r="A175" s="118" t="s">
         <v>2664</v>
       </c>
       <c r="B175" t="s">
@@ -27778,7 +28308,7 @@
       <c r="E175" s="2" t="s">
         <v>2666</v>
       </c>
-      <c r="F175" s="124"/>
+      <c r="F175" s="119"/>
       <c r="G175" s="22"/>
       <c r="J175"/>
       <c r="M175" s="39" t="s">
@@ -27906,27 +28436,27 @@
       <c r="J184"/>
     </row>
     <row r="187" spans="1:20">
-      <c r="A187" s="119" t="s">
+      <c r="A187" s="124" t="s">
         <v>144</v>
       </c>
-      <c r="B187" s="119"/>
-      <c r="C187" s="119"/>
-      <c r="D187" s="119"/>
-      <c r="E187" s="119"/>
-      <c r="F187" s="119"/>
-      <c r="G187" s="119"/>
-      <c r="H187" s="119"/>
-      <c r="I187" s="119"/>
-      <c r="J187" s="119"/>
-      <c r="K187" s="119"/>
-      <c r="L187" s="119"/>
-      <c r="M187" s="119"/>
-      <c r="N187" s="119"/>
-      <c r="O187" s="119"/>
-      <c r="P187" s="119"/>
-      <c r="Q187" s="119"/>
-      <c r="R187" s="119"/>
-      <c r="S187" s="119"/>
+      <c r="B187" s="124"/>
+      <c r="C187" s="124"/>
+      <c r="D187" s="124"/>
+      <c r="E187" s="124"/>
+      <c r="F187" s="124"/>
+      <c r="G187" s="124"/>
+      <c r="H187" s="124"/>
+      <c r="I187" s="124"/>
+      <c r="J187" s="124"/>
+      <c r="K187" s="124"/>
+      <c r="L187" s="124"/>
+      <c r="M187" s="124"/>
+      <c r="N187" s="124"/>
+      <c r="O187" s="124"/>
+      <c r="P187" s="124"/>
+      <c r="Q187" s="124"/>
+      <c r="R187" s="124"/>
+      <c r="S187" s="124"/>
     </row>
     <row r="188" spans="1:20">
       <c r="A188" t="s">
@@ -34576,27 +35106,27 @@
       </c>
     </row>
     <row r="413" spans="1:22">
-      <c r="A413" s="119" t="s">
+      <c r="A413" s="124" t="s">
         <v>160</v>
       </c>
-      <c r="B413" s="119"/>
-      <c r="C413" s="119"/>
-      <c r="D413" s="119"/>
-      <c r="E413" s="119"/>
-      <c r="F413" s="119"/>
-      <c r="G413" s="119"/>
-      <c r="H413" s="119"/>
-      <c r="I413" s="119"/>
-      <c r="J413" s="119"/>
-      <c r="K413" s="119"/>
-      <c r="L413" s="119"/>
-      <c r="M413" s="119"/>
-      <c r="N413" s="119"/>
-      <c r="O413" s="119"/>
-      <c r="P413" s="119"/>
-      <c r="Q413" s="119"/>
-      <c r="R413" s="119"/>
-      <c r="S413" s="119"/>
+      <c r="B413" s="124"/>
+      <c r="C413" s="124"/>
+      <c r="D413" s="124"/>
+      <c r="E413" s="124"/>
+      <c r="F413" s="124"/>
+      <c r="G413" s="124"/>
+      <c r="H413" s="124"/>
+      <c r="I413" s="124"/>
+      <c r="J413" s="124"/>
+      <c r="K413" s="124"/>
+      <c r="L413" s="124"/>
+      <c r="M413" s="124"/>
+      <c r="N413" s="124"/>
+      <c r="O413" s="124"/>
+      <c r="P413" s="124"/>
+      <c r="Q413" s="124"/>
+      <c r="R413" s="124"/>
+      <c r="S413" s="124"/>
     </row>
     <row r="414" spans="1:22" ht="28.8">
       <c r="A414" t="s">
@@ -35135,7 +35665,7 @@
     <mergeCell ref="A187:S187"/>
     <mergeCell ref="A413:S413"/>
   </mergeCells>
-  <phoneticPr fontId="42" type="noConversion"/>
+  <phoneticPr fontId="43" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E449" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
     <hyperlink ref="E423" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>

</xml_diff>

<commit_message>
Megred Acuity Qucik link data sheet of firm contact and label sheet
</commit_message>
<xml_diff>
--- a/AcuityDataSheet.xlsx
+++ b/AcuityDataSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Kumar\git\PE4.7Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C9C226-F587-426C-9425-766E06499B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BB255C-3CB5-4EEE-8459-F542F39B017B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomMetaData" sheetId="15" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5114" uniqueCount="3101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5198" uniqueCount="3160">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -9389,6 +9389,183 @@
   </si>
   <si>
     <t>Advisory Services&lt;break&gt;Capital Raise</t>
+  </si>
+  <si>
+    <t>Acuity Quick Links</t>
+  </si>
+  <si>
+    <t>AQLIns1</t>
+  </si>
+  <si>
+    <t>Test Demo Company 1</t>
+  </si>
+  <si>
+    <t>AQLIns2</t>
+  </si>
+  <si>
+    <t>Test Demo Company 2</t>
+  </si>
+  <si>
+    <t>AQLIns3</t>
+  </si>
+  <si>
+    <t>Test Demo Company 3</t>
+  </si>
+  <si>
+    <t>AQLIns4</t>
+  </si>
+  <si>
+    <t>Test Demo Company 4</t>
+  </si>
+  <si>
+    <t>AQLIns41</t>
+  </si>
+  <si>
+    <t>Test Demo Company 5</t>
+  </si>
+  <si>
+    <t>AQLIns42</t>
+  </si>
+  <si>
+    <t>Test Demo Company 7</t>
+  </si>
+  <si>
+    <t>AQLIns43</t>
+  </si>
+  <si>
+    <t>Test Demo Company 8</t>
+  </si>
+  <si>
+    <t>AQLIns5</t>
+  </si>
+  <si>
+    <t>Demo Company !@#$%^&amp;&amp;&amp;*())))))))_+_)(*&amp;^%$#@!@#$%^&amp;*()(*&amp;^%$#@!</t>
+  </si>
+  <si>
+    <t>AQLIns6</t>
+  </si>
+  <si>
+    <t>Testing Demo Account 1</t>
+  </si>
+  <si>
+    <t>AQLIns7</t>
+  </si>
+  <si>
+    <t>AQLIns8</t>
+  </si>
+  <si>
+    <t>New Demo Company</t>
+  </si>
+  <si>
+    <t>AQLContact1</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Kristian</t>
+  </si>
+  <si>
+    <t>Testdemoinstitution1@gmail.com</t>
+  </si>
+  <si>
+    <t>AQLContact2</t>
+  </si>
+  <si>
+    <t>Kristian !@#$%^&amp;&amp;&amp;*())))))))_+_)(*&amp;^%$#@!@#$%^&amp;*()(*&amp;^%$#@!</t>
+  </si>
+  <si>
+    <t>AQLContact3</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Tye</t>
+  </si>
+  <si>
+    <t>andrewtyedemo@gmail.com</t>
+  </si>
+  <si>
+    <t>AQLContact4</t>
+  </si>
+  <si>
+    <t>Mathew</t>
+  </si>
+  <si>
+    <t>Hayden</t>
+  </si>
+  <si>
+    <t>mathewhaydendemogmail.com</t>
+  </si>
+  <si>
+    <t>AQLContact5</t>
+  </si>
+  <si>
+    <t>Haydengergrsegogegergegetgrthyjthtjyktyk</t>
+  </si>
+  <si>
+    <t>mathewhaydendemo@gmail.com</t>
+  </si>
+  <si>
+    <t>AQLContact6</t>
+  </si>
+  <si>
+    <t>Shane</t>
+  </si>
+  <si>
+    <t>Watson</t>
+  </si>
+  <si>
+    <t>shanewatsondemo@gmail.com</t>
+  </si>
+  <si>
+    <t>AQLContact7</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Marsh</t>
+  </si>
+  <si>
+    <t>AQLContact8</t>
+  </si>
+  <si>
+    <t>AQLContact9</t>
+  </si>
+  <si>
+    <t>Aston</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>AQ_AccountLabel01</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>AQ_AccountLabel02</t>
+  </si>
+  <si>
+    <t>Phone number validation</t>
+  </si>
+  <si>
+    <t>AQ_AccountLabel03</t>
+  </si>
+  <si>
+    <t>LEN(SUBSTITUTE(Phone, ' ', NULL)) &gt;= 10</t>
+  </si>
+  <si>
+    <t>AQ_AccountLabel04</t>
+  </si>
+  <si>
+    <t>Mobile number should not more than 10 digit</t>
+  </si>
+  <si>
+    <t>AQ_AccountLabel05</t>
   </si>
 </sst>
 </file>
@@ -9977,7 +10154,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="40" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -10232,13 +10409,20 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="40" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
@@ -10247,13 +10431,11 @@
     <xf numFmtId="0" fontId="42" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10538,7 +10720,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -10947,11 +11129,11 @@
       </c>
     </row>
     <row r="35" spans="1:12" s="16" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A35" s="136" t="s">
+      <c r="A35" s="137" t="s">
         <v>2163</v>
       </c>
-      <c r="B35" s="136"/>
-      <c r="C35" s="136"/>
+      <c r="B35" s="137"/>
+      <c r="C35" s="137"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" t="s">
@@ -16322,39 +16504,39 @@
       </c>
     </row>
     <row r="212" spans="1:31">
-      <c r="A212" s="138" t="s">
+      <c r="A212" s="140" t="s">
         <v>144</v>
       </c>
-      <c r="B212" s="138"/>
-      <c r="C212" s="138"/>
-      <c r="D212" s="138"/>
-      <c r="E212" s="138"/>
-      <c r="F212" s="138"/>
-      <c r="G212" s="138"/>
-      <c r="H212" s="138"/>
-      <c r="I212" s="138"/>
-      <c r="J212" s="138"/>
-      <c r="K212" s="138"/>
-      <c r="L212" s="138"/>
-      <c r="M212" s="138"/>
-      <c r="N212" s="138"/>
-      <c r="O212" s="138"/>
-      <c r="P212" s="138"/>
-      <c r="Q212" s="138"/>
-      <c r="R212" s="138"/>
-      <c r="S212" s="138"/>
-      <c r="T212" s="138"/>
-      <c r="U212" s="138"/>
-      <c r="V212" s="138"/>
-      <c r="W212" s="138"/>
-      <c r="X212" s="138"/>
-      <c r="Y212" s="138"/>
-      <c r="Z212" s="138"/>
-      <c r="AA212" s="138"/>
-      <c r="AB212" s="138"/>
-      <c r="AC212" s="138"/>
-      <c r="AD212" s="138"/>
-      <c r="AE212" s="138"/>
+      <c r="B212" s="140"/>
+      <c r="C212" s="140"/>
+      <c r="D212" s="140"/>
+      <c r="E212" s="140"/>
+      <c r="F212" s="140"/>
+      <c r="G212" s="140"/>
+      <c r="H212" s="140"/>
+      <c r="I212" s="140"/>
+      <c r="J212" s="140"/>
+      <c r="K212" s="140"/>
+      <c r="L212" s="140"/>
+      <c r="M212" s="140"/>
+      <c r="N212" s="140"/>
+      <c r="O212" s="140"/>
+      <c r="P212" s="140"/>
+      <c r="Q212" s="140"/>
+      <c r="R212" s="140"/>
+      <c r="S212" s="140"/>
+      <c r="T212" s="140"/>
+      <c r="U212" s="140"/>
+      <c r="V212" s="140"/>
+      <c r="W212" s="140"/>
+      <c r="X212" s="140"/>
+      <c r="Y212" s="140"/>
+      <c r="Z212" s="140"/>
+      <c r="AA212" s="140"/>
+      <c r="AB212" s="140"/>
+      <c r="AC212" s="140"/>
+      <c r="AD212" s="140"/>
+      <c r="AE212" s="140"/>
     </row>
     <row r="213" spans="1:31">
       <c r="A213" t="s">
@@ -16617,39 +16799,39 @@
       </c>
     </row>
     <row r="247" spans="1:38">
-      <c r="A247" s="138" t="s">
+      <c r="A247" s="140" t="s">
         <v>144</v>
       </c>
-      <c r="B247" s="138"/>
-      <c r="C247" s="138"/>
-      <c r="D247" s="138"/>
-      <c r="E247" s="138"/>
-      <c r="F247" s="138"/>
-      <c r="G247" s="138"/>
-      <c r="H247" s="138"/>
-      <c r="I247" s="138"/>
-      <c r="J247" s="138"/>
-      <c r="K247" s="138"/>
-      <c r="L247" s="138"/>
-      <c r="M247" s="138"/>
-      <c r="N247" s="138"/>
-      <c r="O247" s="138"/>
-      <c r="P247" s="138"/>
-      <c r="Q247" s="138"/>
-      <c r="R247" s="138"/>
-      <c r="S247" s="138"/>
-      <c r="T247" s="138"/>
-      <c r="U247" s="138"/>
-      <c r="V247" s="138"/>
-      <c r="W247" s="138"/>
-      <c r="X247" s="138"/>
-      <c r="Y247" s="138"/>
-      <c r="Z247" s="138"/>
-      <c r="AA247" s="138"/>
-      <c r="AB247" s="138"/>
-      <c r="AC247" s="138"/>
-      <c r="AD247" s="138"/>
-      <c r="AE247" s="138"/>
+      <c r="B247" s="140"/>
+      <c r="C247" s="140"/>
+      <c r="D247" s="140"/>
+      <c r="E247" s="140"/>
+      <c r="F247" s="140"/>
+      <c r="G247" s="140"/>
+      <c r="H247" s="140"/>
+      <c r="I247" s="140"/>
+      <c r="J247" s="140"/>
+      <c r="K247" s="140"/>
+      <c r="L247" s="140"/>
+      <c r="M247" s="140"/>
+      <c r="N247" s="140"/>
+      <c r="O247" s="140"/>
+      <c r="P247" s="140"/>
+      <c r="Q247" s="140"/>
+      <c r="R247" s="140"/>
+      <c r="S247" s="140"/>
+      <c r="T247" s="140"/>
+      <c r="U247" s="140"/>
+      <c r="V247" s="140"/>
+      <c r="W247" s="140"/>
+      <c r="X247" s="140"/>
+      <c r="Y247" s="140"/>
+      <c r="Z247" s="140"/>
+      <c r="AA247" s="140"/>
+      <c r="AB247" s="140"/>
+      <c r="AC247" s="140"/>
+      <c r="AD247" s="140"/>
+      <c r="AE247" s="140"/>
     </row>
     <row r="248" spans="1:38">
       <c r="A248" t="s">
@@ -17083,8 +17265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -17124,26 +17306,26 @@
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="141" t="s">
+      <c r="A9" s="138" t="s">
         <v>2717</v>
       </c>
-      <c r="B9" s="141"/>
-      <c r="C9" s="141"/>
-      <c r="D9" s="141"/>
-      <c r="E9" s="141"/>
-      <c r="F9" s="141"/>
-      <c r="G9" s="141"/>
-      <c r="H9" s="141"/>
-      <c r="I9" s="141"/>
-      <c r="J9" s="141"/>
-      <c r="K9" s="141"/>
-      <c r="L9" s="141"/>
-      <c r="M9" s="141"/>
-      <c r="N9" s="141"/>
-      <c r="O9" s="141"/>
-      <c r="P9" s="141"/>
-      <c r="Q9" s="141"/>
-      <c r="R9" s="141"/>
+      <c r="B9" s="138"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="138"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="138"/>
+      <c r="J9" s="138"/>
+      <c r="K9" s="138"/>
+      <c r="L9" s="138"/>
+      <c r="M9" s="138"/>
+      <c r="N9" s="138"/>
+      <c r="O9" s="138"/>
+      <c r="P9" s="138"/>
+      <c r="Q9" s="138"/>
+      <c r="R9" s="138"/>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
@@ -17979,7 +18161,7 @@
       <c r="A98" t="s">
         <v>3037</v>
       </c>
-      <c r="S98" s="143" t="s">
+      <c r="S98" s="136" t="s">
         <v>3038</v>
       </c>
     </row>
@@ -18216,12 +18398,12 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="141" t="s">
+      <c r="A2" s="138" t="s">
         <v>2717</v>
       </c>
-      <c r="B2" s="141"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="12" t="s">
@@ -18538,13 +18720,13 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="137" t="s">
+      <c r="A19" s="139" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="137"/>
-      <c r="C19" s="137"/>
-      <c r="D19" s="137"/>
-      <c r="E19" s="137"/>
+      <c r="B19" s="139"/>
+      <c r="C19" s="139"/>
+      <c r="D19" s="139"/>
+      <c r="E19" s="139"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="86" t="s">
@@ -18578,11 +18760,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" s="16" customFormat="1">
-      <c r="A25" s="136" t="s">
+      <c r="A25" s="137" t="s">
         <v>2180</v>
       </c>
-      <c r="B25" s="136"/>
-      <c r="C25" s="136"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="137"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
@@ -18822,22 +19004,22 @@
     </row>
     <row r="9" spans="1:15" ht="19.5" customHeight="1"/>
     <row r="10" spans="1:15">
-      <c r="A10" s="139" t="s">
+      <c r="A10" s="142" t="s">
         <v>144</v>
       </c>
-      <c r="B10" s="139"/>
-      <c r="C10" s="139"/>
-      <c r="D10" s="139"/>
-      <c r="E10" s="139"/>
-      <c r="F10" s="139"/>
-      <c r="G10" s="139"/>
-      <c r="H10" s="139"/>
-      <c r="I10" s="139"/>
-      <c r="J10" s="139"/>
-      <c r="K10" s="139"/>
-      <c r="L10" s="139"/>
-      <c r="M10" s="139"/>
-      <c r="N10" s="139"/>
+      <c r="B10" s="142"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
+      <c r="F10" s="142"/>
+      <c r="G10" s="142"/>
+      <c r="H10" s="142"/>
+      <c r="I10" s="142"/>
+      <c r="J10" s="142"/>
+      <c r="K10" s="142"/>
+      <c r="L10" s="142"/>
+      <c r="M10" s="142"/>
+      <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="86" t="s">
@@ -18882,22 +19064,22 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="140" t="s">
+      <c r="A16" s="143" t="s">
         <v>1241</v>
       </c>
-      <c r="B16" s="140"/>
-      <c r="C16" s="140"/>
-      <c r="D16" s="140"/>
-      <c r="E16" s="140"/>
-      <c r="F16" s="140"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="140"/>
-      <c r="I16" s="140"/>
-      <c r="J16" s="140"/>
-      <c r="K16" s="140"/>
-      <c r="L16" s="140"/>
-      <c r="M16" s="140"/>
-      <c r="N16" s="140"/>
+      <c r="B16" s="143"/>
+      <c r="C16" s="143"/>
+      <c r="D16" s="143"/>
+      <c r="E16" s="143"/>
+      <c r="F16" s="143"/>
+      <c r="G16" s="143"/>
+      <c r="H16" s="143"/>
+      <c r="I16" s="143"/>
+      <c r="J16" s="143"/>
+      <c r="K16" s="143"/>
+      <c r="L16" s="143"/>
+      <c r="M16" s="143"/>
+      <c r="N16" s="143"/>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
@@ -18968,11 +19150,11 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="16" customFormat="1">
-      <c r="A25" s="136" t="s">
+      <c r="A25" s="137" t="s">
         <v>2180</v>
       </c>
-      <c r="B25" s="136"/>
-      <c r="C25" s="136"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="137"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="12" t="s">
@@ -19324,13 +19506,13 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="142" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="139"/>
-      <c r="C3" s="139"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="139"/>
+      <c r="B3" s="142"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
       <c r="F3" s="61"/>
       <c r="G3" s="62"/>
       <c r="H3" s="62"/>
@@ -19365,11 +19547,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A130" sqref="A130:XFD140"/>
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -19402,11 +19584,11 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="137" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="136"/>
-      <c r="C3" s="136"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -19882,13 +20064,13 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="137" t="s">
+      <c r="A64" s="139" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="137"/>
-      <c r="C64" s="137"/>
-      <c r="D64" s="137"/>
-      <c r="E64" s="137"/>
+      <c r="B64" s="139"/>
+      <c r="C64" s="139"/>
+      <c r="D64" s="139"/>
+      <c r="E64" s="139"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
@@ -20060,13 +20242,13 @@
       <c r="C82" s="86"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="137" t="s">
+      <c r="A85" s="139" t="s">
         <v>159</v>
       </c>
-      <c r="B85" s="137"/>
-      <c r="C85" s="137"/>
-      <c r="D85" s="137"/>
-      <c r="E85" s="137"/>
+      <c r="B85" s="139"/>
+      <c r="C85" s="139"/>
+      <c r="D85" s="139"/>
+      <c r="E85" s="139"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
@@ -20189,11 +20371,11 @@
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="136" t="s">
+      <c r="A101" s="137" t="s">
         <v>2180</v>
       </c>
-      <c r="B101" s="136"/>
-      <c r="C101" s="136"/>
+      <c r="B101" s="137"/>
+      <c r="C101" s="137"/>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
@@ -20428,11 +20610,11 @@
       </c>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="136" t="s">
+      <c r="A125" s="137" t="s">
         <v>2163</v>
       </c>
-      <c r="B125" s="136"/>
-      <c r="C125" s="136"/>
+      <c r="B125" s="137"/>
+      <c r="C125" s="137"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
@@ -20457,17 +20639,17 @@
       </c>
     </row>
     <row r="130" spans="1:9">
-      <c r="A130" s="141" t="s">
+      <c r="A130" s="138" t="s">
         <v>2717</v>
       </c>
-      <c r="B130" s="141"/>
-      <c r="C130" s="141"/>
-      <c r="D130" s="141"/>
-      <c r="E130" s="141"/>
-      <c r="F130" s="141"/>
-      <c r="G130" s="141"/>
-      <c r="H130" s="141"/>
-      <c r="I130" s="141"/>
+      <c r="B130" s="138"/>
+      <c r="C130" s="138"/>
+      <c r="D130" s="138"/>
+      <c r="E130" s="138"/>
+      <c r="F130" s="138"/>
+      <c r="G130" s="138"/>
+      <c r="H130" s="138"/>
+      <c r="I130" s="138"/>
     </row>
     <row r="132" spans="1:9">
       <c r="A132" t="s">
@@ -20541,8 +20723,134 @@
         <v>2820</v>
       </c>
     </row>
+    <row r="142" spans="1:9">
+      <c r="A142" s="137" t="s">
+        <v>3101</v>
+      </c>
+      <c r="B142" s="137"/>
+      <c r="C142" s="137"/>
+    </row>
+    <row r="143" spans="1:9">
+      <c r="A143" t="s">
+        <v>3102</v>
+      </c>
+      <c r="B143" s="144" t="s">
+        <v>3103</v>
+      </c>
+      <c r="C143" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
+      <c r="A144" t="s">
+        <v>3104</v>
+      </c>
+      <c r="B144" t="s">
+        <v>3105</v>
+      </c>
+      <c r="C144" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
+        <v>3106</v>
+      </c>
+      <c r="B145" s="144" t="s">
+        <v>3107</v>
+      </c>
+      <c r="C145" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>3108</v>
+      </c>
+      <c r="B146" t="s">
+        <v>3109</v>
+      </c>
+      <c r="C146" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
+        <v>3110</v>
+      </c>
+      <c r="B147" t="s">
+        <v>3111</v>
+      </c>
+      <c r="C147" t="s">
+        <v>2191</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
+        <v>3112</v>
+      </c>
+      <c r="B148" t="s">
+        <v>3113</v>
+      </c>
+      <c r="C148" t="s">
+        <v>2197</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="s">
+        <v>3114</v>
+      </c>
+      <c r="B149" t="s">
+        <v>3115</v>
+      </c>
+      <c r="C149" t="s">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="s">
+        <v>3116</v>
+      </c>
+      <c r="B150" t="s">
+        <v>3117</v>
+      </c>
+      <c r="C150" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B151" t="s">
+        <v>3119</v>
+      </c>
+      <c r="C151" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
+        <v>3120</v>
+      </c>
+      <c r="B152" t="s">
+        <v>3119</v>
+      </c>
+      <c r="C152" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
+        <v>3121</v>
+      </c>
+      <c r="C153" t="s">
+        <v>3122</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A142:C142"/>
     <mergeCell ref="A130:I130"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A64:E64"/>
@@ -20713,10 +21021,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -20734,12 +21042,12 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="139" t="s">
         <v>1271</v>
       </c>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
@@ -20837,7 +21145,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>1286</v>
       </c>
@@ -20845,7 +21153,7 @@
         <v>2714</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:4">
       <c r="A18" s="86" t="s">
         <v>1956</v>
       </c>
@@ -20853,9 +21161,58 @@
         <v>1940</v>
       </c>
     </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="146" t="s">
+        <v>3101</v>
+      </c>
+      <c r="B20" s="139"/>
+      <c r="C20" s="139"/>
+      <c r="D20" s="139"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="145" t="s">
+        <v>3151</v>
+      </c>
+      <c r="B21" s="145" t="s">
+        <v>3152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="145" t="s">
+        <v>3153</v>
+      </c>
+      <c r="B22" s="145" t="s">
+        <v>3154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="145" t="s">
+        <v>3155</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="145" t="s">
+        <v>3157</v>
+      </c>
+      <c r="B24" s="145" t="s">
+        <v>3158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="145" t="s">
+        <v>3159</v>
+      </c>
+      <c r="B25" s="145" t="s">
+        <v>1569</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20884,14 +21241,14 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="137" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="136"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="136"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -20958,12 +21315,12 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="137" t="s">
+      <c r="A13" s="139" t="s">
         <v>1271</v>
       </c>
-      <c r="B13" s="137"/>
-      <c r="C13" s="137"/>
-      <c r="D13" s="137"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="139"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="86" t="s">
@@ -21187,10 +21544,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="139" t="s">
         <v>177</v>
       </c>
-      <c r="B3" s="137"/>
+      <c r="B3" s="139"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
@@ -21438,11 +21795,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:N147"/>
+  <dimension ref="A1:N159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A142" sqref="A142:XFD147"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -22226,17 +22583,17 @@
       <c r="F56" s="2"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="138" t="s">
+      <c r="A58" s="140" t="s">
         <v>144</v>
       </c>
-      <c r="B58" s="138"/>
-      <c r="C58" s="138"/>
-      <c r="D58" s="138"/>
-      <c r="E58" s="138"/>
-      <c r="F58" s="138"/>
-      <c r="G58" s="138"/>
-      <c r="H58" s="138"/>
-      <c r="I58" s="138"/>
+      <c r="B58" s="140"/>
+      <c r="C58" s="140"/>
+      <c r="D58" s="140"/>
+      <c r="E58" s="140"/>
+      <c r="F58" s="140"/>
+      <c r="G58" s="140"/>
+      <c r="H58" s="140"/>
+      <c r="I58" s="140"/>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
@@ -22456,17 +22813,17 @@
       <c r="I76" s="86"/>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="138" t="s">
+      <c r="A80" s="140" t="s">
         <v>334</v>
       </c>
-      <c r="B80" s="138"/>
-      <c r="C80" s="138"/>
-      <c r="D80" s="138"/>
-      <c r="E80" s="138"/>
-      <c r="F80" s="138"/>
-      <c r="G80" s="138"/>
-      <c r="H80" s="138"/>
-      <c r="I80" s="138"/>
+      <c r="B80" s="140"/>
+      <c r="C80" s="140"/>
+      <c r="D80" s="140"/>
+      <c r="E80" s="140"/>
+      <c r="F80" s="140"/>
+      <c r="G80" s="140"/>
+      <c r="H80" s="140"/>
+      <c r="I80" s="140"/>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
@@ -22573,11 +22930,11 @@
       </c>
     </row>
     <row r="96" spans="1:8" s="16" customFormat="1">
-      <c r="A96" s="136" t="s">
+      <c r="A96" s="137" t="s">
         <v>2180</v>
       </c>
-      <c r="B96" s="136"/>
-      <c r="C96" s="136"/>
+      <c r="B96" s="137"/>
+      <c r="C96" s="137"/>
       <c r="H96"/>
     </row>
     <row r="97" spans="1:9">
@@ -23065,11 +23422,11 @@
       </c>
     </row>
     <row r="130" spans="1:7">
-      <c r="A130" s="136" t="s">
+      <c r="A130" s="137" t="s">
         <v>2163</v>
       </c>
-      <c r="B130" s="136"/>
-      <c r="C130" s="136"/>
+      <c r="B130" s="137"/>
+      <c r="C130" s="137"/>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
@@ -23199,11 +23556,11 @@
       </c>
     </row>
     <row r="142" spans="1:7">
-      <c r="A142" s="136" t="s">
+      <c r="A142" s="137" t="s">
         <v>2717</v>
       </c>
-      <c r="B142" s="136"/>
-      <c r="C142" s="136"/>
+      <c r="B142" s="137"/>
+      <c r="C142" s="137"/>
     </row>
     <row r="144" spans="1:7">
       <c r="A144" t="s">
@@ -23213,7 +23570,7 @@
         <v>2822</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:9">
       <c r="A145" t="s">
         <v>2823</v>
       </c>
@@ -23221,7 +23578,7 @@
         <v>2824</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:9">
       <c r="A146" t="s">
         <v>2825</v>
       </c>
@@ -23229,13 +23586,184 @@
         <v>2826</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:9">
       <c r="A147" t="s">
         <v>2827</v>
       </c>
     </row>
+    <row r="150" spans="1:9">
+      <c r="A150" s="137" t="s">
+        <v>3101</v>
+      </c>
+      <c r="B150" s="137"/>
+      <c r="C150" s="137"/>
+      <c r="D150" s="16"/>
+      <c r="E150" s="16"/>
+      <c r="F150" s="16"/>
+      <c r="G150" s="16"/>
+      <c r="H150" s="16"/>
+      <c r="I150" s="16"/>
+    </row>
+    <row r="151" spans="1:9">
+      <c r="A151" s="145" t="s">
+        <v>3123</v>
+      </c>
+      <c r="B151" s="145" t="s">
+        <v>3124</v>
+      </c>
+      <c r="C151" s="145" t="s">
+        <v>3125</v>
+      </c>
+      <c r="D151" t="str">
+        <f>_xlfn.CONCAT(B151," ",C151)</f>
+        <v>Daniel Kristian</v>
+      </c>
+      <c r="E151" s="144" t="s">
+        <v>3103</v>
+      </c>
+      <c r="F151" t="s">
+        <v>3126</v>
+      </c>
+      <c r="H151">
+        <v>8979151245</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9">
+      <c r="A152" s="145" t="s">
+        <v>3127</v>
+      </c>
+      <c r="B152" s="145" t="s">
+        <v>3124</v>
+      </c>
+      <c r="C152" t="s">
+        <v>3128</v>
+      </c>
+      <c r="E152" s="144" t="s">
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9">
+      <c r="A153" s="145" t="s">
+        <v>3129</v>
+      </c>
+      <c r="B153" t="s">
+        <v>3130</v>
+      </c>
+      <c r="C153" s="145" t="s">
+        <v>3131</v>
+      </c>
+      <c r="F153" t="s">
+        <v>3132</v>
+      </c>
+      <c r="H153">
+        <v>8979161289</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9">
+      <c r="A154" s="145" t="s">
+        <v>3133</v>
+      </c>
+      <c r="B154" t="s">
+        <v>3134</v>
+      </c>
+      <c r="C154" t="s">
+        <v>3135</v>
+      </c>
+      <c r="E154" s="144" t="s">
+        <v>3103</v>
+      </c>
+      <c r="F154" t="s">
+        <v>3136</v>
+      </c>
+      <c r="H154">
+        <v>8802654738</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
+      <c r="A155" s="145" t="s">
+        <v>3137</v>
+      </c>
+      <c r="B155" s="145" t="s">
+        <v>3134</v>
+      </c>
+      <c r="C155" t="s">
+        <v>3138</v>
+      </c>
+      <c r="E155" s="144" t="s">
+        <v>3103</v>
+      </c>
+      <c r="F155" t="s">
+        <v>3139</v>
+      </c>
+      <c r="H155">
+        <v>8802654738</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9">
+      <c r="A156" s="145" t="s">
+        <v>3140</v>
+      </c>
+      <c r="B156" t="s">
+        <v>3141</v>
+      </c>
+      <c r="C156" s="145" t="s">
+        <v>3142</v>
+      </c>
+      <c r="E156" t="s">
+        <v>3105</v>
+      </c>
+      <c r="F156" s="102" t="s">
+        <v>3143</v>
+      </c>
+      <c r="H156">
+        <v>8979161267</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
+      <c r="A157" s="145" t="s">
+        <v>3144</v>
+      </c>
+      <c r="B157" t="s">
+        <v>3145</v>
+      </c>
+      <c r="C157" t="s">
+        <v>3146</v>
+      </c>
+      <c r="E157" s="144" t="s">
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
+      <c r="A158" s="145" t="s">
+        <v>3147</v>
+      </c>
+      <c r="B158" t="s">
+        <v>3145</v>
+      </c>
+      <c r="C158" t="s">
+        <v>3146</v>
+      </c>
+      <c r="E158" s="144" t="s">
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="A159" s="145" t="s">
+        <v>3148</v>
+      </c>
+      <c r="B159" t="s">
+        <v>3149</v>
+      </c>
+      <c r="C159" t="s">
+        <v>3150</v>
+      </c>
+      <c r="H159">
+        <v>89791612345</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A150:C150"/>
     <mergeCell ref="A58:I58"/>
     <mergeCell ref="A80:I80"/>
     <mergeCell ref="A96:C96"/>
@@ -23595,16 +24123,16 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="137" t="s">
+      <c r="A29" s="139" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="137"/>
-      <c r="C29" s="137"/>
-      <c r="D29" s="137"/>
-      <c r="E29" s="137"/>
-      <c r="F29" s="137"/>
-      <c r="G29" s="137"/>
-      <c r="H29" s="137"/>
+      <c r="B29" s="139"/>
+      <c r="C29" s="139"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="139"/>
+      <c r="H29" s="139"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="86" t="s">
@@ -23706,17 +24234,17 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="142" t="s">
+      <c r="A46" s="141" t="s">
         <v>2717</v>
       </c>
-      <c r="B46" s="142"/>
-      <c r="C46" s="142"/>
-      <c r="D46" s="142"/>
-      <c r="E46" s="142"/>
-      <c r="F46" s="142"/>
-      <c r="G46" s="142"/>
-      <c r="H46" s="142"/>
-      <c r="I46" s="142"/>
+      <c r="B46" s="141"/>
+      <c r="C46" s="141"/>
+      <c r="D46" s="141"/>
+      <c r="E46" s="141"/>
+      <c r="F46" s="141"/>
+      <c r="G46" s="141"/>
+      <c r="H46" s="141"/>
+      <c r="I46" s="141"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
@@ -25555,11 +26083,11 @@
       </c>
     </row>
     <row r="14" spans="1:6" s="16" customFormat="1">
-      <c r="A14" s="136" t="s">
+      <c r="A14" s="137" t="s">
         <v>2180</v>
       </c>
-      <c r="B14" s="136"/>
-      <c r="C14" s="136"/>
+      <c r="B14" s="137"/>
+      <c r="C14" s="137"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
@@ -26147,11 +26675,11 @@
       </c>
       <c r="J5" s="23" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>12/16/2023</v>
+        <v>01/07/2024</v>
       </c>
       <c r="K5" t="str">
         <f ca="1">TEXT(TODAY()+25,"mm/dd/yyyy")</f>
-        <v>12/16/2023</v>
+        <v>01/07/2024</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="28.8">
@@ -31280,27 +31808,27 @@
       <c r="J184"/>
     </row>
     <row r="187" spans="1:20">
-      <c r="A187" s="138" t="s">
+      <c r="A187" s="140" t="s">
         <v>144</v>
       </c>
-      <c r="B187" s="138"/>
-      <c r="C187" s="138"/>
-      <c r="D187" s="138"/>
-      <c r="E187" s="138"/>
-      <c r="F187" s="138"/>
-      <c r="G187" s="138"/>
-      <c r="H187" s="138"/>
-      <c r="I187" s="138"/>
-      <c r="J187" s="138"/>
-      <c r="K187" s="138"/>
-      <c r="L187" s="138"/>
-      <c r="M187" s="138"/>
-      <c r="N187" s="138"/>
-      <c r="O187" s="138"/>
-      <c r="P187" s="138"/>
-      <c r="Q187" s="138"/>
-      <c r="R187" s="138"/>
-      <c r="S187" s="138"/>
+      <c r="B187" s="140"/>
+      <c r="C187" s="140"/>
+      <c r="D187" s="140"/>
+      <c r="E187" s="140"/>
+      <c r="F187" s="140"/>
+      <c r="G187" s="140"/>
+      <c r="H187" s="140"/>
+      <c r="I187" s="140"/>
+      <c r="J187" s="140"/>
+      <c r="K187" s="140"/>
+      <c r="L187" s="140"/>
+      <c r="M187" s="140"/>
+      <c r="N187" s="140"/>
+      <c r="O187" s="140"/>
+      <c r="P187" s="140"/>
+      <c r="Q187" s="140"/>
+      <c r="R187" s="140"/>
+      <c r="S187" s="140"/>
     </row>
     <row r="188" spans="1:20">
       <c r="A188" t="s">
@@ -37950,27 +38478,27 @@
       </c>
     </row>
     <row r="413" spans="1:22">
-      <c r="A413" s="138" t="s">
+      <c r="A413" s="140" t="s">
         <v>159</v>
       </c>
-      <c r="B413" s="138"/>
-      <c r="C413" s="138"/>
-      <c r="D413" s="138"/>
-      <c r="E413" s="138"/>
-      <c r="F413" s="138"/>
-      <c r="G413" s="138"/>
-      <c r="H413" s="138"/>
-      <c r="I413" s="138"/>
-      <c r="J413" s="138"/>
-      <c r="K413" s="138"/>
-      <c r="L413" s="138"/>
-      <c r="M413" s="138"/>
-      <c r="N413" s="138"/>
-      <c r="O413" s="138"/>
-      <c r="P413" s="138"/>
-      <c r="Q413" s="138"/>
-      <c r="R413" s="138"/>
-      <c r="S413" s="138"/>
+      <c r="B413" s="140"/>
+      <c r="C413" s="140"/>
+      <c r="D413" s="140"/>
+      <c r="E413" s="140"/>
+      <c r="F413" s="140"/>
+      <c r="G413" s="140"/>
+      <c r="H413" s="140"/>
+      <c r="I413" s="140"/>
+      <c r="J413" s="140"/>
+      <c r="K413" s="140"/>
+      <c r="L413" s="140"/>
+      <c r="M413" s="140"/>
+      <c r="N413" s="140"/>
+      <c r="O413" s="140"/>
+      <c r="P413" s="140"/>
+      <c r="Q413" s="140"/>
+      <c r="R413" s="140"/>
+      <c r="S413" s="140"/>
     </row>
     <row r="414" spans="1:22" ht="28.8">
       <c r="A414" t="s">

</xml_diff>